<commit_message>
build up to wk3
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
   <si>
     <t>Finals Week</t>
   </si>
@@ -66,14 +66,7 @@
     <t>Topics</t>
   </si>
   <si>
-    <t>* Orientation to the class
-* QFT walk-through</t>
-  </si>
-  <si>
     <t>New tools,  Projects &amp;  Data Prep, Multiple Regression</t>
-  </si>
-  <si>
-    <t>Model Building, Moderation, Interactions</t>
   </si>
   <si>
     <t>* Fit and interpret models with categorical predictors
@@ -82,26 +75,6 @@
 * Fit and interpret an interaction model</t>
   </si>
   <si>
-    <t xml:space="preserve">* Join the #introductions, #assignments and #classwork Slack channels. 
-* Introduce yourself to the class (who/year/major/non-stat interests)
-* 2-3 min video Project Proposal. Post link to YouTube in #projects channel by Friday EOD. </t>
-  </si>
-  <si>
-    <t>* QFT on Model Building
-* Categorical variables</t>
-  </si>
-  <si>
-    <t>* Moderation and stratification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Adding interaction terms into the model
-* How to compare between models
-</t>
-  </si>
-  <si>
-    <t>* Multiple Regression (Notebook ch 2)</t>
-  </si>
-  <si>
     <t>* Learn how to develop good questions
 * Get connected with modern collaboration tools
 * Review data preparation methods
@@ -116,28 +89,7 @@
 * Data preparation (Notebook Ch 1)</t>
   </si>
   <si>
-    <t>* Identify confounding factors
-* Use model fit statistics to compare between competing models
-* Identify a handful of problems that can creep up when building a model</t>
-  </si>
-  <si>
-    <t>Confounding &amp; Variable Selection, Model Selection &amp;  Special Considerations</t>
-  </si>
-  <si>
-    <t>* Open work day</t>
-  </si>
-  <si>
     <t>* Model building homework (Due 2/11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Watch project proposals videos and fill out [this survey]() to report who you want to work with. </t>
-  </si>
-  <si>
-    <t>* Identifying confounding effects in the model building process
-* Comparing between models, and deciding when enough is enough and just stop tweaking the model!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* All the things that can show up to grief you during model building. </t>
   </si>
   <si>
     <t>* [Notebook Ch 3](https://norcalbiostat.github.io/MATH456_notes/model-building)</t>
@@ -218,101 +170,187 @@
     <t>Factor Analysis, , Cluster Analysis</t>
   </si>
   <si>
-    <t xml:space="preserve">* Join our Slack Channel
-* Install the Slack phone app
+    <t>Project Updates (use R Studio to make a X min presentation)</t>
+  </si>
+  <si>
+    <t>* Project Update Presentations (Mon)
+* Exam 1 (Fri)</t>
+  </si>
+  <si>
+    <t>* Project Update Presentations (Fri)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time Series, Spatial Modeling, </t>
+  </si>
+  <si>
+    <t>Correlated Data,  Random Intercept Models,</t>
+  </si>
+  <si>
+    <t>Missing Data Identification, Multiple Imputation, MICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Install the `mice` package. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Take Home Final distributed by Wed EOD. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'll answer questions about the final exam, otherwise the period is yours to work on the exam, projects, or any remaining homework. </t>
+  </si>
+  <si>
+    <t>ded week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Afifi Ch 18
+* https://www.jaredknowles.com/journal/2013/11/25/getting-started-with-mixed-effect-models-in-r </t>
+  </si>
+  <si>
+    <t>* Install the `lme4` and `arm` packages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Linear algebra incoming. </t>
+  </si>
+  <si>
+    <t>* Small area estimates using census data</t>
+  </si>
+  <si>
+    <t>https://d4tagirl.com/2017/05/how-to-plot-animated-maps-with-gganimate</t>
+  </si>
+  <si>
+    <t>Making awesome animated maps</t>
+  </si>
+  <si>
+    <t>* Install the `plotly`,  `ggthemes`, and `gganimate` packages</t>
+  </si>
+  <si>
+    <t>* Afifi Ch 15, 16
+* https://d4tagirl.com/2017/01/rpart-who-voted-for-trump</t>
+  </si>
+  <si>
+    <t>https://data.nasa.gov/Space-Science/Meteorite-Landings/gh4g-9sfh</t>
+  </si>
+  <si>
+    <t>meteorite landings since 1400</t>
+  </si>
+  <si>
+    <t>classification, mass, year, geoloc</t>
+  </si>
+  <si>
+    <t>https://data.nasa.gov/Space-Science/WISE-NEA-COMET-DISCOVERY-STATISTICS/7qz6-zrqt</t>
+  </si>
+  <si>
+    <t>comet discoveries</t>
+  </si>
+  <si>
+    <t>nasa earth exchange on AWS</t>
+  </si>
+  <si>
+    <t>https://nex.nasa.gov/nex/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=8Vw4eJLoXUQ</t>
+  </si>
+  <si>
+    <t>the amazing world of charts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Join our Slack Channel &amp; Install the phone app
 * Update R &amp; R Studio to current versions
 * Install LaTeX (if not already done). Time to up the game on your report appearance. </t>
   </si>
   <si>
-    <t>Project Updates (use R Studio to make a X min presentation)</t>
-  </si>
-  <si>
-    <t>* Project Update Presentations (Mon)
-* Exam 1 (Fri)</t>
-  </si>
-  <si>
-    <t>* Project Update Presentations (Fri)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time Series, Spatial Modeling, </t>
-  </si>
-  <si>
-    <t>Correlated Data,  Random Intercept Models,</t>
-  </si>
-  <si>
-    <t>Missing Data Identification, Multiple Imputation, MICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Install the `mice` package. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Take Home Final distributed by Wed EOD. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I'll answer questions about the final exam, otherwise the period is yours to work on the exam, projects, or any remaining homework. </t>
-  </si>
-  <si>
-    <t>ded week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Afifi Ch 18
-* https://www.jaredknowles.com/journal/2013/11/25/getting-started-with-mixed-effect-models-in-r </t>
-  </si>
-  <si>
-    <t>* Install the `lme4` and `arm` packages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Linear algebra incoming. </t>
-  </si>
-  <si>
-    <t>* Small area estimates using census data</t>
-  </si>
-  <si>
-    <t>https://d4tagirl.com/2017/05/how-to-plot-animated-maps-with-gganimate</t>
-  </si>
-  <si>
-    <t>Making awesome animated maps</t>
-  </si>
-  <si>
-    <t>* Install the `plotly`,  `ggthemes`, and `gganimate` packages</t>
-  </si>
-  <si>
-    <t>* Afifi Ch 15, 16
-* https://d4tagirl.com/2017/01/rpart-who-voted-for-trump</t>
-  </si>
-  <si>
-    <t>https://data.nasa.gov/Space-Science/Meteorite-Landings/gh4g-9sfh</t>
-  </si>
-  <si>
-    <t>meteorite landings since 1400</t>
-  </si>
-  <si>
-    <t>classification, mass, year, geoloc</t>
-  </si>
-  <si>
-    <t>https://data.nasa.gov/Space-Science/WISE-NEA-COMET-DISCOVERY-STATISTICS/7qz6-zrqt</t>
-  </si>
-  <si>
-    <t>comet discoveries</t>
-  </si>
-  <si>
-    <t>nasa earth exchange on AWS</t>
-  </si>
-  <si>
-    <t>https://nex.nasa.gov/nex/</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=8Vw4eJLoXUQ</t>
-  </si>
-  <si>
-    <t>the amazing world of charts</t>
+    <t>* Linear  Regression (Notebook ch 2)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* Join the #introductions, #assignments and #classwork Slack channels. 
+* Introduce yourself to the class (who/year/major/non-stat interests)
+* 2-3 min video Project Proposal. Post link to YouTube in #projects channel by Friday EOD. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>* Data Camp</t>
+    </r>
+  </si>
+  <si>
+    <t>* Orientation to the class
+* Question Formulation Technique (QFT) walk-through</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* Watch project proposals videos and fill out </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[this survey]() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">to report who you want to work with. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">* What are stratified models and subgroup analysis. 
+* How does stratification relate to moderation? 
+* How do these concepts differ from interactions? </t>
+  </si>
+  <si>
+    <t>Model Building, Moderation &amp; Interactions, Model fit &amp; variable selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Measures of model fit. 
+* How to choose variables for inclusion in a model
+* Comparing between models, and deciding when enough is enough and just stop tweaking the model!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Identify a handful of problems that can creep up when building a model
+* Conduct a fully reproducible analysis that includes and data preparation, exploration, and analysis steps including model building. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* All the things that can show up to grief you during model building. 
+</t>
+  </si>
+  <si>
+    <t>Special Considerations, , Team Check ins</t>
+  </si>
+  <si>
+    <t>* Team check-ups. How are things going? What problems are arising? How can we help troubleshoot as a class? 
+* Open work time to work on your modeling assignment, or in your groups on current analyses</t>
+  </si>
+  <si>
+    <t>* QFT on Model Building
+* Team assignments
+* Categorical variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robin in Sacramento for a conference. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Start working on the model building homework. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -361,8 +399,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,6 +428,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66CCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,7 +582,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -581,6 +631,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="89" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="90">
@@ -677,6 +733,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66CCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1012,9 +1073,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE672480-34D8-4AD4-9F60-F23A82615206}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1059,40 +1120,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:10" ht="141" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>41660</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
       <c r="B3" s="3">
@@ -1100,32 +1161,32 @@
         <v>41667</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    </row>
+    <row r="4" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18">
         <v>3</v>
       </c>
       <c r="B4" s="3">
@@ -1133,25 +1194,29 @@
         <v>41674</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="F4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="179.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -1162,26 +1227,26 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="6" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1193,22 +1258,22 @@
         <v>41688</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="6"/>
       <c r="G6" s="7" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1220,24 +1285,24 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="6" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1249,18 +1314,18 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1280,10 +1345,10 @@
       <c r="G9" s="7"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1306,17 +1371,17 @@
         <v>41723</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1331,7 +1396,7 @@
         <v>41730</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1340,7 +1405,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1352,14 +1417,14 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="4"/>
@@ -1375,11 +1440,11 @@
         <v>41744</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
@@ -1430,7 +1495,7 @@
         <v>41765</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1438,10 +1503,10 @@
       <c r="G17" s="7"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1476,7 +1541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43BB1120-E55B-4CB9-AE22-5C9F3F8B8D47}">
   <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1488,37 +1553,37 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove first bullet problem on schedule
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>Finals Week</t>
   </si>
@@ -94,19 +94,6 @@
   <si>
     <t>* [Notebook Ch 3](https://norcalbiostat.github.io/MATH456_notes/model-building)
 * Afifi Ch 7, 8.5, Ch 9</t>
-  </si>
-  <si>
-    <t>* Fit and interpret the output from a Logistic Regression model.
-* Use  Logistic Regression to classify observations into two groups
-* Interpret a confusion matrix
-* Calculate and explain terms such as Sensitivity, Specificity, and Accuracy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Fitting and interpreting Logistic Regression models. 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Demystfying the confusion matrix by calculating varying measures of model utility such as sensitivity, accuracy, and false positive rate. </t>
   </si>
   <si>
     <t>Open work day</t>
@@ -315,15 +302,6 @@
 </t>
   </si>
   <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>* Read Afifi Ch 12</t>
-  </si>
-  <si>
-    <t>* [Confusion Matrix](https://en.wikipedia.org/wiki/Receiver_operating_characteristic)</t>
-  </si>
-  <si>
     <t>* http://rmarkdown.rstudio.com/lesson-11.html</t>
   </si>
   <si>
@@ -336,12 +314,30 @@
     <t>Generalized Linear Models, Fitted Probabilities, Classification</t>
   </si>
   <si>
-    <t xml:space="preserve">* Logistic regression is one of the more common classification models. You're calculating the probability of being in group 1 (Y=0) or group 2 (Y=1).  
+    <t>* We use Receiver operating characteristic  (ROC) curves to determine how well a binary classifier (like logistic regression) discriminates between two groups as the threshold (p(y=1)) is changed. 
+* Confusion matricies are used to determine how well a model does in classifying observations.  They're not that confusing to make, but are involved in a TON of new terminoloty
+* Important measures are accuracy/sensitvity/specificity/false positive rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Fitting and interpreting Logistic Regression models. 
+* Odds Ratios are always the odds of an event for one group compared to another group. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* LogReg models the probability of being in group 1 (Y=1) compared to group 2 (Y=0).  
+* Thus it can be used to classify individuals into two groups, or predict the risk of an event. 
+* Logistic regression is one of the more common classification models.
 </t>
   </si>
   <si>
-    <t>* We use Receiver operating characteristic  (ROC) curves to determine how well a binary classifier (like logistic regression) discriminates between two groups as the threshold (p(y=1)) is changed. 
-* Confusion matricies are used to determine how well a model does in classifying observations.  They're not that confusing to make, but are involved in a TON of new terminoloty</t>
+    <t>* Fit and interpret the output from a Logistic Regression model.
+* Use  Logistic Regression to classify observations into two groups
+* Create and interpret a ROC curve
+* Create a confusion matrix
+* Calculate and explain terms such as Sensitivity, Specificity, and Accuracy</t>
+  </si>
+  <si>
+    <t>* Read Afifi Ch 12
+* Install the caret and ROCR packages</t>
   </si>
   <si>
     <r>
@@ -355,7 +351,17 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>* Afifi Ch 12</t>
+      <t xml:space="preserve">* Afifi Ch 12
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">* [Confusion Matrix](https://en.wikipedia.org/wiki/Confusion_matrix)
+* ROC curves http://blog.revolutionanalytics.com/2016/08/roc-curves-in-two-lines-of-code.html </t>
     </r>
   </si>
 </sst>
@@ -1087,8 +1093,8 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1147,22 +1153,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1174,25 +1180,25 @@
         <v>41667</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J3" s="17" t="s">
         <v>17</v>
@@ -1207,31 +1213,31 @@
         <v>41674</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J4" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="192" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1240,31 +1246,31 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="G5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="J5" s="17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1272,22 +1278,14 @@
         <f t="shared" si="0"/>
         <v>41688</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="C6" s="2"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="17" t="s">
-        <v>72</v>
-      </c>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -1298,24 +1296,24 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="I7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1327,18 +1325,18 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1354,18 +1352,18 @@
       <c r="C9" s="2"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1388,17 +1386,17 @@
         <v>41723</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1413,7 +1411,7 @@
         <v>41730</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1422,7 +1420,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1434,14 +1432,14 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="4"/>
@@ -1457,11 +1455,11 @@
         <v>41744</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
@@ -1512,7 +1510,7 @@
         <v>41765</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1520,10 +1518,10 @@
       <c r="G17" s="7"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1570,37 +1568,37 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add wk 4 and 5
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="107">
   <si>
     <t>Finals Week</t>
   </si>
@@ -86,16 +87,6 @@
 * Data preparation (Notebook Ch 1)</t>
   </si>
   <si>
-    <t>* Model building homework (Due 2/11)</t>
-  </si>
-  <si>
-    <t>* [Notebook Ch 3](https://norcalbiostat.github.io/MATH456_notes/model-building)</t>
-  </si>
-  <si>
-    <t>* [Notebook Ch 3](https://norcalbiostat.github.io/MATH456_notes/model-building)
-* Afifi Ch 7, 8.5, Ch 9</t>
-  </si>
-  <si>
     <t>Open work day</t>
   </si>
   <si>
@@ -206,33 +197,102 @@
     <t>the amazing world of charts</t>
   </si>
   <si>
-    <t xml:space="preserve">* Join our Slack Channel &amp; Install the phone app
-* Update R &amp; R Studio to current versions
-* Install LaTeX (if not already done). Time to up the game on your report appearance. </t>
-  </si>
-  <si>
     <t>* Linear  Regression (Notebook ch 2)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">* Join the #introductions, #assignments and #classwork Slack channels. 
-* Introduce yourself to the class (who/year/major/non-stat interests)
-* 2-3 min video Project Proposal. Post link to YouTube in #projects channel by Friday EOD. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>* Data Camp</t>
-    </r>
   </si>
   <si>
     <t>* Orientation to the class
 * Question Formulation Technique (QFT) walk-through</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* What are stratified models and subgroup analysis. 
+* How does stratification relate to moderation? 
+* How do these concepts differ from interactions? </t>
+  </si>
+  <si>
+    <t>Model Building, Moderation &amp; Interactions, Model fit &amp; variable selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Measures of model fit. 
+* How to choose variables for inclusion in a model
+* Comparing between models, and deciding when enough is enough and just stop tweaking the model!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Identify a handful of problems that can creep up when building a model
+* Conduct a fully reproducible analysis that includes and data preparation, exploration, and analysis steps including model building. </t>
+  </si>
+  <si>
+    <t>Special Considerations, , Team Check ins</t>
+  </si>
+  <si>
+    <t>* Team check-ups. How are things going? What problems are arising? How can we help troubleshoot as a class? 
+* Open work time to work on your modeling assignment, or in your groups on current analyses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robin in Sacramento for a conference. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Start working on the model building homework. </t>
+  </si>
+  <si>
+    <t>* http://rmarkdown.rstudio.com/lesson-11.html</t>
+  </si>
+  <si>
+    <t>* Project Update Presentations. X minute group presentations with slides prepared in R Markdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Review the different methods to make a [presentation in R Studio](http://rmarkdown.rstudio.com/lesson-11.html). Decide on an output amongst your team. </t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Catgory</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Exam</t>
+  </si>
+  <si>
+    <t>Data Camp</t>
+  </si>
+  <si>
+    <t>Slack Introductions</t>
+  </si>
+  <si>
+    <t>Multiple Regression</t>
+  </si>
+  <si>
+    <t>Model Building</t>
+  </si>
+  <si>
+    <t>Peer Review Model Building</t>
+  </si>
+  <si>
+    <t>Project Updates</t>
+  </si>
+  <si>
+    <t>Poster Presentations</t>
   </si>
   <si>
     <r>
@@ -254,90 +314,90 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">to report who you want to work with. </t>
+      <t>to report who you want to work with. 
+* All follow-up questions should go into the #projects Slack channel</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">* What are stratified models and subgroup analysis. 
-* How does stratification relate to moderation? 
-* How do these concepts differ from interactions? </t>
-  </si>
-  <si>
-    <t>Model Building, Moderation &amp; Interactions, Model fit &amp; variable selection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Measures of model fit. 
-* How to choose variables for inclusion in a model
-* Comparing between models, and deciding when enough is enough and just stop tweaking the model!
+    <t xml:space="preserve">* Join our Slack Team at math456.slack.com &amp; Install the phone app
+* Update R &amp; R Studio to current versions
+* Install LaTeX (if not already done). Time to up the game on your report appearance. </t>
+  </si>
+  <si>
+    <t>* Multiple Regression assignment (Due Wed 2/7)
+* Model building assignment (Due Fri 2/9)</t>
+  </si>
+  <si>
+    <t>* Multiple Regression assignment (Due Wed 2/7)
+* Model building assignment (Due Fri 2/9)
+* Peer Review Model Building report (Due Sun 2/11)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* Join the #introductions, #assignments and #classwork Slack channels. 
+* Introduce yourself to the class (who/year/major/non-stat interests) (Due Sun 1/28)
+* 2-3 min video Project Proposal. Post link to YouTube in #projects channel by Friday EOD. 
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Identify a handful of problems that can creep up when building a model
-* Conduct a fully reproducible analysis that includes and data preparation, exploration, and analysis steps including model building. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* All the things that can show up to grief you during model building. 
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>* Data Camp (TBD)</t>
+    </r>
+  </si>
+  <si>
+    <t>* Project Team assignments
+* Categorical variables (PMA5 Ch 9.3)</t>
+  </si>
+  <si>
+    <t>* [Notebook Ch 3](https://norcalbiostat.github.io/MATH456_notes/model-building)
+* Afifi Ch 7, 8.4-8.7, selections from Ch 9</t>
+  </si>
+  <si>
+    <t>* [Notebook Ch 3](https://norcalbiostat.github.io/MATH456_notes/model-building)
+* PMA5 Ch 9.2, 9.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* QFT Model Building
+* Missing Data (PMA5 9.2) -- Just Intro. We'll come back to this topic in more detail later. 
+* Multicollinearity (PMA5 9.5)
 </t>
   </si>
   <si>
-    <t>Special Considerations, , Team Check ins</t>
-  </si>
-  <si>
-    <t>* Team check-ups. How are things going? What problems are arising? How can we help troubleshoot as a class? 
-* Open work time to work on your modeling assignment, or in your groups on current analyses</t>
-  </si>
-  <si>
-    <t>* QFT on Model Building
-* Team assignments
-* Categorical variables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robin in Sacramento for a conference. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Start working on the model building homework. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Logistic regression and classification assignment (Due 2/25)
+    <t xml:space="preserve">* Read Afifi Ch 12
 </t>
   </si>
   <si>
-    <t>* http://rmarkdown.rstudio.com/lesson-11.html</t>
-  </si>
-  <si>
-    <t>* Project Update Presentations. X minute group presentations with slides prepared in R Markdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Review the different methods to make a [presentation in R Studio](http://rmarkdown.rstudio.com/lesson-11.html). Decide on an output amongst your team. </t>
-  </si>
-  <si>
-    <t>Generalized Linear Models, Fitted Probabilities, Classification</t>
-  </si>
-  <si>
-    <t>* We use Receiver operating characteristic  (ROC) curves to determine how well a binary classifier (like logistic regression) discriminates between two groups as the threshold (p(y=1)) is changed. 
-* Confusion matricies are used to determine how well a model does in classifying observations.  They're not that confusing to make, but are involved in a TON of new terminoloty
-* Important measures are accuracy/sensitvity/specificity/false positive rate</t>
+    <t>* Install the caret and ROCR packages</t>
+  </si>
+  <si>
+    <t>* LogReg models the probability of being in group 1 (Y=1) compared to group 2 (Y=0).  
+* Thus it can be used to classify individuals into two groups, or predict the risk of an event. 
+* Logistic regression is one of the more common classification models.</t>
   </si>
   <si>
     <t xml:space="preserve">* Fitting and interpreting Logistic Regression models. 
-* Odds Ratios are always the odds of an event for one group compared to another group. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* LogReg models the probability of being in group 1 (Y=1) compared to group 2 (Y=0).  
-* Thus it can be used to classify individuals into two groups, or predict the risk of an event. 
-* Logistic regression is one of the more common classification models.
+* Odds Ratios are always the odds of an event for one group compared to another group. 
 </t>
   </si>
   <si>
-    <t>* Fit and interpret the output from a Logistic Regression model.
-* Use  Logistic Regression to classify observations into two groups
-* Create and interpret a ROC curve
-* Create a confusion matrix
-* Calculate and explain terms such as Sensitivity, Specificity, and Accuracy</t>
-  </si>
-  <si>
-    <t>* Read Afifi Ch 12
-* Install the caret and ROCR packages</t>
+    <t>Generalized Linear Models, Predicted Probabilities</t>
+  </si>
+  <si>
+    <t>Classification, ROC curves, Confusion Matrix</t>
+  </si>
+  <si>
+    <t>* Poisson regression can be used to model count data (truncated at 0, whole integer values) (Reading: PMA5 12.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* PMA5 Ch 12.8 (Start p 295) , 12.3 (What to watch out for)
+* [Confusion Matrix](https://en.wikipedia.org/wiki/Confusion_matrix)
+* [ROC curves](http://blog.revolutionanalytics.com/2016/08/roc-curves-in-two-lines-of-code.html)
+</t>
   </si>
   <si>
     <r>
@@ -351,25 +411,100 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">* Afifi Ch 12
+      <t>* Afifi Ch 12.1-12.7, p. 289
+* [Goodness of Fit](https://www.r-bloggers.com/logistic-regression-in-r-part-two/)
+* PMA5 Ch 12.11 (Poisson Regression)</t>
+    </r>
+  </si>
+  <si>
+    <t>* Most common measure of model fit for logistic regression is the goodness of fit chi-squared statistic. (Reading:PMA5 p. 289)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Build and interpret a Logistic regression model on binary data
+* Assess how well a logistic model fits using a goodness of fit measure. 
+* Build and interpret a Poisson model on count data. 
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* Use  Logistic Regression to classify observations into two groups
 </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">* [Confusion Matrix](https://en.wikipedia.org/wiki/Confusion_matrix)
-* ROC curves http://blog.revolutionanalytics.com/2016/08/roc-curves-in-two-lines-of-code.html </t>
+      <t>* Identify the optimal cutoff point for a binary classifier</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>* Create and interpret a ROC curve</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>* Create a confusion matrix
+* Calculate and explain terms such as Sensitivity, Specificity, and Accuracy</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">* Assess the proportion of individuals correctly classified as the cutoff  is changed.  (Reading: PMA5 Ch 12.8, start @ p 295)
+* Confusion matricies are used to determine how well a model does in classifying observations.  
+* Important measures are accuracy/sensitvity/specificity/false positive rate
+</t>
+  </si>
+  <si>
+    <t>GLM Assignment</t>
+  </si>
+  <si>
+    <t>Peer Review GLM Assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* GLM assignment (Due Fri 2/23)
+</t>
+  </si>
+  <si>
+    <t>* GLM assignment (Due Fri 2/23)
+* Peer Review GLM Assignment (Due Sun 2/25)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -424,6 +559,29 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -457,7 +615,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -508,8 +666,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="90">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -600,8 +778,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -657,8 +838,50 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="91" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="91" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="90" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="92" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="4" xfId="91" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="90">
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -702,6 +925,7 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Heading 2" xfId="91" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -748,7 +972,9 @@
     <cellStyle name="Hyperlink" xfId="89" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Percent" xfId="90" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Total" xfId="92" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1094,14 +1320,15 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="25.25" style="5" customWidth="1"/>
-    <col min="5" max="6" width="14.875" style="5"/>
-    <col min="7" max="7" width="17.75" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.875" style="5"/>
+    <col min="6" max="6" width="21.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="23.125" style="5" customWidth="1"/>
     <col min="8" max="8" width="32.875" style="5" customWidth="1"/>
     <col min="9" max="9" width="36.25" style="5" customWidth="1"/>
     <col min="10" max="10" width="24.125" style="5" customWidth="1"/>
@@ -1139,7 +1366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="141" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -1153,25 +1380,25 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -1180,31 +1407,31 @@
         <v>41667</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -1213,32 +1440,32 @@
         <v>41674</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="192" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+        <v>58</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
       <c r="B5" s="3">
@@ -1246,46 +1473,62 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>77</v>
+        <v>94</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>100</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+        <v>99</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
         <v>5</v>
       </c>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
         <v>41688</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="17"/>
+      <c r="C6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="34" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -1296,24 +1539,24 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="I7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1325,18 +1568,18 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1352,18 +1595,18 @@
       <c r="C9" s="2"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1386,17 +1629,17 @@
         <v>41723</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1411,7 +1654,7 @@
         <v>41730</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1420,7 +1663,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1432,14 +1675,14 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="4"/>
@@ -1455,11 +1698,11 @@
         <v>41744</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
@@ -1510,7 +1753,7 @@
         <v>41765</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1518,10 +1761,10 @@
       <c r="G17" s="7"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1553,6 +1796,883 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF4A7D6-99F8-47F5-800F-D0D81251D4B0}">
+  <dimension ref="A1:J86"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="25"/>
+    <col min="2" max="2" width="32.25" style="25" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="7.75" style="25"/>
+    <col min="5" max="5" width="9.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.125" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="10" style="21" customWidth="1"/>
+    <col min="9" max="9" width="7.75" style="21"/>
+    <col min="10" max="10" width="4.75" style="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="21">
+        <v>1</v>
+      </c>
+      <c r="E2" s="31">
+        <v>41666</v>
+      </c>
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>1</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="21">
+        <v>50</v>
+      </c>
+      <c r="E3" s="31">
+        <v>41772</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="21">
+        <f t="shared" ref="H2:H8" si="0">SUMIF($C$2:$C$77,G3,$D$2:$D$77)</f>
+        <v>25</v>
+      </c>
+      <c r="I3" s="24">
+        <f t="shared" ref="I2:I8" si="1">H3/$H$9</f>
+        <v>0.11682242990654206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>2</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="21">
+        <v>10</v>
+      </c>
+      <c r="E4" s="31">
+        <v>41676</v>
+      </c>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I4" s="24">
+        <f t="shared" si="1"/>
+        <v>4.6728971962616819E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>3</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="21">
+        <v>5</v>
+      </c>
+      <c r="E5" s="31">
+        <v>41678</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="21">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="I5" s="24">
+        <f t="shared" si="1"/>
+        <v>0.23364485981308411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
+        <v>3</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="21">
+        <v>4</v>
+      </c>
+      <c r="E6" s="31">
+        <v>41680</v>
+      </c>
+      <c r="G6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="21">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I6" s="24">
+        <f t="shared" si="1"/>
+        <v>3.7383177570093455E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>4</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="21">
+        <v>10</v>
+      </c>
+      <c r="E7" s="31">
+        <v>41694</v>
+      </c>
+      <c r="G7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="21">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I7" s="24">
+        <f t="shared" si="1"/>
+        <v>0.46728971962616822</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>5</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="21">
+        <v>4</v>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="21">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I8" s="24">
+        <f t="shared" si="1"/>
+        <v>0.14018691588785046</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21">
+        <v>6</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="31"/>
+      <c r="H9" s="27">
+        <f>SUM(H2:H8)</f>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <v>7</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>8</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="21">
+        <v>10</v>
+      </c>
+      <c r="E11" s="31">
+        <v>41713</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="31"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="31"/>
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="31"/>
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="31"/>
+      <c r="H15"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="31"/>
+      <c r="H16"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="31"/>
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <v>14</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="21">
+        <v>20</v>
+      </c>
+      <c r="E18" s="31"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="31"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
+        <v>16</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="21">
+        <v>100</v>
+      </c>
+      <c r="E20" s="31"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="31"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="31"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="31"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="31"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="31"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="31"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="31"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="31"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="31"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="31"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="31"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="28"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="31"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="31"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="31"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="31"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="31"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="31"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="28"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="28"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="28"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="28"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="28"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="21"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="28"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="28"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="28"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="21"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="28"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="21"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="28"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="21"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="28"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="28"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="28"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="28"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="28"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="21"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="28"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="21"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="28"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="21"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="28"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="21"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="28"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="25"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="21"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="25"/>
+      <c r="I59" s="25"/>
+      <c r="J59" s="25"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="21"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="28"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="21"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="28"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="21"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="28"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="21"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="28"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="21"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="28"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="22"/>
+      <c r="B65" s="22"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="28"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="22"/>
+      <c r="B66" s="22"/>
+      <c r="C66" s="22"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="32"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="22"/>
+      <c r="B67" s="22"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="32"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="22"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="32"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="22"/>
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="32"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="22"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="32"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="22"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="32"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="22"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="26"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="22"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="26"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="22"/>
+      <c r="B74" s="22"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="26"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="22"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="32"/>
+      <c r="H75"/>
+      <c r="I75"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="22"/>
+      <c r="B76" s="22"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="32"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="22"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="32"/>
+      <c r="H77"/>
+      <c r="I77"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="22"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="32"/>
+      <c r="H78"/>
+      <c r="I78"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="22"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="32"/>
+      <c r="H79"/>
+      <c r="I79"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="22"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="32"/>
+      <c r="H80"/>
+      <c r="I80"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="22"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="32"/>
+      <c r="H81"/>
+      <c r="I81"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="22"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="32"/>
+      <c r="H82"/>
+      <c r="I82"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="22"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="32"/>
+      <c r="H83"/>
+      <c r="I83"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="22"/>
+      <c r="B84" s="22"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="32"/>
+      <c r="H84"/>
+      <c r="I84"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="22"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="32"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="29"/>
+      <c r="B86" s="29"/>
+      <c r="D86" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43BB1120-E55B-4CB9-AE22-5C9F3F8B8D47}">
   <dimension ref="A2:C5"/>
   <sheetViews>
@@ -1568,37 +2688,37 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add wk7 and 8. rebuild.
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="150">
   <si>
     <t>Finals Week</t>
   </si>
@@ -84,16 +84,7 @@
 * Afifi Ch 1-5</t>
   </si>
   <si>
-    <t>* Project proposals
-* Data preparation (Notebook Ch 1)</t>
-  </si>
-  <si>
     <t>Open work day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* QFT n&lt;&lt;&lt;p
-* The curse of dimensionality
-* We'll explore the mathmatical model behind PCA. </t>
   </si>
   <si>
     <t xml:space="preserve">* We'll fit and interpret a few PCA models. 
@@ -131,10 +122,6 @@
     <t>* Install the `plotly`,  `ggthemes`, and `gganimate` packages</t>
   </si>
   <si>
-    <t>* Afifi Ch 15, 16
-* https://d4tagirl.com/2017/01/rpart-who-voted-for-trump</t>
-  </si>
-  <si>
     <t>https://data.nasa.gov/Space-Science/Meteorite-Landings/gh4g-9sfh</t>
   </si>
   <si>
@@ -163,10 +150,6 @@
   </si>
   <si>
     <t>* Linear  Regression (Notebook ch 2)</t>
-  </si>
-  <si>
-    <t>* Orientation to the class
-* Question Formulation Technique (QFT) walk-through</t>
   </si>
   <si>
     <t xml:space="preserve">* What are stratified models and subgroup analysis. 
@@ -201,9 +184,6 @@
   </si>
   <si>
     <t>* Project Update Presentations. X minute group presentations with slides prepared in R Markdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Review the different methods to make a [presentation in R Studio](http://rmarkdown.rstudio.com/lesson-11.html). Decide on an output amongst your team. </t>
   </si>
   <si>
     <t>%</t>
@@ -278,14 +258,6 @@
 * Categorical variables (PMA5 Ch 9.3)</t>
   </si>
   <si>
-    <t>* [Notebook Ch 3](https://norcalbiostat.github.io/MATH456_notes/model-building)
-* Afifi Ch 7, 8.4-8.7, selections from Ch 9</t>
-  </si>
-  <si>
-    <t>* [Notebook Ch 3](https://norcalbiostat.github.io/MATH456_notes/model-building)
-* PMA5 Ch 9.2, 9.5</t>
-  </si>
-  <si>
     <t xml:space="preserve">* QFT Model Building
 * Missing Data (PMA5 9.2) -- Just Intro. We'll come back to this topic in more detail later. 
 * Multicollinearity (PMA5 9.5)
@@ -333,12 +305,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">* Assess the proportion of individuals correctly classified as the cutoff  is changed.  (Reading: PMA5 Ch 12.8, start @ p 295)
-* Confusion matricies are used to determine how well a model does in classifying observations.  
-* Important measures are accuracy/sensitvity/specificity/false positive rate
-</t>
-  </si>
-  <si>
     <t>GLM Assignment</t>
   </si>
   <si>
@@ -347,12 +313,6 @@
   <si>
     <t>* GLM assignment (Due Fri 2/23)
 * Peer Review GLM Assignment (Due Sun 2/25)</t>
-  </si>
-  <si>
-    <t>* [Notebook Ch 4](https://norcalbiostat.github.io/MATH456_notes/glm)
-* Afifi Ch 12.1-12.7, p. 289
-* [Goodness of Fit](https://www.r-bloggers.com/logistic-regression-in-r-part-two/)
-* PMA5 Ch 12.11 (Poisson Regression)</t>
   </si>
   <si>
     <t>Robin in Sacramento for a conference. Edward Cover Class</t>
@@ -431,9 +391,6 @@
     <t>PR Correlated Data</t>
   </si>
   <si>
-    <t>Midterm,, Project presentations</t>
-  </si>
-  <si>
     <t>Midterm Review</t>
   </si>
   <si>
@@ -489,6 +446,124 @@
   </si>
   <si>
     <t>Manipulating data:C ase study</t>
+  </si>
+  <si>
+    <t>* PCA / FA assignment (Due Fri 3/9)
+* Peer Review (Due Sun 3/11)</t>
+  </si>
+  <si>
+    <t>In class Midterm</t>
+  </si>
+  <si>
+    <t>* Missing Data Assignment (Due Fri 5/4)
+* Peer Review (Due Sun 5/6)</t>
+  </si>
+  <si>
+    <t>* Take home portion of Final exam distributed Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* In class exam (May ??)
+* Take home portion (Due before in class exam)
+</t>
+  </si>
+  <si>
+    <t>* Correlated Data assignment (Due Fri 4/6) - tentative
+* PR Correlated data (Due Sun 4/8) - tentative</t>
+  </si>
+  <si>
+    <t>* Spatio-Temporal assignment due (Fri 4/20) - tentative
+* PR Spatio-Temporal (Sun 4/22) - tentative</t>
+  </si>
+  <si>
+    <t>PR Spatio-Temporal</t>
+  </si>
+  <si>
+    <t>QFT Spatio-Temporal</t>
+  </si>
+  <si>
+    <t>Spatio-Temporal analysis</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Spatial-Temporal Modeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable Overload, Principal Component Analysis, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factor Analysis, , </t>
+  </si>
+  <si>
+    <t>QFT n&lt;&lt;p</t>
+  </si>
+  <si>
+    <t>* QFT Correlated Data</t>
+  </si>
+  <si>
+    <t>* QFT Spatio-Temporal Data</t>
+  </si>
+  <si>
+    <t>* Explain the difference between PCA and FA</t>
+  </si>
+  <si>
+    <t>* In class portion of Midterm Exam (Wed 3/14) 
+* Take home portion of Midterm Exam (Due Friday 3/16)
+* Project Update Presentations (Fri 3/16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Assess the proportion of individuals correctly classified as the cutoff  is changed.  (Reading: PMA5 Ch 12.8, start @ p 295)
+* Confusion matrices are used to determine how well a model does in classifying observations.  
+* Important measures are accuracy/sensitivity/specificity/false positive rate
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* QFT n&lt;&lt;&lt;p
+* The curse of dimensionality
+* We'll explore the mathematical model behind PCA. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Another dimension reduction technique: Factor Analysis. Similar, but different.  Used in different situations. 
+* Exploratory vs Confirmatory Factor Analysis. </t>
+  </si>
+  <si>
+    <t>* Fine tuning your factor model by rotating the axes
+* Using FA as a modeling tool by creating factor scores</t>
+  </si>
+  <si>
+    <t>* PMA5 Ch 9.2, 9.5</t>
+  </si>
+  <si>
+    <t>* PMA5 Ch 12.1-12.7, p. 289
+* [Goodness of Fit](https://www.r-bloggers.com/logistic-regression-in-r-part-two/)
+* PMA5 Ch 12.11 (Poisson Regression)</t>
+  </si>
+  <si>
+    <t>* PMA5 Ch 7, 8.4-8.7, selections from Ch 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* PMA5 Ch 15
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* PMA5 Ch 14
+* [[Open Psychology Data]](https://openpsychometrics.org/_rawdata/ )
+</t>
+  </si>
+  <si>
+    <t>Review, Midterm, Project presentations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Review the different methods to make a [presentation in R Studio](http://rmarkdown.rstudio.com/lesson-11.html). Decide on an output style amongst your team before you start. </t>
+  </si>
+  <si>
+    <t>* Orientation to the class
+* New tools: Hack MD, Slack
+* Question Formulation Technique (QFT) walk-through</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * Data preparation (Notebook Ch 1)</t>
   </si>
   <si>
     <r>
@@ -503,82 +578,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>* Earn ~20k experience in Data Camp - End of Semester(5/14)</t>
+      <t>* Continuing education: Earn ~20k experience in Data Camp by end of Semester (5/14)</t>
     </r>
-  </si>
-  <si>
-    <t>* PCA / FA assignment (Due Fri 3/9)
-* Peer Review (Due Sun 3/11)</t>
-  </si>
-  <si>
-    <t>In class Midterm</t>
-  </si>
-  <si>
-    <t>* In class portion of Midterm Exam (Wed 3/14) 
-* Take home portion of Midtrem Exam (Due Friday 3/16)
-* Project Update Presentations (Fri 3/16)</t>
-  </si>
-  <si>
-    <t>* Missing Data Assignment (Due Fri 5/4)
-* Peer Review (Due Sun 5/6)</t>
-  </si>
-  <si>
-    <t>* Take home portion of Final exam distributed Friday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* In class exam (May ??)
-* Take home portion (Due before in class exam)
-</t>
-  </si>
-  <si>
-    <t>* Correlated Data assignment (Due Fri 4/6) - tentative
-* PR Correlated data (Due Sun 4/8) - tentative</t>
-  </si>
-  <si>
-    <t>* Spatio-Temporal assignment due (Fri 4/20) - tentative
-* PR Spatio-Temporal (Sun 4/22) - tentative</t>
-  </si>
-  <si>
-    <t>PR Spatio-Temporal</t>
-  </si>
-  <si>
-    <t>QFT Spatio-Temporal</t>
-  </si>
-  <si>
-    <t>Spatio-Temporal analysis</t>
-  </si>
-  <si>
-    <t>Topic</t>
-  </si>
-  <si>
-    <t>Spatial-Temporal Modeling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variable Overload, Principal Component Analysis, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Factor Analysis, , </t>
-  </si>
-  <si>
-    <t>* Another dimension reduction technique: Factor Analysis. Similar, but different.  Used in different situations. 
-* Exploratory vs Confirmatory Factor Analysis. 
-* Fine tuning your factor model by rotating the axes
-* Using FA as a modeling tool by creating factor scores</t>
-  </si>
-  <si>
-    <t>QFT n&lt;&lt;p</t>
-  </si>
-  <si>
-    <t>* QFT Correlated Data</t>
-  </si>
-  <si>
-    <t>* QFT Spatio-Temporal Data</t>
-  </si>
-  <si>
-    <t>* Afifi Ch 14, 15
-* [[Open Psychology Data]](https://openpsychometrics.org/_rawdata/ )
-* [[STDHA tutorial on PCA]](http://www.sthda.com/english/articles/31-principal-component-methods-in-r-practical-guide/112-pca-principal-component-analysis-essentials/)
-* [[FA Tutorial in R from Stanford]](https://web.stanford.edu/class/psych253/tutorials/FactorAnalysis.html)</t>
   </si>
 </sst>
 </file>
@@ -1444,7 +1445,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1490,7 +1491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -1504,22 +1505,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>16</v>
+        <v>148</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1531,28 +1532,28 @@
         <v>41667</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1564,29 +1565,29 @@
         <v>41674</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J4" s="28"/>
     </row>
-    <row r="5" spans="1:11" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <v>4</v>
       </c>
@@ -1595,28 +1596,28 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1628,30 +1629,30 @@
         <v>41688</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>81</v>
+        <v>136</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" s="28"/>
     </row>
-    <row r="7" spans="1:11" ht="204.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="7" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
         <v>6</v>
       </c>
       <c r="B7" s="3">
@@ -1659,32 +1660,32 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>18</v>
+        <v>137</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
         <v>7</v>
       </c>
       <c r="B8" s="3">
@@ -1692,22 +1693,28 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>130</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>30</v>
+        <v>143</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+        <v>138</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="17">
         <v>8</v>
       </c>
       <c r="B9" s="3">
@@ -1715,28 +1722,28 @@
         <v>41709</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1759,22 +1766,22 @@
         <v>41723</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1804,18 +1811,18 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="16"/>
       <c r="G13" s="7" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1844,20 +1851,20 @@
         <v>41751</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1886,22 +1893,22 @@
         <v>41765</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1922,23 +1929,23 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:10" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1973,25 +1980,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1999,16 +2006,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D2" s="41">
         <v>5</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G2" s="38">
         <f>SUMIF($C$2:$C$86,F2,$D$2:$D$86)</f>
@@ -2024,16 +2031,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D3" s="41">
         <v>20</v>
       </c>
       <c r="F3" s="42" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G3" s="41">
         <f>SUMIF($C$2:$C$86,F3,$D$2:$D$86)</f>
@@ -2049,16 +2056,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D4" s="35">
         <v>10</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G4" s="32">
         <f>SUMIF($C$2:$C$86,F4,$D$2:$D$86)</f>
@@ -2074,16 +2081,16 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D5" s="41">
         <v>5</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G5" s="31">
         <f>SUMIF($C$2:$C$86,F5,$D$2:$D$86)</f>
@@ -2099,10 +2106,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D6" s="35">
         <v>10</v>
@@ -2117,10 +2124,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D7" s="41">
         <v>5</v>
@@ -2131,10 +2138,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D8" s="35">
         <v>20</v>
@@ -2145,10 +2152,10 @@
         <v>3.1</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D9" s="41">
         <v>5</v>
@@ -2159,10 +2166,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D10" s="41">
         <v>5</v>
@@ -2173,10 +2180,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D11" s="35">
         <v>20</v>
@@ -2188,10 +2195,10 @@
         <v>4.2</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C12" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D12" s="41">
         <v>5</v>
@@ -2203,10 +2210,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D13" s="41">
         <v>5</v>
@@ -2218,10 +2225,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D14" s="32">
         <v>100</v>
@@ -2233,10 +2240,10 @@
         <v>6</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D15" s="31">
         <v>25</v>
@@ -2248,10 +2255,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D16" s="41">
         <v>5</v>
@@ -2263,10 +2270,10 @@
         <v>7.1</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D17" s="35">
         <v>20</v>
@@ -2278,10 +2285,10 @@
         <v>7.2</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D18" s="41">
         <v>5</v>
@@ -2293,10 +2300,10 @@
         <v>8</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D19" s="41">
         <v>5</v>
@@ -2308,10 +2315,10 @@
         <v>8.1</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D20" s="35">
         <v>20</v>
@@ -2323,10 +2330,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D21" s="41">
         <v>5</v>
@@ -2338,10 +2345,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D22" s="41">
         <v>5</v>
@@ -2352,10 +2359,10 @@
         <v>9.1</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D23" s="35">
         <v>20</v>
@@ -2366,10 +2373,10 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D24" s="41">
         <v>5</v>
@@ -2380,10 +2387,10 @@
         <v>10</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D25" s="31">
         <v>25</v>
@@ -2394,10 +2401,10 @@
         <v>11</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C26" s="41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D26" s="41">
         <v>5</v>
@@ -2411,7 +2418,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D27" s="32">
         <v>100</v>
@@ -2896,37 +2903,37 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2951,33 +2958,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -2985,13 +2992,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -2999,7 +3006,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -3007,7 +3014,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3015,10 +3022,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F10" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3026,7 +3033,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3034,7 +3041,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3042,7 +3049,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3050,7 +3057,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3058,7 +3065,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
add OH, ignore _render_week, rebuild
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -223,30 +223,6 @@
   </si>
   <si>
     <t>Poster Presentations</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">* Watch project proposals videos and fill out </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[this survey]() </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>to report who you want to work with. 
-* All follow-up questions should go into the #projects Slack channel</t>
-    </r>
   </si>
   <si>
     <t>* Multiple Regression assignment (Due Wed 2/7)
@@ -581,11 +557,15 @@
       <t>* Continuing education: Earn ~20k experience in Data Camp by end of Semester (5/14)</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">* Watch project proposals videos and DM Robin in slack with your top 3 choices. 
+* All follow-up questions should go into the #projects Slack channel as a reply to the proposer. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1096,9 +1076,9 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
     <cellStyle name="Percent" xfId="90" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Percent 2" xfId="52"/>
     <cellStyle name="Total" xfId="92" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1440,12 +1420,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE672480-34D8-4AD4-9F60-F23A82615206}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1505,22 +1485,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>148</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1538,13 +1518,13 @@
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>60</v>
+        <v>149</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>38</v>
@@ -1553,7 +1533,7 @@
         <v>40</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1574,13 +1554,13 @@
         <v>44</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>43</v>
@@ -1596,28 +1576,28 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1629,22 +1609,22 @@
         <v>41688</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>16</v>
@@ -1660,19 +1640,19 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>17</v>
@@ -1681,7 +1661,7 @@
         <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1693,20 +1673,20 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G8" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>16</v>
@@ -1722,28 +1702,28 @@
         <v>41709</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>46</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1776,12 +1756,12 @@
         <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1811,18 +1791,18 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="16"/>
       <c r="G13" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1859,12 +1839,12 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1899,16 +1879,16 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1929,7 +1909,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1950,7 +1930,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F20" r:id="rId1" xr:uid="{B108864C-74A1-4DB0-BF76-6134A099EE4C}"/>
+    <hyperlink ref="F20" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1958,7 +1938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF4A7D6-99F8-47F5-800F-D0D81251D4B0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1980,7 +1960,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>48</v>
@@ -2006,7 +1986,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" s="41" t="s">
         <v>52</v>
@@ -2081,7 +2061,7 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>52</v>
@@ -2138,7 +2118,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="35" t="s">
         <v>48</v>
@@ -2152,7 +2132,7 @@
         <v>3.1</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="41" t="s">
         <v>52</v>
@@ -2166,7 +2146,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" s="41" t="s">
         <v>52</v>
@@ -2180,7 +2160,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="35" t="s">
         <v>48</v>
@@ -2195,7 +2175,7 @@
         <v>4.2</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="41" t="s">
         <v>52</v>
@@ -2210,7 +2190,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="41" t="s">
         <v>52</v>
@@ -2225,7 +2205,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>53</v>
@@ -2255,7 +2235,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="41" t="s">
         <v>52</v>
@@ -2270,7 +2250,7 @@
         <v>7.1</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17" s="35" t="s">
         <v>48</v>
@@ -2285,7 +2265,7 @@
         <v>7.2</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="41" t="s">
         <v>52</v>
@@ -2300,7 +2280,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" s="41" t="s">
         <v>52</v>
@@ -2315,7 +2295,7 @@
         <v>8.1</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" s="35" t="s">
         <v>48</v>
@@ -2330,7 +2310,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C21" s="41" t="s">
         <v>52</v>
@@ -2345,7 +2325,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="41" t="s">
         <v>52</v>
@@ -2359,7 +2339,7 @@
         <v>9.1</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="35" t="s">
         <v>48</v>
@@ -2373,7 +2353,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="41" t="s">
         <v>52</v>
@@ -2401,7 +2381,7 @@
         <v>11</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="41" t="s">
         <v>52</v>
@@ -2888,7 +2868,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43BB1120-E55B-4CB9-AE22-5C9F3F8B8D47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2942,7 +2922,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D3D8A2-979C-4BB4-9449-E424C93F4175}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2958,33 +2938,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
         <v>101</v>
       </c>
-      <c r="C4" t="s">
-        <v>102</v>
-      </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" t="s">
         <v>101</v>
-      </c>
-      <c r="G4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" t="s">
         <v>105</v>
-      </c>
-      <c r="F5" t="s">
-        <v>106</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -2992,13 +2972,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -3006,7 +2986,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -3014,7 +2994,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3022,10 +3002,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" t="s">
         <v>110</v>
-      </c>
-      <c r="F10" t="s">
-        <v>111</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3033,7 +3013,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3041,7 +3021,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3049,7 +3029,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3057,7 +3037,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3065,7 +3045,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
upd schedule, rebuild wk2
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="151">
   <si>
     <t>Finals Week</t>
   </si>
@@ -223,15 +223,6 @@
   </si>
   <si>
     <t>Poster Presentations</t>
-  </si>
-  <si>
-    <t>* Multiple Regression assignment (Due Wed 2/7)
-* Model building assignment (Due Fri 2/9)
-* Peer Review Model Building report (Due Sun 2/11)</t>
-  </si>
-  <si>
-    <t>* Project Team assignments
-* Categorical variables (PMA5 Ch 9.3)</t>
   </si>
   <si>
     <t xml:space="preserve">* QFT Model Building
@@ -516,9 +507,6 @@
 * PMA5 Ch 12.11 (Poisson Regression)</t>
   </si>
   <si>
-    <t>* PMA5 Ch 7, 8.4-8.7, selections from Ch 9</t>
-  </si>
-  <si>
     <t xml:space="preserve">* PMA5 Ch 15
 </t>
   </si>
@@ -545,7 +533,8 @@
     <r>
       <t xml:space="preserve">* Join the #introductions, #assignments and #classwork Slack channels. 
 * Introduce yourself to the class (who/year/major/non-stat interests) (Due Sun 1/28)
-* 2-3 min video Project Proposal. Post link to YouTube in #projects channel by Friday EOD. 
+* 2-3 min video Project Proposal. Post link to YouTube in #projects channel (Due Friday 1/26)
+* Non-proposers: Watch project proposals videos and DM Robin in Slack with your top 3 choices (Due Sun 1/28) 
 </t>
     </r>
     <r>
@@ -554,12 +543,30 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>* Continuing education: Earn ~20k experience in Data Camp by end of Semester (5/14)</t>
+      <t>* Continuing education: Earn ~20k experience in Data Camp by end of Semester (Due 5/14)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">* Watch project proposals videos and DM Robin in slack with your top 3 choices. 
-* All follow-up questions should go into the #projects Slack channel as a reply to the proposer. </t>
+    <t xml:space="preserve">* Read selected sections from PMA5
+* Review the Course Notebook Ch3 (Model Building). Prepare to answer questions posed in the notes and in the daily list below. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Project Team assignments
+* How can we include non-numeric data in a model? 
+* What problems can we encounter when using such data? </t>
+  </si>
+  <si>
+    <t>* Multiple Regression assignment (Due Wed 2/7)
+* Model building assignment (Due Fri 2/9)
+* Peer Review Model Building report (Due Sun 2/11)
+* Team project Research proposal (Due  2/16)</t>
+  </si>
+  <si>
+    <t>* PMA5 Ch 7, 8.4-8.7, selections from Ch 9
+* [[Article on how to prepare a research proposal]](https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3282423/)</t>
+  </si>
+  <si>
+    <t>Research Proposal</t>
   </si>
 </sst>
 </file>
@@ -1425,7 +1432,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1436,7 +1443,7 @@
     <col min="7" max="7" width="30.125" style="5" customWidth="1"/>
     <col min="8" max="8" width="32.875" style="5" customWidth="1"/>
     <col min="9" max="9" width="30.5" style="5" customWidth="1"/>
-    <col min="10" max="10" width="24.125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="36.75" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1471,7 +1478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -1485,22 +1492,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1518,13 +1525,13 @@
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>141</v>
-      </c>
       <c r="G3" s="7" t="s">
-        <v>61</v>
+        <v>147</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>38</v>
@@ -1533,7 +1540,7 @@
         <v>40</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>60</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1554,13 +1561,13 @@
         <v>44</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>43</v>
@@ -1576,28 +1583,28 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" s="28" t="s">
-        <v>69</v>
-      </c>
       <c r="J5" s="28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1609,22 +1616,22 @@
         <v>41688</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>16</v>
@@ -1640,19 +1647,19 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>17</v>
@@ -1661,7 +1668,7 @@
         <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1673,20 +1680,20 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>16</v>
@@ -1702,28 +1709,28 @@
         <v>41709</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>46</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1756,12 +1763,12 @@
         <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1791,18 +1798,18 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="16"/>
       <c r="G13" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1839,12 +1846,12 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1879,16 +1886,16 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1909,7 +1916,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1939,10 +1946,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D27"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1960,7 +1967,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>48</v>
@@ -1986,7 +1993,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" s="41" t="s">
         <v>52</v>
@@ -1998,12 +2005,12 @@
         <v>48</v>
       </c>
       <c r="G2" s="38">
-        <f>SUMIF($C$2:$C$86,F2,$D$2:$D$86)</f>
+        <f>SUMIF($C$2:$C$87,F2,$D$2:$D$87)</f>
         <v>120</v>
       </c>
       <c r="H2" s="40">
         <f>G2/$G$6</f>
-        <v>0.2608695652173913</v>
+        <v>0.25531914893617019</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2023,12 +2030,12 @@
         <v>52</v>
       </c>
       <c r="G3" s="41">
-        <f>SUMIF($C$2:$C$86,F3,$D$2:$D$86)</f>
+        <f>SUMIF($C$2:$C$87,F3,$D$2:$D$87)</f>
         <v>90</v>
       </c>
       <c r="H3" s="43">
         <f>G3/$G$6</f>
-        <v>0.19565217391304349</v>
+        <v>0.19148936170212766</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2048,12 +2055,12 @@
         <v>53</v>
       </c>
       <c r="G4" s="32">
-        <f>SUMIF($C$2:$C$86,F4,$D$2:$D$86)</f>
+        <f>SUMIF($C$2:$C$87,F4,$D$2:$D$87)</f>
         <v>200</v>
       </c>
       <c r="H4" s="34">
         <f>G4/$G$6</f>
-        <v>0.43478260869565216</v>
+        <v>0.42553191489361702</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2061,7 +2068,7 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>52</v>
@@ -2073,12 +2080,12 @@
         <v>49</v>
       </c>
       <c r="G5" s="31">
-        <f>SUMIF($C$2:$C$86,F5,$D$2:$D$86)</f>
-        <v>50</v>
+        <f>SUMIF($C$2:$C$87,F5,$D$2:$D$87)</f>
+        <v>60</v>
       </c>
       <c r="H5" s="37">
         <f>G5/$G$6</f>
-        <v>0.10869565217391304</v>
+        <v>0.1276595744680851</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2096,7 +2103,7 @@
       </c>
       <c r="G6" s="25">
         <f>SUM(G2:G5)</f>
-        <v>460</v>
+        <v>470</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2115,38 +2122,38 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="35">
-        <v>20</v>
+        <v>150</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="31">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="41">
-        <v>5</v>
+        <v>71</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="35">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
-        <v>4</v>
+        <v>3.1</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>130</v>
+        <v>72</v>
       </c>
       <c r="C10" s="41" t="s">
         <v>52</v>
@@ -2157,40 +2164,40 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
-        <v>4.0999999999999996</v>
+        <v>4</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="35">
-        <v>20</v>
+        <v>128</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="41">
+        <v>5</v>
       </c>
       <c r="G11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="41">
-        <v>5</v>
+        <v>79</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="35">
+        <v>20</v>
       </c>
       <c r="G12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C13" s="41" t="s">
         <v>52</v>
@@ -2202,85 +2209,85 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
-        <v>5.0999999999999996</v>
+        <v>5</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="32">
-        <v>100</v>
+        <v>88</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="41">
+        <v>5</v>
       </c>
       <c r="G14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
-        <v>6</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="31">
-        <v>25</v>
+        <v>89</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="32">
+        <v>100</v>
       </c>
       <c r="G15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="41">
-        <v>5</v>
+        <v>58</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="31">
+        <v>20</v>
       </c>
       <c r="G16"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
-        <v>7.1</v>
+        <v>7</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="35">
-        <v>20</v>
+        <v>86</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="41">
+        <v>5</v>
       </c>
       <c r="G17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="41">
-        <v>5</v>
+        <v>81</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="35">
+        <v>20</v>
       </c>
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
-        <v>8</v>
+        <v>7.2</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="C19" s="41" t="s">
         <v>52</v>
@@ -2292,40 +2299,40 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
-        <v>8.1</v>
+        <v>8</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="C20" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="35">
-        <v>20</v>
+        <v>122</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="41">
+        <v>5</v>
       </c>
       <c r="G20"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
-        <v>8.1999999999999993</v>
+        <v>8.1</v>
       </c>
       <c r="B21" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="41">
-        <v>5</v>
+      <c r="C21" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="35">
+        <v>20</v>
       </c>
       <c r="G21"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
-        <v>9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="C22" s="41" t="s">
         <v>52</v>
@@ -2336,76 +2343,87 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="35">
-        <v>20</v>
+        <v>87</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="41">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
-        <v>9.1999999999999993</v>
+        <v>9.1</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="41">
-        <v>5</v>
+        <v>82</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="35">
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
-        <v>10</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="31">
-        <v>25</v>
+        <v>83</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="41">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="41">
-        <v>5</v>
+        <v>59</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="31">
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
+        <v>11</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="20">
         <v>11.1</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C28" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D28" s="32">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
@@ -2415,9 +2433,6 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
@@ -2708,10 +2723,10 @@
       <c r="E73" s="26"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="21"/>
-      <c r="B74" s="21"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="21"/>
+      <c r="A74" s="20"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="21"/>
@@ -2855,9 +2870,15 @@
       <c r="D94" s="21"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="27"/>
-      <c r="B95" s="27"/>
-      <c r="D95" s="27"/>
+      <c r="A95" s="21"/>
+      <c r="B95" s="21"/>
+      <c r="C95" s="21"/>
+      <c r="D95" s="21"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
+      <c r="D96" s="27"/>
     </row>
   </sheetData>
   <sortState ref="A2:D98">
@@ -2938,33 +2959,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" t="s">
         <v>101</v>
       </c>
-      <c r="E4" t="s">
-        <v>103</v>
-      </c>
       <c r="F4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -2972,13 +2993,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -2986,7 +3007,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -2994,7 +3015,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3002,10 +3023,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3013,7 +3034,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3021,7 +3042,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3029,7 +3050,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3037,7 +3058,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3045,7 +3066,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
adj schedule. rebuild wk 2 and 3
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -166,20 +166,9 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">* Identify a handful of problems that can creep up when building a model
-* Conduct a fully reproducible analysis that includes and data preparation, exploration, and analysis steps including model building. </t>
-  </si>
-  <si>
     <t>Special Considerations, , Team Check ins</t>
   </si>
   <si>
-    <t>* Team check-ups. How are things going? What problems are arising? How can we help troubleshoot as a class? 
-* Open work time to work on your modeling assignment, or in your groups on current analyses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Start working on the model building homework. </t>
-  </si>
-  <si>
     <t>* http://rmarkdown.rstudio.com/lesson-11.html</t>
   </si>
   <si>
@@ -223,16 +212,6 @@
   </si>
   <si>
     <t>Poster Presentations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* QFT Model Building
-* Missing Data (PMA5 9.2) -- Just Intro. We'll come back to this topic in more detail later. 
-* Multicollinearity (PMA5 9.5)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Read Afifi Ch 12
-</t>
   </si>
   <si>
     <t>* Install the caret and ROCR packages</t>
@@ -559,17 +538,39 @@
 * Team project Research proposal (Due  2/16)</t>
   </si>
   <si>
-    <t>* PMA5 Ch 7, 8.4-8.7, selections from Ch 9
-* [[Article on how to prepare a research proposal]](https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3282423/)</t>
-  </si>
-  <si>
     <t>Research Proposal</t>
+  </si>
+  <si>
+    <t>* PMA5 Ch 7, 8.4-8.7, 9.3
+* [[Article on how to prepare a research proposal]](https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3282423/)
+* [[Article on how to control confounding effects by statistical analysis]](https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4017459/)</t>
+  </si>
+  <si>
+    <t>* Open work time to work on your modeling assignment, or in your groups on current analyses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Start working on the model building homework. 
+* Have met with your team at least once by now. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* QFT Model Building
+* Model  building: What to watch out for
+* Team check-ins: How are things going? What problems are arising? How can we help troubleshoot as a class? 
+</t>
+  </si>
+  <si>
+    <t>* Identify a handful of problems that can creep up when building a model
+* Conduct a fully reproducible analysis that includes and data preparation, exploration, and analysis steps including model building. 
+* Interpret a bivariate relationship between two categorical variables</t>
+  </si>
+  <si>
+    <t>* 2x2 tables, Odds Ratios, Risk Ratios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -620,12 +621,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -648,8 +643,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -701,6 +702,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -868,11 +875,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -898,9 +905,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -925,10 +929,10 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="91" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="91" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="91" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="91" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -942,7 +946,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="92" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="92" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -955,9 +959,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -988,6 +989,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="90" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="93">
@@ -1080,9 +1090,9 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
     <cellStyle name="Percent" xfId="90" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Percent 2" xfId="52"/>
     <cellStyle name="Total" xfId="92" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1424,12 +1434,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1444,13 +1454,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1459,7 +1469,7 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1471,12 +1481,12 @@
       <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
       <c r="B2" s="3">
@@ -1489,26 +1499,26 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="G2" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" s="43" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
         <v>2</v>
       </c>
       <c r="B3" s="3">
@@ -1522,26 +1532,26 @@
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="H3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="28" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17">
+      <c r="J3" s="27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
         <v>3</v>
       </c>
       <c r="B4" s="3">
@@ -1549,28 +1559,30 @@
         <v>41674</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>41</v>
+        <v>148</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" s="28"/>
+        <v>147</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
+      <c r="A5" s="16">
         <v>4</v>
       </c>
       <c r="B5" s="3">
@@ -1578,32 +1590,30 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="E5" s="4"/>
       <c r="F5" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J5" s="28" t="s">
-        <v>73</v>
+      <c r="I5" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
       <c r="B6" s="3">
@@ -1611,30 +1621,30 @@
         <v>41688</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>74</v>
+        <v>61</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>69</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="28"/>
+      <c r="J6" s="27"/>
     </row>
     <row r="7" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <v>6</v>
       </c>
       <c r="B7" s="3">
@@ -1642,19 +1652,19 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>17</v>
@@ -1663,11 +1673,11 @@
         <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
         <v>7</v>
       </c>
       <c r="B8" s="3">
@@ -1675,20 +1685,20 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>16</v>
@@ -1696,7 +1706,7 @@
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
+      <c r="A9" s="16">
         <v>8</v>
       </c>
       <c r="B9" s="3">
@@ -1704,41 +1714,41 @@
         <v>41709</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
@@ -1758,12 +1768,12 @@
         <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1793,18 +1803,18 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="16"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1841,12 +1851,12 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1881,16 +1891,16 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1911,7 +1921,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1923,7 +1933,7 @@
       <c r="E20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="15" t="s">
         <v>25</v>
       </c>
       <c r="J20" s="4" t="s">
@@ -1932,7 +1942,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F20" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1940,7 +1950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1949,931 +1959,931 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="23"/>
-    <col min="2" max="2" width="32.25" style="23" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="7.75" style="23"/>
+    <col min="1" max="1" width="9" style="22"/>
+    <col min="2" max="2" width="32.25" style="22" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="7.75" style="22"/>
     <col min="5" max="5" width="5.125" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="10" style="20" customWidth="1"/>
-    <col min="8" max="8" width="7.75" style="20"/>
-    <col min="9" max="9" width="4.75" style="20" customWidth="1"/>
+    <col min="7" max="7" width="10" style="19" customWidth="1"/>
+    <col min="8" max="8" width="7.75" style="19"/>
+    <col min="9" max="9" width="4.75" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>47</v>
       </c>
+      <c r="G1" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="41">
+      <c r="B2" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="39">
         <v>5</v>
       </c>
-      <c r="F2" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="38">
+      <c r="F2" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="36">
         <f>SUMIF($C$2:$C$87,F2,$D$2:$D$87)</f>
         <v>120</v>
       </c>
-      <c r="H2" s="40">
+      <c r="H2" s="38">
         <f>G2/$G$6</f>
         <v>0.25531914893617019</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20">
+      <c r="A3" s="19">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="41">
+      <c r="B3" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="39">
         <v>20</v>
       </c>
-      <c r="F3" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="41">
+      <c r="F3" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="39">
         <f>SUMIF($C$2:$C$87,F3,$D$2:$D$87)</f>
         <v>90</v>
       </c>
-      <c r="H3" s="43">
+      <c r="H3" s="41">
         <f>G3/$G$6</f>
         <v>0.19148936170212766</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
+      <c r="A4" s="19">
         <v>2</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="35">
+      <c r="B4" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="33">
         <v>10</v>
       </c>
-      <c r="F4" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="32">
+      <c r="F4" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="30">
         <f>SUMIF($C$2:$C$87,F4,$D$2:$D$87)</f>
         <v>200</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H4" s="32">
         <f>G4/$G$6</f>
         <v>0.42553191489361702</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="A5" s="19">
         <v>2.1</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="41">
+      <c r="B5" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="39">
         <v>5</v>
       </c>
-      <c r="F5" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="31">
+      <c r="F5" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="29">
         <f>SUMIF($C$2:$C$87,F5,$D$2:$D$87)</f>
         <v>60</v>
       </c>
-      <c r="H5" s="37">
+      <c r="H5" s="35">
         <f>G5/$G$6</f>
         <v>0.1276595744680851</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20">
+      <c r="A6" s="19">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="35">
+      <c r="B6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="33">
         <v>10</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="24">
         <f>SUM(G2:G5)</f>
         <v>470</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="A7" s="19">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="41">
+      <c r="B7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="39">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+      <c r="A8" s="19">
         <v>2.4</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="19">
+        <v>3</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
+        <v>3.1</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="31">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
-        <v>3</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="35">
+      <c r="D10" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="19">
+        <v>4</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="39">
+        <v>5</v>
+      </c>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="33">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
-        <v>3.1</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="41">
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="19">
+        <v>4.2</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="39">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
-        <v>4</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="41">
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
         <v>5</v>
       </c>
-      <c r="G11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="35">
+      <c r="B14" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="39">
+        <v>5</v>
+      </c>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="19">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="30">
+        <v>100</v>
+      </c>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="19">
+        <v>6</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="29">
         <v>20</v>
       </c>
-      <c r="G12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="20">
-        <v>4.2</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="41">
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="19">
+        <v>7</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="39">
         <v>5</v>
       </c>
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="19">
+        <v>7.1</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="33">
+        <v>20</v>
+      </c>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="19">
+        <v>7.2</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="39">
         <v>5</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="41">
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
+        <v>8</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="39">
         <v>5</v>
       </c>
-      <c r="G14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="32">
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="19">
+        <v>8.1</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="33">
+        <v>20</v>
+      </c>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="19">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="19">
+        <v>9</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="19">
+        <v>9.1</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="19">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="19">
+        <v>10</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="19">
+        <v>11</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="19">
+        <v>11.1</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="30">
         <v>100</v>
       </c>
-      <c r="G15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
-        <v>6</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="31">
-        <v>20</v>
-      </c>
-      <c r="G16"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
-        <v>7</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="41">
-        <v>5</v>
-      </c>
-      <c r="G17"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
-        <v>7.1</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="35">
-        <v>20</v>
-      </c>
-      <c r="G18"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
-        <v>7.2</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="41">
-        <v>5</v>
-      </c>
-      <c r="G19"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
-        <v>8</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="41">
-        <v>5</v>
-      </c>
-      <c r="G20"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
-        <v>8.1</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="35">
-        <v>20</v>
-      </c>
-      <c r="G21"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="41">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
-        <v>9</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="41">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="20">
-        <v>9.1</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="35">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="20">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="41">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="20">
-        <v>10</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="31">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="20">
-        <v>11</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="41">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="20">
-        <v>11.1</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="32">
-        <v>100</v>
-      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="19"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="19"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="19"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="26"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="25"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
+      <c r="A42" s="19"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="26"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="25"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="26"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="25"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="26"/>
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="25"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="26"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="25"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="26"/>
+      <c r="A51" s="19"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="25"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="26"/>
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="25"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="26"/>
+      <c r="A53" s="19"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="25"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="26"/>
+      <c r="A54" s="19"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="25"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="26"/>
+      <c r="A55" s="19"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="25"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="20"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="26"/>
+      <c r="A56" s="19"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="25"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="26"/>
+      <c r="A57" s="19"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="25"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="26"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="25"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="20"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="26"/>
+      <c r="A59" s="19"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="25"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="20"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="26"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="25"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="26"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="25"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="20"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="26"/>
+      <c r="A62" s="19"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="25"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="26"/>
+      <c r="A63" s="19"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="25"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="24"/>
-      <c r="G64" s="23"/>
-      <c r="H64" s="23"/>
+      <c r="A64" s="19"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="22"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="23"/>
-      <c r="H65" s="23"/>
+      <c r="A65" s="19"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="22"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="20"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="22"/>
-      <c r="I66" s="23"/>
+      <c r="A66" s="19"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="21"/>
+      <c r="I66" s="22"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
-      <c r="B67" s="20"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="22"/>
-      <c r="I67" s="23"/>
+      <c r="A67" s="19"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="21"/>
+      <c r="I67" s="22"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="26"/>
+      <c r="A68" s="19"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="25"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="26"/>
+      <c r="A69" s="19"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="25"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="26"/>
+      <c r="A70" s="19"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="25"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="20"/>
-      <c r="B71" s="20"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="26"/>
+      <c r="A71" s="19"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="25"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
-      <c r="B72" s="20"/>
-      <c r="C72" s="20"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="26"/>
+      <c r="A72" s="19"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="25"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="20"/>
-      <c r="B73" s="20"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="26"/>
+      <c r="A73" s="19"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="25"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="20"/>
-      <c r="B74" s="20"/>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20"/>
+      <c r="A74" s="19"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="21"/>
-      <c r="B75" s="21"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
+      <c r="A75" s="20"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="21"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="21"/>
-      <c r="D76" s="21"/>
+      <c r="A76" s="20"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="21"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
+      <c r="A77" s="20"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="20"/>
+      <c r="D77" s="20"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="21"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
+      <c r="A78" s="20"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="20"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="21"/>
-      <c r="B79" s="21"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
+      <c r="A79" s="20"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="20"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="21"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
-      <c r="E80" s="24"/>
+      <c r="A80" s="20"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="23"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="21"/>
-      <c r="B81" s="21"/>
-      <c r="C81" s="21"/>
-      <c r="D81" s="21"/>
-      <c r="E81" s="24"/>
+      <c r="A81" s="20"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="23"/>
       <c r="G81"/>
       <c r="H81"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="21"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
-      <c r="E82" s="24"/>
+      <c r="A82" s="20"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="23"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="21"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="21"/>
-      <c r="D83" s="21"/>
+      <c r="A83" s="20"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="20"/>
       <c r="G83"/>
       <c r="H83"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="21"/>
-      <c r="B84" s="21"/>
-      <c r="C84" s="21"/>
-      <c r="D84" s="21"/>
+      <c r="A84" s="20"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
       <c r="G84"/>
       <c r="H84"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="21"/>
-      <c r="B85" s="21"/>
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
+      <c r="A85" s="20"/>
+      <c r="B85" s="20"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="20"/>
       <c r="G85"/>
       <c r="H85"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="21"/>
-      <c r="B86" s="21"/>
-      <c r="C86" s="21"/>
-      <c r="D86" s="21"/>
+      <c r="A86" s="20"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="20"/>
       <c r="G86"/>
       <c r="H86"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="21"/>
-      <c r="B87" s="21"/>
-      <c r="C87" s="21"/>
-      <c r="D87" s="21"/>
+      <c r="A87" s="20"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="20"/>
       <c r="G87"/>
       <c r="H87"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="21"/>
-      <c r="B88" s="21"/>
-      <c r="C88" s="21"/>
-      <c r="D88" s="21"/>
+      <c r="A88" s="20"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="20"/>
+      <c r="D88" s="20"/>
       <c r="G88"/>
       <c r="H88"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="21"/>
-      <c r="B89" s="21"/>
-      <c r="C89" s="21"/>
-      <c r="D89" s="21"/>
+      <c r="A89" s="20"/>
+      <c r="B89" s="20"/>
+      <c r="C89" s="20"/>
+      <c r="D89" s="20"/>
       <c r="G89"/>
       <c r="H89"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="21"/>
-      <c r="B90" s="21"/>
-      <c r="C90" s="21"/>
-      <c r="D90" s="21"/>
+      <c r="A90" s="20"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="20"/>
       <c r="G90"/>
       <c r="H90"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="21"/>
-      <c r="B91" s="21"/>
-      <c r="C91" s="21"/>
-      <c r="D91" s="21"/>
+      <c r="A91" s="20"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="20"/>
+      <c r="D91" s="20"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="21"/>
-      <c r="B92" s="21"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="21"/>
+      <c r="A92" s="20"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="20"/>
+      <c r="D92" s="20"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="21"/>
-      <c r="B93" s="21"/>
-      <c r="C93" s="21"/>
-      <c r="D93" s="21"/>
+      <c r="A93" s="20"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="20"/>
+      <c r="D93" s="20"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="21"/>
-      <c r="B94" s="21"/>
-      <c r="C94" s="21"/>
-      <c r="D94" s="21"/>
+      <c r="A94" s="20"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="20"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="21"/>
-      <c r="B95" s="21"/>
-      <c r="C95" s="21"/>
-      <c r="D95" s="21"/>
+      <c r="A95" s="20"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="20"/>
+      <c r="D95" s="20"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="27"/>
-      <c r="B96" s="27"/>
-      <c r="D96" s="27"/>
+      <c r="A96" s="26"/>
+      <c r="B96" s="26"/>
+      <c r="D96" s="26"/>
     </row>
   </sheetData>
   <sortState ref="A2:D98">
@@ -2884,7 +2894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2938,7 +2948,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2954,33 +2964,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -2988,13 +2998,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -3002,7 +3012,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -3010,7 +3020,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3018,10 +3028,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F10" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3029,7 +3039,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3037,7 +3047,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3045,7 +3055,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3053,7 +3063,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3061,7 +3071,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
remove hard coding from wk3 topic
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -166,9 +166,6 @@
 </t>
   </si>
   <si>
-    <t>Special Considerations, , Team Check ins</t>
-  </si>
-  <si>
     <t>* http://rmarkdown.rstudio.com/lesson-11.html</t>
   </si>
   <si>
@@ -565,6 +562,9 @@
   </si>
   <si>
     <t>* 2x2 tables, Odds Ratios, Risk Ratios</t>
+  </si>
+  <si>
+    <t>Model building recap, Team Check ins, bivariate categorical analysis</t>
   </si>
 </sst>
 </file>
@@ -1439,7 +1439,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1499,22 +1499,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" s="43" t="s">
         <v>137</v>
-      </c>
-      <c r="H2" s="43" t="s">
-        <v>138</v>
       </c>
       <c r="I2" s="43" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1532,13 +1532,13 @@
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="42" t="s">
         <v>140</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>141</v>
       </c>
       <c r="H3" s="43" t="s">
         <v>38</v>
@@ -1547,7 +1547,7 @@
         <v>40</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1559,25 +1559,25 @@
         <v>41674</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>149</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I4" s="44" t="s">
         <v>148</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="I4" s="44" t="s">
-        <v>149</v>
       </c>
       <c r="J4" s="27"/>
     </row>
@@ -1590,26 +1590,26 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1621,22 +1621,22 @@
         <v>41688</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>16</v>
@@ -1652,19 +1652,19 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>17</v>
@@ -1673,7 +1673,7 @@
         <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1685,20 +1685,20 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G8" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>16</v>
@@ -1714,28 +1714,28 @@
         <v>41709</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="F9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="J9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1768,12 +1768,12 @@
         <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1803,18 +1803,18 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="15"/>
       <c r="G13" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1891,16 +1891,16 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1921,7 +1921,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1972,25 +1972,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>48</v>
-      </c>
       <c r="F1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>48</v>
-      </c>
       <c r="H1" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1998,16 +1998,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="39">
         <v>5</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="36">
         <f>SUMIF($C$2:$C$87,F2,$D$2:$D$87)</f>
@@ -2023,16 +2023,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="39">
         <v>20</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3" s="39">
         <f>SUMIF($C$2:$C$87,F3,$D$2:$D$87)</f>
@@ -2048,16 +2048,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="33">
         <v>10</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" s="30">
         <f>SUMIF($C$2:$C$87,F4,$D$2:$D$87)</f>
@@ -2073,16 +2073,16 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="39">
         <v>5</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" s="29">
         <f>SUMIF($C$2:$C$87,F5,$D$2:$D$87)</f>
@@ -2098,10 +2098,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="33">
         <v>10</v>
@@ -2116,10 +2116,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="39">
         <v>5</v>
@@ -2130,10 +2130,10 @@
         <v>2.4</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="29">
         <v>15</v>
@@ -2144,10 +2144,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="33">
         <v>20</v>
@@ -2158,10 +2158,10 @@
         <v>3.1</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="39">
         <v>5</v>
@@ -2172,10 +2172,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="39">
         <v>5</v>
@@ -2187,10 +2187,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="33">
         <v>20</v>
@@ -2202,10 +2202,10 @@
         <v>4.2</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="39">
         <v>5</v>
@@ -2217,10 +2217,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="39">
         <v>5</v>
@@ -2232,10 +2232,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="30">
         <v>100</v>
@@ -2247,10 +2247,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="29">
         <v>20</v>
@@ -2262,10 +2262,10 @@
         <v>7</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="39">
         <v>5</v>
@@ -2277,10 +2277,10 @@
         <v>7.1</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="33">
         <v>20</v>
@@ -2292,10 +2292,10 @@
         <v>7.2</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="39">
         <v>5</v>
@@ -2307,10 +2307,10 @@
         <v>8</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="39">
         <v>5</v>
@@ -2322,10 +2322,10 @@
         <v>8.1</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="33">
         <v>20</v>
@@ -2337,10 +2337,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C22" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="39">
         <v>5</v>
@@ -2351,10 +2351,10 @@
         <v>9</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="39">
         <v>5</v>
@@ -2365,10 +2365,10 @@
         <v>9.1</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="33">
         <v>20</v>
@@ -2379,10 +2379,10 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="39">
         <v>5</v>
@@ -2393,10 +2393,10 @@
         <v>10</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D26" s="29">
         <v>25</v>
@@ -2407,10 +2407,10 @@
         <v>11</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="39">
         <v>5</v>
@@ -2424,7 +2424,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="30">
         <v>100</v>
@@ -2964,33 +2964,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
         <v>92</v>
       </c>
-      <c r="C4" t="s">
-        <v>93</v>
-      </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" t="s">
         <v>92</v>
-      </c>
-      <c r="G4" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="s">
         <v>96</v>
-      </c>
-      <c r="F5" t="s">
-        <v>97</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -2998,13 +2998,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -3012,7 +3012,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -3020,7 +3020,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3028,10 +3028,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" t="s">
         <v>101</v>
-      </c>
-      <c r="F10" t="s">
-        <v>102</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3039,7 +3039,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3047,7 +3047,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3055,7 +3055,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3063,7 +3063,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3071,7 +3071,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
add bold to due dates in schedule
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -254,10 +254,6 @@
     <t>Peer Review GLM Assignment</t>
   </si>
   <si>
-    <t>* GLM assignment (Due Fri 2/23)
-* Peer Review GLM Assignment (Due Sun 2/25)</t>
-  </si>
-  <si>
     <t>* Use  Logistic Regression to classify observations into two groups
 * Identify the optimal cutoff point for a binary classifier
 * Create and interpret a ROC curve
@@ -470,9 +466,6 @@
   <si>
     <t>* Fine tuning your factor model by rotating the axes
 * Using FA as a modeling tool by creating factor scores</t>
-  </si>
-  <si>
-    <t>* PMA5 Ch 9.2, 9.5</t>
   </si>
   <si>
     <t>* PMA5 Ch 12.1-12.7, p. 289
@@ -558,24 +551,33 @@
 * Interpret a bivariate relationship between two categorical variables</t>
   </si>
   <si>
-    <t>* 2x2 tables, Odds Ratios, Risk Ratios</t>
-  </si>
-  <si>
-    <t>Model building recap, Team Check ins, bivariate categorical analysis</t>
-  </si>
-  <si>
     <t>* Structural and content expectations for Model Building Report 
 * Open work time to work on your modeling assignment, or in your groups on current analyses</t>
   </si>
   <si>
     <t>Class Cancelled - Robin speaking at the [Global Women in Data Science Conference](http://www.widsconference.org/). Live stream available!</t>
+  </si>
+  <si>
+    <t>* Worksheet on translating research questions from english, to mathmatical notation, to code
+* 2x2 tables, Odds Ratios, Risk Ratios</t>
+  </si>
+  <si>
+    <t>Model building recap &amp;  Team Check ins, Expectations for HW1,  Model writing and Odds Ratios</t>
+  </si>
+  <si>
+    <t>* PMA5 Ch 9.2, 9.5
+* [[Notes on Odds Ratios]](www.norcalbiostat.com/lec/cda/)</t>
+  </si>
+  <si>
+    <t>* GLM assignment (Due Fri 2/23)
+* Peer Review GLM Assignment (Due Sun 2/25)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -646,12 +648,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -889,7 +885,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1004,9 +1000,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1448,25 +1441,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="28.125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="27.75" style="5" customWidth="1"/>
-    <col min="6" max="6" width="21.875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="30.125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="32.875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="30.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="28.125" style="5" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="27.75" style="5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="21.875" style="5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="30.125" style="5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="32.875" style="5" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5" style="5" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="36.75" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -1498,7 +1491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -1512,25 +1505,25 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H2" s="43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I2" s="43" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -1545,13 +1538,13 @@
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H3" s="43" t="s">
         <v>38</v>
@@ -1560,11 +1553,11 @@
         <v>40</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="44">
         <v>3</v>
       </c>
       <c r="B4" s="3">
@@ -1575,26 +1568,26 @@
         <v>148</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="I4" s="44" t="s">
+      <c r="I4" s="28" t="s">
         <v>147</v>
       </c>
       <c r="J4" s="27"/>
     </row>
-    <row r="5" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -1610,7 +1603,7 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G5" s="28" t="s">
         <v>58</v>
@@ -1622,11 +1615,11 @@
         <v>61</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="45">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="44">
         <v>5</v>
       </c>
       <c r="B6" s="3">
@@ -1637,7 +1630,7 @@
         <v>60</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>56</v>
@@ -1646,17 +1639,17 @@
         <v>62</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>57</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J6" s="27"/>
     </row>
-    <row r="7" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>6</v>
       </c>
@@ -1665,19 +1658,19 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>17</v>
@@ -1686,10 +1679,10 @@
         <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>7</v>
       </c>
@@ -1698,27 +1691,27 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G8" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>8</v>
       </c>
@@ -1727,31 +1720,31 @@
         <v>41709</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>42</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="10"/>
@@ -1763,7 +1756,7 @@
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1781,15 +1774,15 @@
         <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1805,9 +1798,8 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1816,21 +1808,21 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="15"/>
       <c r="G13" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1847,7 +1839,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:11" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1864,15 +1856,15 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1904,16 +1896,16 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1934,7 +1926,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1985,7 +1977,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>44</v>
@@ -2011,7 +2003,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="39" t="s">
         <v>48</v>
@@ -2086,7 +2078,7 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="39" t="s">
         <v>48</v>
@@ -2143,7 +2135,7 @@
         <v>2.4</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>45</v>
@@ -2185,7 +2177,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C11" s="39" t="s">
         <v>48</v>
@@ -2200,7 +2192,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="33" t="s">
         <v>44</v>
@@ -2215,7 +2207,7 @@
         <v>4.2</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="39" t="s">
         <v>48</v>
@@ -2230,7 +2222,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="39" t="s">
         <v>48</v>
@@ -2245,7 +2237,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="30" t="s">
         <v>49</v>
@@ -2275,7 +2267,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" s="39" t="s">
         <v>48</v>
@@ -2290,7 +2282,7 @@
         <v>7.1</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="33" t="s">
         <v>44</v>
@@ -2305,7 +2297,7 @@
         <v>7.2</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" s="39" t="s">
         <v>48</v>
@@ -2320,7 +2312,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20" s="39" t="s">
         <v>48</v>
@@ -2335,7 +2327,7 @@
         <v>8.1</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21" s="33" t="s">
         <v>44</v>
@@ -2350,7 +2342,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C22" s="39" t="s">
         <v>48</v>
@@ -2364,7 +2356,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" s="39" t="s">
         <v>48</v>
@@ -2378,7 +2370,7 @@
         <v>9.1</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="33" t="s">
         <v>44</v>
@@ -2392,7 +2384,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="39" t="s">
         <v>48</v>
@@ -2420,7 +2412,7 @@
         <v>11</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" s="39" t="s">
         <v>48</v>
@@ -2977,33 +2969,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
-        <v>92</v>
-      </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" t="s">
         <v>91</v>
-      </c>
-      <c r="G4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s">
         <v>95</v>
-      </c>
-      <c r="F5" t="s">
-        <v>96</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -3011,13 +3003,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -3025,7 +3017,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -3033,7 +3025,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3041,10 +3033,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" t="s">
         <v>100</v>
-      </c>
-      <c r="F10" t="s">
-        <v>101</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3052,7 +3044,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3060,7 +3052,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3068,7 +3060,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3076,7 +3068,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3084,7 +3076,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
add wk4 announcements, rebuild wk4/wk5
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="152">
   <si>
     <t>Finals Week</t>
   </si>
@@ -222,9 +222,6 @@
     <t xml:space="preserve">* Fitting and interpreting Logistic Regression models. 
 * Odds Ratios are always the odds of an event for one group compared to another group. 
 </t>
-  </si>
-  <si>
-    <t>Generalized Linear Models, Predicted Probabilities</t>
   </si>
   <si>
     <t>Classification, ROC curves, Confusion Matrix</t>
@@ -466,11 +463,6 @@
   <si>
     <t>* Fine tuning your factor model by rotating the axes
 * Using FA as a modeling tool by creating factor scores</t>
-  </si>
-  <si>
-    <t>* PMA5 Ch 12.1-12.7, p. 289
-* [Goodness of Fit](https://www.r-bloggers.com/logistic-regression-in-r-part-two/)
-* PMA5 Ch 12.11 (Poisson Regression)</t>
   </si>
   <si>
     <t xml:space="preserve">* PMA5 Ch 15
@@ -571,6 +563,19 @@
   <si>
     <t>* PMA5 Ch 9.2, 9.5
 * [[Notes on Odds Ratios]](http://www.norcalbiostat.com/lec/cda/)</t>
+  </si>
+  <si>
+    <t>Generalized Linear Models, Predicted Probabilities, Count data</t>
+  </si>
+  <si>
+    <t>* Read selected book chapters. 
+* Notebook Chapter 5.1, 5.21.-5.2.4 (Binary Data), 5.4(Count data)</t>
+  </si>
+  <si>
+    <t>* PMA5 Ch 12.1-12.7, p. 289
+* PMA5 Ch 12.11 (Poisson Regression)
+* Notebook Chapter 5.1, 5.21.-5.2.4 (Binary Data), 5.4(Count data)
+* [Goodness of Fit notes](https://www.r-bloggers.com/logistic-regression-in-r-part-two/)</t>
   </si>
 </sst>
 </file>
@@ -650,7 +655,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -708,12 +713,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1002,8 +1001,8 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="93">
@@ -1444,8 +1443,8 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4:H4"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1505,22 +1504,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H2" s="43" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I2" s="43" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1538,13 +1537,13 @@
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H3" s="43" t="s">
         <v>38</v>
@@ -1553,7 +1552,7 @@
         <v>40</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1565,29 +1564,29 @@
         <v>41674</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>150</v>
-      </c>
       <c r="G4" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="I4" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="I4" s="28" t="s">
-        <v>147</v>
-      </c>
       <c r="J4" s="27"/>
     </row>
-    <row r="5" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -1596,30 +1595,32 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>149</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="F5" s="8" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="G5" s="28" t="s">
         <v>58</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="44">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
       <c r="B6" s="3">
@@ -1627,25 +1628,25 @@
         <v>41688</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>57</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J6" s="27"/>
     </row>
@@ -1658,19 +1659,19 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>17</v>
@@ -1679,7 +1680,7 @@
         <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1691,20 +1692,20 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G8" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>16</v>
@@ -1720,28 +1721,28 @@
         <v>41709</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>42</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1774,12 +1775,12 @@
         <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1808,18 +1809,18 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="15"/>
       <c r="G13" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1856,12 +1857,12 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1896,16 +1897,16 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1926,7 +1927,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1977,7 +1978,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>44</v>
@@ -2003,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="39" t="s">
         <v>48</v>
@@ -2078,7 +2079,7 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="39" t="s">
         <v>48</v>
@@ -2135,7 +2136,7 @@
         <v>2.4</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>45</v>
@@ -2149,7 +2150,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>44</v>
@@ -2163,7 +2164,7 @@
         <v>3.1</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="39" t="s">
         <v>48</v>
@@ -2177,7 +2178,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" s="39" t="s">
         <v>48</v>
@@ -2192,7 +2193,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="33" t="s">
         <v>44</v>
@@ -2207,7 +2208,7 @@
         <v>4.2</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="39" t="s">
         <v>48</v>
@@ -2222,7 +2223,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="39" t="s">
         <v>48</v>
@@ -2237,7 +2238,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="30" t="s">
         <v>49</v>
@@ -2267,7 +2268,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="39" t="s">
         <v>48</v>
@@ -2282,7 +2283,7 @@
         <v>7.1</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="33" t="s">
         <v>44</v>
@@ -2297,7 +2298,7 @@
         <v>7.2</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="39" t="s">
         <v>48</v>
@@ -2312,7 +2313,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" s="39" t="s">
         <v>48</v>
@@ -2327,7 +2328,7 @@
         <v>8.1</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" s="33" t="s">
         <v>44</v>
@@ -2342,7 +2343,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22" s="39" t="s">
         <v>48</v>
@@ -2356,7 +2357,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" s="39" t="s">
         <v>48</v>
@@ -2370,7 +2371,7 @@
         <v>9.1</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="33" t="s">
         <v>44</v>
@@ -2384,7 +2385,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="39" t="s">
         <v>48</v>
@@ -2412,7 +2413,7 @@
         <v>11</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="39" t="s">
         <v>48</v>
@@ -2969,33 +2970,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
         <v>90</v>
       </c>
-      <c r="C4" t="s">
-        <v>91</v>
-      </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" t="s">
         <v>90</v>
-      </c>
-      <c r="G4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" t="s">
         <v>94</v>
-      </c>
-      <c r="F5" t="s">
-        <v>95</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -3003,13 +3004,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -3017,7 +3018,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -3025,7 +3026,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3033,10 +3034,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" t="s">
         <v>99</v>
-      </c>
-      <c r="F10" t="s">
-        <v>100</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3044,7 +3045,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3052,7 +3053,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3060,7 +3061,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3068,7 +3069,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3076,7 +3077,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
fix week 5 schedule
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="154">
   <si>
     <t>Finals Week</t>
   </si>
@@ -214,17 +214,9 @@
     <t>* Install the caret and ROCR packages</t>
   </si>
   <si>
-    <t>* LogReg models the probability of being in group 1 (Y=1) compared to group 2 (Y=0).  
-* Thus it can be used to classify individuals into two groups, or predict the risk of an event. 
-* Logistic regression is one of the more common classification models.</t>
-  </si>
-  <si>
     <t xml:space="preserve">* Fitting and interpreting Logistic Regression models. 
 * Odds Ratios are always the odds of an event for one group compared to another group. 
 </t>
-  </si>
-  <si>
-    <t>Classification, ROC curves, Confusion Matrix</t>
   </si>
   <si>
     <t>* Poisson regression can be used to model count data (truncated at 0, whole integer values) (Reading: PMA5 12.11)</t>
@@ -251,13 +243,6 @@
     <t>Peer Review GLM Assignment</t>
   </si>
   <si>
-    <t>* Use  Logistic Regression to classify observations into two groups
-* Identify the optimal cutoff point for a binary classifier
-* Create and interpret a ROC curve
-* Create a confusion matrix
-* Calculate and explain terms such as Sensitivity, Specificity, and Accuracy</t>
-  </si>
-  <si>
     <t>* Explain how PCA can be used as a dimension reduction technique
 * Explain the difference between multivariate and multivariable
 * Conduct a PCA using both the correlation and covariance matrix
@@ -444,12 +429,6 @@
     <t>* In class portion of Midterm Exam (Wed 3/14) 
 * Take home portion of Midterm Exam (Due Friday 3/16)
 * Project Update Presentations (Fri 3/16)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Assess the proportion of individuals correctly classified as the cutoff  is changed.  (Reading: PMA5 Ch 12.8, start @ p 295)
-* Confusion matrices are used to determine how well a model does in classifying observations.  
-* Important measures are accuracy/sensitivity/specificity/false positive rate
-</t>
   </si>
   <si>
     <t xml:space="preserve">* QFT n&lt;&lt;&lt;p
@@ -576,6 +555,36 @@
 * PMA5 Ch 12.11 (Poisson Regression)
 * Notebook Chapter 5.1, 5.21.-5.2.4 (Binary Data), 5.4(Count data)
 * [Goodness of Fit notes](https://www.r-bloggers.com/logistic-regression-in-r-part-two/)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday I went into ROC curves b/c discussion went that way.  But that screwed up my schedule. Really just talk about all the logreg things before poisson next time. 
+Friday example was a disaster. Can't interpret rate of siblings, and I didn't exponentiate the results anyhow, nor provide interpretation. Shitty lecture. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* LogReg models the probability of being in group 1 (Y=1) compared to group 2 (Y=0).  
+* Thus it can be used to classify individuals into two groups, or predict the risk of an event. 
+* Logistic regression is one of the more common classification models.
+* Assess the proportion of individuals correctly classified as the cutoff  is changed.  (Reading: PMA5 Ch 12.8, start @ p 295)
+* Confusion matrices are used to determine how well a model does in classifying observations.  
+* Important measures are accuracy/sensitivity/specificity/false positive rate
+</t>
+  </si>
+  <si>
+    <t>* Translate english research questions to mathmatical notation, and R code. 
+* Use  Logistic Regression to classify observations into two groups
+* Identify the optimal cutoff point for a binary classifier
+* Create and interpret a ROC curve
+* Create a confusion matrix
+* Calculate and explain terms such as Sensitivity, Specificity, and Accuracy</t>
+  </si>
+  <si>
+    <t>Worksheet on model formulation. Write answers in Google Doc</t>
+  </si>
+  <si>
+    <t>* Answers to Model formulation worksheet written in Google Docs (Due Mon 2/19)</t>
+  </si>
+  <si>
+    <t>Model writing, Classification practice</t>
   </si>
 </sst>
 </file>
@@ -655,7 +664,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -713,6 +722,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,7 +899,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -961,9 +976,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1003,6 +1015,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="93">
@@ -1440,11 +1458,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1456,9 +1474,10 @@
     <col min="8" max="8" width="32.875" style="5" customWidth="1"/>
     <col min="9" max="9" width="30.5" style="5" customWidth="1"/>
     <col min="10" max="10" width="36.75" style="5" customWidth="1"/>
+    <col min="11" max="11" width="43.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -1490,7 +1509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -1504,25 +1523,25 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H2" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="I2" s="43" t="s">
+      <c r="G2" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" s="42" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -1537,25 +1556,25 @@
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" s="43" t="s">
+      <c r="G3" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="42" t="s">
         <v>40</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -1564,29 +1583,29 @@
         <v>41674</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G4" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="G4" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="I4" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="H4" s="43" t="s">
-        <v>143</v>
-      </c>
-      <c r="I4" s="44" t="s">
-        <v>145</v>
-      </c>
       <c r="J4" s="27"/>
     </row>
-    <row r="5" spans="1:10" ht="141" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -1595,31 +1614,34 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="G5" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>60</v>
-      </c>
       <c r="J5" s="27" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+      <c r="K5" s="45" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="230.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -1628,29 +1650,31 @@
         <v>41688</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>153</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>57</v>
+        <v>149</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="J6" s="27"/>
-    </row>
-    <row r="7" spans="1:10" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>6</v>
       </c>
@@ -1659,19 +1683,19 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>17</v>
@@ -1680,10 +1704,10 @@
         <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>7</v>
       </c>
@@ -1692,27 +1716,27 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>127</v>
+        <v>140</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>122</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>8</v>
       </c>
@@ -1721,31 +1745,31 @@
         <v>41709</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>42</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="10"/>
@@ -1757,7 +1781,7 @@
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1775,15 +1799,15 @@
         <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1800,7 +1824,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1809,21 +1833,21 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="15"/>
       <c r="G13" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1840,7 +1864,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1857,15 +1881,15 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1897,16 +1921,16 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1927,7 +1951,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1978,7 +2002,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>44</v>
@@ -2004,22 +2028,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D2" s="38">
         <v>5</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="36">
+      <c r="G2" s="35">
         <f>SUMIF($C$2:$C$87,F2,$D$2:$D$87)</f>
         <v>120</v>
       </c>
-      <c r="H2" s="38">
+      <c r="H2" s="37">
         <f>G2/$G$6</f>
         <v>0.25531914893617019</v>
       </c>
@@ -2031,20 +2055,20 @@
       <c r="B3" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D3" s="38">
         <v>20</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="39">
+      <c r="G3" s="38">
         <f>SUMIF($C$2:$C$87,F3,$D$2:$D$87)</f>
         <v>90</v>
       </c>
-      <c r="H3" s="41">
+      <c r="H3" s="40">
         <f>G3/$G$6</f>
         <v>0.19148936170212766</v>
       </c>
@@ -2056,20 +2080,20 @@
       <c r="B4" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="32">
         <v>10</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="29">
         <f>SUMIF($C$2:$C$87,F4,$D$2:$D$87)</f>
         <v>200</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="31">
         <f>G4/$G$6</f>
         <v>0.42553191489361702</v>
       </c>
@@ -2079,22 +2103,22 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="38">
         <v>5</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="28">
         <f>SUMIF($C$2:$C$87,F5,$D$2:$D$87)</f>
         <v>60</v>
       </c>
-      <c r="H5" s="35">
+      <c r="H5" s="34">
         <f>G5/$G$6</f>
         <v>0.1276595744680851</v>
       </c>
@@ -2106,10 +2130,10 @@
       <c r="B6" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="32">
         <v>10</v>
       </c>
       <c r="G6" s="24">
@@ -2124,10 +2148,10 @@
       <c r="B7" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="38">
         <v>5</v>
       </c>
     </row>
@@ -2136,12 +2160,12 @@
         <v>2.4</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="28">
         <v>15</v>
       </c>
     </row>
@@ -2150,12 +2174,12 @@
         <v>3</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="32">
         <v>20</v>
       </c>
     </row>
@@ -2164,12 +2188,12 @@
         <v>3.1</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="38">
         <v>5</v>
       </c>
     </row>
@@ -2178,12 +2202,12 @@
         <v>4</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="C11" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="38">
         <v>5</v>
       </c>
       <c r="G11"/>
@@ -2193,12 +2217,12 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="32">
         <v>20</v>
       </c>
       <c r="G12"/>
@@ -2208,12 +2232,12 @@
         <v>4.2</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="38">
         <v>5</v>
       </c>
       <c r="G13"/>
@@ -2223,12 +2247,12 @@
         <v>5</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="39">
+      <c r="D14" s="38">
         <v>5</v>
       </c>
       <c r="G14"/>
@@ -2238,12 +2262,12 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="29">
         <v>100</v>
       </c>
       <c r="G15"/>
@@ -2255,10 +2279,10 @@
       <c r="B16" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="28">
         <v>20</v>
       </c>
       <c r="G16"/>
@@ -2268,12 +2292,12 @@
         <v>7</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="39">
+      <c r="D17" s="38">
         <v>5</v>
       </c>
       <c r="G17"/>
@@ -2283,12 +2307,12 @@
         <v>7.1</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="32">
         <v>20</v>
       </c>
       <c r="G18"/>
@@ -2298,12 +2322,12 @@
         <v>7.2</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="39">
+      <c r="D19" s="38">
         <v>5</v>
       </c>
       <c r="G19"/>
@@ -2313,12 +2337,12 @@
         <v>8</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="C20" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="39">
+      <c r="D20" s="38">
         <v>5</v>
       </c>
       <c r="G20"/>
@@ -2328,12 +2352,12 @@
         <v>8.1</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="C21" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="32">
         <v>20</v>
       </c>
       <c r="G21"/>
@@ -2343,12 +2367,12 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="38">
         <v>5</v>
       </c>
     </row>
@@ -2357,12 +2381,12 @@
         <v>9</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="39">
+      <c r="D23" s="38">
         <v>5</v>
       </c>
     </row>
@@ -2371,12 +2395,12 @@
         <v>9.1</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="33">
+      <c r="D24" s="32">
         <v>20</v>
       </c>
     </row>
@@ -2385,12 +2409,12 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="39">
+      <c r="D25" s="38">
         <v>5</v>
       </c>
     </row>
@@ -2401,10 +2425,10 @@
       <c r="B26" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="28">
         <v>25</v>
       </c>
     </row>
@@ -2413,12 +2437,12 @@
         <v>11</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="39">
+      <c r="D27" s="38">
         <v>5</v>
       </c>
     </row>
@@ -2429,10 +2453,10 @@
       <c r="B28" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="30">
+      <c r="D28" s="29">
         <v>100</v>
       </c>
     </row>
@@ -2970,33 +2994,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
         <v>89</v>
       </c>
-      <c r="C4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" t="s">
-        <v>92</v>
-      </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -3004,13 +3028,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -3018,7 +3042,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -3026,7 +3050,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3034,10 +3058,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3045,7 +3069,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3053,7 +3077,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3061,7 +3085,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3069,7 +3093,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3077,7 +3101,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
add wk8 and update schedule
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C773DD3-5308-4A71-9EC9-490A9B6DA6A8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E47E39-5914-4B99-94FB-BA81FCBACB6E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="159">
   <si>
     <t>Finals Week</t>
   </si>
@@ -170,9 +170,6 @@
     <t>* http://rmarkdown.rstudio.com/lesson-11.html</t>
   </si>
   <si>
-    <t>* Project Update Presentations. X minute group presentations with slides prepared in R Markdown</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -365,9 +362,6 @@
 * Peer Review (Due Sun 3/11)</t>
   </si>
   <si>
-    <t>In class Midterm</t>
-  </si>
-  <si>
     <t>* Missing Data Assignment (Due Fri 5/4)
 * Peer Review (Due Sun 5/6)</t>
   </si>
@@ -419,11 +413,6 @@
   </si>
   <si>
     <t>* Explain the difference between PCA and FA</t>
-  </si>
-  <si>
-    <t>* In class portion of Midterm Exam (Wed 3/14) 
-* Take home portion of Midterm Exam (Due Friday 3/16)
-* Project Update Presentations (Fri 3/16)</t>
   </si>
   <si>
     <t xml:space="preserve">* QFT n&lt;&lt;&lt;p
@@ -596,6 +585,34 @@
   </si>
   <si>
     <t>Classification Practice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forgot to do QFT. Turned this into a reading quiz on FA for following Wednesday. They failed miserably. 
+Seemed to not blow their mind with PCA. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FA == mind blown. Big time. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* In class portion of Midterm Exam (Wed 3/14) 
+* Project Update Presentations (Fri 3/16)
+* Take home portion of Midterm Exam (Due Sunday 3/18)
+</t>
+  </si>
+  <si>
+    <t>* In class Midterm (60%)
+* Take home portion (40%) posted in Slack #assignments by EOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Project Update Presentations. 5 minute group presentations with slides prepared in R Markdown
+* This means no more than 3-4 slides per group.
+* This is worth 20 pts, so make it good. You have 4-5 minutes and 3-4 slides to show me that
+* you know what your data consists of
+* you have gotten it into R and started exploring/visualizing/cleaning
+* you should be starting to do bivariate comparisons at this point
+* you have a clear idea of what model you are working towards
+* and that EVERYONE is contributing. Everyone must share in the presentation
+  </t>
   </si>
 </sst>
 </file>
@@ -1477,9 +1494,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1540,22 +1557,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H2" s="42" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I2" s="42" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1573,13 +1590,13 @@
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H3" s="42" t="s">
         <v>38</v>
@@ -1588,7 +1605,7 @@
         <v>40</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1600,25 +1617,25 @@
         <v>41674</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="43" t="s">
         <v>137</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G4" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="H4" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="I4" s="43" t="s">
-        <v>140</v>
       </c>
       <c r="J4" s="27"/>
     </row>
@@ -1631,31 +1648,31 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="K5" s="45" t="s">
         <v>144</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="G5" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="K5" s="45" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="230.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1667,31 +1684,31 @@
         <v>41688</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="K6" s="47" t="s">
         <v>151</v>
-      </c>
-      <c r="K6" s="47" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1703,19 +1720,19 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
+      </c>
+      <c r="G7" s="46" t="s">
+        <v>117</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>17</v>
@@ -1724,7 +1741,10 @@
         <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="K7" s="47" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1736,27 +1756,30 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="243" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>8</v>
       </c>
@@ -1765,28 +1788,28 @@
         <v>41709</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>102</v>
+        <v>157</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>42</v>
+        <v>158</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1819,12 +1842,12 @@
         <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1853,18 +1876,18 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="15"/>
       <c r="G13" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1901,12 +1924,12 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1941,16 +1964,16 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1971,7 +1994,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2003,7 +2026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12:D12"/>
     </sheetView>
   </sheetViews>
@@ -2022,25 +2045,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>47</v>
-      </c>
       <c r="F1" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>47</v>
-      </c>
       <c r="H1" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2048,16 +2071,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="38">
         <v>5</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2" s="35">
         <f>SUMIF($C$2:$C$89,F2,$D$2:$D$89)</f>
@@ -2073,16 +2096,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="38">
         <v>20</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="38">
         <f>SUMIF($C$2:$C$89,F3,$D$2:$D$89)</f>
@@ -2098,16 +2121,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="32">
         <v>10</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="29">
         <f>SUMIF($C$2:$C$89,F4,$D$2:$D$89)</f>
@@ -2123,16 +2146,16 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="38">
         <v>5</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="28">
         <f>SUMIF($C$2:$C$89,F5,$D$2:$D$89)</f>
@@ -2148,10 +2171,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="32">
         <v>10</v>
@@ -2166,10 +2189,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="38">
         <v>5</v>
@@ -2180,10 +2203,10 @@
         <v>2.4</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="28">
         <v>15</v>
@@ -2194,10 +2217,10 @@
         <v>2.5</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="38">
         <v>5</v>
@@ -2208,10 +2231,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="32">
         <v>20</v>
@@ -2222,10 +2245,10 @@
         <v>3.1</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="38">
         <v>5</v>
@@ -2236,10 +2259,10 @@
         <v>3.2</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="38">
         <v>5</v>
@@ -2250,10 +2273,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="38">
         <v>5</v>
@@ -2265,10 +2288,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="32">
         <v>20</v>
@@ -2280,10 +2303,10 @@
         <v>4.2</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="38">
         <v>5</v>
@@ -2295,10 +2318,10 @@
         <v>5</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="38">
         <v>5</v>
@@ -2310,10 +2333,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="29">
         <v>100</v>
@@ -2325,10 +2348,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="28">
         <v>20</v>
@@ -2340,10 +2363,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="38">
         <v>5</v>
@@ -2355,10 +2378,10 @@
         <v>7.1</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="32">
         <v>20</v>
@@ -2370,10 +2393,10 @@
         <v>7.2</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="38">
         <v>5</v>
@@ -2385,10 +2408,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="38">
         <v>5</v>
@@ -2400,10 +2423,10 @@
         <v>8.1</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="32">
         <v>20</v>
@@ -2415,10 +2438,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="38">
         <v>5</v>
@@ -2429,10 +2452,10 @@
         <v>9</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" s="38">
         <v>5</v>
@@ -2443,10 +2466,10 @@
         <v>9.1</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="32">
         <v>20</v>
@@ -2457,10 +2480,10 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="38">
         <v>5</v>
@@ -2471,10 +2494,10 @@
         <v>10</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="28">
         <v>25</v>
@@ -2485,10 +2508,10 @@
         <v>11</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="38">
         <v>5</v>
@@ -2502,7 +2525,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" s="29">
         <v>100</v>
@@ -3042,33 +3065,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
         <v>85</v>
       </c>
-      <c r="C4" t="s">
-        <v>86</v>
-      </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
         <v>85</v>
-      </c>
-      <c r="G4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" t="s">
         <v>89</v>
-      </c>
-      <c r="F5" t="s">
-        <v>90</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -3076,13 +3099,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -3090,7 +3113,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -3098,7 +3121,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3106,10 +3129,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" t="s">
         <v>94</v>
-      </c>
-      <c r="F10" t="s">
-        <v>95</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3117,7 +3140,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3125,7 +3148,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3133,7 +3156,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3141,7 +3164,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3149,7 +3172,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
add wk10 and rebuild
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306F7AF0-BFDD-4FA1-A5BF-9AD91B3E2986}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7F8220-267E-4127-AADA-ACB9A41FE877}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="180">
   <si>
     <t>Finals Week</t>
   </si>
@@ -95,15 +95,6 @@
     <t>Correlated Data,  Random Intercept Models,</t>
   </si>
   <si>
-    <t>Missing Data Identification, Multiple Imputation, MICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Install the `mice` package. </t>
-  </si>
-  <si>
-    <t>ded week</t>
-  </si>
-  <si>
     <t>https://data.nasa.gov/Space-Science/Meteorite-Landings/gh4g-9sfh</t>
   </si>
   <si>
@@ -249,9 +240,6 @@
     <t>QFT Model Building</t>
   </si>
   <si>
-    <t>* QFT Missing Data</t>
-  </si>
-  <si>
     <t>QFT Correlated Data</t>
   </si>
   <si>
@@ -268,9 +256,6 @@
   </si>
   <si>
     <t>Final Exam Review</t>
-  </si>
-  <si>
-    <t>Final Project Presentations</t>
   </si>
   <si>
     <t>* Join our Slack Team at math456.slack.com &amp; Install the phone app
@@ -347,14 +332,6 @@
 * Peer Review (Due Sun 5/6)</t>
   </si>
   <si>
-    <t>* Take home portion of Final exam distributed Friday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* In class exam (May ??)
-* Take home portion (Due before in class exam)
-</t>
-  </si>
-  <si>
     <t>* Spatio-Temporal assignment due (Fri 4/20) - tentative
 * PR Spatio-Temporal (Sun 4/22) - tentative</t>
   </si>
@@ -369,9 +346,6 @@
   </si>
   <si>
     <t>Topic</t>
-  </si>
-  <si>
-    <t>Spatial-Temporal Modeling</t>
   </si>
   <si>
     <t xml:space="preserve">Variable Overload, Principal Component Analysis, </t>
@@ -601,14 +575,7 @@
 * Intro to Correlated Data</t>
   </si>
   <si>
-    <t>* Random vs fixed effects</t>
-  </si>
-  <si>
     <t>open work day</t>
-  </si>
-  <si>
-    <t>* Explain the concept of information pooling
-* Demonstrate how to specify and fit a random intercept model</t>
   </si>
   <si>
     <t>* Correlated Data assignment - PMA6 18.2 - 18.6 (Due Fri 4/6)
@@ -617,6 +584,122 @@
   <si>
     <t xml:space="preserve">https://d4tagirl.com/2017/05/how-to-plot-animated-maps-with-gganimate
 * small area estimates using census data? </t>
+  </si>
+  <si>
+    <t>No School</t>
+  </si>
+  <si>
+    <t>* Random Intercept Models (Notebook 11-11.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Sometimes we may have an idea of how the clusters should be correlated. 
+* How can we change or control the correlation structure between individuals or groups? 
+* What impact can that have on the model results and interpretations? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Open work day. 
+* Finish homework
+* Work on your project - Many of you have models that have a clustered or correlated nature. </t>
+  </si>
+  <si>
+    <t>Fitting RI models in R, Controlling the covariance structure, Open work day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitudinal models, </t>
+  </si>
+  <si>
+    <t>* Effects of non-response
+* Missing data mechanisms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Install the `mice` and `VIM` packages. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* What strategies can we use to deal with missing data in an appropriate manner? </t>
+  </si>
+  <si>
+    <t>* Notebook Ch 14</t>
+  </si>
+  <si>
+    <t>Final Exam - Wed at 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final exam review part II (Time TBD) Poll will go out. </t>
+  </si>
+  <si>
+    <t>Geospatial models</t>
+  </si>
+  <si>
+    <t>Missing Data Identification, Impact, Strategies</t>
+  </si>
+  <si>
+    <t>* Explain the concept of information pooling
+* Write a multi-level model mathematically</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Fit a Random intercept model in R
+* Allow for different correlations by changing the correlation structure
+ * Explain the impact model-misspecification can have on the results. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Use the Random Intercept model to account for geographically correlated data. 
+* Learn what other methods exist to model spatial data. 
+* Create simple maps to visualize the results of spatial models. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Use the Random intercept model to account for temporally correlated data. 
+* Learn what  other methods exist to model time series data? 
+* Create visualizations for longitudinal data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Explain the effects of missing data. 
+* List and define the different missing data mechanisms. 
+* Explain the typical methods of handling missing data and the problems with each. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Explain the mathematical model behind multiple imputation using chained equations
+* Conduct multiple imputation on a data set and analyze the results. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* What types of models are you interested in that we didn’t cover? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Contribute to the Google Doc for topics to discuss early next week. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other topics, Final exam review, Open work day. </t>
+  </si>
+  <si>
+    <t>Multiple Imputation, MICE</t>
+  </si>
+  <si>
+    <t>* College of Natural Science Poster Presentation
+* Short Lecture so you can get your posters up
+* Multiple imputation is the gold standard of how to analyze data with missing values. We'll go over what this general algorithm is all about</t>
+  </si>
+  <si>
+    <t>* In depth detail for one specific method called MICE: Multiple Imputation using Chained Equations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* In class exam (Wed 5/16 at 10am)
+* Take home portion (Due Friday 12 noon FIRM)
+</t>
+  </si>
+  <si>
+    <t>* Submit your CNS Poster Session abstract as a class project to https://www.csuchico.edu/nsci/event/poster.shtml (Due 5pm Mon 16th FIRM)</t>
+  </si>
+  <si>
+    <t>* Fitting RI models in R * Including covariates, and centering covariates</t>
+  </si>
+  <si>
+    <t>* Notebook Ch 11.4-11.6</t>
+  </si>
+  <si>
+    <t>* Read Lecture notes
+* Install package `sjPlot`
+* Replicate models and plots in notes
+* Make a schedule to meet with your group to work on the project. 
+* Review the Poster session guidelines and submission instructions</t>
   </si>
 </sst>
 </file>
@@ -696,7 +779,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,6 +843,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6D6D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -931,7 +1020,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1058,6 +1147,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1160,6 +1255,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF6D6D"/>
       <color rgb="FF66CCFF"/>
     </mruColors>
   </colors>
@@ -1496,11 +1592,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1561,22 +1657,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="41" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H2" s="42" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="I2" s="42" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1584,32 +1680,32 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <f t="shared" ref="B3:B18" si="0">B2+7</f>
+        <f t="shared" ref="B3:B17" si="0">B2+7</f>
         <v>41667</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="H3" s="42" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I3" s="42" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1621,25 +1717,25 @@
         <v>41674</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>132</v>
-      </c>
       <c r="G4" s="42" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H4" s="42" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I4" s="43" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="J4" s="27"/>
     </row>
@@ -1652,31 +1748,31 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G5" s="43" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H5" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I5" s="44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="K5" s="45" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="230.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1688,31 +1784,31 @@
         <v>41688</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="K6" s="47" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1724,19 +1820,19 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>17</v>
@@ -1745,10 +1841,10 @@
         <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="K7" s="47" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1760,27 +1856,27 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="47" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="243" thickBot="1" x14ac:dyDescent="0.3">
@@ -1792,28 +1888,28 @@
         <v>41709</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1839,29 +1935,29 @@
         <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>149</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="K11" s="47"/>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1869,16 +1965,32 @@
         <f t="shared" si="0"/>
         <v>41730</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1887,24 +1999,26 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D13" s="4"/>
+        <v>154</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>166</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="15"/>
       <c r="G13" s="7" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1912,8 +2026,12 @@
         <f t="shared" si="0"/>
         <v>41744</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>165</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
@@ -1921,7 +2039,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:11" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1930,23 +2048,31 @@
         <v>41751</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>162</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="E15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+        <v>156</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="J15" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1954,16 +2080,28 @@
         <f t="shared" si="0"/>
         <v>41758</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="4"/>
+      <c r="C16" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>168</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="49" t="s">
+        <v>173</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1972,52 +2110,43 @@
         <v>41765</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>21</v>
+        <v>171</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>72</v>
+        <v>169</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>96</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" si="0"/>
-        <v>41772</v>
+        <v>41774</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>1</v>
+        <v>159</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>160</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="2"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="15"/>
-      <c r="J20" s="4"/>
+        <v>175</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2051,25 +2180,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>40</v>
-      </c>
       <c r="F1" s="18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2077,16 +2206,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="38">
         <v>5</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G2" s="35">
         <f>SUMIF($C$2:$C$89,F2,$D$2:$D$89)</f>
@@ -2102,16 +2231,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3" s="38">
         <v>20</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G3" s="38">
         <f>SUMIF($C$2:$C$89,F3,$D$2:$D$89)</f>
@@ -2127,16 +2256,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D4" s="32">
         <v>10</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G4" s="29">
         <f>SUMIF($C$2:$C$89,F4,$D$2:$D$89)</f>
@@ -2152,16 +2281,16 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D5" s="38">
         <v>5</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G5" s="28">
         <f>SUMIF($C$2:$C$89,F5,$D$2:$D$89)</f>
@@ -2177,10 +2306,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" s="32">
         <v>10</v>
@@ -2195,10 +2324,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D7" s="38">
         <v>5</v>
@@ -2209,10 +2338,10 @@
         <v>2.4</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D8" s="28">
         <v>15</v>
@@ -2223,10 +2352,10 @@
         <v>2.5</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D9" s="38">
         <v>5</v>
@@ -2237,10 +2366,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D10" s="32">
         <v>20</v>
@@ -2251,10 +2380,10 @@
         <v>3.1</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11" s="38">
         <v>5</v>
@@ -2265,10 +2394,10 @@
         <v>3.2</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D12" s="38">
         <v>5</v>
@@ -2279,10 +2408,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D13" s="38">
         <v>5</v>
@@ -2294,10 +2423,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D14" s="32">
         <v>20</v>
@@ -2309,10 +2438,10 @@
         <v>4.2</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D15" s="38">
         <v>5</v>
@@ -2324,10 +2453,10 @@
         <v>5</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" s="38">
         <v>5</v>
@@ -2339,10 +2468,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D17" s="29">
         <v>100</v>
@@ -2354,10 +2483,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D18" s="28">
         <v>20</v>
@@ -2369,10 +2498,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D19" s="38">
         <v>5</v>
@@ -2384,10 +2513,10 @@
         <v>7.1</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D20" s="32">
         <v>20</v>
@@ -2399,10 +2528,10 @@
         <v>7.2</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D21" s="38">
         <v>5</v>
@@ -2414,10 +2543,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D22" s="38">
         <v>5</v>
@@ -2429,10 +2558,10 @@
         <v>8.1</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D23" s="32">
         <v>20</v>
@@ -2444,10 +2573,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D24" s="38">
         <v>5</v>
@@ -2458,10 +2587,10 @@
         <v>9</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D25" s="38">
         <v>5</v>
@@ -2472,10 +2601,10 @@
         <v>9.1</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D26" s="32">
         <v>20</v>
@@ -2486,10 +2615,10 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D27" s="38">
         <v>5</v>
@@ -2500,10 +2629,10 @@
         <v>10</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D28" s="28">
         <v>25</v>
@@ -2514,10 +2643,10 @@
         <v>11</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D29" s="38">
         <v>5</v>
@@ -2531,7 +2660,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D30" s="29">
         <v>100</v>
@@ -3016,37 +3145,37 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3071,33 +3200,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -3105,13 +3234,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -3119,7 +3248,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -3127,7 +3256,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3135,10 +3264,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3146,7 +3275,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3154,7 +3283,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3162,7 +3291,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3170,7 +3299,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3178,7 +3307,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
add wk 11 and rebuild
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7F8220-267E-4127-AADA-ACB9A41FE877}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B9E6B8-F201-4E16-BEAA-2EC9F90C527F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="184">
   <si>
     <t>Finals Week</t>
   </si>
@@ -92,9 +92,6 @@
 * Learning the Elbow Rule? Hint, it has nothing to do with your ear. </t>
   </si>
   <si>
-    <t>Correlated Data,  Random Intercept Models,</t>
-  </si>
-  <si>
     <t>https://data.nasa.gov/Space-Science/Meteorite-Landings/gh4g-9sfh</t>
   </si>
   <si>
@@ -332,10 +329,6 @@
 * Peer Review (Due Sun 5/6)</t>
   </si>
   <si>
-    <t>* Spatio-Temporal assignment due (Fri 4/20) - tentative
-* PR Spatio-Temporal (Sun 4/22) - tentative</t>
-  </si>
-  <si>
     <t>PR Spatio-Temporal</t>
   </si>
   <si>
@@ -355,9 +348,6 @@
   </si>
   <si>
     <t>QFT n&lt;&lt;p</t>
-  </si>
-  <si>
-    <t>* QFT Spatio-Temporal Data</t>
   </si>
   <si>
     <t>* Explain the difference between PCA and FA</t>
@@ -605,9 +595,6 @@
     <t>Fitting RI models in R, Controlling the covariance structure, Open work day</t>
   </si>
   <si>
-    <t xml:space="preserve">Longitudinal models, </t>
-  </si>
-  <si>
     <t>* Effects of non-response
 * Missing data mechanisms</t>
   </si>
@@ -622,9 +609,6 @@
   </si>
   <si>
     <t>Final Exam - Wed at 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Final exam review part II (Time TBD) Poll will go out. </t>
   </si>
   <si>
     <t>Geospatial models</t>
@@ -647,11 +631,6 @@
 * Create simple maps to visualize the results of spatial models. </t>
   </si>
   <si>
-    <t xml:space="preserve">* Use the Random intercept model to account for temporally correlated data. 
-* Learn what  other methods exist to model time series data? 
-* Create visualizations for longitudinal data. </t>
-  </si>
-  <si>
     <t xml:space="preserve">* Explain the effects of missing data. 
 * List and define the different missing data mechanisms. 
 * Explain the typical methods of handling missing data and the problems with each. </t>
@@ -661,18 +640,6 @@
 * Conduct multiple imputation on a data set and analyze the results. </t>
   </si>
   <si>
-    <t xml:space="preserve">* What types of models are you interested in that we didn’t cover? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Contribute to the Google Doc for topics to discuss early next week. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other topics, Final exam review, Open work day. </t>
-  </si>
-  <si>
-    <t>Multiple Imputation, MICE</t>
-  </si>
-  <si>
     <t>* College of Natural Science Poster Presentation
 * Short Lecture so you can get your posters up
 * Multiple imputation is the gold standard of how to analyze data with missing values. We'll go over what this general algorithm is all about</t>
@@ -687,9 +654,6 @@
   </si>
   <si>
     <t>* Submit your CNS Poster Session abstract as a class project to https://www.csuchico.edu/nsci/event/poster.shtml (Due 5pm Mon 16th FIRM)</t>
-  </si>
-  <si>
-    <t>* Fitting RI models in R * Including covariates, and centering covariates</t>
   </si>
   <si>
     <t>* Notebook Ch 11.4-11.6</t>
@@ -700,6 +664,62 @@
 * Replicate models and plots in notes
 * Make a schedule to meet with your group to work on the project. 
 * Review the Poster session guidelines and submission instructions</t>
+  </si>
+  <si>
+    <t>* Fitting RI models in R 
+* Including covariates, and centering covariates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">had to go through homework. Question out of book are confusingly worded, R code to center variables not known. Important for the entire homework, yet not really emphasized during lecture. Move earlier. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Create visualizations for longitudinal data. 
+* Analyze temporal data using standard methods
+* Use the Random intercept model to account for temporally correlated data. 
+</t>
+  </si>
+  <si>
+    <t>Visualizing longitudinal data, analyzing longitudinal data, writing contrasts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* QFT Spatio-Temporal Data
+* Introduction to longitudinal data
+* How do we visualize temporally correlated data? 
+* Introduction to the Pediatric pain data. </t>
+  </si>
+  <si>
+    <t>* Notebook Ch 12</t>
+  </si>
+  <si>
+    <t>* Notebook Ch 13</t>
+  </si>
+  <si>
+    <t>* We'll explore different ways to analyze repeated measures data
+* Most initial approaches don't need fancy models like the random intercept model, we'll look at a bunch of t-tests</t>
+  </si>
+  <si>
+    <t>Project presentations</t>
+  </si>
+  <si>
+    <t>Project presentations (MW) , , Final exam review (F)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Spatio-Temporal assignment due (Fri 4/20)
+* PR Spatio-Temporal (Sun 4/22) 
+* In person SET's on Friday. Attendance mandatory </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Often in fully interaction models we need to write contrast statements to assess specific effects. 
+* This requires multiplying matricies, which the notes walk you through doing. Don't worry, it's the simplest example of matrix multiplication that there is. </t>
+  </si>
+  <si>
+    <t>Correlated Data,  Random Intercept Models, No school</t>
+  </si>
+  <si>
+    <t>Multiple Imputation, MICE, Open work day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Download the mice and ozone data from my data webpage for the homework. </t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1040,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1154,6 +1174,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="93">
@@ -1594,9 +1620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1657,22 +1683,22 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="41" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H2" s="42" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I2" s="42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1684,28 +1710,28 @@
         <v>41667</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H3" s="42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1717,25 +1743,25 @@
         <v>41674</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="43" t="s">
         <v>118</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="G4" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="H4" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="I4" s="43" t="s">
-        <v>121</v>
       </c>
       <c r="J4" s="27"/>
     </row>
@@ -1748,31 +1774,31 @@
         <v>41681</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="K5" s="45" t="s">
         <v>125</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G5" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="K5" s="45" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="230.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1784,31 +1810,31 @@
         <v>41688</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="K6" s="47" t="s">
         <v>132</v>
-      </c>
-      <c r="K6" s="47" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1820,19 +1846,19 @@
         <v>41695</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>17</v>
@@ -1841,10 +1867,10 @@
         <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K7" s="47" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1856,27 +1882,27 @@
         <v>41702</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="47" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="243" thickBot="1" x14ac:dyDescent="0.3">
@@ -1888,28 +1914,28 @@
         <v>41709</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1932,28 +1958,28 @@
         <v>41723</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>181</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I11" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="K11" s="47"/>
     </row>
@@ -1966,31 +1992,34 @@
         <v>41730</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
+      </c>
+      <c r="I12" s="50" t="s">
+        <v>149</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+      <c r="K12" s="47" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1999,24 +2028,30 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="15"/>
+        <v>171</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F13" s="51" t="s">
+        <v>174</v>
+      </c>
       <c r="G13" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+        <v>173</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>180</v>
+      </c>
       <c r="J13" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>148</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
@@ -2027,17 +2062,22 @@
         <v>41744</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G14" s="7"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
+      <c r="K14" s="15" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
@@ -2048,28 +2088,28 @@
         <v>41751</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2081,27 +2121,25 @@
         <v>41758</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
       <c r="G16" s="49" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2110,19 +2148,19 @@
         <v>41765</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>67</v>
+        <v>177</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="J17" s="4"/>
     </row>
@@ -2134,23 +2172,21 @@
         <v>41774</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="7" t="s">
-        <v>160</v>
-      </c>
+      <c r="G18" s="7"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K13" r:id="rId1" xr:uid="{80D4A954-358D-4F10-94B1-96CBF123A2A4}"/>
+    <hyperlink ref="K14" r:id="rId1" xr:uid="{24F4B91A-3558-4E59-B7D9-1042EB8C4863}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2180,25 +2216,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>37</v>
-      </c>
       <c r="F1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2206,16 +2242,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="38">
         <v>5</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" s="35">
         <f>SUMIF($C$2:$C$89,F2,$D$2:$D$89)</f>
@@ -2231,16 +2267,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="38">
         <v>20</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="38">
         <f>SUMIF($C$2:$C$89,F3,$D$2:$D$89)</f>
@@ -2256,16 +2292,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="32">
         <v>10</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="29">
         <f>SUMIF($C$2:$C$89,F4,$D$2:$D$89)</f>
@@ -2281,16 +2317,16 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="38">
         <v>5</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="28">
         <f>SUMIF($C$2:$C$89,F5,$D$2:$D$89)</f>
@@ -2306,10 +2342,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="32">
         <v>10</v>
@@ -2324,10 +2360,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="38">
         <v>5</v>
@@ -2338,10 +2374,10 @@
         <v>2.4</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="28">
         <v>15</v>
@@ -2352,10 +2388,10 @@
         <v>2.5</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="38">
         <v>5</v>
@@ -2366,10 +2402,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="32">
         <v>20</v>
@@ -2380,10 +2416,10 @@
         <v>3.1</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="38">
         <v>5</v>
@@ -2394,10 +2430,10 @@
         <v>3.2</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="38">
         <v>5</v>
@@ -2408,10 +2444,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="38">
         <v>5</v>
@@ -2423,10 +2459,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="32">
         <v>20</v>
@@ -2438,10 +2474,10 @@
         <v>4.2</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="38">
         <v>5</v>
@@ -2453,10 +2489,10 @@
         <v>5</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="38">
         <v>5</v>
@@ -2468,10 +2504,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="29">
         <v>100</v>
@@ -2483,10 +2519,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="28">
         <v>20</v>
@@ -2498,10 +2534,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="38">
         <v>5</v>
@@ -2513,10 +2549,10 @@
         <v>7.1</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="32">
         <v>20</v>
@@ -2528,10 +2564,10 @@
         <v>7.2</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="38">
         <v>5</v>
@@ -2543,10 +2579,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="38">
         <v>5</v>
@@ -2558,10 +2594,10 @@
         <v>8.1</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="32">
         <v>20</v>
@@ -2573,10 +2609,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="38">
         <v>5</v>
@@ -2587,10 +2623,10 @@
         <v>9</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="38">
         <v>5</v>
@@ -2601,10 +2637,10 @@
         <v>9.1</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="32">
         <v>20</v>
@@ -2615,10 +2651,10 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="38">
         <v>5</v>
@@ -2629,10 +2665,10 @@
         <v>10</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="28">
         <v>25</v>
@@ -2643,10 +2679,10 @@
         <v>11</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="38">
         <v>5</v>
@@ -2660,7 +2696,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="29">
         <v>100</v>
@@ -3145,37 +3181,37 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3200,33 +3236,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
         <v>73</v>
       </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
         <v>73</v>
-      </c>
-      <c r="G4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
         <v>77</v>
-      </c>
-      <c r="F5" t="s">
-        <v>78</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -3234,13 +3270,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -3248,7 +3284,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -3256,7 +3292,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3264,10 +3300,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" t="s">
         <v>82</v>
-      </c>
-      <c r="F10" t="s">
-        <v>83</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3275,7 +3311,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3283,7 +3319,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3291,7 +3327,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3299,7 +3335,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3307,7 +3343,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
add hw to wk11
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B9E6B8-F201-4E16-BEAA-2EC9F90C527F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EBD93C-FE23-4BC1-9A21-51E1E5D7D707}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="187">
   <si>
     <t>Finals Week</t>
   </si>
@@ -673,12 +673,6 @@
     <t xml:space="preserve">had to go through homework. Question out of book are confusingly worded, R code to center variables not known. Important for the entire homework, yet not really emphasized during lecture. Move earlier. </t>
   </si>
   <si>
-    <t xml:space="preserve">* Create visualizations for longitudinal data. 
-* Analyze temporal data using standard methods
-* Use the Random intercept model to account for temporally correlated data. 
-</t>
-  </si>
-  <si>
     <t>Visualizing longitudinal data, analyzing longitudinal data, writing contrasts</t>
   </si>
   <si>
@@ -688,16 +682,6 @@
 * Introduction to the Pediatric pain data. </t>
   </si>
   <si>
-    <t>* Notebook Ch 12</t>
-  </si>
-  <si>
-    <t>* Notebook Ch 13</t>
-  </si>
-  <si>
-    <t>* We'll explore different ways to analyze repeated measures data
-* Most initial approaches don't need fancy models like the random intercept model, we'll look at a bunch of t-tests</t>
-  </si>
-  <si>
     <t>Project presentations</t>
   </si>
   <si>
@@ -720,13 +704,44 @@
   </si>
   <si>
     <t xml:space="preserve">* Download the mice and ozone data from my data webpage for the homework. </t>
+  </si>
+  <si>
+    <t>Data Fest Weekend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* We'll explore the use of an extension of lme4 called lme4qtl to fit a random intercept to a spatial model, where we define the nearest neighbor matrix. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* We'll see how to make some maps in R using shapefiles
+* We'll draft up a nearest neighbor matrix - as a way to hand create a Conditionally Autoregressive Model (CAR)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Notebook Ch 13
+* http://www.statsref.com/HTML/index.html?car_models.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Notebook Ch 12
+* https://onlinecourses.science.psu.edu/stat510/node/61 </t>
+  </si>
+  <si>
+    <t>* Recap the difference between longitudinal data and time series data
+* We'll explore different ways to analyze repeated measures data
+* Most initial approaches don't need fancy models like the random intercept model, we'll look at a bunch of t-tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Create visualizations for longitudinal data. 
+* Define autocorrelation
+* Analyze temporal data using standard methods
+* Use the Random intercept model to account for temporally correlated data. 
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -794,6 +809,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1040,7 +1062,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1178,8 +1200,9 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="93">
@@ -1620,9 +1643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1958,7 +1981,7 @@
         <v>41723</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>158</v>
@@ -2019,7 +2042,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -2028,28 +2051,28 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F13" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="F13" s="51" t="s">
-        <v>174</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>173</v>
-      </c>
       <c r="H13" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>180</v>
-      </c>
       <c r="J13" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K13" s="15"/>
     </row>
@@ -2069,11 +2092,17 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+        <v>183</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="J14" s="4"/>
       <c r="K14" s="15" t="s">
         <v>145</v>
@@ -2111,6 +2140,9 @@
       <c r="J15" s="4" t="s">
         <v>89</v>
       </c>
+      <c r="K15" s="51" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
@@ -2121,7 +2153,7 @@
         <v>41758</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>162</v>
@@ -2148,16 +2180,16 @@
         <v>41765</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
add week 13 info
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EBD93C-FE23-4BC1-9A21-51E1E5D7D707}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="189">
   <si>
     <t>Finals Week</t>
   </si>
@@ -602,16 +601,10 @@
     <t xml:space="preserve">* Install the `mice` and `VIM` packages. </t>
   </si>
   <si>
-    <t xml:space="preserve">* What strategies can we use to deal with missing data in an appropriate manner? </t>
-  </si>
-  <si>
     <t>* Notebook Ch 14</t>
   </si>
   <si>
     <t>Final Exam - Wed at 10</t>
-  </si>
-  <si>
-    <t>Geospatial models</t>
   </si>
   <si>
     <t>Missing Data Identification, Impact, Strategies</t>
@@ -626,11 +619,6 @@
  * Explain the impact model-misspecification can have on the results. </t>
   </si>
   <si>
-    <t xml:space="preserve">* Use the Random Intercept model to account for geographically correlated data. 
-* Learn what other methods exist to model spatial data. 
-* Create simple maps to visualize the results of spatial models. </t>
-  </si>
-  <si>
     <t xml:space="preserve">* Explain the effects of missing data. 
 * List and define the different missing data mechanisms. 
 * Explain the typical methods of handling missing data and the problems with each. </t>
@@ -638,11 +626,6 @@
   <si>
     <t xml:space="preserve">* Explain the mathematical model behind multiple imputation using chained equations
 * Conduct multiple imputation on a data set and analyze the results. </t>
-  </si>
-  <si>
-    <t>* College of Natural Science Poster Presentation
-* Short Lecture so you can get your posters up
-* Multiple imputation is the gold standard of how to analyze data with missing values. We'll go over what this general algorithm is all about</t>
   </si>
   <si>
     <t>* In depth detail for one specific method called MICE: Multiple Imputation using Chained Equations</t>
@@ -712,15 +695,6 @@
     <t xml:space="preserve">* We'll explore the use of an extension of lme4 called lme4qtl to fit a random intercept to a spatial model, where we define the nearest neighbor matrix. </t>
   </si>
   <si>
-    <t xml:space="preserve">* We'll see how to make some maps in R using shapefiles
-* We'll draft up a nearest neighbor matrix - as a way to hand create a Conditionally Autoregressive Model (CAR)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Notebook Ch 13
-* http://www.statsref.com/HTML/index.html?car_models.html </t>
-  </si>
-  <si>
     <t xml:space="preserve">* Notebook Ch 12
 * https://onlinecourses.science.psu.edu/stat510/node/61 </t>
   </si>
@@ -736,11 +710,46 @@
 * Use the Random intercept model to account for temporally correlated data. 
 </t>
   </si>
+  <si>
+    <t>* Notebook Ch 13</t>
+  </si>
+  <si>
+    <t>Terminology &amp; mapping, Spatial influence, open work day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Start out with some terminology
+* Then make some maps using shapes and points. 
+* How do we identify neighbors? 
+</t>
+  </si>
+  <si>
+    <t>* Create maps using shapes and points in R. 
+* Identify spatial neighbors using borders and distances. 
+* Use the Random Intercept model to account for geographically correlated data. 
+* Plot the results of a model onto a map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* College of Natural Science Poster Presentation - no class. 
+</t>
+  </si>
+  <si>
+    <t>* What strategies can we use to deal with missing data in an appropriate manner? 
+* What are some methods for imputation? 
+* Multiple imputation is the gold standard of how to analyze data with missing values. We'll go over what this general algorithm is all about</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* 10 minute project presentations. Randomly chosen on Monday. 
+* Must use slides, but not restricted to R presentation slides. </t>
+  </si>
+  <si>
+    <t>* Replicate all examples in the notes. 
+* New packages: spdep, sp, ggmap, maps, lme4qtl</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1295,9 +1304,9 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
     <cellStyle name="Percent" xfId="90" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Percent 2" xfId="52"/>
     <cellStyle name="Total" xfId="92" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1640,12 +1649,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1981,10 +1990,10 @@
         <v>41723</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>141</v>
@@ -2018,16 +2027,16 @@
         <v>150</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>148</v>
@@ -2036,10 +2045,10 @@
         <v>149</v>
       </c>
       <c r="J12" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="K12" s="47" t="s">
         <v>166</v>
-      </c>
-      <c r="K12" s="47" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2051,32 +2060,32 @@
         <v>41737</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" s="52" t="s">
+        <v>178</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="F13" s="52" t="s">
-        <v>184</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>175</v>
-      </c>
       <c r="K13" s="15"/>
     </row>
-    <row r="14" spans="1:11" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -2085,20 +2094,22 @@
         <v>41744</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E14" s="4"/>
+        <v>184</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="F14" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>182</v>
-      </c>
       <c r="H14" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>16</v>
@@ -2108,7 +2119,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -2117,22 +2128,22 @@
         <v>41751</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>152</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>151</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>153</v>
+        <v>186</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>143</v>
@@ -2141,10 +2152,10 @@
         <v>89</v>
       </c>
       <c r="K15" s="51" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -2153,18 +2164,18 @@
         <v>41758</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
       <c r="G16" s="49" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>143</v>
@@ -2180,16 +2191,18 @@
         <v>41765</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>187</v>
+      </c>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>66</v>
@@ -2204,7 +2217,7 @@
         <v>41774</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -2213,12 +2226,12 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K14" r:id="rId1" xr:uid="{24F4B91A-3558-4E59-B7D9-1042EB8C4863}"/>
+    <hyperlink ref="K14" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2226,7 +2239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3198,7 +3211,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3252,7 +3265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
update schedule add items
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH456/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FFC5A2-A280-454F-A87C-91CFB929C7EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561F434C-5B76-554A-86EB-959B5EA987FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="161">
   <si>
     <t>Finals Week</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Week</t>
   </si>
   <si>
-    <t>Participation</t>
-  </si>
-  <si>
     <t>Reading</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
   </si>
   <si>
     <t>Cesar Chavez day - Campus closed</t>
-  </si>
-  <si>
-    <t>Assignments / activities</t>
   </si>
   <si>
     <t>Moderation and Confounding</t>
@@ -157,15 +151,6 @@
     <t>Dead week</t>
   </si>
   <si>
-    <t>Introduction to the instructor, class structure, materials, requirements, expectations and resources. 
-Blackboard usage (grading)
-Online materials (google drive, website, slack)
-Physical materials (course notes, textbook)
-Learning Techniques (learning journal, group quizzes, exam error assessments, peer grading)
-Support structures (community coding, Slack, OH)
-Group research project</t>
-  </si>
-  <si>
     <t>Project selection</t>
   </si>
   <si>
@@ -173,33 +158,6 @@
   </si>
   <si>
     <t>Learning Activity</t>
-  </si>
-  <si>
-    <t>Familiarize yourself with this website and required course materials. 
-Obtain the textbook and setup an online learning journal.
-Join the Slack workspace and post an introduction
-Update R, R Studio and associated packages</t>
-  </si>
-  <si>
-    <t>Post introduction on Slack (Due XX/XX )
-PM Dr. D the link to your Learning Journal (Due XX/XX)</t>
-  </si>
-  <si>
-    <t>QFT: Preparing data for analysis
-LJ: MLR</t>
-  </si>
-  <si>
-    <t>Question formation technique (QFT) 
-Review data preparation methods
-Revisit fitting multiple linear regression models</t>
-  </si>
-  <si>
-    <t>Describe how to ensure your success in this class
-Get to know your classmates
-Start to develop good questions</t>
-  </si>
-  <si>
-    <t>Interpreting different types of predictors</t>
   </si>
   <si>
     <t>Interaction models and contrasts
@@ -234,19 +192,10 @@
     <t>GLM Assignment</t>
   </si>
   <si>
-    <t>QFT n&lt;&lt;p</t>
-  </si>
-  <si>
     <t>PCA/FA Assignment</t>
   </si>
   <si>
-    <t>Peer Review PCA/FA Assignment</t>
-  </si>
-  <si>
     <t>PR Correlated Data</t>
-  </si>
-  <si>
-    <t>QFT Missing Data</t>
   </si>
   <si>
     <t>PR Missing Data</t>
@@ -382,9 +331,6 @@
     <t>Project Presentations, Project report due</t>
   </si>
   <si>
-    <t>Project update (1pg)</t>
-  </si>
-  <si>
     <t>Project Update Presentations</t>
   </si>
   <si>
@@ -472,13 +418,6 @@
     <t>Install packages: caret, ROCR</t>
   </si>
   <si>
-    <t xml:space="preserve">install packages: mice, </t>
-  </si>
-  <si>
-    <t>Build and interpret a Logistic regression model on binary data
-Build and interpret a Poisson model on count data</t>
-  </si>
-  <si>
     <t>Generalized Linear Models
 (Binary and Count outcomes)</t>
   </si>
@@ -497,39 +436,16 @@
     <t>HW 03: GLM</t>
   </si>
   <si>
-    <t xml:space="preserve">Class logistics, Data preparation review
-</t>
-  </si>
-  <si>
     <t>HW: Statistical Modeling</t>
   </si>
   <si>
-    <t>Slack Intro: Who are you, what do you hope to get out of this class, how will you ensure your success in this class? 
-Write instructions on how to prepare data for analysis</t>
-  </si>
-  <si>
-    <t>Data Preparation</t>
-  </si>
-  <si>
     <t>PR Statistical Modeling</t>
   </si>
   <si>
-    <t>QFT/LJ GLM</t>
-  </si>
-  <si>
     <t>PR GLM Assignmnt</t>
   </si>
   <si>
-    <t>QFT Survival Analysis</t>
-  </si>
-  <si>
     <t>PR Survival Analysis</t>
-  </si>
-  <si>
-    <t>Pre-Learning</t>
-  </si>
-  <si>
-    <t>Post-Learning</t>
   </si>
   <si>
     <t>Midterm Review</t>
@@ -554,27 +470,9 @@
     <t>Preparing Data for Analysis</t>
   </si>
   <si>
-    <t>HW 00: Data Prep Instructions</t>
-  </si>
-  <si>
-    <t>QFT/LJ: Success in this Class</t>
-  </si>
-  <si>
     <t>Community Coding (5x)</t>
   </si>
   <si>
-    <t>QFT Statistical Modeling</t>
-  </si>
-  <si>
-    <t>Quiz: PCA &amp; FA</t>
-  </si>
-  <si>
-    <t>Quiz: Survival Analysis</t>
-  </si>
-  <si>
-    <t>Quiz 00</t>
-  </si>
-  <si>
     <t>HW 04: Correlated Outcomes</t>
   </si>
   <si>
@@ -609,6 +507,95 @@
   </si>
   <si>
     <t>HW PCA &amp; FA</t>
+  </si>
+  <si>
+    <t>Model formulation wksheet</t>
+  </si>
+  <si>
+    <t>PR  PCA/FA Assignment</t>
+  </si>
+  <si>
+    <t>External Talk</t>
+  </si>
+  <si>
+    <t>PR Project Presentations</t>
+  </si>
+  <si>
+    <t>Data Preparation ref sheet</t>
+  </si>
+  <si>
+    <t>Fix my notes</t>
+  </si>
+  <si>
+    <t>PCA &amp; FA Quiz</t>
+  </si>
+  <si>
+    <t>Survival Analysis Quiz</t>
+  </si>
+  <si>
+    <t>Interpreting predictors in a multiple variable regression model</t>
+  </si>
+  <si>
+    <t>Writing models worksheet</t>
+  </si>
+  <si>
+    <t>Start to develop good questions
+Build and interpret a Logistic regression model on binary data
+Build and interpret a Poisson model on count data</t>
+  </si>
+  <si>
+    <t>Introduction to the instructor, class structure, materials, requirements, expectations and resources. 
+Blackboard usage (grading )
+Online materials (google drive, website, slack)
+Physical materials (course notes, textbook)
+Learning Techniques (learning journal, group quizzes, exam error assessments, peer grading)
+Support structures (community coding, Slack, OH)
+Group research project</t>
+  </si>
+  <si>
+    <t>[[Quiz 00]]()(Due 1/23)</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 3</t>
+  </si>
+  <si>
+    <t>Syllabus</t>
+  </si>
+  <si>
+    <t>Draft report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">install packages: mice
+Watch seminar on Missing Data: https://media.csuchico.edu/media/0_tgnydpgf </t>
+  </si>
+  <si>
+    <t>Familiarize yourself with this website and required course materials. 
+Review the syllabus and first homework assignment. 
+Read PMA6 - Chapter 3 (Before Friday)</t>
+  </si>
+  <si>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>[[HW 00: Getting Started]](hw00-getting-started.html) (Due Sun 1/26 )</t>
+  </si>
+  <si>
+    <t>[[Review Overview]](project.html)</t>
+  </si>
+  <si>
+    <t>hw00-getting-started</t>
+  </si>
+  <si>
+    <t>Quiz on Data preparation &amp; class logistics
+Create a Data preparation reference flowchart</t>
+  </si>
+  <si>
+    <t>Describe how to ensure your success in this class
+Get to know your classmates
+Describe what Self Regulated Learning means to you</t>
+  </si>
+  <si>
+    <t>Class logistics, Data preparation review</t>
   </si>
 </sst>
 </file>
@@ -981,7 +968,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1055,9 +1042,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1165,6 +1149,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -1590,7 +1580,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1606,22 +1596,22 @@
   <sheetData>
     <row r="1" spans="1:8" s="15" customFormat="1" ht="17" thickBot="1">
       <c r="A1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>27</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>6</v>
@@ -1630,7 +1620,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="68">
+    <row r="2" spans="1:8" ht="17">
       <c r="A2" s="20">
         <v>1.1000000000000001</v>
       </c>
@@ -1638,13 +1628,19 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>46</v>
+        <v>27</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1652,10 +1648,10 @@
         <v>1.2</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
-      </c>
-      <c r="G3" t="s">
-        <v>145</v>
+        <v>122</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1666,16 +1662,16 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>98</v>
+        <v>90</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>85</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1687,12 +1683,12 @@
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="16"/>
       <c r="G5" s="26"/>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="34">
@@ -1703,16 +1699,16 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>142</v>
+        <v>118</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>120</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1723,13 +1719,13 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
-      </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
+        <v>117</v>
+      </c>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="26"/>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17">
@@ -1739,15 +1735,15 @@
       <c r="B8" s="15">
         <v>6</v>
       </c>
-      <c r="D8" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="37" t="s">
-        <v>100</v>
+      <c r="D8" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="37"/>
+      <c r="F8" s="36" t="s">
+        <v>87</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1758,10 +1754,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="37"/>
+        <v>54</v>
+      </c>
+      <c r="E9" s="37"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:8" ht="34">
@@ -1772,15 +1768,15 @@
         <v>8</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="28" t="s">
-        <v>104</v>
+        <v>78</v>
+      </c>
+      <c r="E10" s="37"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="27" t="s">
+        <v>91</v>
       </c>
       <c r="H10" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1790,12 +1786,12 @@
       <c r="B11" s="15">
         <v>8</v>
       </c>
-      <c r="D11" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="32"/>
+      <c r="D11" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" spans="1:8" ht="24" customHeight="1">
       <c r="A12" s="20">
@@ -1805,16 +1801,16 @@
         <v>9</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="G12" s="69" t="s">
-        <v>152</v>
+        <v>97</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="68" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1825,8 +1821,8 @@
         <v>10</v>
       </c>
       <c r="D13" s="26"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="31"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="30"/>
       <c r="G13" s="26"/>
     </row>
     <row r="14" spans="1:8" ht="26" customHeight="1">
@@ -1837,14 +1833,14 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="35"/>
+      <c r="F14" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="31" t="s">
-        <v>102</v>
-      </c>
       <c r="G14" s="26" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1855,15 +1851,15 @@
         <v>12</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="31"/>
+        <v>76</v>
+      </c>
+      <c r="E15" s="35"/>
+      <c r="F15" s="30"/>
       <c r="G15" s="26" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="H15" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="17">
@@ -1874,14 +1870,14 @@
         <v>13</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E16" s="18"/>
-      <c r="F16" s="31" t="s">
-        <v>161</v>
+      <c r="F16" s="30" t="s">
+        <v>133</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1891,7 +1887,7 @@
       <c r="B17" s="15">
         <v>14</v>
       </c>
-      <c r="F17" s="31"/>
+      <c r="F17" s="30"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="20">
@@ -1901,11 +1897,11 @@
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="31"/>
+        <v>38</v>
+      </c>
+      <c r="F18" s="30"/>
       <c r="H18" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="51">
@@ -1918,8 +1914,8 @@
       <c r="D19" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="39" t="s">
-        <v>106</v>
+      <c r="G19" s="38" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1935,21 +1931,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.1640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="36.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="55.5" style="7" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" style="7" customWidth="1"/>
     <col min="6" max="6" width="34.6640625" style="7" customWidth="1"/>
     <col min="7" max="8" width="38" style="7" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="35.83203125" style="6" customWidth="1"/>
     <col min="10" max="10" width="24.6640625" style="6" customWidth="1"/>
     <col min="11" max="16384" width="14.83203125" style="6"/>
   </cols>
@@ -1980,46 +1976,44 @@
         <v>18</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>44</v>
+        <v>154</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="176">
-      <c r="A2" s="27">
+      <c r="A2" s="69">
         <v>1</v>
       </c>
       <c r="B2" s="11">
         <v>42389</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>159</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>48</v>
+        <v>158</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>47</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="112">
-      <c r="A3" s="27">
+      <c r="A3" s="69">
         <v>2</v>
       </c>
       <c r="B3" s="11">
@@ -2027,28 +2021,28 @@
         <v>42396</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="7" t="s">
-        <v>50</v>
+      <c r="F3" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10" ht="48">
-      <c r="A4" s="27">
+      <c r="A4" s="69">
         <v>3</v>
       </c>
       <c r="B4" s="11">
@@ -2056,69 +2050,69 @@
         <v>42403</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>83</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="80">
-      <c r="A5" s="27">
+      <c r="A5" s="69">
         <v>4</v>
       </c>
       <c r="B5" s="11">
         <f>B4+7</f>
         <v>42410</v>
       </c>
-      <c r="C5" s="61" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="64" t="s">
-        <v>121</v>
+      <c r="C5" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="63" t="s">
+        <v>146</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="141" thickBot="1">
-      <c r="A6" s="27">
+      <c r="A6" s="69">
         <v>5</v>
       </c>
       <c r="B6" s="11">
         <f t="shared" si="0"/>
         <v>42417</v>
       </c>
-      <c r="C6" s="61" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="64" t="s">
-        <v>118</v>
+      <c r="C6" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>105</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="113" thickBot="1">
-      <c r="A7" s="27">
+      <c r="A7" s="69">
         <v>6</v>
       </c>
       <c r="B7" s="11">
@@ -2126,32 +2120,32 @@
         <v>42424</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="F7" s="59" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="59" t="s">
-        <v>73</v>
+        <v>60</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="F7" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="58" t="s">
+        <v>61</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="112">
-      <c r="A8" s="27">
+      <c r="A8" s="69">
         <v>7</v>
       </c>
       <c r="B8" s="11">
@@ -2159,21 +2153,21 @@
         <v>42431</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="6" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2185,16 +2179,16 @@
         <v>42438</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16">
@@ -2204,22 +2198,22 @@
         <v>42445</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="112">
@@ -2231,18 +2225,18 @@
         <v>42452</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="56">
@@ -2257,13 +2251,13 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="62" t="s">
-        <v>79</v>
-      </c>
-      <c r="H12" s="61" t="s">
-        <v>80</v>
+        <v>30</v>
+      </c>
+      <c r="G12" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="60" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="128">
@@ -2275,25 +2269,25 @@
         <v>42466</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="61" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="61" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="61" t="s">
-        <v>85</v>
+        <v>45</v>
+      </c>
+      <c r="E13" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="60" t="s">
+        <v>73</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="80">
@@ -2305,13 +2299,13 @@
         <v>42473</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="9"/>
@@ -2326,7 +2320,7 @@
         <v>42480</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2347,7 +2341,7 @@
       <c r="E16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="6" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="16">
@@ -2359,18 +2353,18 @@
         <v>42494</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="32">
@@ -2391,9 +2385,9 @@
     <row r="23" spans="1:9" ht="16" thickBot="1">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="61"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="60"/>
       <c r="H23" s="1"/>
       <c r="I23" s="12"/>
     </row>
@@ -2401,8 +2395,8 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="59"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="58"/>
       <c r="H24" s="1"/>
     </row>
   </sheetData>
@@ -2413,18 +2407,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0647D9F9-0194-9C4A-8769-507350581DA1}">
-  <dimension ref="A1:M101"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="38"/>
-    <col min="2" max="2" width="32.1640625" style="38" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="38"/>
+    <col min="1" max="1" width="8.83203125" style="37"/>
+    <col min="2" max="2" width="32.1640625" style="37" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="37" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" style="37" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="10" style="15" customWidth="1"/>
@@ -2434,16 +2428,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1">
-      <c r="A1" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="40" t="s">
+      <c r="A1" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -2469,25 +2463,25 @@
       <c r="A2" s="15">
         <v>0</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="41">
+      <c r="C2" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="40">
         <v>5</v>
       </c>
-      <c r="F2" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="G2" s="41">
-        <f>SUMIF($C$2:$C$92,F2,$D$2:$D$92)</f>
-        <v>40</v>
-      </c>
-      <c r="H2" s="46">
-        <f>G2/$G$8</f>
-        <v>9.0909090909090912E-2</v>
+      <c r="F2" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="42">
+        <f>SUMIF($C$2:$C$87,F2,$D$2:$D$87)</f>
+        <v>130</v>
+      </c>
+      <c r="H2" s="43">
+        <f>G2/$G$7</f>
+        <v>0.26804123711340205</v>
       </c>
       <c r="K2" t="s">
         <v>7</v>
@@ -2495,7 +2489,7 @@
       <c r="L2">
         <v>120</v>
       </c>
-      <c r="M2" s="58">
+      <c r="M2" s="57">
         <v>0.24</v>
       </c>
     </row>
@@ -2503,25 +2497,25 @@
       <c r="A3" s="15">
         <v>0</v>
       </c>
-      <c r="B3" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="41">
+      <c r="B3" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="40">
         <v>10</v>
       </c>
-      <c r="F3" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="43">
-        <f>SUMIF($C$2:$C$92,F3,$D$2:$D$92)</f>
-        <v>130</v>
-      </c>
-      <c r="H3" s="44">
-        <f>G3/$G$8</f>
-        <v>0.29545454545454547</v>
+      <c r="F3" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="40">
+        <f>SUMIF($C$2:$C$87,F3,$D$2:$D$87)</f>
+        <v>125</v>
+      </c>
+      <c r="H3" s="45">
+        <f>G3/$G$7</f>
+        <v>0.25773195876288657</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
@@ -2529,7 +2523,7 @@
       <c r="L3">
         <v>100</v>
       </c>
-      <c r="M3" s="58">
+      <c r="M3" s="57">
         <v>0.2</v>
       </c>
     </row>
@@ -2537,23 +2531,25 @@
       <c r="A4" s="15">
         <v>0</v>
       </c>
-      <c r="B4" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="F4" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="G4" s="41">
-        <f>SUMIF($C$2:$C$92,F4,$D$2:$D$92)</f>
-        <v>55</v>
-      </c>
-      <c r="H4" s="46">
-        <f>G4/$G$8</f>
-        <v>0.125</v>
+      <c r="B4" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="40">
+        <v>20</v>
+      </c>
+      <c r="F4" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="64">
+        <f>SUMIF($C$2:$C$87,F4,$D$2:$D$87)</f>
+        <v>70</v>
+      </c>
+      <c r="H4" s="66">
+        <f>G4/$G$7</f>
+        <v>0.14432989690721648</v>
       </c>
       <c r="K4" t="s">
         <v>13</v>
@@ -2561,33 +2557,33 @@
       <c r="L4">
         <v>200</v>
       </c>
-      <c r="M4" s="58">
+      <c r="M4" s="57">
         <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="15">
-        <v>1.2</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="65">
-        <v>5</v>
-      </c>
-      <c r="F5" s="66" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="65">
-        <f>SUMIF($C$2:$C$92,F5,$D$2:$D$92)</f>
-        <v>65</v>
-      </c>
-      <c r="H5" s="67">
-        <f>G5/$G$8</f>
-        <v>0.14772727272727273</v>
+        <v>0</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="40">
+        <v>10</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="48">
+        <f>SUMIF($C$2:$C$87,F5,$D$2:$D$87)</f>
+        <v>100</v>
+      </c>
+      <c r="H5" s="49">
+        <f>G5/$G$7</f>
+        <v>0.20618556701030927</v>
       </c>
       <c r="K5" t="s">
         <v>14</v>
@@ -2595,118 +2591,107 @@
       <c r="L5">
         <v>80</v>
       </c>
-      <c r="M5" s="58">
+      <c r="M5" s="57">
         <v>0.16</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="15">
-        <v>1</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" s="41">
-        <v>5</v>
-      </c>
-      <c r="F6" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="49">
-        <f>SUMIF($C$2:$C$92,F6,$D$2:$D$92)</f>
-        <v>100</v>
-      </c>
-      <c r="H6" s="50">
-        <f>G6/$G$8</f>
-        <v>0.22727272727272727</v>
+        <v>0</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="40">
+        <v>10</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="51">
+        <f>SUMIF($C$2:$C$87,F6,$D$2:$D$87)</f>
+        <v>60</v>
+      </c>
+      <c r="H6" s="52">
+        <f>G6/$G$7</f>
+        <v>0.12371134020618557</v>
       </c>
       <c r="L6">
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" ht="17" thickBot="1">
       <c r="A7" s="15">
+        <v>1</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="46">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3">
+        <f>SUM(G2:G6)</f>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="15" customFormat="1" ht="17" thickTop="1">
+      <c r="A8" s="15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="47">
+      <c r="B8" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="64">
         <v>10</v>
       </c>
-      <c r="F7" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="52">
-        <f>SUMIF($C$2:$C$92,F7,$D$2:$D$92)</f>
-        <v>50</v>
-      </c>
-      <c r="H7" s="53">
-        <f>G7/$G$8</f>
-        <v>0.11363636363636363</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="15" customFormat="1" ht="17" thickBot="1">
-      <c r="A8" s="68">
-        <v>2.1</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="47">
-        <v>20</v>
-      </c>
       <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8" s="3">
-        <f>SUM(G2:G7)</f>
-        <v>440</v>
-      </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
     </row>
-    <row r="9" spans="1:13" s="15" customFormat="1" ht="17" thickTop="1">
-      <c r="A9" s="68">
+    <row r="9" spans="1:13" s="15" customFormat="1">
+      <c r="A9" s="67">
         <v>2</v>
       </c>
-      <c r="B9" s="38" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="D9" s="41">
-        <v>5</v>
+      <c r="B9" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="46">
+        <v>20</v>
       </c>
       <c r="E9"/>
+      <c r="F9"/>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
       <c r="M9"/>
     </row>
     <row r="10" spans="1:13" s="15" customFormat="1">
-      <c r="A10" s="68">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" s="41">
-        <v>10</v>
+      <c r="A10" s="15">
+        <v>2.1</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="46">
+        <v>5</v>
       </c>
       <c r="E10"/>
       <c r="F10"/>
@@ -2716,16 +2701,16 @@
       <c r="M10"/>
     </row>
     <row r="11" spans="1:13" s="15" customFormat="1">
-      <c r="A11" s="68">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="65">
+      <c r="A11" s="67">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="40">
         <v>10</v>
       </c>
       <c r="E11"/>
@@ -2736,20 +2721,21 @@
       <c r="M11"/>
     </row>
     <row r="12" spans="1:13" s="15" customFormat="1">
-      <c r="A12" s="15">
-        <v>3</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="D12" s="41">
-        <v>5</v>
+      <c r="A12" s="67">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="64">
+        <v>10</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
+      <c r="G12"/>
       <c r="J12"/>
       <c r="K12"/>
       <c r="L12"/>
@@ -2759,17 +2745,18 @@
       <c r="A13" s="15">
         <v>3.1</v>
       </c>
-      <c r="B13" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="47" t="s">
+      <c r="B13" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="46">
         <v>20</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
+      <c r="G13"/>
       <c r="J13"/>
       <c r="K13"/>
       <c r="L13"/>
@@ -2779,17 +2766,18 @@
       <c r="A14" s="15">
         <v>3.2</v>
       </c>
-      <c r="B14" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="D14" s="41">
+      <c r="B14" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="40">
         <v>10</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
+      <c r="G14"/>
       <c r="J14"/>
       <c r="K14"/>
       <c r="L14"/>
@@ -2799,13 +2787,13 @@
       <c r="A15" s="15">
         <v>3.3</v>
       </c>
-      <c r="B15" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="C15" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="65">
+      <c r="B15" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="64">
         <v>10</v>
       </c>
       <c r="E15"/>
@@ -2818,16 +2806,16 @@
     </row>
     <row r="16" spans="1:13" s="15" customFormat="1">
       <c r="A16" s="15">
-        <v>4</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="D16" s="41">
-        <v>5</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="46">
+        <v>20</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
@@ -2839,16 +2827,16 @@
     </row>
     <row r="17" spans="1:13" s="15" customFormat="1">
       <c r="A17" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>156</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="47">
-        <v>20</v>
+        <v>4.2</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="40">
+        <v>10</v>
       </c>
       <c r="E17"/>
       <c r="F17"/>
@@ -2860,15 +2848,15 @@
     </row>
     <row r="18" spans="1:13" s="15" customFormat="1">
       <c r="A18" s="15">
-        <v>4.2</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="D18" s="41">
+        <v>4.3</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="64">
         <v>10</v>
       </c>
       <c r="E18"/>
@@ -2881,16 +2869,16 @@
     </row>
     <row r="19" spans="1:13" s="15" customFormat="1">
       <c r="A19" s="15">
-        <v>4.3</v>
-      </c>
-      <c r="B19" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="C19" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="65">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="40">
+        <v>5</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
@@ -2902,16 +2890,16 @@
     </row>
     <row r="20" spans="1:13" s="15" customFormat="1">
       <c r="A20" s="15">
-        <v>5</v>
-      </c>
-      <c r="B20" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="D20" s="41">
-        <v>5</v>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="48">
+        <v>50</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -2923,20 +2911,19 @@
     </row>
     <row r="21" spans="1:13" s="15" customFormat="1">
       <c r="A21" s="15">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B21" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="49">
-        <v>50</v>
+        <v>6.1</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="46">
+        <v>20</v>
       </c>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21"/>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
@@ -2944,20 +2931,19 @@
     </row>
     <row r="22" spans="1:13" s="15" customFormat="1">
       <c r="A22" s="15">
-        <v>6</v>
-      </c>
-      <c r="B22" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" s="41">
-        <v>5</v>
+        <v>6.2</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="40">
+        <v>10</v>
       </c>
       <c r="E22"/>
       <c r="F22"/>
-      <c r="G22"/>
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
@@ -2965,20 +2951,19 @@
     </row>
     <row r="23" spans="1:13" s="15" customFormat="1">
       <c r="A23" s="15">
-        <v>6.1</v>
-      </c>
-      <c r="B23" s="38" t="s">
-        <v>158</v>
-      </c>
-      <c r="C23" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="47">
-        <v>20</v>
+        <v>6.3</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="64">
+        <v>10</v>
       </c>
       <c r="E23"/>
       <c r="F23"/>
-      <c r="G23"/>
       <c r="J23"/>
       <c r="K23"/>
       <c r="L23"/>
@@ -2986,20 +2971,19 @@
     </row>
     <row r="24" spans="1:13" s="15" customFormat="1">
       <c r="A24" s="15">
-        <v>6.2</v>
-      </c>
-      <c r="B24" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="D24" s="41">
-        <v>10</v>
+        <v>7.1</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="46">
+        <v>20</v>
       </c>
       <c r="E24"/>
       <c r="F24"/>
-      <c r="G24"/>
       <c r="J24"/>
       <c r="K24"/>
       <c r="L24"/>
@@ -3007,257 +2991,196 @@
     </row>
     <row r="25" spans="1:13" s="15" customFormat="1">
       <c r="A25" s="15">
-        <v>6.3</v>
-      </c>
-      <c r="B25" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="C25" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="65">
+        <v>7.2</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="40">
         <v>10</v>
       </c>
       <c r="E25"/>
       <c r="F25"/>
-      <c r="G25"/>
       <c r="J25"/>
       <c r="K25"/>
       <c r="L25"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" s="15" customFormat="1">
+    <row r="26" spans="1:13">
       <c r="A26" s="15">
+        <v>7.3</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="64">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="15">
+        <v>8.1</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="D26" s="41">
-        <v>5</v>
-      </c>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-    </row>
-    <row r="27" spans="1:13" s="15" customFormat="1">
-      <c r="A27" s="15">
-        <v>7.1</v>
-      </c>
-      <c r="B27" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="47">
+      <c r="D27" s="46">
         <v>20</v>
       </c>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="J27"/>
-      <c r="K27"/>
-      <c r="L27"/>
-      <c r="M27"/>
-    </row>
-    <row r="28" spans="1:13" s="15" customFormat="1">
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="15">
-        <v>7.2</v>
-      </c>
-      <c r="B28" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="D28" s="41">
-        <v>5</v>
-      </c>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="J28"/>
-      <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28"/>
-    </row>
-    <row r="29" spans="1:13" s="15" customFormat="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="15">
-        <v>7.3</v>
-      </c>
-      <c r="B29" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="C29" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="65">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="64">
         <v>10</v>
       </c>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29"/>
-    </row>
-    <row r="30" spans="1:13" s="15" customFormat="1">
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="15">
-        <v>8</v>
-      </c>
-      <c r="B30" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="D30" s="41">
-        <v>5</v>
-      </c>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="J30"/>
-      <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:13" s="15" customFormat="1">
+        <v>10</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="15">
-        <v>8.1</v>
-      </c>
-      <c r="B31" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="C31" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="47">
-        <v>20</v>
-      </c>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
+        <v>10.1</v>
+      </c>
+      <c r="B31" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="51">
+        <v>15</v>
+      </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="15">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="B32" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="C32" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="D32" s="41">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="51">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="15">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="B33" s="38" t="s">
-        <v>150</v>
-      </c>
-      <c r="C33" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" s="65">
-        <v>10</v>
+        <v>10.3</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="51">
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="15">
-        <v>10</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="52" t="s">
+        <v>10.4</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="52">
-        <v>10</v>
+      <c r="D34" s="51">
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="15">
-        <v>10.1</v>
-      </c>
-      <c r="B35" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="52">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="40">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="15">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="B36" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="52">
-        <v>10</v>
+        <v>11.1</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="48">
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="15">
-        <v>10.3</v>
-      </c>
-      <c r="B37" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="C37" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="52">
-        <v>20</v>
-      </c>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="53"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="15">
-        <v>11</v>
-      </c>
-      <c r="B38" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="41">
-        <v>5</v>
-      </c>
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="15">
-        <v>11.1</v>
-      </c>
-      <c r="B39" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="49">
-        <v>50</v>
-      </c>
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="15"/>
@@ -3282,276 +3205,309 @@
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
-      <c r="E43" s="54"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
+      <c r="E44" s="53"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="15"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
+      <c r="E45" s="53"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
+      <c r="E46" s="53"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
       <c r="D47" s="15"/>
+      <c r="E47" s="53"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="15"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="E48" s="53"/>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="15"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="E49" s="53"/>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
-      <c r="E50" s="54"/>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="E50" s="53"/>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="15"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
-      <c r="E51" s="54"/>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="E51" s="53"/>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
-      <c r="E52" s="54"/>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="E52" s="53"/>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
-      <c r="E53" s="54"/>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="E53" s="53"/>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
-      <c r="E54" s="54"/>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="E54" s="53"/>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
       <c r="D55" s="15"/>
-      <c r="E55" s="54"/>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="E55" s="53"/>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
       <c r="D56" s="15"/>
-      <c r="E56" s="54"/>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="E56" s="53"/>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="15"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
       <c r="D57" s="15"/>
-      <c r="E57" s="54"/>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="E57" s="53"/>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="15"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
       <c r="D58" s="15"/>
-      <c r="E58" s="54"/>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="E58" s="53"/>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" s="15"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
       <c r="D59" s="15"/>
-      <c r="E59" s="54"/>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="E59" s="53"/>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" s="15"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
-      <c r="E60" s="54"/>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="E60" s="53"/>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="15"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
-      <c r="E61" s="54"/>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="E61" s="53"/>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="15"/>
       <c r="B62" s="15"/>
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
-      <c r="E62" s="54"/>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="E62" s="53"/>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="15"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
       <c r="E63" s="54"/>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" s="26"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
       <c r="E64" s="54"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="15"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
-      <c r="E65" s="54"/>
+      <c r="E65" s="53"/>
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="15"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
-      <c r="E66" s="54"/>
+      <c r="E66" s="53"/>
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="15"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
       <c r="D67" s="15"/>
-      <c r="E67" s="54"/>
+      <c r="E67" s="53"/>
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="15"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
-      <c r="E68" s="54"/>
+      <c r="E68" s="53"/>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="15"/>
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
       <c r="D69" s="15"/>
-      <c r="E69" s="55"/>
-      <c r="I69" s="38"/>
+      <c r="E69" s="53"/>
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="15"/>
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
       <c r="D70" s="15"/>
-      <c r="E70" s="55"/>
-      <c r="F70" s="26"/>
-      <c r="G70" s="38"/>
-      <c r="H70" s="38"/>
-      <c r="I70" s="38"/>
+      <c r="E70" s="53"/>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="15"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
       <c r="D71" s="15"/>
-      <c r="E71" s="54"/>
-      <c r="F71" s="26"/>
-      <c r="G71" s="38"/>
-      <c r="H71" s="38"/>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="15"/>
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
       <c r="D72" s="15"/>
-      <c r="E72" s="54"/>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="15"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15"/>
       <c r="D73" s="15"/>
-      <c r="E73" s="54"/>
-    </row>
-    <row r="74" spans="1:13">
-      <c r="A74" s="15"/>
-      <c r="B74" s="15"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="54"/>
-    </row>
-    <row r="75" spans="1:13">
-      <c r="A75" s="15"/>
-      <c r="B75" s="15"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="54"/>
-    </row>
-    <row r="76" spans="1:13">
-      <c r="A76" s="15"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="15"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="54"/>
-    </row>
-    <row r="77" spans="1:13">
-      <c r="A77" s="15"/>
-      <c r="B77" s="15"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-    </row>
-    <row r="78" spans="1:13">
-      <c r="A78" s="15"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15"/>
-    </row>
-    <row r="79" spans="1:13">
-      <c r="A79" s="15"/>
-      <c r="B79" s="15"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
+    </row>
+    <row r="74" spans="1:13" s="15" customFormat="1">
+      <c r="E74"/>
+      <c r="F74"/>
+      <c r="J74"/>
+      <c r="K74"/>
+      <c r="L74"/>
+      <c r="M74"/>
+    </row>
+    <row r="75" spans="1:13" s="15" customFormat="1">
+      <c r="A75" s="55"/>
+      <c r="B75" s="55"/>
+      <c r="C75" s="55"/>
+      <c r="D75" s="55"/>
+      <c r="E75"/>
+      <c r="F75"/>
+      <c r="J75"/>
+      <c r="K75"/>
+      <c r="L75"/>
+      <c r="M75"/>
+    </row>
+    <row r="76" spans="1:13" s="15" customFormat="1">
+      <c r="A76" s="55"/>
+      <c r="B76" s="55"/>
+      <c r="C76" s="55"/>
+      <c r="D76" s="55"/>
+      <c r="E76"/>
+      <c r="F76"/>
+      <c r="J76"/>
+      <c r="K76"/>
+      <c r="L76"/>
+      <c r="M76"/>
+    </row>
+    <row r="77" spans="1:13" s="15" customFormat="1">
+      <c r="A77" s="55"/>
+      <c r="B77" s="55"/>
+      <c r="C77" s="55"/>
+      <c r="D77" s="55"/>
+      <c r="E77" s="26"/>
+      <c r="F77"/>
+      <c r="J77"/>
+      <c r="K77"/>
+      <c r="L77"/>
+      <c r="M77"/>
+    </row>
+    <row r="78" spans="1:13" s="15" customFormat="1">
+      <c r="A78" s="55"/>
+      <c r="B78" s="55"/>
+      <c r="C78" s="55"/>
+      <c r="D78" s="55"/>
+      <c r="E78" s="26"/>
+      <c r="F78"/>
+      <c r="J78"/>
+      <c r="K78"/>
+      <c r="L78"/>
+      <c r="M78"/>
+    </row>
+    <row r="79" spans="1:13" s="15" customFormat="1">
+      <c r="A79" s="55"/>
+      <c r="B79" s="55"/>
+      <c r="C79" s="55"/>
+      <c r="D79" s="55"/>
+      <c r="E79" s="26"/>
+      <c r="F79"/>
+      <c r="J79"/>
+      <c r="K79"/>
+      <c r="L79"/>
+      <c r="M79"/>
     </row>
     <row r="80" spans="1:13" s="15" customFormat="1">
-      <c r="A80" s="56"/>
-      <c r="B80" s="56"/>
-      <c r="C80" s="56"/>
-      <c r="D80" s="56"/>
+      <c r="A80" s="55"/>
+      <c r="B80" s="55"/>
+      <c r="C80" s="55"/>
+      <c r="D80" s="55"/>
       <c r="E80"/>
       <c r="F80"/>
+      <c r="G80"/>
+      <c r="H80"/>
       <c r="J80"/>
       <c r="K80"/>
       <c r="L80"/>
       <c r="M80"/>
     </row>
     <row r="81" spans="1:13" s="15" customFormat="1">
-      <c r="A81" s="56"/>
-      <c r="B81" s="56"/>
-      <c r="C81" s="56"/>
-      <c r="D81" s="56"/>
+      <c r="A81" s="55"/>
+      <c r="B81" s="55"/>
+      <c r="C81" s="55"/>
+      <c r="D81" s="55"/>
       <c r="E81"/>
       <c r="F81"/>
       <c r="J81"/>
@@ -3560,70 +3516,80 @@
       <c r="M81"/>
     </row>
     <row r="82" spans="1:13" s="15" customFormat="1">
-      <c r="A82" s="56"/>
-      <c r="B82" s="56"/>
-      <c r="C82" s="56"/>
-      <c r="D82" s="56"/>
+      <c r="A82" s="55"/>
+      <c r="B82" s="55"/>
+      <c r="C82" s="55"/>
+      <c r="D82" s="55"/>
       <c r="E82"/>
       <c r="F82"/>
+      <c r="G82"/>
+      <c r="H82"/>
       <c r="J82"/>
       <c r="K82"/>
       <c r="L82"/>
       <c r="M82"/>
     </row>
     <row r="83" spans="1:13" s="15" customFormat="1">
-      <c r="A83" s="56"/>
-      <c r="B83" s="56"/>
-      <c r="C83" s="56"/>
-      <c r="D83" s="56"/>
-      <c r="E83" s="26"/>
+      <c r="A83" s="55"/>
+      <c r="B83" s="55"/>
+      <c r="C83" s="55"/>
+      <c r="D83" s="55"/>
+      <c r="E83"/>
       <c r="F83"/>
+      <c r="G83"/>
+      <c r="H83"/>
       <c r="J83"/>
       <c r="K83"/>
       <c r="L83"/>
       <c r="M83"/>
     </row>
     <row r="84" spans="1:13" s="15" customFormat="1">
-      <c r="A84" s="56"/>
-      <c r="B84" s="56"/>
-      <c r="C84" s="56"/>
-      <c r="D84" s="56"/>
-      <c r="E84" s="26"/>
+      <c r="A84" s="55"/>
+      <c r="B84" s="55"/>
+      <c r="C84" s="55"/>
+      <c r="D84" s="55"/>
+      <c r="E84"/>
       <c r="F84"/>
+      <c r="G84"/>
+      <c r="H84"/>
       <c r="J84"/>
       <c r="K84"/>
       <c r="L84"/>
       <c r="M84"/>
     </row>
     <row r="85" spans="1:13" s="15" customFormat="1">
-      <c r="A85" s="56"/>
-      <c r="B85" s="56"/>
-      <c r="C85" s="56"/>
-      <c r="D85" s="56"/>
-      <c r="E85" s="26"/>
+      <c r="A85" s="55"/>
+      <c r="B85" s="55"/>
+      <c r="C85" s="55"/>
+      <c r="D85" s="55"/>
+      <c r="E85"/>
       <c r="F85"/>
+      <c r="G85"/>
+      <c r="H85"/>
       <c r="J85"/>
       <c r="K85"/>
       <c r="L85"/>
       <c r="M85"/>
     </row>
     <row r="86" spans="1:13" s="15" customFormat="1">
-      <c r="A86" s="56"/>
-      <c r="B86" s="56"/>
-      <c r="C86" s="56"/>
-      <c r="D86" s="56"/>
+      <c r="A86" s="55"/>
+      <c r="B86" s="55"/>
+      <c r="C86" s="55"/>
+      <c r="D86" s="55"/>
       <c r="E86"/>
       <c r="F86"/>
+      <c r="G86"/>
+      <c r="H86"/>
       <c r="J86"/>
       <c r="K86"/>
       <c r="L86"/>
       <c r="M86"/>
     </row>
     <row r="87" spans="1:13" s="15" customFormat="1">
-      <c r="A87" s="56"/>
-      <c r="B87" s="56"/>
-      <c r="C87" s="56"/>
-      <c r="D87" s="56"/>
+      <c r="A87" s="55"/>
+      <c r="B87" s="55"/>
+      <c r="C87" s="55"/>
+      <c r="D87" s="55"/>
       <c r="E87"/>
       <c r="F87"/>
       <c r="G87"/>
@@ -3634,22 +3600,24 @@
       <c r="M87"/>
     </row>
     <row r="88" spans="1:13" s="15" customFormat="1">
-      <c r="A88" s="56"/>
-      <c r="B88" s="56"/>
-      <c r="C88" s="56"/>
-      <c r="D88" s="56"/>
+      <c r="A88" s="55"/>
+      <c r="B88" s="55"/>
+      <c r="C88" s="55"/>
+      <c r="D88" s="55"/>
       <c r="E88"/>
       <c r="F88"/>
+      <c r="G88"/>
+      <c r="H88"/>
       <c r="J88"/>
       <c r="K88"/>
       <c r="L88"/>
       <c r="M88"/>
     </row>
     <row r="89" spans="1:13" s="15" customFormat="1">
-      <c r="A89" s="56"/>
-      <c r="B89" s="56"/>
-      <c r="C89" s="56"/>
-      <c r="D89" s="56"/>
+      <c r="A89" s="55"/>
+      <c r="B89" s="55"/>
+      <c r="C89" s="55"/>
+      <c r="D89" s="55"/>
       <c r="E89"/>
       <c r="F89"/>
       <c r="G89"/>
@@ -3659,130 +3627,50 @@
       <c r="L89"/>
       <c r="M89"/>
     </row>
-    <row r="90" spans="1:13" s="15" customFormat="1">
-      <c r="A90" s="56"/>
-      <c r="B90" s="56"/>
-      <c r="C90" s="56"/>
-      <c r="D90" s="56"/>
-      <c r="E90"/>
-      <c r="F90"/>
-      <c r="G90"/>
-      <c r="H90"/>
-      <c r="J90"/>
-      <c r="K90"/>
-      <c r="L90"/>
-      <c r="M90"/>
-    </row>
-    <row r="91" spans="1:13" s="15" customFormat="1">
-      <c r="A91" s="56"/>
-      <c r="B91" s="56"/>
-      <c r="C91" s="56"/>
-      <c r="D91" s="56"/>
-      <c r="E91"/>
-      <c r="F91"/>
-      <c r="G91"/>
-      <c r="H91"/>
-      <c r="J91"/>
-      <c r="K91"/>
-      <c r="L91"/>
-      <c r="M91"/>
-    </row>
-    <row r="92" spans="1:13" s="15" customFormat="1">
-      <c r="A92" s="56"/>
-      <c r="B92" s="56"/>
-      <c r="C92" s="56"/>
-      <c r="D92" s="56"/>
-      <c r="E92"/>
-      <c r="F92"/>
-      <c r="G92"/>
-      <c r="H92"/>
-      <c r="J92"/>
-      <c r="K92"/>
-      <c r="L92"/>
-      <c r="M92"/>
-    </row>
-    <row r="93" spans="1:13" s="15" customFormat="1">
-      <c r="A93" s="56"/>
-      <c r="B93" s="56"/>
-      <c r="C93" s="56"/>
-      <c r="D93" s="56"/>
-      <c r="E93"/>
-      <c r="F93"/>
-      <c r="G93"/>
-      <c r="H93"/>
-      <c r="J93"/>
-      <c r="K93"/>
-      <c r="L93"/>
-      <c r="M93"/>
-    </row>
-    <row r="94" spans="1:13" s="15" customFormat="1">
-      <c r="A94" s="56"/>
-      <c r="B94" s="56"/>
-      <c r="C94" s="56"/>
-      <c r="D94" s="56"/>
-      <c r="E94"/>
-      <c r="F94"/>
-      <c r="G94"/>
-      <c r="H94"/>
-      <c r="J94"/>
-      <c r="K94"/>
-      <c r="L94"/>
-      <c r="M94"/>
-    </row>
-    <row r="95" spans="1:13" s="15" customFormat="1">
-      <c r="A95" s="56"/>
-      <c r="B95" s="56"/>
-      <c r="C95" s="56"/>
-      <c r="D95" s="56"/>
-      <c r="E95"/>
-      <c r="F95"/>
-      <c r="G95"/>
-      <c r="H95"/>
-      <c r="J95"/>
-      <c r="K95"/>
-      <c r="L95"/>
-      <c r="M95"/>
+    <row r="90" spans="1:13">
+      <c r="A90" s="55"/>
+      <c r="B90" s="55"/>
+      <c r="C90" s="55"/>
+      <c r="D90" s="55"/>
+    </row>
+    <row r="91" spans="1:13">
+      <c r="A91" s="55"/>
+      <c r="B91" s="55"/>
+      <c r="C91" s="55"/>
+      <c r="D91" s="55"/>
+    </row>
+    <row r="92" spans="1:13">
+      <c r="A92" s="55"/>
+      <c r="B92" s="55"/>
+      <c r="C92" s="55"/>
+      <c r="D92" s="55"/>
+    </row>
+    <row r="93" spans="1:13">
+      <c r="A93" s="55"/>
+      <c r="B93" s="55"/>
+      <c r="C93" s="55"/>
+      <c r="D93" s="55"/>
+    </row>
+    <row r="94" spans="1:13">
+      <c r="A94" s="55"/>
+      <c r="B94" s="55"/>
+      <c r="C94" s="55"/>
+      <c r="D94" s="55"/>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95" s="55"/>
+      <c r="B95" s="55"/>
+      <c r="C95" s="55"/>
+      <c r="D95" s="55"/>
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="56"/>
       <c r="B96" s="56"/>
-      <c r="C96" s="56"/>
       <c r="D96" s="56"/>
-      <c r="G96"/>
-      <c r="H96"/>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="56"/>
-      <c r="B97" s="56"/>
-      <c r="C97" s="56"/>
-      <c r="D97" s="56"/>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="56"/>
-      <c r="B98" s="56"/>
-      <c r="C98" s="56"/>
-      <c r="D98" s="56"/>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="56"/>
-      <c r="B99" s="56"/>
-      <c r="C99" s="56"/>
-      <c r="D99" s="56"/>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="56"/>
-      <c r="B100" s="56"/>
-      <c r="C100" s="56"/>
-      <c r="D100" s="56"/>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="57"/>
-      <c r="B101" s="57"/>
-      <c r="D101" s="57"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D105">
-    <sortCondition ref="A2:A105"/>
+  <sortState ref="A2:D103">
+    <sortCondition ref="A2:A103"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add OH form to HW00
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH456/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B3BE1A-11FE-E04A-9B59-ABC2317D89BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683231E6-5755-C14C-92DC-E1EA34A028DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="162">
   <si>
     <t>Finals Week</t>
   </si>
@@ -596,6 +596,9 @@
   </si>
   <si>
     <t>Review project webpage</t>
+  </si>
+  <si>
+    <t>Jane Teach</t>
   </si>
 </sst>
 </file>
@@ -729,7 +732,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -811,6 +814,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -968,7 +977,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1155,6 +1164,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -1579,7 +1591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1931,9 +1943,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15"/>
@@ -2059,11 +2071,11 @@
       <c r="F4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="71" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="80">
@@ -2109,6 +2121,9 @@
       </c>
       <c r="F6" s="7" t="s">
         <v>109</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="113" thickBot="1">

</xml_diff>

<commit_message>
adjust schedule spacing. fix broken link
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,27 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH456/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683231E6-5755-C14C-92DC-E1EA34A028DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF583185-174A-4A83-A32D-80DBA21E4C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30690" yWindow="585" windowWidth="25905" windowHeight="14430" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
     <sheet name="slo_detail" sheetId="5" r:id="rId2"/>
     <sheet name="points" sheetId="11" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -577,9 +585,6 @@
     <t>todo</t>
   </si>
   <si>
-    <t>[[HW 00: Getting Started]](hw00-getting-started.html) (Due Sun 1/26 )</t>
-  </si>
-  <si>
     <t>hw00-getting-started</t>
   </si>
   <si>
@@ -599,13 +604,16 @@
   </si>
   <si>
     <t>Jane Teach</t>
+  </si>
+  <si>
+    <t>[[HW 00: Getting Started]](hw/hw00-getting-started.html) (Due Sun 1/26 )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1595,18 +1603,18 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="15"/>
-    <col min="3" max="3" width="5.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" style="15" customWidth="1"/>
+    <col min="1" max="2" width="8.875" style="15"/>
+    <col min="3" max="3" width="5.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" customWidth="1"/>
+    <col min="5" max="5" width="11.125" style="15" customWidth="1"/>
     <col min="6" max="6" width="18" style="25" customWidth="1"/>
     <col min="7" max="7" width="33" customWidth="1"/>
     <col min="8" max="8" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="15" customFormat="1" ht="17" thickBot="1">
+    <row r="1" spans="1:8" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>25</v>
       </c>
@@ -1632,7 +1640,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>1.1000000000000001</v>
       </c>
@@ -1649,13 +1657,13 @@
         <v>148</v>
       </c>
       <c r="G2" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>1.2</v>
       </c>
@@ -1666,7 +1674,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>2.1</v>
       </c>
@@ -1686,7 +1694,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>3.1</v>
       </c>
@@ -1703,7 +1711,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="34">
+    <row r="6" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>4.0999999999999996</v>
       </c>
@@ -1723,7 +1731,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>5.0999999999999996</v>
       </c>
@@ -1740,7 +1748,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>6.1</v>
       </c>
@@ -1758,7 +1766,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>7.1</v>
       </c>
@@ -1772,7 +1780,7 @@
       <c r="F9" s="36"/>
       <c r="G9" s="26"/>
     </row>
-    <row r="10" spans="1:8" ht="34">
+    <row r="10" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>9.1</v>
       </c>
@@ -1791,7 +1799,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>8</v>
       </c>
@@ -1805,7 +1813,7 @@
       <c r="F11" s="33"/>
       <c r="G11" s="31"/>
     </row>
-    <row r="12" spans="1:8" ht="24" customHeight="1">
+    <row r="12" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>10.1</v>
       </c>
@@ -1825,7 +1833,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>11.1</v>
       </c>
@@ -1837,7 +1845,7 @@
       <c r="F13" s="30"/>
       <c r="G13" s="26"/>
     </row>
-    <row r="14" spans="1:8" ht="26" customHeight="1">
+    <row r="14" spans="1:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>12.1</v>
       </c>
@@ -1855,7 +1863,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>13.1</v>
       </c>
@@ -1874,7 +1882,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>15.1</v>
       </c>
@@ -1892,7 +1900,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>16.100000000000001</v>
       </c>
@@ -1901,7 +1909,7 @@
       </c>
       <c r="F17" s="30"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>17.100000000000001</v>
       </c>
@@ -1916,7 +1924,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="51">
+    <row r="19" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>18.100000000000001</v>
       </c>
@@ -1931,7 +1939,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A21:G24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:G24">
     <sortCondition ref="B21:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1948,21 +1956,21 @@
       <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.875" style="6" customWidth="1"/>
     <col min="4" max="4" width="36.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="34.6640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="38.375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="34.625" style="7" customWidth="1"/>
     <col min="7" max="8" width="38" style="7" customWidth="1"/>
-    <col min="9" max="9" width="35.83203125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="14.83203125" style="6"/>
+    <col min="9" max="9" width="35.875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="24.625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="14.875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1994,7 +2002,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="176">
+    <row r="2" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="69">
         <v>1</v>
       </c>
@@ -2002,10 +2010,10 @@
         <v>42389</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>153</v>
@@ -2017,14 +2025,14 @@
         <v>147</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J2" s="12"/>
     </row>
-    <row r="3" spans="1:10" ht="112">
+    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="69">
         <v>2</v>
       </c>
@@ -2053,7 +2061,7 @@
       </c>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10" ht="48">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="69">
         <v>3</v>
       </c>
@@ -2072,13 +2080,13 @@
         <v>33</v>
       </c>
       <c r="G4" s="71" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="80">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="69">
         <v>4</v>
       </c>
@@ -2102,7 +2110,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="141" thickBot="1">
+    <row r="6" spans="1:10" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="69">
         <v>5</v>
       </c>
@@ -2126,7 +2134,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="113" thickBot="1">
+    <row r="7" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="69">
         <v>6</v>
       </c>
@@ -2159,7 +2167,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="112">
+    <row r="8" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="69">
         <v>7</v>
       </c>
@@ -2185,7 +2193,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -2206,7 +2214,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11">
         <f t="shared" si="0"/>
@@ -2231,7 +2239,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="112">
+    <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -2254,7 +2262,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="56">
+    <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -2275,7 +2283,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="128">
+    <row r="13" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -2305,7 +2313,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="80">
+    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -2326,7 +2334,7 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:10" ht="16">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -2343,7 +2351,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -2359,7 +2367,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -2382,7 +2390,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="32">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>0</v>
       </c>
@@ -2397,7 +2405,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="16" thickBot="1">
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="60"/>
@@ -2406,7 +2414,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" ht="16" thickBot="1">
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -2428,21 +2436,21 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="37"/>
-    <col min="2" max="2" width="32.1640625" style="37" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" style="37" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="5.1640625" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="37"/>
+    <col min="2" max="2" width="32.125" style="37" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="37" customWidth="1"/>
+    <col min="4" max="4" width="6.375" style="37" customWidth="1"/>
+    <col min="5" max="5" width="5.125" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="10" style="15" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="15"/>
-    <col min="9" max="9" width="4.6640625" style="15" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="15"/>
+    <col min="9" max="9" width="4.625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" thickBot="1">
+    <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="39" t="s">
         <v>23</v>
       </c>
@@ -2474,7 +2482,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17" thickTop="1">
+    <row r="2" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>0</v>
       </c>
@@ -2508,7 +2516,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>0</v>
       </c>
@@ -2542,7 +2550,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>0</v>
       </c>
@@ -2576,7 +2584,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>0</v>
       </c>
@@ -2610,7 +2618,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>0</v>
       </c>
@@ -2638,7 +2646,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17" thickBot="1">
+    <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>1</v>
       </c>
@@ -2656,7 +2664,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="15" customFormat="1" ht="17" thickTop="1">
+    <row r="8" spans="1:13" s="15" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>1.1000000000000001</v>
       </c>
@@ -2675,7 +2683,7 @@
       <c r="L8"/>
       <c r="M8"/>
     </row>
-    <row r="9" spans="1:13" s="15" customFormat="1">
+    <row r="9" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="67">
         <v>2</v>
       </c>
@@ -2695,7 +2703,7 @@
       <c r="L9"/>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:13" s="15" customFormat="1">
+    <row r="10" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>2.1</v>
       </c>
@@ -2715,7 +2723,7 @@
       <c r="L10"/>
       <c r="M10"/>
     </row>
-    <row r="11" spans="1:13" s="15" customFormat="1">
+    <row r="11" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="67">
         <v>2.2000000000000002</v>
       </c>
@@ -2735,7 +2743,7 @@
       <c r="L11"/>
       <c r="M11"/>
     </row>
-    <row r="12" spans="1:13" s="15" customFormat="1">
+    <row r="12" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="67">
         <v>2.2999999999999998</v>
       </c>
@@ -2756,7 +2764,7 @@
       <c r="L12"/>
       <c r="M12"/>
     </row>
-    <row r="13" spans="1:13" s="15" customFormat="1">
+    <row r="13" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>3.1</v>
       </c>
@@ -2777,7 +2785,7 @@
       <c r="L13"/>
       <c r="M13"/>
     </row>
-    <row r="14" spans="1:13" s="15" customFormat="1">
+    <row r="14" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>3.2</v>
       </c>
@@ -2798,7 +2806,7 @@
       <c r="L14"/>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:13" s="15" customFormat="1">
+    <row r="15" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>3.3</v>
       </c>
@@ -2819,7 +2827,7 @@
       <c r="L15"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:13" s="15" customFormat="1">
+    <row r="16" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>4.0999999999999996</v>
       </c>
@@ -2840,7 +2848,7 @@
       <c r="L16"/>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" s="15" customFormat="1">
+    <row r="17" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>4.2</v>
       </c>
@@ -2861,7 +2869,7 @@
       <c r="L17"/>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" s="15" customFormat="1">
+    <row r="18" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>4.3</v>
       </c>
@@ -2882,7 +2890,7 @@
       <c r="L18"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" s="15" customFormat="1">
+    <row r="19" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>5</v>
       </c>
@@ -2903,7 +2911,7 @@
       <c r="L19"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" s="15" customFormat="1">
+    <row r="20" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>5.0999999999999996</v>
       </c>
@@ -2924,7 +2932,7 @@
       <c r="L20"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" s="15" customFormat="1">
+    <row r="21" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>6.1</v>
       </c>
@@ -2944,7 +2952,7 @@
       <c r="L21"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" s="15" customFormat="1">
+    <row r="22" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>6.2</v>
       </c>
@@ -2964,7 +2972,7 @@
       <c r="L22"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" s="15" customFormat="1">
+    <row r="23" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>6.3</v>
       </c>
@@ -2984,7 +2992,7 @@
       <c r="L23"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" s="15" customFormat="1">
+    <row r="24" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>7.1</v>
       </c>
@@ -3004,7 +3012,7 @@
       <c r="L24"/>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" s="15" customFormat="1">
+    <row r="25" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>7.2</v>
       </c>
@@ -3024,7 +3032,7 @@
       <c r="L25"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>7.3</v>
       </c>
@@ -3038,7 +3046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>8.1</v>
       </c>
@@ -3052,7 +3060,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>8.1999999999999993</v>
       </c>
@@ -3066,7 +3074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>8.3000000000000007</v>
       </c>
@@ -3080,7 +3088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>10</v>
       </c>
@@ -3094,7 +3102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>10.1</v>
       </c>
@@ -3108,7 +3116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>10.199999999999999</v>
       </c>
@@ -3122,7 +3130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>10.3</v>
       </c>
@@ -3136,7 +3144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>10.4</v>
       </c>
@@ -3150,7 +3158,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>11</v>
       </c>
@@ -3164,7 +3172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>11.1</v>
       </c>
@@ -3178,183 +3186,183 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="53"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
       <c r="D40" s="15"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="15"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
       <c r="E44" s="53"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
       <c r="E45" s="53"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
       <c r="E46" s="53"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
       <c r="D47" s="15"/>
       <c r="E47" s="53"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
       <c r="E48" s="53"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
       <c r="E49" s="53"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
       <c r="E50" s="53"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
       <c r="E51" s="53"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
       <c r="E52" s="53"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
       <c r="E53" s="53"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
       <c r="E54" s="53"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
       <c r="D55" s="15"/>
       <c r="E55" s="53"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
       <c r="D56" s="15"/>
       <c r="E56" s="53"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
       <c r="D57" s="15"/>
       <c r="E57" s="53"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
       <c r="D58" s="15"/>
       <c r="E58" s="53"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="15"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
       <c r="D59" s="15"/>
       <c r="E59" s="53"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
       <c r="E60" s="53"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
       <c r="E61" s="53"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="15"/>
       <c r="B62" s="15"/>
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
       <c r="E62" s="53"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
@@ -3365,7 +3373,7 @@
       <c r="H63" s="37"/>
       <c r="I63" s="37"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
@@ -3376,67 +3384,67 @@
       <c r="H64" s="37"/>
       <c r="I64" s="37"/>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="15"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
       <c r="E65" s="53"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="15"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
       <c r="E66" s="53"/>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="15"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
       <c r="D67" s="15"/>
       <c r="E67" s="53"/>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="15"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
       <c r="E68" s="53"/>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="15"/>
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
       <c r="D69" s="15"/>
       <c r="E69" s="53"/>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="15"/>
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
       <c r="D70" s="15"/>
       <c r="E70" s="53"/>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="15"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
       <c r="D71" s="15"/>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="15"/>
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
       <c r="D72" s="15"/>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="15"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15"/>
       <c r="D73" s="15"/>
     </row>
-    <row r="74" spans="1:13" s="15" customFormat="1">
+    <row r="74" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E74"/>
       <c r="F74"/>
       <c r="J74"/>
@@ -3444,7 +3452,7 @@
       <c r="L74"/>
       <c r="M74"/>
     </row>
-    <row r="75" spans="1:13" s="15" customFormat="1">
+    <row r="75" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="55"/>
       <c r="B75" s="55"/>
       <c r="C75" s="55"/>
@@ -3456,7 +3464,7 @@
       <c r="L75"/>
       <c r="M75"/>
     </row>
-    <row r="76" spans="1:13" s="15" customFormat="1">
+    <row r="76" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="55"/>
       <c r="B76" s="55"/>
       <c r="C76" s="55"/>
@@ -3468,7 +3476,7 @@
       <c r="L76"/>
       <c r="M76"/>
     </row>
-    <row r="77" spans="1:13" s="15" customFormat="1">
+    <row r="77" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="55"/>
       <c r="B77" s="55"/>
       <c r="C77" s="55"/>
@@ -3480,7 +3488,7 @@
       <c r="L77"/>
       <c r="M77"/>
     </row>
-    <row r="78" spans="1:13" s="15" customFormat="1">
+    <row r="78" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="55"/>
       <c r="B78" s="55"/>
       <c r="C78" s="55"/>
@@ -3492,7 +3500,7 @@
       <c r="L78"/>
       <c r="M78"/>
     </row>
-    <row r="79" spans="1:13" s="15" customFormat="1">
+    <row r="79" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="55"/>
       <c r="B79" s="55"/>
       <c r="C79" s="55"/>
@@ -3504,7 +3512,7 @@
       <c r="L79"/>
       <c r="M79"/>
     </row>
-    <row r="80" spans="1:13" s="15" customFormat="1">
+    <row r="80" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="55"/>
       <c r="B80" s="55"/>
       <c r="C80" s="55"/>
@@ -3518,7 +3526,7 @@
       <c r="L80"/>
       <c r="M80"/>
     </row>
-    <row r="81" spans="1:13" s="15" customFormat="1">
+    <row r="81" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="55"/>
       <c r="B81" s="55"/>
       <c r="C81" s="55"/>
@@ -3530,7 +3538,7 @@
       <c r="L81"/>
       <c r="M81"/>
     </row>
-    <row r="82" spans="1:13" s="15" customFormat="1">
+    <row r="82" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="55"/>
       <c r="B82" s="55"/>
       <c r="C82" s="55"/>
@@ -3544,7 +3552,7 @@
       <c r="L82"/>
       <c r="M82"/>
     </row>
-    <row r="83" spans="1:13" s="15" customFormat="1">
+    <row r="83" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="55"/>
       <c r="B83" s="55"/>
       <c r="C83" s="55"/>
@@ -3558,7 +3566,7 @@
       <c r="L83"/>
       <c r="M83"/>
     </row>
-    <row r="84" spans="1:13" s="15" customFormat="1">
+    <row r="84" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="55"/>
       <c r="B84" s="55"/>
       <c r="C84" s="55"/>
@@ -3572,7 +3580,7 @@
       <c r="L84"/>
       <c r="M84"/>
     </row>
-    <row r="85" spans="1:13" s="15" customFormat="1">
+    <row r="85" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="55"/>
       <c r="B85" s="55"/>
       <c r="C85" s="55"/>
@@ -3586,7 +3594,7 @@
       <c r="L85"/>
       <c r="M85"/>
     </row>
-    <row r="86" spans="1:13" s="15" customFormat="1">
+    <row r="86" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="55"/>
       <c r="B86" s="55"/>
       <c r="C86" s="55"/>
@@ -3600,7 +3608,7 @@
       <c r="L86"/>
       <c r="M86"/>
     </row>
-    <row r="87" spans="1:13" s="15" customFormat="1">
+    <row r="87" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="55"/>
       <c r="B87" s="55"/>
       <c r="C87" s="55"/>
@@ -3614,7 +3622,7 @@
       <c r="L87"/>
       <c r="M87"/>
     </row>
-    <row r="88" spans="1:13" s="15" customFormat="1">
+    <row r="88" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="55"/>
       <c r="B88" s="55"/>
       <c r="C88" s="55"/>
@@ -3628,7 +3636,7 @@
       <c r="L88"/>
       <c r="M88"/>
     </row>
-    <row r="89" spans="1:13" s="15" customFormat="1">
+    <row r="89" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="55"/>
       <c r="B89" s="55"/>
       <c r="C89" s="55"/>
@@ -3642,49 +3650,49 @@
       <c r="L89"/>
       <c r="M89"/>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="55"/>
       <c r="B90" s="55"/>
       <c r="C90" s="55"/>
       <c r="D90" s="55"/>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="55"/>
       <c r="B91" s="55"/>
       <c r="C91" s="55"/>
       <c r="D91" s="55"/>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="55"/>
       <c r="B92" s="55"/>
       <c r="C92" s="55"/>
       <c r="D92" s="55"/>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="55"/>
       <c r="B93" s="55"/>
       <c r="C93" s="55"/>
       <c r="D93" s="55"/>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="55"/>
       <c r="B94" s="55"/>
       <c r="C94" s="55"/>
       <c r="D94" s="55"/>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="55"/>
       <c r="B95" s="55"/>
       <c r="C95" s="55"/>
       <c r="D95" s="55"/>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="56"/>
       <c r="B96" s="56"/>
       <c r="D96" s="56"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D103">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D103">
     <sortCondition ref="A2:A103"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add reading and project info
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58BC626-48E2-40EE-8DA0-BEA6C7B994C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F13C65B-5354-4D1C-925D-FC848EDCEB1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29730" yWindow="675" windowWidth="25905" windowHeight="14430" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -23,6 +23,14 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -31,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="167">
   <si>
     <t>Finals Week</t>
   </si>
@@ -594,6 +602,21 @@
   <si>
     <t>Quiz on Data preparation &amp; class logistics
 Create a Data preparation reference flowchart</t>
+  </si>
+  <si>
+    <t>PMA6 CH9, ASCN CH10.5</t>
+  </si>
+  <si>
+    <t>PMA6 CH12, ASCN Ch9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review all listed readings, and any notes you have on modeling from previous classes. 
+Look at Hw01
+</t>
+  </si>
+  <si>
+    <t>MLR: PMA6 Ch8, 10.3, ASCN Ch8   
+Modeling: ASCN Ch10.1-10.3</t>
   </si>
 </sst>
 </file>
@@ -1586,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1661,7 +1684,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>2.1</v>
       </c>
@@ -1671,6 +1694,9 @@
       <c r="D4" t="s">
         <v>81</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="F4" s="34" t="s">
         <v>76</v>
       </c>
@@ -1681,7 +1707,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>3.1</v>
       </c>
@@ -1692,7 +1718,9 @@
       <c r="D5" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="16"/>
+      <c r="E5" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="G5" s="26"/>
       <c r="H5" t="s">
         <v>35</v>
@@ -1707,6 +1735,9 @@
       </c>
       <c r="D6" t="s">
         <v>107</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>164</v>
       </c>
       <c r="F6" s="34" t="s">
         <v>77</v>
@@ -1926,7 +1957,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A21:G24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:G24">
     <sortCondition ref="B21:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1938,9 +1969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,7 +2064,9 @@
       <c r="D3" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>131</v>
       </c>
@@ -2062,7 +2095,9 @@
       <c r="D4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>33</v>
       </c>
@@ -2086,6 +2121,9 @@
       </c>
       <c r="D5" s="63" t="s">
         <v>133</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>164</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>99</v>
@@ -3696,7 +3734,7 @@
       <c r="D97" s="56"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D104">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D104">
     <sortCondition ref="A2:A104"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add due date to hw2
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20356"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D40659C-1CE6-434E-9532-FF904B075975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973389CD-F869-4294-BAC6-00066D4A95D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3915" yWindow="825" windowWidth="23580" windowHeight="14925" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,14 +22,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -608,10 +600,6 @@
     <t>Recruitment video created (Due Mon 2/10 )</t>
   </si>
   <si>
-    <t>HW 02: GLM and Classification
-LJ Check in (Due 2/14 )</t>
-  </si>
-  <si>
     <t>Review on Regression &amp; Variable selection</t>
   </si>
   <si>
@@ -640,6 +628,10 @@
   <si>
     <t xml:space="preserve">Odds Ratios are always the odds of an event for one group compared to another group. 
 Some measures of model fit for Logistic regression is slightly different than for linear regression. </t>
+  </si>
+  <si>
+    <t>HW 02: GLM and Classification (Due 2/23 )
+LJ Check in (Due 2/14 )</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1626,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1750,7 +1742,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>4.0999999999999996</v>
       </c>
@@ -1761,13 +1753,13 @@
         <v>94</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F6" s="34" t="s">
         <v>69</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="H6" t="s">
         <v>162</v>
@@ -1981,7 +1973,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:G24">
+  <sortState ref="A21:G24">
     <sortCondition ref="B21:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2117,10 +2109,10 @@
         <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>159</v>
@@ -2141,22 +2133,22 @@
         <v>42409</v>
       </c>
       <c r="C5" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="F5" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>132</v>
@@ -3773,7 +3765,7 @@
       <c r="D98" s="54"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D105">
+  <sortState ref="A2:D105">
     <sortCondition ref="A2:A105"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish updated info for covid19
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9AF45E-5411-4541-A995-247B8552F768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BA710E-9349-4BB1-A930-3BC3CF58D3E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="points" sheetId="11" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr autoRecover="0" repairLoad="1"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -622,9 +622,6 @@
     <t>finals</t>
   </si>
   <si>
-    <t>Project update (1pg + 5 min show &amp; tell) (Due  03/13 )</t>
-  </si>
-  <si>
     <t>Task distributions, project timeline (Due Sat 2/22 )  
 Printed Team agreements (Due Mon 2/24 )</t>
   </si>
@@ -660,6 +657,9 @@
   </si>
   <si>
     <t>[[Quiz 03]](https://forms.gle/iAHo9yiLrjp8v5266)  (Due 3/5)</t>
+  </si>
+  <si>
+    <t>[[Project update]](project.html#project_update_(wk_8)) (Due  03/13 )</t>
   </si>
 </sst>
 </file>
@@ -1660,7 +1660,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1745,7 +1745,7 @@
         <v>67</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F4" s="34" t="s">
         <v>150</v>
@@ -1787,7 +1787,7 @@
         <v>87</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F6" s="34" t="s">
         <v>162</v>
@@ -1815,7 +1815,7 @@
       <c r="F7" s="36"/>
       <c r="G7" s="26"/>
       <c r="H7" s="38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
@@ -1829,13 +1829,13 @@
         <v>45</v>
       </c>
       <c r="E8" s="72" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="F8" s="36" t="s">
-        <v>176</v>
-      </c>
       <c r="G8" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1867,10 +1867,10 @@
       <c r="E10" s="37"/>
       <c r="F10" s="36"/>
       <c r="G10" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H10" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2267,7 +2267,7 @@
         <v>47</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>126</v>
@@ -2295,7 +2295,7 @@
         <v>24</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
start to update for major changes
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BA710E-9349-4BB1-A930-3BC3CF58D3E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9664DD-DB56-4589-B6FF-78E9B94A12BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="178">
   <si>
     <t>Finals Week</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Project</t>
   </si>
   <si>
-    <t>Final Exam</t>
-  </si>
-  <si>
     <t>Monday</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>Introduction to the class</t>
   </si>
   <si>
-    <t xml:space="preserve">Go relax and take a well deserved break. </t>
-  </si>
-  <si>
     <t>MLK day - Campus closed</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
   </si>
   <si>
     <t>Proposal due for approval</t>
-  </si>
-  <si>
-    <t>Dead week</t>
   </si>
   <si>
     <t>Dimension Reduction - PCA</t>
@@ -163,16 +154,7 @@
 Use latent factors as a predictor in another model</t>
   </si>
   <si>
-    <t>PCA/FA Assignment</t>
-  </si>
-  <si>
-    <t>PR Correlated Data</t>
-  </si>
-  <si>
     <t>PR Missing Data</t>
-  </si>
-  <si>
-    <t>Final Exam Review</t>
   </si>
   <si>
     <t>Project Timeline</t>
@@ -286,17 +268,7 @@
     <t>LJ Check in</t>
   </si>
   <si>
-    <t>Final exam Part take home, Part in class
-Final LJ submission</t>
-  </si>
-  <si>
     <t>4 LJ check ins</t>
-  </si>
-  <si>
-    <t>Project 1 pg &amp; presentations</t>
-  </si>
-  <si>
-    <t>Project reports</t>
   </si>
   <si>
     <t>Correlated Outcomes</t>
@@ -340,12 +312,6 @@
     <t>PR GLM Assignmnt</t>
   </si>
   <si>
-    <t>PR Survival Analysis</t>
-  </si>
-  <si>
-    <t>Midterm Review</t>
-  </si>
-  <si>
     <t>Classification and Prediction</t>
   </si>
   <si>
@@ -373,46 +339,22 @@
     <t>Missing Data Quiz</t>
   </si>
   <si>
-    <t>Correlated Data Assignment</t>
-  </si>
-  <si>
-    <t>Correlated Outcomes Quiz</t>
-  </si>
-  <si>
     <t>HW 05: PCA /FA</t>
   </si>
   <si>
     <t>Quiz 06</t>
   </si>
   <si>
-    <t>HW 06: Survival Analysis</t>
-  </si>
-  <si>
     <t>HW PCA &amp; FA</t>
   </si>
   <si>
-    <t>Model formulation wksheet</t>
-  </si>
-  <si>
-    <t>PR  PCA/FA Assignment</t>
-  </si>
-  <si>
     <t>External Talk</t>
   </si>
   <si>
-    <t>PR Project Presentations</t>
-  </si>
-  <si>
     <t>Data Preparation ref sheet</t>
   </si>
   <si>
     <t>Fix my notes</t>
-  </si>
-  <si>
-    <t>PCA &amp; FA Quiz</t>
-  </si>
-  <si>
-    <t>Survival Analysis Quiz</t>
   </si>
   <si>
     <t>PMA6 Ch 3</t>
@@ -659,14 +601,76 @@
     <t>[[Quiz 03]](https://forms.gle/iAHo9yiLrjp8v5266)  (Due 3/5)</t>
   </si>
   <si>
-    <t>[[Project update]](project.html#project_update_(wk_8)) (Due  03/13 )</t>
+    <t xml:space="preserve">Practice social distancing, get outdoors, get some exercise, and just hang in there. </t>
+  </si>
+  <si>
+    <t>HW 06: Cluster Analysis</t>
+  </si>
+  <si>
+    <t>PMA6 CH 14
+ASCN Ch 13</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 15
+ASCN Ch 14</t>
+  </si>
+  <si>
+    <t>[[Project update]](project.html#project_update_I) (Due  03/27 )</t>
+  </si>
+  <si>
+    <t>PR Draft report</t>
+  </si>
+  <si>
+    <t>Final report</t>
+  </si>
+  <si>
+    <t>Cluster Analysis</t>
+  </si>
+  <si>
+    <t>Pre-topic QFT</t>
+  </si>
+  <si>
+    <t>PCA / FA</t>
+  </si>
+  <si>
+    <t>PR Assignment</t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t>Pre-topic QFT (LJ + group)</t>
+  </si>
+  <si>
+    <t>Discussion - Question + Answers</t>
+  </si>
+  <si>
+    <t>Correlated Data</t>
+  </si>
+  <si>
+    <t>Project check in: Report &amp; Presentation</t>
+  </si>
+  <si>
+    <t>Project check in: Team Eval</t>
+  </si>
+  <si>
+    <t>Project check in: Questions/Discussion</t>
+  </si>
+  <si>
+    <t>Final presentation</t>
+  </si>
+  <si>
+    <t>Draft report: Team Eval</t>
+  </si>
+  <si>
+    <t>Final report: Individual member eval</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -791,6 +795,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="16">
@@ -1038,7 +1050,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1235,6 +1247,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -1657,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1676,22 +1694,22 @@
   <sheetData>
     <row r="1" spans="1:8" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>26</v>
-      </c>
       <c r="C1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>20</v>
-      </c>
       <c r="F1" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>6</v>
@@ -1708,19 +1726,19 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="67" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="G2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="H2" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1728,10 +1746,10 @@
         <v>1.2</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -1742,19 +1760,19 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1766,14 +1784,14 @@
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
@@ -1784,19 +1802,19 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="H6" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
@@ -1807,15 +1825,15 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="F7" s="36"/>
       <c r="G7" s="26"/>
       <c r="H7" s="38" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
@@ -1826,16 +1844,16 @@
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E8" s="72" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1846,10 +1864,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="F9" s="36"/>
       <c r="G9" s="26"/>
@@ -1862,15 +1880,12 @@
         <v>8</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="36"/>
       <c r="G10" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="H10" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1878,63 +1893,61 @@
         <v>8</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
       <c r="E11" s="32"/>
       <c r="F11" s="33"/>
       <c r="G11" s="31"/>
     </row>
-    <row r="12" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>10.1</v>
       </c>
       <c r="B12" s="15">
         <v>9</v>
       </c>
-      <c r="D12" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>74</v>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="73" t="s">
+        <v>159</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="66" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>11.1</v>
       </c>
       <c r="B13" s="15">
         <v>10</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="26"/>
-    </row>
-    <row r="14" spans="1:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="73" t="s">
+        <v>160</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>12.1</v>
       </c>
       <c r="B14" s="15">
         <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1944,16 +1957,11 @@
       <c r="B15" s="15">
         <v>12</v>
       </c>
-      <c r="D15" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="30"/>
       <c r="G15" s="26" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H15" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1963,15 +1971,13 @@
       <c r="B16" s="15">
         <v>13</v>
       </c>
-      <c r="D16" s="26" t="s">
-        <v>79</v>
-      </c>
+      <c r="D16" s="26"/>
       <c r="E16" s="18"/>
       <c r="F16" s="30" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>99</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1990,27 +1996,39 @@
       <c r="B18" s="15">
         <v>15</v>
       </c>
-      <c r="D18" t="s">
-        <v>33</v>
-      </c>
       <c r="F18" s="30"/>
       <c r="H18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>18.100000000000001</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="38" t="s">
-        <v>69</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="G19" s="38"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="66" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="26"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="26"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:G24">
@@ -2061,19 +2079,19 @@
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="I1" s="24" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2084,25 +2102,25 @@
         <v>42388</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="J2" s="12"/>
     </row>
@@ -2115,25 +2133,25 @@
         <v>42395</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="J3" s="12"/>
     </row>
@@ -2146,22 +2164,22 @@
         <v>42402</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="G4" s="68" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2173,25 +2191,25 @@
         <v>42409</v>
       </c>
       <c r="C5" s="58" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2203,22 +2221,22 @@
         <v>42416</v>
       </c>
       <c r="C6" s="58" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D6" s="61" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2230,26 +2248,26 @@
         <v>42423</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="E7" s="57"/>
       <c r="F7" s="56" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G7" s="56" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2261,20 +2279,20 @@
         <v>42430</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2286,19 +2304,19 @@
         <v>42437</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2308,22 +2326,22 @@
         <v>42444</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2335,18 +2353,18 @@
         <v>42451</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.25">
@@ -2361,13 +2379,13 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G12" s="59" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H12" s="58" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2379,25 +2397,25 @@
         <v>42465</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E13" s="58" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F13" s="58" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G13" s="58" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2409,13 +2427,13 @@
         <v>42472</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="9"/>
@@ -2430,7 +2448,7 @@
         <v>42479</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2451,7 +2469,7 @@
       <c r="E16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2463,18 +2481,18 @@
         <v>42493</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2517,16 +2535,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0647D9F9-0194-9C4A-8769-507350581DA1}">
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.875" style="37"/>
-    <col min="2" max="2" width="32.125" style="37" customWidth="1"/>
+    <col min="2" max="2" width="35" style="37" customWidth="1"/>
     <col min="3" max="3" width="11.125" style="37" customWidth="1"/>
     <col min="4" max="4" width="6.375" style="37" customWidth="1"/>
     <col min="5" max="5" width="6" style="15" customWidth="1"/>
@@ -2539,7 +2557,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="39" t="s">
         <v>7</v>
@@ -2551,7 +2569,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="39" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
@@ -2586,18 +2604,18 @@
         <v>4</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="42">
-        <f>SUMIF($C$2:$C$89,F2,$D$2:$D$89)</f>
-        <v>130</v>
+        <f>SUMIF($C$2:$C$95,F2,$D$2:$D$95)</f>
+        <v>125</v>
       </c>
       <c r="H2" s="43">
         <f>G2/$G$7</f>
-        <v>0.28260869565217389</v>
+        <v>0.26881720430107525</v>
       </c>
       <c r="K2" t="s">
         <v>7</v>
@@ -2614,7 +2632,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="C3" s="40" t="s">
         <v>12</v>
@@ -2623,18 +2641,18 @@
         <v>6</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="F3" s="44" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="40">
-        <f>SUMIF($C$2:$C$89,F3,$D$2:$D$89)</f>
-        <v>110</v>
+        <f>SUMIF($C$2:$C$95,F3,$D$2:$D$95)</f>
+        <v>130</v>
       </c>
       <c r="H3" s="45">
         <f>G3/$G$7</f>
-        <v>0.2391304347826087</v>
+        <v>0.27956989247311825</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
@@ -2651,7 +2669,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>12</v>
@@ -2660,18 +2678,18 @@
         <v>8</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="F4" s="63" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="62">
-        <f>SUMIF($C$2:$C$89,F4,$D$2:$D$89)-10</f>
+        <f>SUMIF($C$2:$C$95,F4,$D$2:$D$95)-10</f>
         <v>60</v>
       </c>
       <c r="H4" s="64">
         <f>G4/$G$7</f>
-        <v>0.13043478260869565</v>
+        <v>0.12903225806451613</v>
       </c>
       <c r="K4" t="s">
         <v>13</v>
@@ -2688,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>12</v>
@@ -2697,18 +2715,18 @@
         <v>20</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="F5" s="47" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="48">
-        <f>SUMIF($C$2:$C$89,F5,$D$2:$D$89)</f>
-        <v>100</v>
+        <f>SUMIF($C$2:$C$95,F5,$D$2:$D$95)</f>
+        <v>50</v>
       </c>
       <c r="H5" s="49">
         <f>G5/$G$7</f>
-        <v>0.21739130434782608</v>
+        <v>0.10752688172043011</v>
       </c>
       <c r="K5" t="s">
         <v>14</v>
@@ -2725,7 +2743,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C6" s="40" t="s">
         <v>12</v>
@@ -2734,18 +2752,18 @@
         <v>5</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="F6" s="50" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="51">
-        <f>SUMIF($C$2:$C$89,F6,$D$2:$D$89)</f>
-        <v>60</v>
+        <f>SUMIF($C$2:$C$95,F6,$D$2:$D$95)</f>
+        <v>100</v>
       </c>
       <c r="H6" s="52">
         <f>G6/$G$7</f>
-        <v>0.13043478260869565</v>
+        <v>0.21505376344086022</v>
       </c>
       <c r="L6">
         <v>500</v>
@@ -2756,7 +2774,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C7" s="40" t="s">
         <v>12</v>
@@ -2765,11 +2783,11 @@
         <v>5</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
-        <v>460</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2777,7 +2795,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="C8" s="46" t="s">
         <v>7</v>
@@ -2786,7 +2804,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -2795,7 +2813,7 @@
         <v>1.2</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>12</v>
@@ -2804,7 +2822,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
@@ -2816,16 +2834,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C10" s="62" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="62">
         <v>10</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="F10"/>
       <c r="J10"/>
@@ -2838,7 +2856,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C11" s="46" t="s">
         <v>7</v>
@@ -2847,7 +2865,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="F11"/>
       <c r="J11"/>
@@ -2856,19 +2874,23 @@
       <c r="M11"/>
     </row>
     <row r="12" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
-        <v>2.1</v>
+      <c r="A12" s="65">
+        <v>2.2000000000000002</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="46">
-        <v>5</v>
+        <v>73</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="40">
+        <v>8</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>126</v>
       </c>
       <c r="F12"/>
+      <c r="G12"/>
       <c r="J12"/>
       <c r="K12"/>
       <c r="L12"/>
@@ -2876,19 +2898,19 @@
     </row>
     <row r="13" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="65">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="40">
-        <v>8</v>
+        <v>80</v>
+      </c>
+      <c r="C13" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="62">
+        <v>10</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="F13"/>
       <c r="G13"/>
@@ -2898,20 +2920,20 @@
       <c r="M13"/>
     </row>
     <row r="14" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="65">
-        <v>2.2999999999999998</v>
+      <c r="A14" s="15">
+        <v>3.1</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="62" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="62">
-        <v>10</v>
+        <v>104</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="46">
+        <v>20</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -2922,19 +2944,16 @@
     </row>
     <row r="15" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="46">
-        <v>20</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>145</v>
+        <v>74</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="40">
+        <v>8</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
@@ -2945,16 +2964,16 @@
     </row>
     <row r="16" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="40">
-        <v>8</v>
+        <v>79</v>
+      </c>
+      <c r="C16" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="62">
+        <v>10</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -2965,16 +2984,16 @@
     </row>
     <row r="17" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
-        <v>3.3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="62" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="62">
-        <v>10</v>
+        <v>82</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="46">
+        <v>20</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -2985,16 +3004,16 @@
     </row>
     <row r="18" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="C18" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="46">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="40">
+        <v>8</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
@@ -3005,16 +3024,16 @@
     </row>
     <row r="19" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="40">
-        <v>8</v>
+        <v>83</v>
+      </c>
+      <c r="C19" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="62">
+        <v>10</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -3025,19 +3044,18 @@
     </row>
     <row r="20" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="62" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="62">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="48">
+        <v>50</v>
       </c>
       <c r="F20"/>
-      <c r="G20"/>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
@@ -3045,19 +3063,12 @@
     </row>
     <row r="21" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
-        <v>5</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="40">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B21" s="74" t="s">
+        <v>166</v>
       </c>
       <c r="F21"/>
-      <c r="G21"/>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
@@ -3065,16 +3076,16 @@
     </row>
     <row r="22" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
-        <v>5.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="48">
-        <v>50</v>
+        <v>169</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="40">
+        <v>4</v>
       </c>
       <c r="F22"/>
       <c r="J22"/>
@@ -3084,10 +3095,10 @@
     </row>
     <row r="23" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="C23" s="46" t="s">
         <v>7</v>
@@ -3101,56 +3112,46 @@
       <c r="L23"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>40</v>
+        <v>167</v>
       </c>
       <c r="C24" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="40">
-        <v>8</v>
-      </c>
-      <c r="F24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-    </row>
-    <row r="25" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
-        <v>6.3</v>
+        <v>6.4</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="C25" s="62" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" s="62">
         <v>10</v>
       </c>
-      <c r="F25"/>
-      <c r="J25"/>
-      <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25"/>
     </row>
     <row r="26" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
-        <v>7.1</v>
+        <v>6.5</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="46">
-        <v>20</v>
+        <v>170</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="40">
+        <v>10</v>
       </c>
       <c r="F26"/>
       <c r="J26"/>
@@ -3158,40 +3159,44 @@
       <c r="L26"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
-        <v>7.2</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="74" t="s">
+        <v>164</v>
+      </c>
+      <c r="F27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+    </row>
+    <row r="28" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>7.1</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="40">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
-        <v>7.3</v>
-      </c>
-      <c r="B28" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="62" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="62">
-        <v>10</v>
-      </c>
+      <c r="D28" s="40">
+        <v>4</v>
+      </c>
+      <c r="F28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
-        <v>8.1</v>
+        <v>7.2</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="C29" s="46" t="s">
         <v>7</v>
@@ -3202,27 +3207,27 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
-        <v>8.1999999999999993</v>
+        <v>7.3</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
       <c r="C30" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="40">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
-        <v>8.3000000000000007</v>
+        <v>7.4</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>108</v>
+        <v>21</v>
       </c>
       <c r="C31" s="62" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D31" s="62">
         <v>10</v>
@@ -3230,433 +3235,501 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="40">
         <v>10</v>
       </c>
-      <c r="B32" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="51" t="s">
+    </row>
+    <row r="33" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>8</v>
+      </c>
+      <c r="B33" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="F33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+    </row>
+    <row r="34" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <v>8.1</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="40">
+        <v>4</v>
+      </c>
+      <c r="F34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+    </row>
+    <row r="35" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="46">
+        <v>20</v>
+      </c>
+      <c r="F35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+    </row>
+    <row r="36" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="40">
+        <v>4</v>
+      </c>
+      <c r="F36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+    </row>
+    <row r="37" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>8.4</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="62">
+        <v>10</v>
+      </c>
+      <c r="F37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+    </row>
+    <row r="38" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <v>8.5</v>
+      </c>
+      <c r="B38" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="40">
+        <v>10</v>
+      </c>
+      <c r="F38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>10</v>
+      </c>
+      <c r="B39" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="51">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
-        <v>10.1</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="51">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="B34" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="51">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
-        <v>10.3</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="51">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
-        <v>10.4</v>
-      </c>
-      <c r="B36" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="51">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
-        <v>11</v>
-      </c>
-      <c r="B37" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="40">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
-        <v>11.1</v>
-      </c>
-      <c r="B38" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="48">
-        <v>50</v>
-      </c>
-      <c r="E38" s="69"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="69"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="69"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="69"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>10.1</v>
+      </c>
+      <c r="B40" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B41" s="72" t="s">
+        <v>172</v>
+      </c>
+      <c r="C41" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="15">
+        <v>10.3</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
+        <v>10.4</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
+        <v>10.5</v>
+      </c>
+      <c r="B44" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="51">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="15">
+        <v>10.6</v>
+      </c>
+      <c r="B45" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="C45" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
+        <v>10.7</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
+        <v>10.4</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="69"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="C48" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="69"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C49" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
-      <c r="E50" s="69"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
       <c r="E51" s="69"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
       <c r="E52" s="69"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
       <c r="E53" s="69"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
       <c r="E54" s="69"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
       <c r="D55" s="15"/>
       <c r="E55" s="69"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
       <c r="D56" s="15"/>
       <c r="E56" s="69"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
       <c r="D57" s="15"/>
       <c r="E57" s="69"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
       <c r="D58" s="15"/>
       <c r="E58" s="69"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
       <c r="D59" s="15"/>
       <c r="E59" s="69"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
       <c r="E60" s="69"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
       <c r="E61" s="69"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15"/>
       <c r="B62" s="15"/>
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
       <c r="E62" s="69"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
       <c r="E63" s="69"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
-      <c r="E64" s="53"/>
-      <c r="F64" s="26"/>
-      <c r="G64" s="37"/>
-      <c r="H64" s="37"/>
-      <c r="I64" s="37"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E64" s="69"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="15"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
-      <c r="E65" s="53"/>
-      <c r="F65" s="26"/>
-      <c r="G65" s="37"/>
-      <c r="H65" s="37"/>
-      <c r="I65" s="37"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E65" s="69"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="15"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
       <c r="E66" s="69"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="15"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
       <c r="D67" s="15"/>
       <c r="E67" s="69"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="15"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
       <c r="E68" s="69"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="15"/>
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
       <c r="D69" s="15"/>
       <c r="E69" s="69"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="15"/>
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
       <c r="D70" s="15"/>
-      <c r="E70" s="69"/>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E70" s="53"/>
+      <c r="F70" s="26"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="37"/>
+      <c r="I70" s="37"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="15"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
       <c r="D71" s="15"/>
-      <c r="E71" s="69"/>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E71" s="53"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="37"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="37"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="15"/>
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
       <c r="D72" s="15"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E72" s="69"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="15"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15"/>
       <c r="D73" s="15"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E73" s="69"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="15"/>
       <c r="B74" s="15"/>
       <c r="C74" s="15"/>
       <c r="D74" s="15"/>
-    </row>
-    <row r="75" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F75"/>
-      <c r="J75"/>
-      <c r="K75"/>
-      <c r="L75"/>
-      <c r="M75"/>
-    </row>
-    <row r="76" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F76"/>
-      <c r="J76"/>
-      <c r="K76"/>
-      <c r="L76"/>
-      <c r="M76"/>
-    </row>
-    <row r="77" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="53"/>
-      <c r="B77" s="53"/>
-      <c r="C77" s="53"/>
-      <c r="D77" s="53"/>
-      <c r="F77"/>
-      <c r="J77"/>
-      <c r="K77"/>
-      <c r="L77"/>
-      <c r="M77"/>
-    </row>
-    <row r="78" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="53"/>
-      <c r="B78" s="53"/>
-      <c r="C78" s="53"/>
-      <c r="D78" s="53"/>
-      <c r="E78" s="37"/>
-      <c r="F78"/>
-      <c r="J78"/>
-      <c r="K78"/>
-      <c r="L78"/>
-      <c r="M78"/>
-    </row>
-    <row r="79" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="53"/>
-      <c r="B79" s="53"/>
-      <c r="C79" s="53"/>
-      <c r="D79" s="53"/>
-      <c r="E79" s="37"/>
-      <c r="F79"/>
-      <c r="J79"/>
-      <c r="K79"/>
-      <c r="L79"/>
-      <c r="M79"/>
-    </row>
-    <row r="80" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="53"/>
-      <c r="B80" s="53"/>
-      <c r="C80" s="53"/>
-      <c r="D80" s="53"/>
-      <c r="E80" s="37"/>
-      <c r="F80"/>
-      <c r="J80"/>
-      <c r="K80"/>
-      <c r="L80"/>
-      <c r="M80"/>
+      <c r="E74" s="69"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="15"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="69"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="15"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="69"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="15"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="69"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="15"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="15"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="15"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
     </row>
     <row r="81" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="53"/>
-      <c r="B81" s="53"/>
-      <c r="C81" s="53"/>
-      <c r="D81" s="53"/>
       <c r="F81"/>
-      <c r="G81"/>
-      <c r="H81"/>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81"/>
       <c r="M81"/>
     </row>
     <row r="82" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="53"/>
-      <c r="B82" s="53"/>
-      <c r="C82" s="53"/>
-      <c r="D82" s="53"/>
       <c r="F82"/>
       <c r="J82"/>
       <c r="K82"/>
@@ -3669,8 +3742,6 @@
       <c r="C83" s="53"/>
       <c r="D83" s="53"/>
       <c r="F83"/>
-      <c r="G83"/>
-      <c r="H83"/>
       <c r="J83"/>
       <c r="K83"/>
       <c r="L83"/>
@@ -3681,9 +3752,8 @@
       <c r="B84" s="53"/>
       <c r="C84" s="53"/>
       <c r="D84" s="53"/>
+      <c r="E84" s="37"/>
       <c r="F84"/>
-      <c r="G84"/>
-      <c r="H84"/>
       <c r="J84"/>
       <c r="K84"/>
       <c r="L84"/>
@@ -3694,9 +3764,8 @@
       <c r="B85" s="53"/>
       <c r="C85" s="53"/>
       <c r="D85" s="53"/>
+      <c r="E85" s="37"/>
       <c r="F85"/>
-      <c r="G85"/>
-      <c r="H85"/>
       <c r="J85"/>
       <c r="K85"/>
       <c r="L85"/>
@@ -3707,9 +3776,8 @@
       <c r="B86" s="53"/>
       <c r="C86" s="53"/>
       <c r="D86" s="53"/>
+      <c r="E86" s="37"/>
       <c r="F86"/>
-      <c r="G86"/>
-      <c r="H86"/>
       <c r="J86"/>
       <c r="K86"/>
       <c r="L86"/>
@@ -3734,8 +3802,6 @@
       <c r="C88" s="53"/>
       <c r="D88" s="53"/>
       <c r="F88"/>
-      <c r="G88"/>
-      <c r="H88"/>
       <c r="J88"/>
       <c r="K88"/>
       <c r="L88"/>
@@ -3767,41 +3833,83 @@
       <c r="L90"/>
       <c r="M90"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="53"/>
       <c r="B91" s="53"/>
       <c r="C91" s="53"/>
       <c r="D91" s="53"/>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F91"/>
+      <c r="G91"/>
+      <c r="H91"/>
+      <c r="J91"/>
+      <c r="K91"/>
+      <c r="L91"/>
+      <c r="M91"/>
+    </row>
+    <row r="92" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="53"/>
       <c r="B92" s="53"/>
       <c r="C92" s="53"/>
       <c r="D92" s="53"/>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F92"/>
+      <c r="G92"/>
+      <c r="H92"/>
+      <c r="J92"/>
+      <c r="K92"/>
+      <c r="L92"/>
+      <c r="M92"/>
+    </row>
+    <row r="93" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="53"/>
       <c r="B93" s="53"/>
       <c r="C93" s="53"/>
       <c r="D93" s="53"/>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F93"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="J93"/>
+      <c r="K93"/>
+      <c r="L93"/>
+      <c r="M93"/>
+    </row>
+    <row r="94" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="53"/>
       <c r="B94" s="53"/>
       <c r="C94" s="53"/>
       <c r="D94" s="53"/>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="L94"/>
+      <c r="M94"/>
+    </row>
+    <row r="95" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="53"/>
       <c r="B95" s="53"/>
       <c r="C95" s="53"/>
       <c r="D95" s="53"/>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="J95"/>
+      <c r="K95"/>
+      <c r="L95"/>
+      <c r="M95"/>
+    </row>
+    <row r="96" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="53"/>
       <c r="B96" s="53"/>
       <c r="C96" s="53"/>
       <c r="D96" s="53"/>
+      <c r="F96"/>
+      <c r="G96"/>
+      <c r="H96"/>
+      <c r="J96"/>
+      <c r="K96"/>
+      <c r="L96"/>
+      <c r="M96"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="53"/>
@@ -3810,14 +3918,51 @@
       <c r="D97" s="53"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="54"/>
-      <c r="B98" s="54"/>
-      <c r="D98" s="54"/>
+      <c r="A98" s="53"/>
+      <c r="B98" s="53"/>
+      <c r="C98" s="53"/>
+      <c r="D98" s="53"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="53"/>
+      <c r="B99" s="53"/>
+      <c r="C99" s="53"/>
+      <c r="D99" s="53"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="53"/>
+      <c r="B100" s="53"/>
+      <c r="C100" s="53"/>
+      <c r="D100" s="53"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="53"/>
+      <c r="B101" s="53"/>
+      <c r="C101" s="53"/>
+      <c r="D101" s="53"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="53"/>
+      <c r="B102" s="53"/>
+      <c r="C102" s="53"/>
+      <c r="D102" s="53"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="53"/>
+      <c r="B103" s="53"/>
+      <c r="C103" s="53"/>
+      <c r="D103" s="53"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="54"/>
+      <c r="B104" s="54"/>
+      <c r="D104" s="54"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D105">
-    <sortCondition ref="A2:A105"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D111">
+    <sortCondition ref="A2:A111"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update for covid changes
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9664DD-DB56-4589-B6FF-78E9B94A12BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5D5DE8-56C5-4C5D-8FEC-013881E0EF31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="174">
   <si>
     <t>Finals Week</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>MLK day - Campus closed</t>
-  </si>
-  <si>
-    <t>Cesar Chavez day - Campus closed</t>
   </si>
   <si>
     <t>Variable Selection</t>
@@ -196,9 +193,6 @@
 Conduct multiple imputation on a data set and analyze the results.</t>
   </si>
   <si>
-    <t>Project Updates (1pager)</t>
-  </si>
-  <si>
     <t>In class simulation project - using Jerry's package? 
 QFT: Strategies for handling missing data</t>
   </si>
@@ -232,12 +226,6 @@
 Using FA as a modeling tool by creating factor scores and using the scores in a subsequent regression model. </t>
   </si>
   <si>
-    <t xml:space="preserve">Dead Week </t>
-  </si>
-  <si>
-    <t>Final Exam Review Session</t>
-  </si>
-  <si>
     <t>Factor Analysis</t>
   </si>
   <si>
@@ -250,12 +238,6 @@
     <t>Project Presentations</t>
   </si>
   <si>
-    <t>Project Report</t>
-  </si>
-  <si>
-    <t>Project Presentations, Project report due</t>
-  </si>
-  <si>
     <t>Quiz 04</t>
   </si>
   <si>
@@ -263,12 +245,6 @@
   </si>
   <si>
     <t>Statistical Modeling</t>
-  </si>
-  <si>
-    <t>LJ Check in</t>
-  </si>
-  <si>
-    <t>4 LJ check ins</t>
   </si>
   <si>
     <t>Correlated Outcomes</t>
@@ -279,9 +255,6 @@
   <si>
     <t xml:space="preserve">Correlated Outcomes
 </t>
-  </si>
-  <si>
-    <t>QFT/LJ Correlated Data</t>
   </si>
   <si>
     <t xml:space="preserve">Sometimes we may have an idea of how the clusters should be correlated. 
@@ -296,9 +269,6 @@
  Explain the impact model-misspecification can have on the results. </t>
   </si>
   <si>
-    <t>Survival Analysis</t>
-  </si>
-  <si>
     <t xml:space="preserve">Classification and predictions
 </t>
   </si>
@@ -321,9 +291,6 @@
     <t>Preparing Data for Analysis</t>
   </si>
   <si>
-    <t>HW 04: Correlated Outcomes</t>
-  </si>
-  <si>
     <t>GLM and Classification Quiz</t>
   </si>
   <si>
@@ -337,9 +304,6 @@
   </si>
   <si>
     <t>Missing Data Quiz</t>
-  </si>
-  <si>
-    <t>HW 05: PCA /FA</t>
   </si>
   <si>
     <t>Quiz 06</t>
@@ -441,9 +405,6 @@
     <t>[[Quiz 00]](https://forms.gle/fea9qCkhNZrvrdy27)(Due 1/23)</t>
   </si>
   <si>
-    <t>CC / OH (4x)</t>
-  </si>
-  <si>
     <t>Quiz on Data preparation &amp; class logistics
 Create a Data preparation reference flowchart</t>
   </si>
@@ -590,9 +551,6 @@
 Seminar on Missing Data: https://media.csuchico.edu/media/0_tgnydpgf </t>
   </si>
   <si>
-    <t>Project Update Presentations &amp; 1 pager</t>
-  </si>
-  <si>
     <t>PMA6 3.4, 10.2  
 ASCN CH 15
 [FIMD](https://stefvanbuuren.name/fimd/)</t>
@@ -604,9 +562,6 @@
     <t xml:space="preserve">Practice social distancing, get outdoors, get some exercise, and just hang in there. </t>
   </si>
   <si>
-    <t>HW 06: Cluster Analysis</t>
-  </si>
-  <si>
     <t>PMA6 CH 14
 ASCN Ch 13</t>
   </si>
@@ -615,12 +570,6 @@
 ASCN Ch 14</t>
   </si>
   <si>
-    <t>[[Project update]](project.html#project_update_I) (Due  03/27 )</t>
-  </si>
-  <si>
-    <t>PR Draft report</t>
-  </si>
-  <si>
     <t>Final report</t>
   </si>
   <si>
@@ -636,12 +585,6 @@
     <t>PR Assignment</t>
   </si>
   <si>
-    <t>Discussion</t>
-  </si>
-  <si>
-    <t>Pre-topic QFT (LJ + group)</t>
-  </si>
-  <si>
     <t>Discussion - Question + Answers</t>
   </si>
   <si>
@@ -664,6 +607,51 @@
   </si>
   <si>
     <t>Final report: Individual member eval</t>
+  </si>
+  <si>
+    <t>2 LJ check ins</t>
+  </si>
+  <si>
+    <t>CC / OH (1 per topic)</t>
+  </si>
+  <si>
+    <t>Project update presentations</t>
+  </si>
+  <si>
+    <t>[[Project update]](project.html#project_update) (Due  03/27 )</t>
+  </si>
+  <si>
+    <t>HW 04: PCA /FA</t>
+  </si>
+  <si>
+    <t>Cluster analysis</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 16</t>
+  </si>
+  <si>
+    <t>HW 06: Correlated Outcomes</t>
+  </si>
+  <si>
+    <t>HW 05: Cluster Analysis</t>
+  </si>
+  <si>
+    <t>Draft Report (Due 04/18 )</t>
+  </si>
+  <si>
+    <t>Project report &amp; presentations</t>
+  </si>
+  <si>
+    <t>Covid19 Campus Closed</t>
+  </si>
+  <si>
+    <t>Catch up</t>
+  </si>
+  <si>
+    <t>Read PMA6 Chapter 18</t>
+  </si>
+  <si>
+    <t>Read PMA6 Chapter 16</t>
   </si>
 </sst>
 </file>
@@ -1677,8 +1665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1729,16 +1717,16 @@
         <v>26</v>
       </c>
       <c r="E2" s="67" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1746,10 +1734,10 @@
         <v>1.2</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -1760,19 +1748,19 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1784,14 +1772,14 @@
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
@@ -1802,19 +1790,19 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="H6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
@@ -1825,15 +1813,15 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="F7" s="36"/>
       <c r="G7" s="26"/>
       <c r="H7" s="38" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
@@ -1844,16 +1832,16 @@
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="72" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1864,10 +1852,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="F9" s="36"/>
       <c r="G9" s="26"/>
@@ -1880,12 +1868,12 @@
         <v>8</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="36"/>
       <c r="G10" s="27" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1893,10 +1881,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="E11" s="32"/>
       <c r="F11" s="33"/>
@@ -1910,19 +1898,10 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="73" t="s">
-        <v>159</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="26" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="H12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1932,22 +1911,31 @@
       <c r="B13" s="15">
         <v>10</v>
       </c>
-      <c r="D13" s="26" t="s">
-        <v>53</v>
+      <c r="D13" t="s">
+        <v>50</v>
       </c>
       <c r="E13" s="73" t="s">
-        <v>160</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>12.1</v>
       </c>
       <c r="B14" s="15">
         <v>11</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1957,11 +1945,20 @@
       <c r="B15" s="15">
         <v>12</v>
       </c>
-      <c r="G15" s="26" t="s">
-        <v>62</v>
+      <c r="D15" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="66" t="s">
+        <v>167</v>
       </c>
       <c r="H15" t="s">
-        <v>92</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1973,12 +1970,8 @@
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>158</v>
-      </c>
+      <c r="F16" s="30"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
@@ -1987,7 +1980,18 @@
       <c r="B17" s="15">
         <v>14</v>
       </c>
-      <c r="F17" s="30"/>
+      <c r="D17" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
@@ -1997,31 +2001,17 @@
         <v>15</v>
       </c>
       <c r="F18" s="30"/>
-      <c r="H18" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>18.100000000000001</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="G19" s="38"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D23" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="G23" s="66" t="s">
-        <v>78</v>
+      <c r="H19" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2043,9 +2033,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,10 +2078,10 @@
         <v>17</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2102,25 +2092,25 @@
         <v>42388</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="J2" s="12"/>
     </row>
@@ -2133,25 +2123,25 @@
         <v>42395</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="J3" s="12"/>
     </row>
@@ -2164,22 +2154,22 @@
         <v>42402</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="G4" s="68" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2191,25 +2181,25 @@
         <v>42409</v>
       </c>
       <c r="C5" s="58" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2221,22 +2211,22 @@
         <v>42416</v>
       </c>
       <c r="C6" s="58" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D6" s="61" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2248,26 +2238,26 @@
         <v>42423</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E7" s="57"/>
       <c r="F7" s="56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2279,20 +2269,20 @@
         <v>42430</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2307,16 +2297,13 @@
         <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>42</v>
+      <c r="H9" s="8" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2344,7 +2331,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -2352,22 +2339,20 @@
         <f t="shared" si="0"/>
         <v>42451</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+      <c r="C11" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -2375,20 +2360,24 @@
         <f t="shared" si="0"/>
         <v>42458</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="59" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H12" s="58" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -2397,28 +2386,26 @@
         <v>42465</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="58" t="s">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="F13" s="58" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G13" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="H13" s="1"/>
       <c r="I13" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -2426,14 +2413,11 @@
         <f t="shared" si="0"/>
         <v>42472</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>35</v>
+      <c r="C14" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>47</v>
+        <v>173</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="9"/>
@@ -2447,16 +2431,14 @@
         <f t="shared" si="0"/>
         <v>42479</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -2464,13 +2446,19 @@
         <f t="shared" si="0"/>
         <v>42486</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="6" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -2480,20 +2468,12 @@
         <f t="shared" si="0"/>
         <v>42493</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
@@ -2509,6 +2489,9 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
@@ -2535,10 +2518,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0647D9F9-0194-9C4A-8769-507350581DA1}">
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2569,7 +2552,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="39" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
@@ -2604,18 +2587,18 @@
         <v>4</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="42">
-        <f>SUMIF($C$2:$C$95,F2,$D$2:$D$95)</f>
+        <f>SUMIF($C$2:$C$94,F2,$D$2:$D$94)</f>
         <v>125</v>
       </c>
       <c r="H2" s="43">
         <f>G2/$G$7</f>
-        <v>0.26881720430107525</v>
+        <v>0.28409090909090912</v>
       </c>
       <c r="K2" t="s">
         <v>7</v>
@@ -2632,27 +2615,27 @@
         <v>0</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C3" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="40">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F3" s="44" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="40">
-        <f>SUMIF($C$2:$C$95,F3,$D$2:$D$95)</f>
-        <v>130</v>
+        <f>SUMIF($C$2:$C$94,F3,$D$2:$D$94)</f>
+        <v>80</v>
       </c>
       <c r="H3" s="45">
         <f>G3/$G$7</f>
-        <v>0.27956989247311825</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
@@ -2669,7 +2652,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>12</v>
@@ -2678,18 +2661,18 @@
         <v>8</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F4" s="63" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="62">
-        <f>SUMIF($C$2:$C$95,F4,$D$2:$D$95)-10</f>
-        <v>60</v>
+        <f>SUMIF($C$2:$C$94,F4,$D$2:$D$94)-10</f>
+        <v>90</v>
       </c>
       <c r="H4" s="64">
         <f>G4/$G$7</f>
-        <v>0.12903225806451613</v>
+        <v>0.20454545454545456</v>
       </c>
       <c r="K4" t="s">
         <v>13</v>
@@ -2706,27 +2689,27 @@
         <v>0</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="40">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F5" s="47" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="48">
-        <f>SUMIF($C$2:$C$95,F5,$D$2:$D$95)</f>
+        <f>SUMIF($C$2:$C$94,F5,$D$2:$D$94)</f>
         <v>50</v>
       </c>
       <c r="H5" s="49">
         <f>G5/$G$7</f>
-        <v>0.10752688172043011</v>
+        <v>0.11363636363636363</v>
       </c>
       <c r="K5" t="s">
         <v>14</v>
@@ -2743,27 +2726,27 @@
         <v>0</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C6" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F6" s="50" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="51">
-        <f>SUMIF($C$2:$C$95,F6,$D$2:$D$95)</f>
-        <v>100</v>
+        <f>SUMIF($C$2:$C$94,F6,$D$2:$D$94)</f>
+        <v>95</v>
       </c>
       <c r="H6" s="52">
         <f>G6/$G$7</f>
-        <v>0.21505376344086022</v>
+        <v>0.21590909090909091</v>
       </c>
       <c r="L6">
         <v>500</v>
@@ -2774,20 +2757,20 @@
         <v>0</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C7" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
-        <v>465</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2795,7 +2778,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C8" s="46" t="s">
         <v>7</v>
@@ -2804,7 +2787,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -2813,7 +2796,7 @@
         <v>1.2</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>12</v>
@@ -2822,7 +2805,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
@@ -2834,7 +2817,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C10" s="62" t="s">
         <v>21</v>
@@ -2843,7 +2826,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F10"/>
       <c r="J10"/>
@@ -2856,7 +2839,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C11" s="46" t="s">
         <v>7</v>
@@ -2865,7 +2848,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F11"/>
       <c r="J11"/>
@@ -2878,7 +2861,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C12" s="40" t="s">
         <v>12</v>
@@ -2887,7 +2870,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
@@ -2901,7 +2884,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C13" s="62" t="s">
         <v>21</v>
@@ -2910,7 +2893,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F13"/>
       <c r="G13"/>
@@ -2924,7 +2907,7 @@
         <v>3.1</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C14" s="46" t="s">
         <v>7</v>
@@ -2933,7 +2916,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -2947,13 +2930,16 @@
         <v>3.2</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C15" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="40">
         <v>8</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
@@ -2967,13 +2953,16 @@
         <v>3.3</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C16" s="62" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="62">
         <v>10</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -2987,13 +2976,16 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C17" s="46" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="46">
         <v>20</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -3007,13 +2999,16 @@
         <v>4.2</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="40">
         <v>8</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
@@ -3027,13 +3022,16 @@
         <v>4.3</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C19" s="62" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="62">
         <v>10</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -3055,6 +3053,9 @@
       <c r="D20" s="48">
         <v>50</v>
       </c>
+      <c r="E20" s="15" t="s">
+        <v>113</v>
+      </c>
       <c r="F20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -3066,7 +3067,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="F21"/>
       <c r="J21"/>
@@ -3079,13 +3080,16 @@
         <v>6.1</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="C22" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="40">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F22"/>
       <c r="J22"/>
@@ -3098,13 +3102,16 @@
         <v>6.2</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>7</v>
+        <v>151</v>
       </c>
       <c r="C23" s="46" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="46">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F23"/>
       <c r="J23"/>
@@ -3117,13 +3124,16 @@
         <v>6.3</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C24" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="40">
         <v>4</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -3131,13 +3141,16 @@
         <v>6.4</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="62" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="62">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="46">
+        <v>15</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -3145,13 +3158,16 @@
         <v>6.5</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="40">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="C26" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="62">
+        <v>20</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F26"/>
       <c r="J26"/>
@@ -3164,7 +3180,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="74" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="F27"/>
       <c r="J27"/>
@@ -3177,13 +3193,16 @@
         <v>7.1</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C28" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="40">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F28"/>
       <c r="J28"/>
@@ -3196,13 +3215,16 @@
         <v>7.2</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>7</v>
+        <v>151</v>
       </c>
       <c r="C29" s="46" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="46">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -3210,13 +3232,16 @@
         <v>7.3</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C30" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="40">
         <v>4</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -3224,13 +3249,16 @@
         <v>7.4</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="62" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="62">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C31" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="46">
+        <v>15</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -3238,13 +3266,16 @@
         <v>7.5</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="C32" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="40">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="C32" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="62">
+        <v>20</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -3252,7 +3283,7 @@
         <v>8</v>
       </c>
       <c r="B33" s="74" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="F33"/>
       <c r="J33"/>
@@ -3265,13 +3296,16 @@
         <v>8.1</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C34" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D34" s="40">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F34"/>
       <c r="J34"/>
@@ -3284,13 +3318,16 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>7</v>
+        <v>151</v>
       </c>
       <c r="C35" s="46" t="s">
         <v>7</v>
       </c>
       <c r="D35" s="46">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F35"/>
       <c r="J35"/>
@@ -3303,13 +3340,16 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C36" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D36" s="40">
         <v>4</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F36"/>
       <c r="J36"/>
@@ -3322,13 +3362,16 @@
         <v>8.4</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="62" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="62">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="46">
+        <v>15</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F37"/>
       <c r="J37"/>
@@ -3341,13 +3384,16 @@
         <v>8.5</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="C38" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="40">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="C38" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="62">
+        <v>20</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="F38"/>
       <c r="J38"/>
@@ -3370,13 +3416,16 @@
         <v>10.1</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" s="51" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="51">
         <v>10</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -3384,13 +3433,16 @@
         <v>10.199999999999999</v>
       </c>
       <c r="B41" s="72" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="C41" s="51" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="51">
         <v>20</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -3398,13 +3450,16 @@
         <v>10.3</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C42" s="51" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="51">
         <v>5</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -3412,13 +3467,16 @@
         <v>10.4</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="C43" s="51" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="51">
         <v>5</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -3426,7 +3484,7 @@
         <v>10.5</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C44" s="51" t="s">
         <v>14</v>
@@ -3434,13 +3492,16 @@
       <c r="D44" s="51">
         <v>15</v>
       </c>
+      <c r="E44" s="15" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
-        <v>10.6</v>
-      </c>
-      <c r="B45" s="37" t="s">
-        <v>162</v>
+        <v>10.7</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>157</v>
       </c>
       <c r="C45" s="51" t="s">
         <v>14</v>
@@ -3448,13 +3509,16 @@
       <c r="D45" s="51">
         <v>5</v>
       </c>
+      <c r="E45" s="15" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
-        <v>10.7</v>
+        <v>10.4</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="C46" s="51" t="s">
         <v>14</v>
@@ -3462,50 +3526,52 @@
       <c r="D46" s="51">
         <v>5</v>
       </c>
+      <c r="E46" s="15" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="15">
-        <v>10.4</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>177</v>
+      <c r="A47" s="15"/>
+      <c r="B47" s="37" t="s">
+        <v>146</v>
       </c>
       <c r="C47" s="51" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="51">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
-      <c r="B48" s="37" t="s">
-        <v>163</v>
+      <c r="B48" s="15" t="s">
+        <v>156</v>
       </c>
       <c r="C48" s="51" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="51">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
-      <c r="B49" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="C49" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="51">
-        <v>10</v>
-      </c>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
+      <c r="E50" s="69"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
@@ -3605,42 +3671,46 @@
       <c r="D64" s="15"/>
       <c r="E64" s="69"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="15"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
       <c r="E65" s="69"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="15"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
       <c r="E66" s="69"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="15"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
       <c r="D67" s="15"/>
       <c r="E67" s="69"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="15"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
       <c r="E68" s="69"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="15"/>
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
       <c r="D69" s="15"/>
-      <c r="E69" s="69"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E69" s="53"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="37"/>
+      <c r="I69" s="37"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="15"/>
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
@@ -3651,76 +3721,72 @@
       <c r="H70" s="37"/>
       <c r="I70" s="37"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="15"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
       <c r="D71" s="15"/>
-      <c r="E71" s="53"/>
-      <c r="F71" s="26"/>
-      <c r="G71" s="37"/>
-      <c r="H71" s="37"/>
-      <c r="I71" s="37"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E71" s="69"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="15"/>
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
       <c r="D72" s="15"/>
       <c r="E72" s="69"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="15"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15"/>
       <c r="D73" s="15"/>
       <c r="E73" s="69"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="15"/>
       <c r="B74" s="15"/>
       <c r="C74" s="15"/>
       <c r="D74" s="15"/>
       <c r="E74" s="69"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="15"/>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>
       <c r="D75" s="15"/>
       <c r="E75" s="69"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="15"/>
       <c r="B76" s="15"/>
       <c r="C76" s="15"/>
       <c r="D76" s="15"/>
       <c r="E76" s="69"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="15"/>
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
       <c r="D77" s="15"/>
-      <c r="E77" s="69"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="15"/>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
       <c r="D78" s="15"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="15"/>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
       <c r="D79" s="15"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="15"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
+    <row r="80" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F80"/>
+      <c r="J80"/>
+      <c r="K80"/>
+      <c r="L80"/>
+      <c r="M80"/>
     </row>
     <row r="81" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F81"/>
@@ -3730,6 +3796,10 @@
       <c r="M81"/>
     </row>
     <row r="82" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="53"/>
+      <c r="B82" s="53"/>
+      <c r="C82" s="53"/>
+      <c r="D82" s="53"/>
       <c r="F82"/>
       <c r="J82"/>
       <c r="K82"/>
@@ -3741,6 +3811,7 @@
       <c r="B83" s="53"/>
       <c r="C83" s="53"/>
       <c r="D83" s="53"/>
+      <c r="E83" s="37"/>
       <c r="F83"/>
       <c r="J83"/>
       <c r="K83"/>
@@ -3776,8 +3847,9 @@
       <c r="B86" s="53"/>
       <c r="C86" s="53"/>
       <c r="D86" s="53"/>
-      <c r="E86" s="37"/>
       <c r="F86"/>
+      <c r="G86"/>
+      <c r="H86"/>
       <c r="J86"/>
       <c r="K86"/>
       <c r="L86"/>
@@ -3789,8 +3861,6 @@
       <c r="C87" s="53"/>
       <c r="D87" s="53"/>
       <c r="F87"/>
-      <c r="G87"/>
-      <c r="H87"/>
       <c r="J87"/>
       <c r="K87"/>
       <c r="L87"/>
@@ -3802,6 +3872,8 @@
       <c r="C88" s="53"/>
       <c r="D88" s="53"/>
       <c r="F88"/>
+      <c r="G88"/>
+      <c r="H88"/>
       <c r="J88"/>
       <c r="K88"/>
       <c r="L88"/>
@@ -3898,18 +3970,11 @@
       <c r="L95"/>
       <c r="M95"/>
     </row>
-    <row r="96" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="53"/>
       <c r="B96" s="53"/>
       <c r="C96" s="53"/>
       <c r="D96" s="53"/>
-      <c r="F96"/>
-      <c r="G96"/>
-      <c r="H96"/>
-      <c r="J96"/>
-      <c r="K96"/>
-      <c r="L96"/>
-      <c r="M96"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="53"/>
@@ -3948,19 +4013,13 @@
       <c r="D102" s="53"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="53"/>
-      <c r="B103" s="53"/>
-      <c r="C103" s="53"/>
-      <c r="D103" s="53"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="54"/>
-      <c r="B104" s="54"/>
-      <c r="D104" s="54"/>
+      <c r="A103" s="54"/>
+      <c r="B103" s="54"/>
+      <c r="D103" s="54"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D111">
-    <sortCondition ref="A2:A111"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D110">
+    <sortCondition ref="A2:A110"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add quiz and LJ dates to schedule
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D01D1FA-A1F4-4FA4-BDA4-D04517FE16E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6C207E-107D-4866-8471-6DF5E0C2BFDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="178">
   <si>
     <t>Finals Week</t>
   </si>
@@ -205,12 +205,6 @@
     <t>Project Presentations</t>
   </si>
   <si>
-    <t>Quiz 04</t>
-  </si>
-  <si>
-    <t>Quiz 05</t>
-  </si>
-  <si>
     <t>Statistical Modeling</t>
   </si>
   <si>
@@ -273,9 +267,6 @@
     <t>Missing Data Quiz</t>
   </si>
   <si>
-    <t>Quiz 06</t>
-  </si>
-  <si>
     <t>External Talk</t>
   </si>
   <si>
@@ -591,12 +582,6 @@
     <t>PMA6 Ch 16</t>
   </si>
   <si>
-    <t>HW 06: Correlated Outcomes</t>
-  </si>
-  <si>
-    <t>HW 05: Cluster Analysis</t>
-  </si>
-  <si>
     <t>Draft Report (Due 04/18 )</t>
   </si>
   <si>
@@ -649,6 +634,30 @@
     <t xml:space="preserve">Review the QFT prompt and generate questions in your LJ
 Join the #topic-04 Slack channel
 </t>
+  </si>
+  <si>
+    <t>[[Quiz 04]](https://forms.gle/mirjk4xDsFk8HtHQA) (Due 4/9 )</t>
+  </si>
+  <si>
+    <t>Quiz 05 (Due 4/23 )</t>
+  </si>
+  <si>
+    <t>Quiz 06 (Due 5/7 )</t>
+  </si>
+  <si>
+    <t>HW 06: Correlated Outcomes (Draft due 5/5, Final due 5/9 )</t>
+  </si>
+  <si>
+    <t>HW 05: Cluster Analysis (Draft 4/21, Final 4/25 )</t>
+  </si>
+  <si>
+    <t>Pre-topic LJ check in. (Mon 4/27 AM)</t>
+  </si>
+  <si>
+    <t>Pre-topic LJ check in. (Mon 4/13 AM)</t>
+  </si>
+  <si>
+    <t>Friday 12-2pm</t>
   </si>
 </sst>
 </file>
@@ -1653,7 +1662,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1704,16 +1713,16 @@
         <v>26</v>
       </c>
       <c r="E2" s="66" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1721,10 +1730,10 @@
         <v>1.2</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -1735,16 +1744,16 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -1762,11 +1771,11 @@
         <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
@@ -1777,19 +1786,19 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
@@ -1800,15 +1809,15 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F7" s="35"/>
       <c r="G7" s="25"/>
       <c r="H7" s="37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
@@ -1822,13 +1831,13 @@
         <v>38</v>
       </c>
       <c r="E8" s="71" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1839,10 +1848,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F9" s="35"/>
       <c r="G9" s="25"/>
@@ -1860,7 +1869,7 @@
       <c r="E10" s="36"/>
       <c r="F10" s="35"/>
       <c r="G10" s="26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1868,10 +1877,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="32"/>
@@ -1885,10 +1894,10 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1899,16 +1908,14 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>137</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="G13" s="65"/>
+    </row>
+    <row r="14" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>12.1</v>
       </c>
@@ -1919,10 +1926,13 @@
         <v>44</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>47</v>
+        <v>170</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1933,19 +1943,19 @@
         <v>12</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>48</v>
+        <v>171</v>
       </c>
       <c r="G15" s="65" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="H15" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1957,8 +1967,9 @@
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="25"/>
+      <c r="G16" s="65" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
@@ -1968,16 +1979,14 @@
         <v>14</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>67</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F17" s="29"/>
       <c r="G17" s="65" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1987,18 +1996,26 @@
       <c r="B18" s="14">
         <v>15</v>
       </c>
-      <c r="F18" s="29"/>
+      <c r="F18" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="G18" s="65" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>18.100000000000001</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="D19" t="s">
+        <v>177</v>
       </c>
       <c r="G19" s="37"/>
       <c r="H19" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2065,7 +2082,7 @@
         <v>17</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J1" s="28" t="s">
         <v>31</v>
@@ -2079,25 +2096,25 @@
         <v>42388</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J2" s="11"/>
     </row>
@@ -2110,25 +2127,25 @@
         <v>42395</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J3" s="11"/>
     </row>
@@ -2144,19 +2161,19 @@
         <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G4" s="67" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2168,25 +2185,25 @@
         <v>42409</v>
       </c>
       <c r="C5" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="I5" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2198,22 +2215,22 @@
         <v>42416</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2228,7 +2245,7 @@
         <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E7" s="56"/>
       <c r="F7" s="55" t="s">
@@ -2238,10 +2255,10 @@
         <v>39</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>41</v>
@@ -2256,16 +2273,16 @@
         <v>42430</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
@@ -2284,13 +2301,13 @@
         <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2327,13 +2344,13 @@
         <v>42451</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>46</v>
@@ -2354,16 +2371,16 @@
         <v>32</v>
       </c>
       <c r="E12" s="57" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G12" s="58" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H12" s="57" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2384,13 +2401,13 @@
         <v>42</v>
       </c>
       <c r="F13" s="57" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G13" s="57" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -2402,17 +2419,17 @@
         <v>42472</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="58" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H14" s="57" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2439,16 +2456,16 @@
         <v>42486</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -2544,7 +2561,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="38" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
@@ -2579,7 +2596,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F2" s="40" t="s">
         <v>7</v>
@@ -2607,7 +2624,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C3" s="39" t="s">
         <v>12</v>
@@ -2616,7 +2633,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F3" s="43" t="s">
         <v>12</v>
@@ -2644,7 +2661,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C4" s="39" t="s">
         <v>12</v>
@@ -2653,7 +2670,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F4" s="62" t="s">
         <v>21</v>
@@ -2681,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C5" s="39" t="s">
         <v>12</v>
@@ -2690,7 +2707,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F5" s="46" t="s">
         <v>13</v>
@@ -2718,7 +2735,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C6" s="39" t="s">
         <v>12</v>
@@ -2727,7 +2744,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F6" s="49" t="s">
         <v>14</v>
@@ -2749,7 +2766,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C7" s="39" t="s">
         <v>12</v>
@@ -2758,7 +2775,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
@@ -2770,7 +2787,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C8" s="45" t="s">
         <v>7</v>
@@ -2779,7 +2796,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -2788,7 +2805,7 @@
         <v>1.2</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C9" s="39" t="s">
         <v>12</v>
@@ -2797,7 +2814,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
@@ -2809,7 +2826,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="61" t="s">
         <v>21</v>
@@ -2818,7 +2835,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F10"/>
       <c r="J10"/>
@@ -2831,7 +2848,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" s="45" t="s">
         <v>7</v>
@@ -2840,7 +2857,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F11"/>
       <c r="J11"/>
@@ -2853,7 +2870,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" s="39" t="s">
         <v>12</v>
@@ -2862,7 +2879,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
@@ -2876,7 +2893,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C13" s="61" t="s">
         <v>21</v>
@@ -2885,7 +2902,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F13"/>
       <c r="G13"/>
@@ -2899,7 +2916,7 @@
         <v>3.1</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C14" s="45" t="s">
         <v>7</v>
@@ -2908,7 +2925,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -2922,7 +2939,7 @@
         <v>3.2</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" s="39" t="s">
         <v>12</v>
@@ -2931,7 +2948,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
@@ -2945,7 +2962,7 @@
         <v>3.3</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C16" s="61" t="s">
         <v>21</v>
@@ -2954,7 +2971,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -2968,7 +2985,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" s="45" t="s">
         <v>7</v>
@@ -2977,7 +2994,7 @@
         <v>20</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -3000,7 +3017,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
@@ -3014,7 +3031,7 @@
         <v>4.3</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" s="61" t="s">
         <v>21</v>
@@ -3023,7 +3040,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -3046,7 +3063,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F20"/>
       <c r="J20"/>
@@ -3059,7 +3076,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="73" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F21"/>
       <c r="J21"/>
@@ -3072,7 +3089,7 @@
         <v>6.1</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C22" s="39" t="s">
         <v>12</v>
@@ -3081,7 +3098,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F22"/>
       <c r="J22"/>
@@ -3094,7 +3111,7 @@
         <v>6.2</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C23" s="45" t="s">
         <v>7</v>
@@ -3103,7 +3120,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F23"/>
       <c r="J23"/>
@@ -3116,7 +3133,7 @@
         <v>6.3</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C24" s="39" t="s">
         <v>12</v>
@@ -3125,7 +3142,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -3142,7 +3159,7 @@
         <v>15</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3159,7 +3176,7 @@
         <v>20</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F26"/>
       <c r="J26"/>
@@ -3172,7 +3189,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F27"/>
       <c r="J27"/>
@@ -3185,7 +3202,7 @@
         <v>7.1</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C28" s="39" t="s">
         <v>12</v>
@@ -3194,7 +3211,7 @@
         <v>6</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F28"/>
       <c r="J28"/>
@@ -3207,7 +3224,7 @@
         <v>7.2</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C29" s="45" t="s">
         <v>7</v>
@@ -3216,7 +3233,7 @@
         <v>5</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -3224,7 +3241,7 @@
         <v>7.3</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C30" s="39" t="s">
         <v>12</v>
@@ -3233,7 +3250,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -3250,7 +3267,7 @@
         <v>15</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -3267,7 +3284,7 @@
         <v>20</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3275,7 +3292,7 @@
         <v>8</v>
       </c>
       <c r="B33" s="73" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F33"/>
       <c r="J33"/>
@@ -3288,7 +3305,7 @@
         <v>8.1</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C34" s="39" t="s">
         <v>12</v>
@@ -3297,7 +3314,7 @@
         <v>6</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F34"/>
       <c r="J34"/>
@@ -3310,7 +3327,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C35" s="45" t="s">
         <v>7</v>
@@ -3319,7 +3336,7 @@
         <v>5</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F35"/>
       <c r="J35"/>
@@ -3332,7 +3349,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C36" s="39" t="s">
         <v>12</v>
@@ -3341,7 +3358,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F36"/>
       <c r="J36"/>
@@ -3363,7 +3380,7 @@
         <v>15</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F37"/>
       <c r="J37"/>
@@ -3385,7 +3402,7 @@
         <v>20</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F38"/>
       <c r="J38"/>
@@ -3417,7 +3434,7 @@
         <v>10</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -3425,7 +3442,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="B41" s="71" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C41" s="50" t="s">
         <v>14</v>
@@ -3434,7 +3451,7 @@
         <v>20</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -3442,7 +3459,7 @@
         <v>10.3</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C42" s="50" t="s">
         <v>14</v>
@@ -3451,7 +3468,7 @@
         <v>5</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -3459,7 +3476,7 @@
         <v>10.4</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C43" s="50" t="s">
         <v>14</v>
@@ -3468,7 +3485,7 @@
         <v>5</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -3476,7 +3493,7 @@
         <v>10.5</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C44" s="50" t="s">
         <v>14</v>
@@ -3485,7 +3502,7 @@
         <v>15</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -3493,7 +3510,7 @@
         <v>10.7</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C45" s="50" t="s">
         <v>14</v>
@@ -3502,7 +3519,7 @@
         <v>5</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -3510,7 +3527,7 @@
         <v>10.4</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C46" s="50" t="s">
         <v>14</v>
@@ -3519,13 +3536,13 @@
         <v>5</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="36" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C47" s="50" t="s">
         <v>14</v>
@@ -3534,13 +3551,13 @@
         <v>20</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="B48" s="14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C48" s="50" t="s">
         <v>14</v>
@@ -3549,7 +3566,7 @@
         <v>10</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add hw5 and wk12
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E364920-5B98-409C-8085-D95A274F6BFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115C662D-0812-4266-BEEC-7DEE51259B4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="420" windowWidth="15270" windowHeight="15030" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -23,6 +23,14 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -31,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="187">
   <si>
     <t>Finals Week</t>
   </si>
@@ -282,9 +290,6 @@
     <t>Syllabus</t>
   </si>
   <si>
-    <t>Draft report</t>
-  </si>
-  <si>
     <t>Familiarize yourself with this website and required course materials. 
 Review the syllabus and first homework assignment. 
 Read PMA6 - Chapter 3 (Before Friday)</t>
@@ -525,9 +530,6 @@
 ASCN Ch 14</t>
   </si>
   <si>
-    <t>Final report</t>
-  </si>
-  <si>
     <t>Cluster Analysis</t>
   </si>
   <si>
@@ -558,9 +560,6 @@
     <t>Final presentation</t>
   </si>
   <si>
-    <t>Draft report: Team Eval</t>
-  </si>
-  <si>
     <t>Final report: Individual member eval</t>
   </si>
   <si>
@@ -580,12 +579,6 @@
   </si>
   <si>
     <t>PMA6 Ch 16</t>
-  </si>
-  <si>
-    <t>Draft Report (Due 04/18 )</t>
-  </si>
-  <si>
-    <t>Project report &amp; presentations</t>
   </si>
   <si>
     <t>Covid19 Campus Closed</t>
@@ -648,9 +641,6 @@
     <t>HW 06: Correlated Outcomes (Draft due 5/5, Final due 5/9 )</t>
   </si>
   <si>
-    <t>HW 05: Cluster Analysis (Draft 4/21, Final 4/25 )</t>
-  </si>
-  <si>
     <t>Pre-topic LJ check in. (Mon 4/27 AM)</t>
   </si>
   <si>
@@ -658,6 +648,51 @@
   </si>
   <si>
     <t>Friday 12-2pm</t>
+  </si>
+  <si>
+    <t>Presentation slides Draft (Due 4/27 PR 4/29)</t>
+  </si>
+  <si>
+    <t>Presentations to be scheduled.</t>
+  </si>
+  <si>
+    <t>10-15 minute final presentations</t>
+  </si>
+  <si>
+    <t>Presentation slides draft</t>
+  </si>
+  <si>
+    <t>PR Presentation slides</t>
+  </si>
+  <si>
+    <t>team effort</t>
+  </si>
+  <si>
+    <t>appropriate method</t>
+  </si>
+  <si>
+    <t>completion status</t>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>Final presentation participation</t>
+  </si>
+  <si>
+    <t>slide quality</t>
+  </si>
+  <si>
+    <t>explanation of methods</t>
+  </si>
+  <si>
+    <t>response to questions</t>
+  </si>
+  <si>
+    <t>smoothness of presentation</t>
+  </si>
+  <si>
+    <t>HW 05: Cluster Analysis [[HTML]](hw/hw05-cluster.html)[[PDF]](hw/hw05-cluster-pdf) (Draft 4/21, Final 4/25 )</t>
   </si>
 </sst>
 </file>
@@ -1661,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1716,13 +1751,13 @@
         <v>69</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1747,13 +1782,13 @@
         <v>47</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -1771,11 +1806,11 @@
         <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
@@ -1789,16 +1824,16 @@
         <v>58</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
@@ -1812,12 +1847,12 @@
         <v>57</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F7" s="35"/>
       <c r="G7" s="25"/>
       <c r="H7" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
@@ -1831,13 +1866,13 @@
         <v>38</v>
       </c>
       <c r="E8" s="71" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="35" t="s">
-        <v>132</v>
-      </c>
       <c r="G8" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1848,10 +1883,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F9" s="35"/>
       <c r="G9" s="25"/>
@@ -1869,7 +1904,7 @@
       <c r="E10" s="36"/>
       <c r="F10" s="35"/>
       <c r="G10" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1877,10 +1912,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="32"/>
@@ -1894,10 +1929,10 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1908,10 +1943,10 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G13" s="65"/>
     </row>
@@ -1926,13 +1961,13 @@
         <v>44</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1943,19 +1978,16 @@
         <v>12</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G15" s="65" t="s">
-        <v>176</v>
-      </c>
-      <c r="H15" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1968,7 +2000,7 @@
       <c r="D16" s="25"/>
       <c r="E16" s="17"/>
       <c r="G16" s="65" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1986,7 +2018,10 @@
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="65" t="s">
-        <v>175</v>
+        <v>169</v>
+      </c>
+      <c r="H17" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1997,10 +2032,10 @@
         <v>15</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G18" s="65" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2008,14 +2043,16 @@
         <v>18.100000000000001</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>177</v>
-      </c>
-      <c r="G19" s="37"/>
+        <v>171</v>
+      </c>
+      <c r="G19" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="H19" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2025,7 +2062,7 @@
       <c r="G24" s="25"/>
     </row>
   </sheetData>
-  <sortState ref="A21:G24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:G24">
     <sortCondition ref="B21:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2082,7 +2119,7 @@
         <v>17</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J1" s="28" t="s">
         <v>31</v>
@@ -2096,25 +2133,25 @@
         <v>42388</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J2" s="11"/>
     </row>
@@ -2130,22 +2167,22 @@
         <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="I3" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J3" s="11"/>
     </row>
@@ -2161,19 +2198,19 @@
         <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="G4" s="67" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2185,25 +2222,25 @@
         <v>42409</v>
       </c>
       <c r="C5" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="F5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="I5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2218,19 +2255,19 @@
         <v>53</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2245,7 +2282,7 @@
         <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" s="56"/>
       <c r="F7" s="55" t="s">
@@ -2255,10 +2292,10 @@
         <v>39</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>41</v>
@@ -2273,16 +2310,16 @@
         <v>42430</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
@@ -2301,13 +2338,13 @@
         <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2344,13 +2381,13 @@
         <v>42451</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>46</v>
@@ -2371,16 +2408,16 @@
         <v>32</v>
       </c>
       <c r="E12" s="57" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G12" s="58" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H12" s="57" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2401,13 +2438,13 @@
         <v>42</v>
       </c>
       <c r="F13" s="57" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G13" s="57" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -2419,17 +2456,17 @@
         <v>42472</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="58" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H14" s="57" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2462,7 +2499,7 @@
         <v>52</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>51</v>
@@ -2529,8 +2566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0647D9F9-0194-9C4A-8769-507350581DA1}">
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2540,7 +2577,7 @@
     <col min="3" max="3" width="11.125" style="36" customWidth="1"/>
     <col min="4" max="4" width="6.375" style="36" customWidth="1"/>
     <col min="5" max="5" width="6" style="14" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="20.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="14" customWidth="1"/>
     <col min="8" max="8" width="8.875" style="14"/>
     <col min="9" max="9" width="4.625" style="14" customWidth="1"/>
@@ -2561,7 +2598,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
@@ -2596,7 +2633,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F2" s="40" t="s">
         <v>7</v>
@@ -2607,7 +2644,7 @@
       </c>
       <c r="H2" s="42">
         <f>G2/$G$7</f>
-        <v>0.27419354838709675</v>
+        <v>0.268018018018018</v>
       </c>
       <c r="K2" t="s">
         <v>7</v>
@@ -2624,7 +2661,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="39" t="s">
         <v>12</v>
@@ -2633,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F3" s="43" t="s">
         <v>12</v>
@@ -2644,7 +2681,7 @@
       </c>
       <c r="H3" s="44">
         <f>G3/$G$7</f>
-        <v>0.18433179723502305</v>
+        <v>0.18018018018018017</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
@@ -2661,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C4" s="39" t="s">
         <v>12</v>
@@ -2670,7 +2707,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="62" t="s">
         <v>21</v>
@@ -2681,7 +2718,7 @@
       </c>
       <c r="H4" s="63">
         <f>G4/$G$7</f>
-        <v>0.20737327188940091</v>
+        <v>0.20270270270270271</v>
       </c>
       <c r="K4" t="s">
         <v>13</v>
@@ -2698,7 +2735,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C5" s="39" t="s">
         <v>12</v>
@@ -2707,7 +2744,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" s="46" t="s">
         <v>13</v>
@@ -2718,7 +2755,7 @@
       </c>
       <c r="H5" s="48">
         <f>G5/$G$7</f>
-        <v>0.1152073732718894</v>
+        <v>0.11261261261261261</v>
       </c>
       <c r="K5" t="s">
         <v>14</v>
@@ -2744,18 +2781,18 @@
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F6" s="49" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="50">
         <f>SUMIF($C$2:$C$94,F6,$D$2:$D$94)</f>
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="H6" s="51">
         <f>G6/$G$7</f>
-        <v>0.21889400921658986</v>
+        <v>0.23648648648648649</v>
       </c>
       <c r="L6">
         <v>500</v>
@@ -2775,11 +2812,11 @@
         <v>0</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
-        <v>434</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2796,7 +2833,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -2805,7 +2842,7 @@
         <v>1.2</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="39" t="s">
         <v>12</v>
@@ -2814,7 +2851,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
@@ -2835,7 +2872,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F10"/>
       <c r="J10"/>
@@ -2857,7 +2894,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F11"/>
       <c r="J11"/>
@@ -2879,7 +2916,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
@@ -2902,7 +2939,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F13"/>
       <c r="G13"/>
@@ -2916,7 +2953,7 @@
         <v>3.1</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" s="45" t="s">
         <v>7</v>
@@ -2925,7 +2962,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -2948,7 +2985,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
@@ -2971,7 +3008,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -2994,7 +3031,7 @@
         <v>20</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -3017,7 +3054,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
@@ -3040,7 +3077,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -3063,7 +3100,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F20"/>
       <c r="J20"/>
@@ -3076,7 +3113,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="73" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F21"/>
       <c r="J21"/>
@@ -3089,7 +3126,7 @@
         <v>6.1</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C22" s="39" t="s">
         <v>12</v>
@@ -3098,7 +3135,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F22"/>
       <c r="J22"/>
@@ -3111,7 +3148,7 @@
         <v>6.2</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C23" s="45" t="s">
         <v>7</v>
@@ -3120,7 +3157,7 @@
         <v>3</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F23"/>
       <c r="J23"/>
@@ -3133,7 +3170,7 @@
         <v>6.3</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C24" s="39" t="s">
         <v>12</v>
@@ -3142,7 +3179,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -3159,7 +3196,7 @@
         <v>15</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3176,7 +3213,7 @@
         <v>20</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F26"/>
       <c r="J26"/>
@@ -3189,7 +3226,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F27"/>
       <c r="J27"/>
@@ -3202,7 +3239,7 @@
         <v>7.1</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C28" s="39" t="s">
         <v>12</v>
@@ -3211,7 +3248,7 @@
         <v>6</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F28"/>
       <c r="J28"/>
@@ -3224,7 +3261,7 @@
         <v>7.2</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C29" s="45" t="s">
         <v>7</v>
@@ -3233,7 +3270,7 @@
         <v>3</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -3241,7 +3278,7 @@
         <v>7.3</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C30" s="39" t="s">
         <v>12</v>
@@ -3250,7 +3287,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -3267,7 +3304,7 @@
         <v>15</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -3284,7 +3321,7 @@
         <v>20</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3292,7 +3329,7 @@
         <v>8</v>
       </c>
       <c r="B33" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F33"/>
       <c r="J33"/>
@@ -3305,7 +3342,7 @@
         <v>8.1</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C34" s="39" t="s">
         <v>12</v>
@@ -3314,7 +3351,7 @@
         <v>6</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F34"/>
       <c r="J34"/>
@@ -3327,7 +3364,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C35" s="45" t="s">
         <v>7</v>
@@ -3336,7 +3373,7 @@
         <v>3</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F35"/>
       <c r="J35"/>
@@ -3349,7 +3386,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C36" s="39" t="s">
         <v>12</v>
@@ -3358,7 +3395,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F36"/>
       <c r="J36"/>
@@ -3380,7 +3417,7 @@
         <v>15</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F37"/>
       <c r="J37"/>
@@ -3402,7 +3439,7 @@
         <v>20</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F38"/>
       <c r="J38"/>
@@ -3434,7 +3471,7 @@
         <v>10</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -3442,7 +3479,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="B41" s="71" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C41" s="50" t="s">
         <v>14</v>
@@ -3451,7 +3488,7 @@
         <v>20</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -3459,7 +3496,7 @@
         <v>10.3</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C42" s="50" t="s">
         <v>14</v>
@@ -3468,7 +3505,7 @@
         <v>5</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -3476,7 +3513,7 @@
         <v>10.4</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C43" s="50" t="s">
         <v>14</v>
@@ -3485,7 +3522,13 @@
         <v>5</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="G43" s="14">
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -3493,16 +3536,22 @@
         <v>10.5</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C44" s="50" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="50">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="G44" s="14">
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -3510,7 +3559,7 @@
         <v>10.7</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="C45" s="50" t="s">
         <v>14</v>
@@ -3519,7 +3568,13 @@
         <v>5</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G45" s="14">
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -3527,7 +3582,7 @@
         <v>10.4</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C46" s="50" t="s">
         <v>14</v>
@@ -3536,144 +3591,171 @@
         <v>5</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="G46" s="14">
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
-      <c r="B47" s="36" t="s">
-        <v>136</v>
+      <c r="B47" s="14" t="s">
+        <v>144</v>
       </c>
       <c r="C47" s="50" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="50">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
-      <c r="B48" s="14" t="s">
-        <v>146</v>
+      <c r="B48" s="36" t="s">
+        <v>181</v>
       </c>
       <c r="C48" s="50" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="50">
-        <v>10</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="G48" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>183</v>
+      </c>
+      <c r="G49" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="68"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>184</v>
+      </c>
+      <c r="G50" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
       <c r="E51" s="68"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>185</v>
+      </c>
+      <c r="G51" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
       <c r="E52" s="68"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
       <c r="E53" s="68"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
       <c r="E54" s="68"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
       <c r="E55" s="68"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
       <c r="E56" s="68"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
       <c r="E57" s="68"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="14"/>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
       <c r="E58" s="68"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
       <c r="E59" s="68"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
       <c r="E60" s="68"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
       <c r="E61" s="68"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
       <c r="E62" s="68"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
       <c r="E63" s="68"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
@@ -4027,7 +4109,7 @@
       <c r="D103" s="53"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D110">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D110">
     <sortCondition ref="A2:A110"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add final project and wk15
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20358"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH456/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504DCBC4-10AB-421A-A978-5B598A798F25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2996BCDF-B206-9A4E-B8C4-C710A3961C3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="420" windowWidth="15270" windowHeight="15030" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="15280" windowHeight="14440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
     <sheet name="slo_detail" sheetId="5" r:id="rId2"/>
     <sheet name="points" sheetId="11" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="182">
   <si>
     <t>Finals Week</t>
   </si>
@@ -621,15 +621,6 @@
     <t>Pre-topic LJ check in. (Mon 4/13 AM)</t>
   </si>
   <si>
-    <t>Friday 12-2pm</t>
-  </si>
-  <si>
-    <t>Presentations to be scheduled.</t>
-  </si>
-  <si>
-    <t>10-15 minute final presentations</t>
-  </si>
-  <si>
     <t>Presentation slides draft</t>
   </si>
   <si>
@@ -673,13 +664,19 @@
   </si>
   <si>
     <t xml:space="preserve">Groups check in with Dr. D. </t>
+  </si>
+  <si>
+    <t>See project page</t>
+  </si>
+  <si>
+    <t>Thursday 2-4pm, OR Friday 12-2pm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1677,21 +1674,21 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="8.875" style="14"/>
-    <col min="3" max="3" width="5.625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.875" customWidth="1"/>
-    <col min="5" max="5" width="11.125" style="14" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" style="14"/>
+    <col min="3" max="3" width="5.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="14" customWidth="1"/>
     <col min="6" max="6" width="18" style="24" customWidth="1"/>
     <col min="7" max="7" width="33" customWidth="1"/>
     <col min="8" max="8" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="14" customFormat="1" ht="17" thickBot="1">
       <c r="A1" s="18" t="s">
         <v>24</v>
       </c>
@@ -1717,7 +1714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="17">
       <c r="A2" s="19">
         <v>1.1000000000000001</v>
       </c>
@@ -1740,7 +1737,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="19">
         <v>1.2</v>
       </c>
@@ -1751,7 +1748,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="128">
       <c r="A4" s="19">
         <v>2.1</v>
       </c>
@@ -1774,7 +1771,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="48">
       <c r="A5" s="20">
         <v>3.1</v>
       </c>
@@ -1793,7 +1790,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="102">
       <c r="A6" s="19">
         <v>4.0999999999999996</v>
       </c>
@@ -1816,7 +1813,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="85">
       <c r="A7" s="19">
         <v>5.0999999999999996</v>
       </c>
@@ -1835,7 +1832,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="119">
       <c r="A8" s="19">
         <v>6.1</v>
       </c>
@@ -1855,7 +1852,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="32">
       <c r="A9" s="19">
         <v>7.1</v>
       </c>
@@ -1871,7 +1868,7 @@
       <c r="F9" s="35"/>
       <c r="G9" s="25"/>
     </row>
-    <row r="10" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="34">
       <c r="A10" s="19">
         <v>9.1</v>
       </c>
@@ -1887,7 +1884,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="19">
         <v>8</v>
       </c>
@@ -1901,7 +1898,7 @@
       <c r="F11" s="32"/>
       <c r="G11" s="30"/>
     </row>
-    <row r="12" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="38.25" customHeight="1">
       <c r="A12" s="19">
         <v>10.1</v>
       </c>
@@ -1915,7 +1912,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="39" customHeight="1">
       <c r="A13" s="19">
         <v>11.1</v>
       </c>
@@ -1930,7 +1927,7 @@
       </c>
       <c r="G13" s="65"/>
     </row>
-    <row r="14" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="68">
       <c r="A14" s="19">
         <v>12.1</v>
       </c>
@@ -1950,7 +1947,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="19">
         <v>13.1</v>
       </c>
@@ -1964,13 +1961,13 @@
         <v>149</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G15" s="65" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="19">
         <v>15.1</v>
       </c>
@@ -1980,10 +1977,10 @@
       <c r="D16" s="25"/>
       <c r="E16" s="17"/>
       <c r="G16" s="65" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="19">
         <v>16.100000000000001</v>
       </c>
@@ -1993,13 +1990,13 @@
       <c r="E17" s="36"/>
       <c r="F17" s="29"/>
       <c r="G17" s="25" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H17" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="19">
         <v>17.100000000000001</v>
       </c>
@@ -2008,10 +2005,10 @@
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="25" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17">
       <c r="A19" s="19">
         <v>18.100000000000001</v>
       </c>
@@ -2019,16 +2016,13 @@
         <v>121</v>
       </c>
       <c r="D19" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="G19" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="H19" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="D24" s="25"/>
       <c r="E24" s="36"/>
       <c r="F24" s="29"/>
@@ -2052,21 +2046,21 @@
       <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="36.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="38.375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="34.625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" style="7" customWidth="1"/>
     <col min="7" max="8" width="38" style="7" customWidth="1"/>
-    <col min="9" max="9" width="35.875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="24.625" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="14.875" style="6"/>
+    <col min="9" max="9" width="35.83203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="14.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -2098,7 +2092,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="80">
       <c r="A2" s="70">
         <v>1</v>
       </c>
@@ -2128,7 +2122,7 @@
       </c>
       <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="80">
       <c r="A3" s="70">
         <v>2</v>
       </c>
@@ -2159,7 +2153,7 @@
       </c>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="64">
       <c r="A4" s="70">
         <v>3</v>
       </c>
@@ -2186,7 +2180,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="80">
       <c r="A5" s="70">
         <v>4</v>
       </c>
@@ -2216,7 +2210,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="113" thickBot="1">
       <c r="A6" s="70">
         <v>5</v>
       </c>
@@ -2243,7 +2237,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="129" thickBot="1">
       <c r="A7" s="69">
         <v>6</v>
       </c>
@@ -2274,7 +2268,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="64">
       <c r="A8" s="69">
         <v>7</v>
       </c>
@@ -2299,7 +2293,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="64">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -2320,7 +2314,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="16">
       <c r="A10" s="9"/>
       <c r="B10" s="10">
         <f t="shared" si="0"/>
@@ -2345,7 +2339,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="16">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -2366,7 +2360,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="128">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -2393,7 +2387,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="80">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -2420,7 +2414,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="70">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -2442,7 +2436,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -2457,7 +2451,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="112">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -2479,7 +2473,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -2494,7 +2488,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="32">
       <c r="A18" s="9" t="s">
         <v>0</v>
       </c>
@@ -2509,10 +2503,10 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="G21" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="16" thickBot="1">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="57"/>
@@ -2521,7 +2515,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="16" thickBot="1">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -2543,21 +2537,21 @@
       <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="36"/>
+    <col min="1" max="1" width="8.83203125" style="36"/>
     <col min="2" max="2" width="35" style="36" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="36" customWidth="1"/>
-    <col min="4" max="4" width="6.375" style="36" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" style="36" customWidth="1"/>
     <col min="5" max="5" width="6" style="14" customWidth="1"/>
-    <col min="6" max="6" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="14" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="14"/>
-    <col min="9" max="9" width="4.625" style="14" customWidth="1"/>
-    <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="14"/>
+    <col min="9" max="9" width="4.6640625" style="14" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="18" thickBot="1">
       <c r="A1" s="38" t="s">
         <v>22</v>
       </c>
@@ -2592,7 +2586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="17" thickTop="1">
       <c r="A2" s="14">
         <v>0</v>
       </c>
@@ -2629,7 +2623,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="14">
         <v>0</v>
       </c>
@@ -2666,7 +2660,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="14">
         <v>0</v>
       </c>
@@ -2703,7 +2697,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="14">
         <v>0</v>
       </c>
@@ -2740,7 +2734,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="14">
         <v>0</v>
       </c>
@@ -2771,7 +2765,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="17" thickBot="1">
       <c r="A7" s="14">
         <v>0</v>
       </c>
@@ -2792,7 +2786,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="18" thickTop="1" thickBot="1">
       <c r="A8" s="14">
         <v>1</v>
       </c>
@@ -2810,7 +2804,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:13" s="14" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="14" customFormat="1" ht="17" thickTop="1">
       <c r="A9" s="64">
         <v>1.2</v>
       </c>
@@ -2831,7 +2825,7 @@
       <c r="L9"/>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="14" customFormat="1">
       <c r="A10" s="14">
         <v>1.1000000000000001</v>
       </c>
@@ -2853,7 +2847,7 @@
       <c r="L10"/>
       <c r="M10"/>
     </row>
-    <row r="11" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="14" customFormat="1">
       <c r="A11" s="64">
         <v>2</v>
       </c>
@@ -2875,7 +2869,7 @@
       <c r="L11"/>
       <c r="M11"/>
     </row>
-    <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="14" customFormat="1">
       <c r="A12" s="64">
         <v>2.2000000000000002</v>
       </c>
@@ -2898,7 +2892,7 @@
       <c r="L12"/>
       <c r="M12"/>
     </row>
-    <row r="13" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="14" customFormat="1">
       <c r="A13" s="64">
         <v>2.2999999999999998</v>
       </c>
@@ -2921,7 +2915,7 @@
       <c r="L13"/>
       <c r="M13"/>
     </row>
-    <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="14" customFormat="1">
       <c r="A14" s="14">
         <v>3.1</v>
       </c>
@@ -2944,7 +2938,7 @@
       <c r="L14"/>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="14" customFormat="1">
       <c r="A15" s="14">
         <v>3.2</v>
       </c>
@@ -2967,7 +2961,7 @@
       <c r="L15"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="14" customFormat="1">
       <c r="A16" s="14">
         <v>3.3</v>
       </c>
@@ -2990,7 +2984,7 @@
       <c r="L16"/>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="14" customFormat="1">
       <c r="A17" s="14">
         <v>4.0999999999999996</v>
       </c>
@@ -3013,7 +3007,7 @@
       <c r="L17"/>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="14" customFormat="1">
       <c r="A18" s="14">
         <v>4.2</v>
       </c>
@@ -3036,7 +3030,7 @@
       <c r="L18"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="14" customFormat="1">
       <c r="A19" s="14">
         <v>4.3</v>
       </c>
@@ -3059,7 +3053,7 @@
       <c r="L19"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="14" customFormat="1">
       <c r="A20" s="14">
         <v>5.0999999999999996</v>
       </c>
@@ -3081,7 +3075,7 @@
       <c r="L20"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="14" customFormat="1">
       <c r="A21" s="14">
         <v>6</v>
       </c>
@@ -3094,7 +3088,7 @@
       <c r="L21"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="14" customFormat="1">
       <c r="A22" s="14">
         <v>6.1</v>
       </c>
@@ -3116,7 +3110,7 @@
       <c r="L22"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="14" customFormat="1">
       <c r="A23" s="14">
         <v>6.2</v>
       </c>
@@ -3138,7 +3132,7 @@
       <c r="L23"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" s="14">
         <v>6.3</v>
       </c>
@@ -3155,7 +3149,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" s="14">
         <v>6.4</v>
       </c>
@@ -3172,7 +3166,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="14" customFormat="1">
       <c r="A26" s="14">
         <v>6.5</v>
       </c>
@@ -3194,7 +3188,7 @@
       <c r="L26"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="14" customFormat="1">
       <c r="A27" s="14">
         <v>7</v>
       </c>
@@ -3207,7 +3201,7 @@
       <c r="L27"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="14" customFormat="1">
       <c r="A28" s="14">
         <v>7.1</v>
       </c>
@@ -3229,7 +3223,7 @@
       <c r="L28"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" s="14">
         <v>7.2</v>
       </c>
@@ -3246,7 +3240,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" s="14">
         <v>7.3</v>
       </c>
@@ -3263,7 +3257,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" s="14">
         <v>7.4</v>
       </c>
@@ -3280,7 +3274,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" s="14">
         <v>7.5</v>
       </c>
@@ -3297,7 +3291,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="14" customFormat="1">
       <c r="A33" s="14">
         <v>8</v>
       </c>
@@ -3310,7 +3304,7 @@
       <c r="L33"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="14" customFormat="1">
       <c r="A34" s="14">
         <v>8.1</v>
       </c>
@@ -3332,7 +3326,7 @@
       <c r="L34"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="14" customFormat="1">
       <c r="A35" s="14">
         <v>8.1999999999999993</v>
       </c>
@@ -3354,7 +3348,7 @@
       <c r="L35"/>
       <c r="M35"/>
     </row>
-    <row r="36" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="14" customFormat="1">
       <c r="A36" s="14">
         <v>8.3000000000000007</v>
       </c>
@@ -3376,7 +3370,7 @@
       <c r="L36"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="14" customFormat="1">
       <c r="A37" s="14">
         <v>8.4</v>
       </c>
@@ -3398,7 +3392,7 @@
       <c r="L37"/>
       <c r="M37"/>
     </row>
-    <row r="38" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="14" customFormat="1">
       <c r="A38" s="14">
         <v>8.5</v>
       </c>
@@ -3420,7 +3414,7 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="A39" s="14">
         <v>10</v>
       </c>
@@ -3430,7 +3424,7 @@
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13">
       <c r="A40" s="14">
         <v>10.1</v>
       </c>
@@ -3447,7 +3441,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="17">
       <c r="A41" s="14">
         <v>10.199999999999999</v>
       </c>
@@ -3464,7 +3458,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="A42" s="14">
         <v>10.3</v>
       </c>
@@ -3481,7 +3475,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13">
       <c r="A43" s="14">
         <v>10.4</v>
       </c>
@@ -3498,18 +3492,18 @@
         <v>100</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G43" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13">
       <c r="A44" s="14">
         <v>10.5</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C44" s="50" t="s">
         <v>14</v>
@@ -3521,18 +3515,18 @@
         <v>100</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G44" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="A45" s="14">
         <v>10.7</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C45" s="50" t="s">
         <v>14</v>
@@ -3544,13 +3538,13 @@
         <v>100</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G45" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" s="14">
         <v>10.4</v>
       </c>
@@ -3567,13 +3561,13 @@
         <v>100</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G46" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13">
       <c r="A47" s="14"/>
       <c r="B47" s="14" t="s">
         <v>142</v>
@@ -3588,10 +3582,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13">
       <c r="A48" s="14"/>
       <c r="B48" s="36" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C48" s="50" t="s">
         <v>14</v>
@@ -3600,170 +3594,170 @@
         <v>5</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G48" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
       <c r="F49" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G49" s="14">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="68"/>
       <c r="F50" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G50" s="14">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
       <c r="E51" s="68"/>
       <c r="F51" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G51" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
       <c r="E52" s="68"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
       <c r="E53" s="68"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
       <c r="E54" s="68"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
       <c r="E55" s="68"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7">
       <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
       <c r="E56" s="68"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
       <c r="E57" s="68"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="A58" s="14"/>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
       <c r="E58" s="68"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" s="14"/>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
       <c r="E59" s="68"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
       <c r="E60" s="68"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
       <c r="E61" s="68"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
       <c r="E62" s="68"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
       <c r="E63" s="68"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7">
       <c r="A64" s="14"/>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
       <c r="E64" s="68"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
       <c r="E65" s="68"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13">
       <c r="A66" s="14"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
       <c r="D66" s="14"/>
       <c r="E66" s="68"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13">
       <c r="A67" s="14"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
       <c r="D67" s="14"/>
       <c r="E67" s="68"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13">
       <c r="A68" s="14"/>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
       <c r="E68" s="68"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13">
       <c r="A69" s="14"/>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
@@ -3774,7 +3768,7 @@
       <c r="H69" s="36"/>
       <c r="I69" s="36"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13">
       <c r="A70" s="14"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
@@ -3785,81 +3779,81 @@
       <c r="H70" s="36"/>
       <c r="I70" s="36"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13">
       <c r="A71" s="14"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
       <c r="D71" s="14"/>
       <c r="E71" s="68"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13">
       <c r="A72" s="14"/>
       <c r="B72" s="14"/>
       <c r="C72" s="14"/>
       <c r="D72" s="14"/>
       <c r="E72" s="68"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13">
       <c r="A73" s="14"/>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
       <c r="D73" s="14"/>
       <c r="E73" s="68"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13">
       <c r="A74" s="14"/>
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
       <c r="D74" s="14"/>
       <c r="E74" s="68"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13">
       <c r="A75" s="14"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
       <c r="D75" s="14"/>
       <c r="E75" s="68"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13">
       <c r="A76" s="14"/>
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
       <c r="D76" s="14"/>
       <c r="E76" s="68"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13">
       <c r="A77" s="14"/>
       <c r="B77" s="14"/>
       <c r="C77" s="14"/>
       <c r="D77" s="14"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13">
       <c r="A78" s="14"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
       <c r="D78" s="14"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13">
       <c r="A79" s="14"/>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
       <c r="D79" s="14"/>
     </row>
-    <row r="80" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" s="14" customFormat="1">
       <c r="F80"/>
       <c r="J80"/>
       <c r="K80"/>
       <c r="L80"/>
       <c r="M80"/>
     </row>
-    <row r="81" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" s="14" customFormat="1">
       <c r="F81"/>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81"/>
       <c r="M81"/>
     </row>
-    <row r="82" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" s="14" customFormat="1">
       <c r="A82" s="52"/>
       <c r="B82" s="52"/>
       <c r="C82" s="52"/>
@@ -3870,7 +3864,7 @@
       <c r="L82"/>
       <c r="M82"/>
     </row>
-    <row r="83" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" s="14" customFormat="1">
       <c r="A83" s="52"/>
       <c r="B83" s="52"/>
       <c r="C83" s="52"/>
@@ -3882,7 +3876,7 @@
       <c r="L83"/>
       <c r="M83"/>
     </row>
-    <row r="84" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" s="14" customFormat="1">
       <c r="A84" s="52"/>
       <c r="B84" s="52"/>
       <c r="C84" s="52"/>
@@ -3894,7 +3888,7 @@
       <c r="L84"/>
       <c r="M84"/>
     </row>
-    <row r="85" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" s="14" customFormat="1">
       <c r="A85" s="52"/>
       <c r="B85" s="52"/>
       <c r="C85" s="52"/>
@@ -3906,7 +3900,7 @@
       <c r="L85"/>
       <c r="M85"/>
     </row>
-    <row r="86" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" s="14" customFormat="1">
       <c r="A86" s="52"/>
       <c r="B86" s="52"/>
       <c r="C86" s="52"/>
@@ -3919,7 +3913,7 @@
       <c r="L86"/>
       <c r="M86"/>
     </row>
-    <row r="87" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" s="14" customFormat="1">
       <c r="A87" s="52"/>
       <c r="B87" s="52"/>
       <c r="C87" s="52"/>
@@ -3930,7 +3924,7 @@
       <c r="L87"/>
       <c r="M87"/>
     </row>
-    <row r="88" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" s="14" customFormat="1">
       <c r="A88" s="52"/>
       <c r="B88" s="52"/>
       <c r="C88" s="52"/>
@@ -3943,7 +3937,7 @@
       <c r="L88"/>
       <c r="M88"/>
     </row>
-    <row r="89" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" s="14" customFormat="1">
       <c r="A89" s="52"/>
       <c r="B89" s="52"/>
       <c r="C89" s="52"/>
@@ -3956,7 +3950,7 @@
       <c r="L89"/>
       <c r="M89"/>
     </row>
-    <row r="90" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" s="14" customFormat="1">
       <c r="A90" s="52"/>
       <c r="B90" s="52"/>
       <c r="C90" s="52"/>
@@ -3969,7 +3963,7 @@
       <c r="L90"/>
       <c r="M90"/>
     </row>
-    <row r="91" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" s="14" customFormat="1">
       <c r="A91" s="52"/>
       <c r="B91" s="52"/>
       <c r="C91" s="52"/>
@@ -3982,7 +3976,7 @@
       <c r="L91"/>
       <c r="M91"/>
     </row>
-    <row r="92" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" s="14" customFormat="1">
       <c r="A92" s="52"/>
       <c r="B92" s="52"/>
       <c r="C92" s="52"/>
@@ -3995,7 +3989,7 @@
       <c r="L92"/>
       <c r="M92"/>
     </row>
-    <row r="93" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" s="14" customFormat="1">
       <c r="A93" s="52"/>
       <c r="B93" s="52"/>
       <c r="C93" s="52"/>
@@ -4008,7 +4002,7 @@
       <c r="L93"/>
       <c r="M93"/>
     </row>
-    <row r="94" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" s="14" customFormat="1">
       <c r="A94" s="52"/>
       <c r="B94" s="52"/>
       <c r="C94" s="52"/>
@@ -4021,7 +4015,7 @@
       <c r="L94"/>
       <c r="M94"/>
     </row>
-    <row r="95" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" s="14" customFormat="1">
       <c r="A95" s="52"/>
       <c r="B95" s="52"/>
       <c r="C95" s="52"/>
@@ -4034,49 +4028,49 @@
       <c r="L95"/>
       <c r="M95"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13">
       <c r="A96" s="52"/>
       <c r="B96" s="52"/>
       <c r="C96" s="52"/>
       <c r="D96" s="52"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" s="52"/>
       <c r="B97" s="52"/>
       <c r="C97" s="52"/>
       <c r="D97" s="52"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" s="52"/>
       <c r="B98" s="52"/>
       <c r="C98" s="52"/>
       <c r="D98" s="52"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" s="52"/>
       <c r="B99" s="52"/>
       <c r="C99" s="52"/>
       <c r="D99" s="52"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" s="52"/>
       <c r="B100" s="52"/>
       <c r="C100" s="52"/>
       <c r="D100" s="52"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" s="52"/>
       <c r="B101" s="52"/>
       <c r="C101" s="52"/>
       <c r="D101" s="52"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" s="52"/>
       <c r="B102" s="52"/>
       <c r="C102" s="52"/>
       <c r="D102" s="52"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" s="53"/>
       <c r="B103" s="53"/>
       <c r="D103" s="53"/>

</xml_diff>

<commit_message>
add links for team eval
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20358"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH456/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2996BCDF-B206-9A4E-B8C4-C710A3961C3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB896D9-1B58-4227-9F15-38332D0908EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="15280" windowHeight="14440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="465" windowWidth="15285" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
     <sheet name="slo_detail" sheetId="5" r:id="rId2"/>
     <sheet name="points" sheetId="11" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -654,9 +654,6 @@
     <t>smoothness of presentation</t>
   </si>
   <si>
-    <t>HW 05: Cluster Analysis [[HTML]](hw/hw05-cluster.html)[[PDF]](hw/hw05-cluster-pdf) (Draft 4/21, Final 4/25 )</t>
-  </si>
-  <si>
     <t>[[Presentation slides Draft]](https://norcalbiostat.github.io/MATH456/project.html#draft_slides) (Due 4/27 PR 4/29)</t>
   </si>
   <si>
@@ -666,17 +663,23 @@
     <t xml:space="preserve">Groups check in with Dr. D. </t>
   </si>
   <si>
-    <t>See project page</t>
-  </si>
-  <si>
     <t>Thursday 2-4pm, OR Friday 12-2pm</t>
+  </si>
+  <si>
+    <t>See project page for details   
+[[Project Scoring]](https://forms.gle/eUYGZqWuMzD5zX2c6)  
+[[Team member evaluation]](https://forms.gle/Fs1k4Mi6VZeU5cCBA)</t>
+  </si>
+  <si>
+    <t>HW 05: Cluster Analysis [[HTML]](hw/hw05-cluster.html)[[PDF]](hw/hw05-cluster-pdf)   
+ (Draft 4/21, Final 4/25 )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1674,21 +1677,21 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="14"/>
-    <col min="3" max="3" width="5.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" style="14" customWidth="1"/>
+    <col min="1" max="2" width="8.875" style="14"/>
+    <col min="3" max="3" width="5.625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" customWidth="1"/>
+    <col min="5" max="5" width="11.125" style="14" customWidth="1"/>
     <col min="6" max="6" width="18" style="24" customWidth="1"/>
     <col min="7" max="7" width="33" customWidth="1"/>
     <col min="8" max="8" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" ht="17" thickBot="1">
+    <row r="1" spans="1:8" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>24</v>
       </c>
@@ -1714,7 +1717,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
         <v>1.1000000000000001</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>1.2</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="128">
+    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>2.1</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="48">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>3.1</v>
       </c>
@@ -1790,7 +1793,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="102">
+    <row r="6" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>4.0999999999999996</v>
       </c>
@@ -1813,7 +1816,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="85">
+    <row r="7" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>5.0999999999999996</v>
       </c>
@@ -1832,7 +1835,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="119">
+    <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>6.1</v>
       </c>
@@ -1852,7 +1855,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="32">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>7.1</v>
       </c>
@@ -1868,7 +1871,7 @@
       <c r="F9" s="35"/>
       <c r="G9" s="25"/>
     </row>
-    <row r="10" spans="1:8" ht="34">
+    <row r="10" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>9.1</v>
       </c>
@@ -1884,7 +1887,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>8</v>
       </c>
@@ -1898,7 +1901,7 @@
       <c r="F11" s="32"/>
       <c r="G11" s="30"/>
     </row>
-    <row r="12" spans="1:8" ht="38.25" customHeight="1">
+    <row r="12" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>10.1</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39" customHeight="1">
+    <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>11.1</v>
       </c>
@@ -1927,7 +1930,7 @@
       </c>
       <c r="G13" s="65"/>
     </row>
-    <row r="14" spans="1:8" ht="68">
+    <row r="14" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>12.1</v>
       </c>
@@ -1947,7 +1950,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>13.1</v>
       </c>
@@ -1961,13 +1964,13 @@
         <v>149</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G15" s="65" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>15.1</v>
       </c>
@@ -1976,11 +1979,11 @@
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="17"/>
-      <c r="G16" s="65" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="G16" s="29" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>16.100000000000001</v>
       </c>
@@ -1990,13 +1993,13 @@
       <c r="E17" s="36"/>
       <c r="F17" s="29"/>
       <c r="G17" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H17" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>17.100000000000001</v>
       </c>
@@ -2005,10 +2008,10 @@
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="25" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="17">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>18.100000000000001</v>
       </c>
@@ -2016,13 +2019,13 @@
         <v>121</v>
       </c>
       <c r="D19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G19" s="37" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" s="25"/>
       <c r="E24" s="36"/>
       <c r="F24" s="29"/>
@@ -2046,21 +2049,21 @@
       <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.875" style="6" customWidth="1"/>
     <col min="4" max="4" width="36.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="34.6640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="38.375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="34.625" style="7" customWidth="1"/>
     <col min="7" max="8" width="38" style="7" customWidth="1"/>
-    <col min="9" max="9" width="35.83203125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="14.83203125" style="6"/>
+    <col min="9" max="9" width="35.875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="24.625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="14.875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -2092,7 +2095,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="80">
+    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="70">
         <v>1</v>
       </c>
@@ -2122,7 +2125,7 @@
       </c>
       <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:10" ht="80">
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="70">
         <v>2</v>
       </c>
@@ -2153,7 +2156,7 @@
       </c>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" ht="64">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="70">
         <v>3</v>
       </c>
@@ -2180,7 +2183,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="80">
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="70">
         <v>4</v>
       </c>
@@ -2210,7 +2213,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="113" thickBot="1">
+    <row r="6" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="70">
         <v>5</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="129" thickBot="1">
+    <row r="7" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="69">
         <v>6</v>
       </c>
@@ -2268,7 +2271,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="64">
+    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="69">
         <v>7</v>
       </c>
@@ -2293,7 +2296,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="64">
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -2314,7 +2317,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="10">
         <f t="shared" si="0"/>
@@ -2339,7 +2342,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -2360,7 +2363,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="128">
+    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -2387,7 +2390,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="80">
+    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -2414,7 +2417,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="70">
+    <row r="14" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -2436,7 +2439,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -2451,7 +2454,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="112">
+    <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -2473,7 +2476,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -2488,7 +2491,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="32">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>0</v>
       </c>
@@ -2503,10 +2506,10 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G21" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="16" thickBot="1">
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="57"/>
@@ -2515,7 +2518,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" ht="16" thickBot="1">
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -2537,21 +2540,21 @@
       <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="36"/>
+    <col min="1" max="1" width="8.875" style="36"/>
     <col min="2" max="2" width="35" style="36" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" style="36" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" style="36" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="36" customWidth="1"/>
+    <col min="4" max="4" width="6.375" style="36" customWidth="1"/>
     <col min="5" max="5" width="6" style="14" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="14" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="14"/>
-    <col min="9" max="9" width="4.6640625" style="14" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="14"/>
+    <col min="9" max="9" width="4.625" style="14" customWidth="1"/>
+    <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" thickBot="1">
+    <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="38" t="s">
         <v>22</v>
       </c>
@@ -2586,7 +2589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17" thickTop="1">
+    <row r="2" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>0</v>
       </c>
@@ -2623,7 +2626,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>0</v>
       </c>
@@ -2660,7 +2663,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>0</v>
       </c>
@@ -2697,7 +2700,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>0</v>
       </c>
@@ -2734,7 +2737,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>0</v>
       </c>
@@ -2765,7 +2768,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17" thickBot="1">
+    <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>0</v>
       </c>
@@ -2786,7 +2789,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18" thickTop="1" thickBot="1">
+    <row r="8" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>1</v>
       </c>
@@ -2804,7 +2807,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:13" s="14" customFormat="1" ht="17" thickTop="1">
+    <row r="9" spans="1:13" s="14" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="64">
         <v>1.2</v>
       </c>
@@ -2825,7 +2828,7 @@
       <c r="L9"/>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:13" s="14" customFormat="1">
+    <row r="10" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>1.1000000000000001</v>
       </c>
@@ -2847,7 +2850,7 @@
       <c r="L10"/>
       <c r="M10"/>
     </row>
-    <row r="11" spans="1:13" s="14" customFormat="1">
+    <row r="11" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="64">
         <v>2</v>
       </c>
@@ -2869,7 +2872,7 @@
       <c r="L11"/>
       <c r="M11"/>
     </row>
-    <row r="12" spans="1:13" s="14" customFormat="1">
+    <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="64">
         <v>2.2000000000000002</v>
       </c>
@@ -2892,7 +2895,7 @@
       <c r="L12"/>
       <c r="M12"/>
     </row>
-    <row r="13" spans="1:13" s="14" customFormat="1">
+    <row r="13" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="64">
         <v>2.2999999999999998</v>
       </c>
@@ -2915,7 +2918,7 @@
       <c r="L13"/>
       <c r="M13"/>
     </row>
-    <row r="14" spans="1:13" s="14" customFormat="1">
+    <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>3.1</v>
       </c>
@@ -2938,7 +2941,7 @@
       <c r="L14"/>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:13" s="14" customFormat="1">
+    <row r="15" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>3.2</v>
       </c>
@@ -2961,7 +2964,7 @@
       <c r="L15"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:13" s="14" customFormat="1">
+    <row r="16" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>3.3</v>
       </c>
@@ -2984,7 +2987,7 @@
       <c r="L16"/>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" s="14" customFormat="1">
+    <row r="17" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>4.0999999999999996</v>
       </c>
@@ -3007,7 +3010,7 @@
       <c r="L17"/>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" s="14" customFormat="1">
+    <row r="18" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>4.2</v>
       </c>
@@ -3030,7 +3033,7 @@
       <c r="L18"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" s="14" customFormat="1">
+    <row r="19" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>4.3</v>
       </c>
@@ -3053,7 +3056,7 @@
       <c r="L19"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" s="14" customFormat="1">
+    <row r="20" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>5.0999999999999996</v>
       </c>
@@ -3075,7 +3078,7 @@
       <c r="L20"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" s="14" customFormat="1">
+    <row r="21" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>6</v>
       </c>
@@ -3088,7 +3091,7 @@
       <c r="L21"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" s="14" customFormat="1">
+    <row r="22" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>6.1</v>
       </c>
@@ -3110,7 +3113,7 @@
       <c r="L22"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" s="14" customFormat="1">
+    <row r="23" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
         <v>6.2</v>
       </c>
@@ -3132,7 +3135,7 @@
       <c r="L23"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>6.3</v>
       </c>
@@ -3149,7 +3152,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>6.4</v>
       </c>
@@ -3166,7 +3169,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="14" customFormat="1">
+    <row r="26" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <v>6.5</v>
       </c>
@@ -3188,7 +3191,7 @@
       <c r="L26"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" s="14" customFormat="1">
+    <row r="27" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
         <v>7</v>
       </c>
@@ -3201,7 +3204,7 @@
       <c r="L27"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" s="14" customFormat="1">
+    <row r="28" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>7.1</v>
       </c>
@@ -3223,7 +3226,7 @@
       <c r="L28"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>7.2</v>
       </c>
@@ -3240,7 +3243,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>7.3</v>
       </c>
@@ -3257,7 +3260,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>7.4</v>
       </c>
@@ -3274,7 +3277,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>7.5</v>
       </c>
@@ -3291,7 +3294,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="14" customFormat="1">
+    <row r="33" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>8</v>
       </c>
@@ -3304,7 +3307,7 @@
       <c r="L33"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="1:13" s="14" customFormat="1">
+    <row r="34" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>8.1</v>
       </c>
@@ -3326,7 +3329,7 @@
       <c r="L34"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="1:13" s="14" customFormat="1">
+    <row r="35" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
         <v>8.1999999999999993</v>
       </c>
@@ -3348,7 +3351,7 @@
       <c r="L35"/>
       <c r="M35"/>
     </row>
-    <row r="36" spans="1:13" s="14" customFormat="1">
+    <row r="36" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>8.3000000000000007</v>
       </c>
@@ -3370,7 +3373,7 @@
       <c r="L36"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="1:13" s="14" customFormat="1">
+    <row r="37" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
         <v>8.4</v>
       </c>
@@ -3392,7 +3395,7 @@
       <c r="L37"/>
       <c r="M37"/>
     </row>
-    <row r="38" spans="1:13" s="14" customFormat="1">
+    <row r="38" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>8.5</v>
       </c>
@@ -3414,7 +3417,7 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
         <v>10</v>
       </c>
@@ -3424,7 +3427,7 @@
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
         <v>10.1</v>
       </c>
@@ -3441,7 +3444,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="17">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
         <v>10.199999999999999</v>
       </c>
@@ -3458,7 +3461,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
         <v>10.3</v>
       </c>
@@ -3475,7 +3478,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="14">
         <v>10.4</v>
       </c>
@@ -3498,7 +3501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="14">
         <v>10.5</v>
       </c>
@@ -3521,7 +3524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
         <v>10.7</v>
       </c>
@@ -3544,7 +3547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
         <v>10.4</v>
       </c>
@@ -3567,7 +3570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="14" t="s">
         <v>142</v>
@@ -3582,7 +3585,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="B48" s="36" t="s">
         <v>171</v>
@@ -3600,7 +3603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
@@ -3612,7 +3615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
@@ -3625,7 +3628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
@@ -3638,126 +3641,126 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
       <c r="E52" s="68"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
       <c r="E53" s="68"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
       <c r="E54" s="68"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
       <c r="E55" s="68"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
       <c r="E56" s="68"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
       <c r="E57" s="68"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="14"/>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
       <c r="E58" s="68"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
       <c r="E59" s="68"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
       <c r="E60" s="68"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
       <c r="E61" s="68"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
       <c r="E62" s="68"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
       <c r="E63" s="68"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
       <c r="E64" s="68"/>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
       <c r="E65" s="68"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="14"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
       <c r="D66" s="14"/>
       <c r="E66" s="68"/>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="14"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
       <c r="D67" s="14"/>
       <c r="E67" s="68"/>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="14"/>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
       <c r="E68" s="68"/>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="14"/>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
@@ -3768,7 +3771,7 @@
       <c r="H69" s="36"/>
       <c r="I69" s="36"/>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="14"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
@@ -3779,81 +3782,81 @@
       <c r="H70" s="36"/>
       <c r="I70" s="36"/>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="14"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
       <c r="D71" s="14"/>
       <c r="E71" s="68"/>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="14"/>
       <c r="B72" s="14"/>
       <c r="C72" s="14"/>
       <c r="D72" s="14"/>
       <c r="E72" s="68"/>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="14"/>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
       <c r="D73" s="14"/>
       <c r="E73" s="68"/>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="14"/>
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
       <c r="D74" s="14"/>
       <c r="E74" s="68"/>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="14"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
       <c r="D75" s="14"/>
       <c r="E75" s="68"/>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="14"/>
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
       <c r="D76" s="14"/>
       <c r="E76" s="68"/>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="14"/>
       <c r="B77" s="14"/>
       <c r="C77" s="14"/>
       <c r="D77" s="14"/>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="14"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
       <c r="D78" s="14"/>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="14"/>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
       <c r="D79" s="14"/>
     </row>
-    <row r="80" spans="1:13" s="14" customFormat="1">
+    <row r="80" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F80"/>
       <c r="J80"/>
       <c r="K80"/>
       <c r="L80"/>
       <c r="M80"/>
     </row>
-    <row r="81" spans="1:13" s="14" customFormat="1">
+    <row r="81" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F81"/>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81"/>
       <c r="M81"/>
     </row>
-    <row r="82" spans="1:13" s="14" customFormat="1">
+    <row r="82" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="52"/>
       <c r="B82" s="52"/>
       <c r="C82" s="52"/>
@@ -3864,7 +3867,7 @@
       <c r="L82"/>
       <c r="M82"/>
     </row>
-    <row r="83" spans="1:13" s="14" customFormat="1">
+    <row r="83" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="52"/>
       <c r="B83" s="52"/>
       <c r="C83" s="52"/>
@@ -3876,7 +3879,7 @@
       <c r="L83"/>
       <c r="M83"/>
     </row>
-    <row r="84" spans="1:13" s="14" customFormat="1">
+    <row r="84" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="52"/>
       <c r="B84" s="52"/>
       <c r="C84" s="52"/>
@@ -3888,7 +3891,7 @@
       <c r="L84"/>
       <c r="M84"/>
     </row>
-    <row r="85" spans="1:13" s="14" customFormat="1">
+    <row r="85" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="52"/>
       <c r="B85" s="52"/>
       <c r="C85" s="52"/>
@@ -3900,7 +3903,7 @@
       <c r="L85"/>
       <c r="M85"/>
     </row>
-    <row r="86" spans="1:13" s="14" customFormat="1">
+    <row r="86" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="52"/>
       <c r="B86" s="52"/>
       <c r="C86" s="52"/>
@@ -3913,7 +3916,7 @@
       <c r="L86"/>
       <c r="M86"/>
     </row>
-    <row r="87" spans="1:13" s="14" customFormat="1">
+    <row r="87" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="52"/>
       <c r="B87" s="52"/>
       <c r="C87" s="52"/>
@@ -3924,7 +3927,7 @@
       <c r="L87"/>
       <c r="M87"/>
     </row>
-    <row r="88" spans="1:13" s="14" customFormat="1">
+    <row r="88" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="52"/>
       <c r="B88" s="52"/>
       <c r="C88" s="52"/>
@@ -3937,7 +3940,7 @@
       <c r="L88"/>
       <c r="M88"/>
     </row>
-    <row r="89" spans="1:13" s="14" customFormat="1">
+    <row r="89" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="52"/>
       <c r="B89" s="52"/>
       <c r="C89" s="52"/>
@@ -3950,7 +3953,7 @@
       <c r="L89"/>
       <c r="M89"/>
     </row>
-    <row r="90" spans="1:13" s="14" customFormat="1">
+    <row r="90" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="52"/>
       <c r="B90" s="52"/>
       <c r="C90" s="52"/>
@@ -3963,7 +3966,7 @@
       <c r="L90"/>
       <c r="M90"/>
     </row>
-    <row r="91" spans="1:13" s="14" customFormat="1">
+    <row r="91" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="52"/>
       <c r="B91" s="52"/>
       <c r="C91" s="52"/>
@@ -3976,7 +3979,7 @@
       <c r="L91"/>
       <c r="M91"/>
     </row>
-    <row r="92" spans="1:13" s="14" customFormat="1">
+    <row r="92" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="52"/>
       <c r="B92" s="52"/>
       <c r="C92" s="52"/>
@@ -3989,7 +3992,7 @@
       <c r="L92"/>
       <c r="M92"/>
     </row>
-    <row r="93" spans="1:13" s="14" customFormat="1">
+    <row r="93" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="52"/>
       <c r="B93" s="52"/>
       <c r="C93" s="52"/>
@@ -4002,7 +4005,7 @@
       <c r="L93"/>
       <c r="M93"/>
     </row>
-    <row r="94" spans="1:13" s="14" customFormat="1">
+    <row r="94" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="52"/>
       <c r="B94" s="52"/>
       <c r="C94" s="52"/>
@@ -4015,7 +4018,7 @@
       <c r="L94"/>
       <c r="M94"/>
     </row>
-    <row r="95" spans="1:13" s="14" customFormat="1">
+    <row r="95" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="52"/>
       <c r="B95" s="52"/>
       <c r="C95" s="52"/>
@@ -4028,49 +4031,49 @@
       <c r="L95"/>
       <c r="M95"/>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="52"/>
       <c r="B96" s="52"/>
       <c r="C96" s="52"/>
       <c r="D96" s="52"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="52"/>
       <c r="B97" s="52"/>
       <c r="C97" s="52"/>
       <c r="D97" s="52"/>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="52"/>
       <c r="B98" s="52"/>
       <c r="C98" s="52"/>
       <c r="D98" s="52"/>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="52"/>
       <c r="B99" s="52"/>
       <c r="C99" s="52"/>
       <c r="D99" s="52"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="52"/>
       <c r="B100" s="52"/>
       <c r="C100" s="52"/>
       <c r="D100" s="52"/>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="52"/>
       <c r="B101" s="52"/>
       <c r="C101" s="52"/>
       <c r="D101" s="52"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="52"/>
       <c r="B102" s="52"/>
       <c r="C102" s="52"/>
       <c r="D102" s="52"/>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="53"/>
       <c r="B103" s="53"/>
       <c r="D103" s="53"/>

</xml_diff>

<commit_message>
add intro and stat modeling
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20358"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB896D9-1B58-4227-9F15-38332D0908EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7623C6-F6C9-4A27-9C4D-504A964B3692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="465" windowWidth="15285" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35220" yWindow="2445" windowWidth="16380" windowHeight="13305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -23,6 +23,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -31,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
   <si>
     <t>Finals Week</t>
   </si>
@@ -118,9 +129,6 @@
   </si>
   <si>
     <t>Variable Selection</t>
-  </si>
-  <si>
-    <t>Proposal due for approval</t>
   </si>
   <si>
     <t>Dimension Reduction - PCA</t>
@@ -270,9 +278,6 @@
     <t>Fix my notes</t>
   </si>
   <si>
-    <t>PMA6 Ch 3</t>
-  </si>
-  <si>
     <t>Syllabus</t>
   </si>
   <si>
@@ -308,9 +313,6 @@
   </si>
   <si>
     <t>Guest Lecture: Penalized methods (LASSO)</t>
-  </si>
-  <si>
-    <t>[[HW 01: Statistical Modeling]](hw/hw01-model-building.html) (Draft 02/09, PR 02/12, Final 02/15 )</t>
   </si>
   <si>
     <t>GLM &amp; Classification Assignment</t>
@@ -345,12 +347,6 @@
 Fit and interpret an interaction model </t>
   </si>
   <si>
-    <t>[[HW 00: Getting Started]](hw/hw00-getting-started.html) (Due 01/26 ) (PR 01/29)</t>
-  </si>
-  <si>
-    <t>[[Quiz 00]](https://forms.gle/fea9qCkhNZrvrdy27)(Due 1/23)</t>
-  </si>
-  <si>
     <t>Quiz on Data preparation &amp; class logistics
 Create a Data preparation reference flowchart</t>
   </si>
@@ -401,9 +397,6 @@
     <t>Slack Participation</t>
   </si>
   <si>
-    <t>PMA6 CH9, ASCN CH 9.5-9.7</t>
-  </si>
-  <si>
     <t xml:space="preserve">QFT: Variable Selection
 </t>
   </si>
@@ -413,12 +406,6 @@
 General F-test for multiple predictors (PMA6 Ch 9.5)</t>
   </si>
   <si>
-    <t>[[Quiz 01]](https://forms.gle/k882tgmNtYwAebv98) (Due 2/10 Before 1pm)</t>
-  </si>
-  <si>
-    <t>Recruitment video created (Due Mon 2/10 )</t>
-  </si>
-  <si>
     <t>Review on Regression &amp; Variable selection</t>
   </si>
   <si>
@@ -449,16 +436,6 @@
 Some measures of model fit for Logistic regression is slightly different than for linear regression. </t>
   </si>
   <si>
-    <t>[Project selection](https://forms.gle/27dgotMRy61DSgtr6) (Due 2/15 )</t>
-  </si>
-  <si>
-    <t>[[HW 02: GLM and Classification]](hw/hw02-glm-classification.html) (Draft 02/23, PR 02/26, Final 02/29 )
-LJ Check in (Due 2/14 )</t>
-  </si>
-  <si>
-    <t>[[Quiz 02]](https://forms.gle/J8M31nsT6bJWFakm8)  (Due 2/25)</t>
-  </si>
-  <si>
     <t>PMA6 11.3-11.4</t>
   </si>
   <si>
@@ -469,28 +446,10 @@
   </si>
   <si>
     <t>finals</t>
-  </si>
-  <si>
-    <t>Task distributions, project timeline (Due Sat 2/22 )  
-Printed Team agreements (Due Mon 2/24 )</t>
-  </si>
-  <si>
-    <t>MLR: PMA6 Ch8, 10.3  
-ASCN Ch8, 9.1-9.4  
-Modeling: ASCN Ch10.1-10.3</t>
   </si>
   <si>
     <t>PMA6 CH12.1-12.8  
 ASCN Ch9.1-9.3</t>
-  </si>
-  <si>
-    <t>HW 03 : Missing Data  
-[[Instructions]](hw/hw03-missing-data.html) [[RMD]](hw/hw03-missing-data-template.Rmd)   
- (Draft 03/04, PR 03/06, Final 03/08 )</t>
-  </si>
-  <si>
-    <t>Midterm (W 03/11 )  
-LJ Check in (F 03/13 )</t>
   </si>
   <si>
     <t xml:space="preserve">install packages: mice, VIM
@@ -505,9 +464,6 @@
     <t>[[Quiz 03]](https://forms.gle/iAHo9yiLrjp8v5266)  (Due 3/5)</t>
   </si>
   <si>
-    <t xml:space="preserve">Practice social distancing, get outdoors, get some exercise, and just hang in there. </t>
-  </si>
-  <si>
     <t>PMA6 CH 14
 ASCN Ch 13</t>
   </si>
@@ -559,12 +515,6 @@
   </si>
   <si>
     <t>[[Project update]](project.html#project_update) (Due  03/27 )</t>
-  </si>
-  <si>
-    <t>Cluster analysis</t>
-  </si>
-  <si>
-    <t>PMA6 Ch 16</t>
   </si>
   <si>
     <t>Covid19 Campus Closed</t>
@@ -618,9 +568,6 @@
     <t>[[Quiz 04]](https://forms.gle/mirjk4xDsFk8HtHQA) (Due 4/9 )</t>
   </si>
   <si>
-    <t>Pre-topic LJ check in. (Mon 4/13 AM)</t>
-  </si>
-  <si>
     <t>Presentation slides draft</t>
   </si>
   <si>
@@ -657,29 +604,97 @@
     <t>[[Presentation slides Draft]](https://norcalbiostat.github.io/MATH456/project.html#draft_slides) (Due 4/27 PR 4/29)</t>
   </si>
   <si>
-    <t>[[Quiz 05]](https://forms.gle/iu3hxM3fpyWSBbxu5) (Due 4/23 )</t>
-  </si>
-  <si>
     <t xml:space="preserve">Groups check in with Dr. D. </t>
   </si>
   <si>
     <t>Thursday 2-4pm, OR Friday 12-2pm</t>
   </si>
   <si>
+    <t xml:space="preserve">Have fun! Relax, rejuvinate yourself. </t>
+  </si>
+  <si>
+    <t>PMA6 Ch 8, 10.3
+ASCN Ch 9</t>
+  </si>
+  <si>
+    <t>[[HW 00: Getting Started]](hw/hw00-getting-started.html) (Due 01/27 ) (PR 01/30)</t>
+  </si>
+  <si>
+    <t>Proposal due for approval (Due Sat 2/4)</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 3
+ASCN Ch 1</t>
+  </si>
+  <si>
+    <t>Review of Simple Linear Regression</t>
+  </si>
+  <si>
+    <t>In class activities</t>
+  </si>
+  <si>
+    <t>flow chart of data preparation</t>
+  </si>
+  <si>
+    <t>pre-work: write down everything you know about LinReg. 
+Compare to a neighbor. Share with class</t>
+  </si>
+  <si>
+    <t>QFT</t>
+  </si>
+  <si>
+    <t>[Project selection]() (Due 2/15 )</t>
+  </si>
+  <si>
+    <t>Recruitment video created (Due Sat 2/11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMA6 Ch8, 10.1-10.3   
+ASCN Ch9-10
+</t>
+  </si>
+  <si>
+    <t>PMA6 Ch9-Ch10   
+ASCN Ch 10.6-10.7</t>
+  </si>
+  <si>
     <t>See project page for details   
-[[Project Scoring]](https://forms.gle/eUYGZqWuMzD5zX2c6)  
-[[Team member evaluation]](https://forms.gle/Fs1k4Mi6VZeU5cCBA)</t>
-  </si>
-  <si>
-    <t>HW 05: Cluster Analysis [[HTML]](hw/hw05-cluster.html)[[PDF]](hw/hw05-cluster-pdf)   
- (Draft 4/21, Final 4/25 )</t>
+[[Project Scoring]]()  
+[[Team member evaluation]]()</t>
+  </si>
+  <si>
+    <t>[[Quiz 00]](https://forms.gle/mizdZk4qw8QC5NXT8)(Due 01/24 )</t>
+  </si>
+  <si>
+    <t>[[Quiz 01]](https://forms.gle/xXoyigprJXnDd5Sn8) (Due 02/02/12 )</t>
+  </si>
+  <si>
+    <t>[[Quiz 02]]()  (Due 2/XX)</t>
+  </si>
+  <si>
+    <t>[[HW 02: GLM and Classification]](hw/hw02-glm-classification.html) (Draft 02/xx, PR 02/xx, Final 02/xx )
+LJ Check in (Due 2/xx )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project timeline &amp; Team Agreements (Due 2/26 )  </t>
+  </si>
+  <si>
+    <t>Midterm  
+LJ Check in</t>
+  </si>
+  <si>
+    <t>[HW 03 : Missing Data [[Instructions]](hw/hw03-missing-data.html) [[RMD]](hw/hw03-missing-data-template.Rmd)   
+ (Draft 03/xx, PR 03/xx, Final 03/xx )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[HW 01: Statistical Modeling]](hw/hw01-model-building.html) (Draft 02/12, PR 02/14, Final 02/18 ) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -802,6 +817,27 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1052,7 +1088,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1122,8 +1158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="81" applyAlignment="1">
@@ -1132,7 +1167,7 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1145,18 +1180,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1191,29 +1214,17 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="82" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="82" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1226,32 +1237,36 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -1674,10 +1689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1687,11 +1702,11 @@
     <col min="4" max="4" width="24.875" customWidth="1"/>
     <col min="5" max="5" width="11.125" style="14" customWidth="1"/>
     <col min="6" max="6" width="18" style="24" customWidth="1"/>
-    <col min="7" max="7" width="33" customWidth="1"/>
-    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="7" max="7" width="19.375" customWidth="1"/>
+    <col min="8" max="8" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>24</v>
       </c>
@@ -1707,7 +1722,7 @@
       <c r="E1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="22" t="s">
@@ -1716,8 +1731,11 @@
       <c r="H1" s="22" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
         <v>1.1000000000000001</v>
       </c>
@@ -1727,313 +1745,311 @@
       <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" t="s">
-        <v>87</v>
+      <c r="E2" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" s="64" t="s">
+        <v>162</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>1.2</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>164</v>
+      </c>
+      <c r="I3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
+        <v>1.3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="19">
         <v>2.1</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B5" s="14">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="66" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" s="64" t="s">
+        <v>182</v>
+      </c>
+      <c r="H5" s="64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="20">
         <v>3.1</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B6" s="15">
         <v>3</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G5" s="25"/>
-      <c r="H5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+      <c r="E6" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="H6" s="64" t="s">
+        <v>171</v>
+      </c>
+      <c r="I6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B7" s="14">
         <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="G6" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="H6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B7" s="14">
-        <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="37" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="H7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B8" s="14">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="H8" s="25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="19">
         <v>6.1</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B9" s="14">
         <v>6</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="71" t="s">
-        <v>128</v>
-      </c>
-      <c r="F8" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
+      <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
         <v>7.1</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B10" s="14">
         <v>7</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="D10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="32"/>
+    </row>
+    <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="19">
         <v>9.1</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B11" s="14">
         <v>8</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="26" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
         <v>8</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11" s="30" t="s">
+      <c r="B12" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19">
+        <v>10.1</v>
+      </c>
+      <c r="B13" s="14">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
         <v>130</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="30"/>
-    </row>
-    <row r="12" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
-        <v>10.1</v>
-      </c>
-      <c r="B12" s="14">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>146</v>
-      </c>
-      <c r="H12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="H13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
         <v>11.1</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B14" s="14">
         <v>10</v>
       </c>
-      <c r="D13" t="s">
-        <v>154</v>
-      </c>
-      <c r="E13" s="72" t="s">
-        <v>131</v>
-      </c>
-      <c r="G13" s="65"/>
-    </row>
-    <row r="14" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="D14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A15" s="19">
         <v>12.1</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B15" s="14">
         <v>11</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="72" t="s">
-        <v>132</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="G15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="19">
         <v>13.1</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B16" s="14">
         <v>12</v>
       </c>
-      <c r="D15" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="G15" s="65" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
-        <v>15.1</v>
-      </c>
-      <c r="B16" s="14">
-        <v>13</v>
-      </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="17"/>
-      <c r="G16" s="29" t="s">
-        <v>181</v>
-      </c>
+      <c r="G16" s="24"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
-        <v>16.100000000000001</v>
+        <v>15.1</v>
       </c>
       <c r="B17" s="14">
-        <v>14</v>
-      </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="H17" t="s">
-        <v>176</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="G17" s="28"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="B18" s="14">
+        <v>14</v>
+      </c>
+      <c r="F18" s="28"/>
+      <c r="G18" t="s">
+        <v>158</v>
+      </c>
+      <c r="H18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="19">
         <v>17.100000000000001</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B19" s="14">
         <v>15</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="25" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="F19" s="28"/>
+      <c r="G19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
         <v>18.100000000000001</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D19" t="s">
-        <v>179</v>
-      </c>
-      <c r="G19" s="37" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="25"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="25"/>
+      <c r="B20" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" t="s">
+        <v>159</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="28"/>
     </row>
   </sheetData>
-  <sortState ref="A21:G24">
-    <sortCondition ref="B21:B24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:G25">
+    <sortCondition ref="B22:B25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2089,44 +2105,44 @@
         <v>17</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>31</v>
+        <v>67</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="70">
+      <c r="A2" s="59">
         <v>1</v>
       </c>
       <c r="B2" s="10">
         <v>42388</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="70">
+      <c r="A3" s="59">
         <v>2</v>
       </c>
       <c r="B3" s="10">
@@ -2134,30 +2150,30 @@
         <v>42395</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="70">
+      <c r="A4" s="59">
         <v>3</v>
       </c>
       <c r="B4" s="10">
@@ -2168,80 +2184,80 @@
         <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="67" t="s">
-        <v>77</v>
+        <v>97</v>
+      </c>
+      <c r="G4" s="57" t="s">
+        <v>75</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="70">
+      <c r="A5" s="59">
         <v>4</v>
       </c>
       <c r="B5" s="10">
         <f>B4+7</f>
         <v>42409</v>
       </c>
-      <c r="C5" s="57" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="60" t="s">
-        <v>113</v>
+      <c r="C5" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>105</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="70">
+      <c r="A6" s="59">
         <v>5</v>
       </c>
       <c r="B6" s="10">
         <f t="shared" si="0"/>
         <v>42416</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="60" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="69">
+      <c r="A7" s="58">
         <v>6</v>
       </c>
       <c r="B7" s="10">
@@ -2249,30 +2265,30 @@
         <v>42423</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="55" t="s">
-        <v>39</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="69">
+      <c r="A8" s="58">
         <v>7</v>
       </c>
       <c r="B8" s="10">
@@ -2280,20 +2296,20 @@
         <v>42430</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2308,13 +2324,13 @@
         <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2351,16 +2367,16 @@
         <v>42451</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2372,22 +2388,22 @@
         <v>42458</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="57" t="s">
-        <v>162</v>
+        <v>31</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>144</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G12" s="58" t="s">
-        <v>157</v>
-      </c>
-      <c r="H12" s="57" t="s">
-        <v>158</v>
+        <v>138</v>
+      </c>
+      <c r="G12" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="H12" s="49" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2399,22 +2415,22 @@
         <v>42465</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="57" t="s">
-        <v>159</v>
-      </c>
-      <c r="G13" s="57" t="s">
-        <v>161</v>
+        <v>41</v>
+      </c>
+      <c r="F13" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="G13" s="49" t="s">
+        <v>143</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -2426,17 +2442,17 @@
         <v>42472</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="58" t="s">
-        <v>157</v>
-      </c>
-      <c r="H14" s="57" t="s">
-        <v>158</v>
+      <c r="G14" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="H14" s="49" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2463,16 +2479,16 @@
         <v>42486</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -2512,9 +2528,9 @@
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="57"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
       <c r="H23" s="1"/>
       <c r="I23" s="11"/>
     </row>
@@ -2522,8 +2538,8 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="55"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="48"/>
       <c r="H24" s="1"/>
     </row>
   </sheetData>
@@ -2534,7 +2550,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0647D9F9-0194-9C4A-8769-507350581DA1}">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:M95"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E48" sqref="E48"/>
@@ -2542,10 +2558,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="36"/>
-    <col min="2" max="2" width="35" style="36" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="36" customWidth="1"/>
-    <col min="4" max="4" width="6.375" style="36" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="14"/>
+    <col min="2" max="2" width="35" style="14" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="6.375" style="14" customWidth="1"/>
     <col min="5" max="5" width="6" style="14" customWidth="1"/>
     <col min="6" max="6" width="20.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="14" customWidth="1"/>
@@ -2555,20 +2571,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="38" t="s">
-        <v>99</v>
+      <c r="E1" s="33" t="s">
+        <v>94</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
@@ -2593,26 +2609,26 @@
       <c r="A2" s="14">
         <v>0</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D2" s="34">
         <v>4</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="41">
+      <c r="G2" s="36">
         <f>SUMIF($C$2:$C$94,F2,$D$2:$D$94)</f>
         <v>119</v>
       </c>
-      <c r="H2" s="42">
+      <c r="H2" s="37">
         <f>G2/$G$7</f>
         <v>0.268018018018018</v>
       </c>
@@ -2622,7 +2638,7 @@
       <c r="L2">
         <v>120</v>
       </c>
-      <c r="M2" s="54">
+      <c r="M2" s="47">
         <v>0.24</v>
       </c>
     </row>
@@ -2630,26 +2646,26 @@
       <c r="A3" s="14">
         <v>0</v>
       </c>
-      <c r="B3" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D3" s="34">
         <v>0</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="39">
+      <c r="G3" s="34">
         <f>SUMIF($C$2:$C$94,F3,$D$2:$D$94)</f>
         <v>80</v>
       </c>
-      <c r="H3" s="44">
+      <c r="H3" s="39">
         <f>G3/$G$7</f>
         <v>0.18018018018018017</v>
       </c>
@@ -2659,7 +2675,7 @@
       <c r="L3">
         <v>100</v>
       </c>
-      <c r="M3" s="54">
+      <c r="M3" s="47">
         <v>0.2</v>
       </c>
     </row>
@@ -2667,26 +2683,26 @@
       <c r="A4" s="14">
         <v>0</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>145</v>
-      </c>
-      <c r="C4" s="39" t="s">
+      <c r="B4" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="39">
+      <c r="D4" s="34">
         <v>8</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="61">
+      <c r="G4" s="52">
         <f>SUMIF($C$2:$C$94,F4,$D$2:$D$94)-10</f>
         <v>90</v>
       </c>
-      <c r="H4" s="63">
+      <c r="H4" s="54">
         <f>G4/$G$7</f>
         <v>0.20270270270270271</v>
       </c>
@@ -2696,7 +2712,7 @@
       <c r="L4">
         <v>200</v>
       </c>
-      <c r="M4" s="54">
+      <c r="M4" s="47">
         <v>0.4</v>
       </c>
     </row>
@@ -2704,26 +2720,26 @@
       <c r="A5" s="14">
         <v>0</v>
       </c>
-      <c r="B5" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" s="39" t="s">
+      <c r="B5" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="34">
         <v>10</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="47">
+      <c r="G5" s="42">
         <f>SUMIF($C$2:$C$94,F5,$D$2:$D$94)</f>
         <v>50</v>
       </c>
-      <c r="H5" s="48">
+      <c r="H5" s="43">
         <f>G5/$G$7</f>
         <v>0.11261261261261261</v>
       </c>
@@ -2733,7 +2749,7 @@
       <c r="L5">
         <v>80</v>
       </c>
-      <c r="M5" s="54">
+      <c r="M5" s="47">
         <v>0.16</v>
       </c>
     </row>
@@ -2741,26 +2757,26 @@
       <c r="A6" s="14">
         <v>0</v>
       </c>
-      <c r="B6" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="39" t="s">
+      <c r="B6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D6" s="34">
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="50">
+      <c r="G6" s="45">
         <f>SUMIF($C$2:$C$94,F6,$D$2:$D$94)</f>
         <v>105</v>
       </c>
-      <c r="H6" s="51">
+      <c r="H6" s="46">
         <f>G6/$G$7</f>
         <v>0.23648648648648649</v>
       </c>
@@ -2772,17 +2788,17 @@
       <c r="A7" s="14">
         <v>0</v>
       </c>
-      <c r="B7" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="39" t="s">
+      <c r="B7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="34">
         <v>0</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
@@ -2793,35 +2809,35 @@
       <c r="A8" s="14">
         <v>1</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="45" t="s">
+      <c r="B8" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="45">
+      <c r="D8" s="40">
         <v>5</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:13" s="14" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="64">
+      <c r="A9" s="55">
         <v>1.2</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="39" t="s">
+      <c r="B9" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="34">
         <v>4</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
@@ -2832,17 +2848,17 @@
       <c r="A10" s="14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B10" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="61" t="s">
+      <c r="B10" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="61">
+      <c r="D10" s="52">
         <v>10</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F10"/>
       <c r="J10"/>
@@ -2851,20 +2867,20 @@
       <c r="M10"/>
     </row>
     <row r="11" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64">
+      <c r="A11" s="55">
         <v>2</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="45" t="s">
+      <c r="B11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="40">
         <v>20</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F11"/>
       <c r="J11"/>
@@ -2873,20 +2889,20 @@
       <c r="M11"/>
     </row>
     <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="64">
+      <c r="A12" s="55">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B12" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="39" t="s">
+      <c r="B12" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="39">
+      <c r="D12" s="34">
         <v>8</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
@@ -2896,20 +2912,20 @@
       <c r="M12"/>
     </row>
     <row r="13" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="64">
+      <c r="A13" s="55">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B13" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="61" t="s">
+      <c r="B13" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="61">
+      <c r="D13" s="52">
         <v>10</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F13"/>
       <c r="G13"/>
@@ -2922,17 +2938,17 @@
       <c r="A14" s="14">
         <v>3.1</v>
       </c>
-      <c r="B14" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="45" t="s">
+      <c r="B14" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="45">
+      <c r="D14" s="40">
         <v>20</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -2945,17 +2961,17 @@
       <c r="A15" s="14">
         <v>3.2</v>
       </c>
-      <c r="B15" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="39" t="s">
+      <c r="B15" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="39">
+      <c r="D15" s="34">
         <v>8</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
@@ -2968,17 +2984,17 @@
       <c r="A16" s="14">
         <v>3.3</v>
       </c>
-      <c r="B16" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="61" t="s">
+      <c r="B16" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="61">
+      <c r="D16" s="52">
         <v>10</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -2991,17 +3007,17 @@
       <c r="A17" s="14">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B17" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="45" t="s">
+      <c r="B17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="45">
+      <c r="D17" s="40">
         <v>20</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -3014,17 +3030,17 @@
       <c r="A18" s="14">
         <v>4.2</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="39" t="s">
+      <c r="B18" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="39">
+      <c r="D18" s="34">
         <v>8</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
@@ -3037,17 +3053,17 @@
       <c r="A19" s="14">
         <v>4.3</v>
       </c>
-      <c r="B19" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="61" t="s">
+      <c r="B19" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="61">
+      <c r="D19" s="52">
         <v>10</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -3060,17 +3076,17 @@
       <c r="A20" s="14">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="47">
+      <c r="D20" s="42">
         <v>50</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F20"/>
       <c r="J20"/>
@@ -3082,8 +3098,8 @@
       <c r="A21" s="14">
         <v>6</v>
       </c>
-      <c r="B21" s="73" t="s">
-        <v>135</v>
+      <c r="B21" s="61" t="s">
+        <v>119</v>
       </c>
       <c r="F21"/>
       <c r="J21"/>
@@ -3095,17 +3111,17 @@
       <c r="A22" s="14">
         <v>6.1</v>
       </c>
-      <c r="B22" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" s="39" t="s">
+      <c r="B22" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="34">
         <v>6</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F22"/>
       <c r="J22"/>
@@ -3117,17 +3133,17 @@
       <c r="A23" s="14">
         <v>6.2</v>
       </c>
-      <c r="B23" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="C23" s="45" t="s">
+      <c r="B23" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="45">
+      <c r="D23" s="40">
         <v>3</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F23"/>
       <c r="J23"/>
@@ -3139,51 +3155,51 @@
       <c r="A24" s="14">
         <v>6.3</v>
       </c>
-      <c r="B24" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="39" t="s">
+      <c r="B24" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="39">
+      <c r="D24" s="34">
         <v>4</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>6.4</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="45">
+      <c r="D25" s="40">
         <v>15</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <v>6.5</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="61" t="s">
+      <c r="C26" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="61">
+      <c r="D26" s="52">
         <v>20</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F26"/>
       <c r="J26"/>
@@ -3195,8 +3211,8 @@
       <c r="A27" s="14">
         <v>7</v>
       </c>
-      <c r="B27" s="73" t="s">
-        <v>133</v>
+      <c r="B27" s="61" t="s">
+        <v>117</v>
       </c>
       <c r="F27"/>
       <c r="J27"/>
@@ -3208,17 +3224,17 @@
       <c r="A28" s="14">
         <v>7.1</v>
       </c>
-      <c r="B28" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" s="39" t="s">
+      <c r="B28" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="39">
+      <c r="D28" s="34">
         <v>6</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F28"/>
       <c r="J28"/>
@@ -3230,76 +3246,76 @@
       <c r="A29" s="14">
         <v>7.2</v>
       </c>
-      <c r="B29" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="C29" s="45" t="s">
+      <c r="B29" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="45">
+      <c r="D29" s="40">
         <v>3</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>7.3</v>
       </c>
-      <c r="B30" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" s="39" t="s">
+      <c r="B30" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="39">
+      <c r="D30" s="34">
         <v>4</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>7.4</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="45">
+      <c r="D31" s="40">
         <v>15</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>7.5</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="61" t="s">
+      <c r="C32" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="61">
+      <c r="D32" s="52">
         <v>20</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>8</v>
       </c>
-      <c r="B33" s="73" t="s">
-        <v>138</v>
+      <c r="B33" s="61" t="s">
+        <v>122</v>
       </c>
       <c r="F33"/>
       <c r="J33"/>
@@ -3311,17 +3327,17 @@
       <c r="A34" s="14">
         <v>8.1</v>
       </c>
-      <c r="B34" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="C34" s="39" t="s">
+      <c r="B34" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="39">
+      <c r="D34" s="34">
         <v>6</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F34"/>
       <c r="J34"/>
@@ -3333,17 +3349,17 @@
       <c r="A35" s="14">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B35" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="C35" s="45" t="s">
+      <c r="B35" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="45">
+      <c r="D35" s="40">
         <v>3</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F35"/>
       <c r="J35"/>
@@ -3355,17 +3371,17 @@
       <c r="A36" s="14">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B36" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="C36" s="39" t="s">
+      <c r="B36" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="39">
+      <c r="D36" s="34">
         <v>4</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F36"/>
       <c r="J36"/>
@@ -3377,17 +3393,17 @@
       <c r="A37" s="14">
         <v>8.4</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="45">
+      <c r="D37" s="40">
         <v>15</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F37"/>
       <c r="J37"/>
@@ -3399,17 +3415,17 @@
       <c r="A38" s="14">
         <v>8.5</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="61" t="s">
+      <c r="C38" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="61">
+      <c r="D38" s="52">
         <v>20</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F38"/>
       <c r="J38"/>
@@ -3421,61 +3437,59 @@
       <c r="A39" s="14">
         <v>10</v>
       </c>
-      <c r="B39" s="73" t="s">
+      <c r="B39" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
         <v>10.1</v>
       </c>
-      <c r="B40" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="50" t="s">
+      <c r="B40" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="50">
+      <c r="D40" s="45">
         <v>10</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
         <v>10.199999999999999</v>
       </c>
-      <c r="B41" s="71" t="s">
-        <v>139</v>
-      </c>
-      <c r="C41" s="50" t="s">
+      <c r="B41" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="50">
+      <c r="D41" s="45">
         <v>20</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
         <v>10.3</v>
       </c>
-      <c r="B42" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" s="50" t="s">
+      <c r="B42" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="50">
+      <c r="D42" s="45">
         <v>5</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -3483,19 +3497,19 @@
         <v>10.4</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="C43" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="50">
+      <c r="D43" s="45">
         <v>5</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="G43" s="14">
         <v>5</v>
@@ -3505,20 +3519,20 @@
       <c r="A44" s="14">
         <v>10.5</v>
       </c>
-      <c r="B44" s="36" t="s">
-        <v>165</v>
-      </c>
-      <c r="C44" s="50" t="s">
+      <c r="B44" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="50">
+      <c r="D44" s="45">
         <v>20</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="G44" s="14">
         <v>5</v>
@@ -3529,19 +3543,19 @@
         <v>10.7</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="C45" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="C45" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="50">
+      <c r="D45" s="45">
         <v>5</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="G45" s="14">
         <v>5</v>
@@ -3552,362 +3566,122 @@
         <v>10.4</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="C46" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="50">
+      <c r="D46" s="45">
         <v>5</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="G46" s="14">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
       <c r="B47" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="C47" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="50">
+      <c r="D47" s="45">
         <v>30</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="C48" s="50" t="s">
+      <c r="B48" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="50">
+      <c r="D48" s="45">
         <v>5</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="G48" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="G49" s="14">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="68"/>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="G50" s="14">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="68"/>
+    <row r="51" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="G51" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="68"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="68"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="68"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="68"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="68"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="68"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="68"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="68"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="68"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="68"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="68"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="68"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="68"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="68"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="68"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="68"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="68"/>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="52"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="36"/>
-      <c r="H69" s="36"/>
-      <c r="I69" s="36"/>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="52"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="36"/>
-      <c r="H70" s="36"/>
-      <c r="I70" s="36"/>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="68"/>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="68"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="68"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="68"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="68"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="68"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A78" s="14"/>
-      <c r="B78" s="14"/>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
-      <c r="B79" s="14"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
-    </row>
-    <row r="80" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F80"/>
       <c r="J80"/>
       <c r="K80"/>
       <c r="L80"/>
       <c r="M80"/>
     </row>
-    <row r="81" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F81"/>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81"/>
       <c r="M81"/>
     </row>
-    <row r="82" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="52"/>
-      <c r="B82" s="52"/>
-      <c r="C82" s="52"/>
-      <c r="D82" s="52"/>
+    <row r="82" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F82"/>
       <c r="J82"/>
       <c r="K82"/>
       <c r="L82"/>
       <c r="M82"/>
     </row>
-    <row r="83" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="52"/>
-      <c r="B83" s="52"/>
-      <c r="C83" s="52"/>
-      <c r="D83" s="52"/>
-      <c r="E83" s="36"/>
+    <row r="83" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F83"/>
       <c r="J83"/>
       <c r="K83"/>
       <c r="L83"/>
       <c r="M83"/>
     </row>
-    <row r="84" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="52"/>
-      <c r="B84" s="52"/>
-      <c r="C84" s="52"/>
-      <c r="D84" s="52"/>
-      <c r="E84" s="36"/>
+    <row r="84" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F84"/>
       <c r="J84"/>
       <c r="K84"/>
       <c r="L84"/>
       <c r="M84"/>
     </row>
-    <row r="85" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="52"/>
-      <c r="B85" s="52"/>
-      <c r="C85" s="52"/>
-      <c r="D85" s="52"/>
-      <c r="E85" s="36"/>
+    <row r="85" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F85"/>
       <c r="J85"/>
       <c r="K85"/>
       <c r="L85"/>
       <c r="M85"/>
     </row>
-    <row r="86" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="52"/>
-      <c r="B86" s="52"/>
-      <c r="C86" s="52"/>
-      <c r="D86" s="52"/>
+    <row r="86" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F86"/>
       <c r="G86"/>
       <c r="H86"/>
@@ -3916,22 +3690,14 @@
       <c r="L86"/>
       <c r="M86"/>
     </row>
-    <row r="87" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="52"/>
-      <c r="B87" s="52"/>
-      <c r="C87" s="52"/>
-      <c r="D87" s="52"/>
+    <row r="87" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F87"/>
       <c r="J87"/>
       <c r="K87"/>
       <c r="L87"/>
       <c r="M87"/>
     </row>
-    <row r="88" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="52"/>
-      <c r="B88" s="52"/>
-      <c r="C88" s="52"/>
-      <c r="D88" s="52"/>
+    <row r="88" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F88"/>
       <c r="G88"/>
       <c r="H88"/>
@@ -3940,11 +3706,7 @@
       <c r="L88"/>
       <c r="M88"/>
     </row>
-    <row r="89" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="52"/>
-      <c r="B89" s="52"/>
-      <c r="C89" s="52"/>
-      <c r="D89" s="52"/>
+    <row r="89" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F89"/>
       <c r="G89"/>
       <c r="H89"/>
@@ -3953,11 +3715,7 @@
       <c r="L89"/>
       <c r="M89"/>
     </row>
-    <row r="90" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="52"/>
-      <c r="B90" s="52"/>
-      <c r="C90" s="52"/>
-      <c r="D90" s="52"/>
+    <row r="90" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F90"/>
       <c r="G90"/>
       <c r="H90"/>
@@ -3966,11 +3724,7 @@
       <c r="L90"/>
       <c r="M90"/>
     </row>
-    <row r="91" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="52"/>
-      <c r="B91" s="52"/>
-      <c r="C91" s="52"/>
-      <c r="D91" s="52"/>
+    <row r="91" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F91"/>
       <c r="G91"/>
       <c r="H91"/>
@@ -3979,11 +3733,7 @@
       <c r="L91"/>
       <c r="M91"/>
     </row>
-    <row r="92" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="52"/>
-      <c r="B92" s="52"/>
-      <c r="C92" s="52"/>
-      <c r="D92" s="52"/>
+    <row r="92" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F92"/>
       <c r="G92"/>
       <c r="H92"/>
@@ -3992,11 +3742,7 @@
       <c r="L92"/>
       <c r="M92"/>
     </row>
-    <row r="93" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="52"/>
-      <c r="B93" s="52"/>
-      <c r="C93" s="52"/>
-      <c r="D93" s="52"/>
+    <row r="93" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F93"/>
       <c r="G93"/>
       <c r="H93"/>
@@ -4005,11 +3751,7 @@
       <c r="L93"/>
       <c r="M93"/>
     </row>
-    <row r="94" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="52"/>
-      <c r="B94" s="52"/>
-      <c r="C94" s="52"/>
-      <c r="D94" s="52"/>
+    <row r="94" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F94"/>
       <c r="G94"/>
       <c r="H94"/>
@@ -4018,11 +3760,7 @@
       <c r="L94"/>
       <c r="M94"/>
     </row>
-    <row r="95" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="52"/>
-      <c r="B95" s="52"/>
-      <c r="C95" s="52"/>
-      <c r="D95" s="52"/>
+    <row r="95" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F95"/>
       <c r="G95"/>
       <c r="H95"/>
@@ -4031,55 +3769,8 @@
       <c r="L95"/>
       <c r="M95"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A96" s="52"/>
-      <c r="B96" s="52"/>
-      <c r="C96" s="52"/>
-      <c r="D96" s="52"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="52"/>
-      <c r="B97" s="52"/>
-      <c r="C97" s="52"/>
-      <c r="D97" s="52"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="52"/>
-      <c r="B98" s="52"/>
-      <c r="C98" s="52"/>
-      <c r="D98" s="52"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="52"/>
-      <c r="B99" s="52"/>
-      <c r="C99" s="52"/>
-      <c r="D99" s="52"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="52"/>
-      <c r="B100" s="52"/>
-      <c r="C100" s="52"/>
-      <c r="D100" s="52"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="52"/>
-      <c r="B101" s="52"/>
-      <c r="C101" s="52"/>
-      <c r="D101" s="52"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="52"/>
-      <c r="B102" s="52"/>
-      <c r="C102" s="52"/>
-      <c r="D102" s="52"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="53"/>
-      <c r="B103" s="53"/>
-      <c r="D103" s="53"/>
-    </row>
   </sheetData>
-  <sortState ref="A2:D110">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D110">
     <sortCondition ref="A2:A110"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revamp assignments to include canvas stuff
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7623C6-F6C9-4A27-9C4D-504A964B3692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A02525-D964-48DE-AD0D-A17901972608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35220" yWindow="2445" windowWidth="16380" windowHeight="13305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="180">
   <si>
     <t>Finals Week</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Factor Analysis</t>
   </si>
   <si>
-    <t>Midterm / Project Updates</t>
-  </si>
-  <si>
     <t>Project Presentations</t>
   </si>
   <si>
@@ -248,9 +245,6 @@
     <t>Classification and Prediction</t>
   </si>
   <si>
-    <t>Generalized Linear Models</t>
-  </si>
-  <si>
     <t>Preparing Data for Analysis</t>
   </si>
   <si>
@@ -298,9 +292,6 @@
   </si>
   <si>
     <t>Class logistics, Data preparation review</t>
-  </si>
-  <si>
-    <t>Review project webpage</t>
   </si>
   <si>
     <t xml:space="preserve">Introduction to the instructor, class structure, materials, requirements, expectations and resources. </t>
@@ -448,10 +439,6 @@
     <t>finals</t>
   </si>
   <si>
-    <t>PMA6 CH12.1-12.8  
-ASCN Ch9.1-9.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">install packages: mice, VIM
 Seminar on Missing Data: https://media.csuchico.edu/media/0_tgnydpgf </t>
   </si>
@@ -461,9 +448,6 @@
 [FIMD](https://stefvanbuuren.name/fimd/)</t>
   </si>
   <si>
-    <t>[[Quiz 03]](https://forms.gle/iAHo9yiLrjp8v5266)  (Due 3/5)</t>
-  </si>
-  <si>
     <t>PMA6 CH 14
 ASCN Ch 13</t>
   </si>
@@ -511,12 +495,6 @@
     <t>CC / OH (1 per topic)</t>
   </si>
   <si>
-    <t>Project update presentations</t>
-  </si>
-  <si>
-    <t>[[Project update]](project.html#project_update) (Due  03/27 )</t>
-  </si>
-  <si>
     <t>Covid19 Campus Closed</t>
   </si>
   <si>
@@ -530,9 +508,6 @@
   </si>
   <si>
     <t>Principal Component Analysis</t>
-  </si>
-  <si>
-    <t>HW 04: Dimension Reduction [[HTML]](hw/hw04-dimension-reduction.html)[[PDF]](hw/hw04-dimension-reduction.pdf)[[RMD]](hw/hw04-dimension-reduction.Rmd)</t>
   </si>
   <si>
     <t xml:space="preserve">Start watching the PCA videos loaded into Google Drive. Follow along with the course notes and book. 
@@ -565,9 +540,6 @@
 </t>
   </si>
   <si>
-    <t>[[Quiz 04]](https://forms.gle/mirjk4xDsFk8HtHQA) (Due 4/9 )</t>
-  </si>
-  <si>
     <t>Presentation slides draft</t>
   </si>
   <si>
@@ -601,33 +573,7 @@
     <t>smoothness of presentation</t>
   </si>
   <si>
-    <t>[[Presentation slides Draft]](https://norcalbiostat.github.io/MATH456/project.html#draft_slides) (Due 4/27 PR 4/29)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Groups check in with Dr. D. </t>
-  </si>
-  <si>
-    <t>Thursday 2-4pm, OR Friday 12-2pm</t>
-  </si>
-  <si>
     <t xml:space="preserve">Have fun! Relax, rejuvinate yourself. </t>
-  </si>
-  <si>
-    <t>PMA6 Ch 8, 10.3
-ASCN Ch 9</t>
-  </si>
-  <si>
-    <t>[[HW 00: Getting Started]](hw/hw00-getting-started.html) (Due 01/27 ) (PR 01/30)</t>
-  </si>
-  <si>
-    <t>Proposal due for approval (Due Sat 2/4)</t>
-  </si>
-  <si>
-    <t>PMA6 Ch 3
-ASCN Ch 1</t>
-  </si>
-  <si>
-    <t>Review of Simple Linear Regression</t>
   </si>
   <si>
     <t>In class activities</t>
@@ -643,51 +589,90 @@
     <t>QFT</t>
   </si>
   <si>
-    <t>[Project selection]() (Due 2/15 )</t>
-  </si>
-  <si>
-    <t>Recruitment video created (Due Sat 2/11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMA6 Ch8, 10.1-10.3   
-ASCN Ch9-10
-</t>
-  </si>
-  <si>
-    <t>PMA6 Ch9-Ch10   
-ASCN Ch 10.6-10.7</t>
-  </si>
-  <si>
-    <t>See project page for details   
-[[Project Scoring]]()  
-[[Team member evaluation]]()</t>
-  </si>
-  <si>
-    <t>[[Quiz 00]](https://forms.gle/mizdZk4qw8QC5NXT8)(Due 01/24 )</t>
-  </si>
-  <si>
-    <t>[[Quiz 01]](https://forms.gle/xXoyigprJXnDd5Sn8) (Due 02/02/12 )</t>
-  </si>
-  <si>
-    <t>[[Quiz 02]]()  (Due 2/XX)</t>
-  </si>
-  <si>
-    <t>[[HW 02: GLM and Classification]](hw/hw02-glm-classification.html) (Draft 02/xx, PR 02/xx, Final 02/xx )
-LJ Check in (Due 2/xx )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project timeline &amp; Team Agreements (Due 2/26 )  </t>
-  </si>
-  <si>
     <t>Midterm  
 LJ Check in</t>
   </si>
   <si>
-    <t>[HW 03 : Missing Data [[Instructions]](hw/hw03-missing-data.html) [[RMD]](hw/hw03-missing-data-template.Rmd)   
- (Draft 03/xx, PR 03/xx, Final 03/xx )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[[HW 01: Statistical Modeling]](hw/hw01-model-building.html) (Draft 02/12, PR 02/14, Final 02/18 ) </t>
+    <t>[[HW 00: Getting Started]](hw/hw00-getting-started.html)</t>
+  </si>
+  <si>
+    <t>[[HW 01: Statistical Modeling]](hw/hw01-model-building.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midterm </t>
+  </si>
+  <si>
+    <t>Model Building</t>
+  </si>
+  <si>
+    <t>Special Topic 1</t>
+  </si>
+  <si>
+    <t>Special Topic 2</t>
+  </si>
+  <si>
+    <t>Final Exam</t>
+  </si>
+  <si>
+    <t>HW05</t>
+  </si>
+  <si>
+    <t>HW 06</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>LJ Check in</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 3  
+ASCN Ch 1</t>
+  </si>
+  <si>
+    <t>ASCN Ch 8</t>
+  </si>
+  <si>
+    <t>Review of Linear Regression</t>
+  </si>
+  <si>
+    <t>ASCN Ch 7, 9</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 12  
+ASCN Ch 11.1-11.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ASCN Ch 10.4-10.5</t>
+  </si>
+  <si>
+    <t>PMA6 Ch9-Ch10   
+ASCN Ch 10</t>
+  </si>
+  <si>
+    <t>Interaction Terms</t>
+  </si>
+  <si>
+    <t>Stratification, Moderation</t>
+  </si>
+  <si>
+    <t>ASCN Ch 10.1</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>HW04</t>
+  </si>
+  <si>
+    <t>HW 03</t>
+  </si>
+  <si>
+    <t>HW 02</t>
+  </si>
+  <si>
+    <t>[[Quiz 01]](https://forms.gle/mizdZk4qw8QC5NXT8)</t>
   </si>
 </sst>
 </file>
@@ -836,8 +821,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1088,7 +1074,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1126,9 +1112,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="81" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1136,46 +1119,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="81" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="81" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="81"/>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="81" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1249,9 +1200,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1265,9 +1213,58 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="81" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="81" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="81" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="81" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="81" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1689,367 +1686,392 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.875" style="14"/>
-    <col min="3" max="3" width="5.625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.875" customWidth="1"/>
-    <col min="5" max="5" width="11.125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="18" style="24" customWidth="1"/>
-    <col min="7" max="7" width="19.375" customWidth="1"/>
-    <col min="8" max="8" width="21.125" customWidth="1"/>
+    <col min="1" max="2" width="8.875" style="57"/>
+    <col min="3" max="3" width="5.625" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" style="59" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="57" customWidth="1"/>
+    <col min="6" max="6" width="18" style="60" customWidth="1"/>
+    <col min="7" max="7" width="19.375" style="59" customWidth="1"/>
+    <col min="8" max="16384" width="8.875" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:8" s="57" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="56" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="58">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B2" s="57">
+        <v>1</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="58">
+        <v>1.2</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="58">
+        <v>1.3</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="H4" s="60" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="58">
+        <v>2.1</v>
+      </c>
+      <c r="B5" s="57">
+        <v>2</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="49"/>
+      <c r="G5" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="61" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" s="49"/>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>3.1</v>
+      </c>
+      <c r="B7" s="14">
+        <v>3</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" s="49"/>
+      <c r="G7" s="50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="58">
+        <v>3.2</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="59" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="58">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B9" s="57">
+        <v>4</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>169</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="62" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="58">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B10" s="57">
+        <v>5</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="57">
+        <v>6.1</v>
+      </c>
+      <c r="B11" s="57">
+        <v>6</v>
+      </c>
+      <c r="D11" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="62" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="58">
+        <v>7.1</v>
+      </c>
+      <c r="B12" s="57">
+        <v>7</v>
+      </c>
+      <c r="D12" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="58">
+        <v>8</v>
+      </c>
+      <c r="B13" s="57">
+        <v>8</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="62" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="58">
+        <v>9</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="66" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" s="67"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="66"/>
+    </row>
+    <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="58">
+        <v>10.1</v>
+      </c>
+      <c r="B15" s="57">
+        <v>9</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="69" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="62" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="58">
+        <v>11.1</v>
+      </c>
+      <c r="B16" s="57">
+        <v>10</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="69" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="70"/>
+      <c r="G16" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="58">
+        <v>12.1</v>
+      </c>
+      <c r="B17" s="57">
+        <v>11</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" s="69"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="62" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="58">
+        <v>13.1</v>
+      </c>
+      <c r="B18" s="57">
+        <v>12</v>
+      </c>
+      <c r="D18" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="69"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="58">
+        <v>14.1</v>
+      </c>
+      <c r="B19" s="57">
+        <v>13</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="70" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="58">
+        <v>15.1</v>
+      </c>
+      <c r="B20" s="57">
         <v>14</v>
       </c>
-      <c r="I1" s="22" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B2" s="14">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="62" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="63" t="s">
+      <c r="D20" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="E20" s="63"/>
+      <c r="G20" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="58">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="B21" s="57">
+        <v>15</v>
+      </c>
+      <c r="D21" s="71" t="s">
         <v>175</v>
       </c>
-      <c r="G2" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="H2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
-        <v>1.2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="65" t="s">
+      <c r="E21" s="63"/>
+      <c r="G21" s="70"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="58">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="B22" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="F22" s="57"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="62"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G23" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="I3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
-        <v>1.3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>161</v>
-      </c>
-      <c r="I4" s="24" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="19">
-        <v>2.1</v>
-      </c>
-      <c r="B5" s="14">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="66" t="s">
-        <v>172</v>
-      </c>
-      <c r="F5" s="63" t="s">
-        <v>176</v>
-      </c>
-      <c r="G5" s="64" t="s">
-        <v>182</v>
-      </c>
-      <c r="H5" s="64" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
-        <v>3.1</v>
-      </c>
-      <c r="B6" s="15">
-        <v>3</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="66" t="s">
-        <v>173</v>
-      </c>
-      <c r="H6" s="64" t="s">
-        <v>171</v>
-      </c>
-      <c r="I6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B7" s="14">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="H7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B8" s="14">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="H8" s="25" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
-        <v>6.1</v>
-      </c>
-      <c r="B9" s="14">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="56" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
-        <v>7.1</v>
-      </c>
-      <c r="B10" s="14">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="F10" s="32"/>
-    </row>
-    <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
-        <v>9.1</v>
-      </c>
-      <c r="B11" s="14">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="25" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
-        <v>8</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="29"/>
-    </row>
-    <row r="13" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
-        <v>10.1</v>
-      </c>
-      <c r="B13" s="14">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>130</v>
-      </c>
-      <c r="H13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
-        <v>11.1</v>
-      </c>
-      <c r="B14" s="14">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E14" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="G14" s="24"/>
-    </row>
-    <row r="15" spans="1:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
-        <v>12.1</v>
-      </c>
-      <c r="B15" s="14">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="G15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
-        <v>13.1</v>
-      </c>
-      <c r="B16" s="14">
-        <v>12</v>
-      </c>
-      <c r="G16" s="24"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
-        <v>15.1</v>
-      </c>
-      <c r="B17" s="14">
-        <v>13</v>
-      </c>
-      <c r="E17" s="17"/>
-      <c r="G17" s="28"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="B18" s="14">
-        <v>14</v>
-      </c>
-      <c r="F18" s="28"/>
-      <c r="G18" t="s">
-        <v>158</v>
-      </c>
-      <c r="H18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="B19" s="14">
-        <v>15</v>
-      </c>
-      <c r="F19" s="28"/>
-      <c r="G19" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" t="s">
-        <v>159</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F25" s="28"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F27" s="70"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:G25">
-    <sortCondition ref="B22:B25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A24:G27">
+    <sortCondition ref="B24:B27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2104,45 +2126,45 @@
       <c r="H1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="J1" s="27" t="s">
+      <c r="I1" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="59">
+      <c r="A2" s="46">
         <v>1</v>
       </c>
       <c r="B2" s="10">
         <v>42388</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="59">
+      <c r="A3" s="46">
         <v>2</v>
       </c>
       <c r="B3" s="10">
@@ -2150,30 +2172,30 @@
         <v>42395</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="59">
+      <c r="A4" s="46">
         <v>3</v>
       </c>
       <c r="B4" s="10">
@@ -2184,80 +2206,80 @@
         <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G4" s="57" t="s">
-        <v>75</v>
+        <v>94</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>72</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="59">
+      <c r="A5" s="46">
         <v>4</v>
       </c>
       <c r="B5" s="10">
         <f>B4+7</f>
         <v>42409</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="I5" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="59">
+      <c r="A6" s="46">
         <v>5</v>
       </c>
       <c r="B6" s="10">
         <f t="shared" si="0"/>
         <v>42416</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>51</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="58">
+      <c r="A7" s="45">
         <v>6</v>
       </c>
       <c r="B7" s="10">
@@ -2268,27 +2290,27 @@
         <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="35" t="s">
         <v>38</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="58">
+      <c r="A8" s="45">
         <v>7</v>
       </c>
       <c r="B8" s="10">
@@ -2296,16 +2318,16 @@
         <v>42430</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
@@ -2324,13 +2346,13 @@
         <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2367,16 +2389,16 @@
         <v>42451</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2393,17 +2415,17 @@
       <c r="D12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="49" t="s">
-        <v>144</v>
+      <c r="E12" s="36" t="s">
+        <v>136</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G12" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="H12" s="49" t="s">
-        <v>140</v>
+        <v>130</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2423,14 +2445,14 @@
       <c r="E13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="G13" s="49" t="s">
-        <v>143</v>
+      <c r="F13" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>135</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -2442,17 +2464,17 @@
         <v>42472</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="H14" s="49" t="s">
-        <v>140</v>
+      <c r="G14" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2479,16 +2501,16 @@
         <v>42486</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -2528,9 +2550,9 @@
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
       <c r="H23" s="1"/>
       <c r="I23" s="11"/>
     </row>
@@ -2538,8 +2560,8 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="48"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="35"/>
       <c r="H24" s="1"/>
     </row>
   </sheetData>
@@ -2558,33 +2580,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="14"/>
-    <col min="2" max="2" width="35" style="14" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="6.375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="6" style="14" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="13"/>
+    <col min="2" max="2" width="35" style="13" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="6.375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="6" style="13" customWidth="1"/>
     <col min="6" max="6" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="14" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="14"/>
-    <col min="9" max="9" width="4.625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="10" style="13" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="13"/>
+    <col min="9" max="9" width="4.625" style="13" customWidth="1"/>
     <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="33" t="s">
-        <v>94</v>
+      <c r="E1" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
@@ -2606,29 +2628,29 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="13">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="21">
         <v>4</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="36">
+      <c r="G2" s="23">
         <f>SUMIF($C$2:$C$94,F2,$D$2:$D$94)</f>
         <v>119</v>
       </c>
-      <c r="H2" s="37">
+      <c r="H2" s="24">
         <f>G2/$G$7</f>
         <v>0.268018018018018</v>
       </c>
@@ -2638,34 +2660,34 @@
       <c r="L2">
         <v>120</v>
       </c>
-      <c r="M2" s="47">
+      <c r="M2" s="34">
         <v>0.24</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="13">
         <v>0</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="34">
+      <c r="D3" s="21">
         <v>0</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="38" t="s">
+      <c r="E3" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="34">
+      <c r="G3" s="21">
         <f>SUMIF($C$2:$C$94,F3,$D$2:$D$94)</f>
         <v>80</v>
       </c>
-      <c r="H3" s="39">
+      <c r="H3" s="26">
         <f>G3/$G$7</f>
         <v>0.18018018018018017</v>
       </c>
@@ -2675,34 +2697,34 @@
       <c r="L3">
         <v>100</v>
       </c>
-      <c r="M3" s="47">
+      <c r="M3" s="34">
         <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="A4" s="13">
         <v>0</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="34" t="s">
+      <c r="B4" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="21">
         <v>8</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="53" t="s">
+      <c r="E4" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="52">
+      <c r="G4" s="39">
         <f>SUMIF($C$2:$C$94,F4,$D$2:$D$94)-10</f>
         <v>90</v>
       </c>
-      <c r="H4" s="54">
+      <c r="H4" s="41">
         <f>G4/$G$7</f>
         <v>0.20270270270270271</v>
       </c>
@@ -2712,34 +2734,34 @@
       <c r="L4">
         <v>200</v>
       </c>
-      <c r="M4" s="47">
+      <c r="M4" s="34">
         <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
         <v>0</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="34" t="s">
+      <c r="B5" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="21">
         <v>10</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="41" t="s">
+      <c r="E5" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="42">
+      <c r="G5" s="29">
         <f>SUMIF($C$2:$C$94,F5,$D$2:$D$94)</f>
         <v>50</v>
       </c>
-      <c r="H5" s="43">
+      <c r="H5" s="30">
         <f>G5/$G$7</f>
         <v>0.11261261261261261</v>
       </c>
@@ -2749,34 +2771,34 @@
       <c r="L5">
         <v>80</v>
       </c>
-      <c r="M5" s="47">
+      <c r="M5" s="34">
         <v>0.16</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="A6" s="13">
         <v>0</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="34" t="s">
+      <c r="B6" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="21">
         <v>0</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" s="44" t="s">
+      <c r="E6" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="45">
+      <c r="G6" s="32">
         <f>SUMIF($C$2:$C$94,F6,$D$2:$D$94)</f>
         <v>105</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="33">
         <f>G6/$G$7</f>
         <v>0.23648648648648649</v>
       </c>
@@ -2785,20 +2807,20 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
+      <c r="A7" s="13">
         <v>0</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="34" t="s">
+      <c r="B7" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="21">
         <v>0</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>95</v>
+      <c r="E7" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
@@ -2806,59 +2828,59 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <v>1</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="40" t="s">
+      <c r="B8" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="27">
         <v>5</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>95</v>
+      <c r="E8" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:13" s="14" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55">
+    <row r="9" spans="1:13" s="13" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="42">
         <v>1.2</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="34" t="s">
+      <c r="B9" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="21">
         <v>4</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>95</v>
+      <c r="E9" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+    <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="52" t="s">
+      <c r="B10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="52">
+      <c r="D10" s="39">
         <v>10</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>95</v>
+      <c r="E10" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F10"/>
       <c r="J10"/>
@@ -2866,21 +2888,21 @@
       <c r="L10"/>
       <c r="M10"/>
     </row>
-    <row r="11" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="55">
+    <row r="11" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="42">
         <v>2</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="40" t="s">
+      <c r="B11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="27">
         <v>20</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>95</v>
+      <c r="E11" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F11"/>
       <c r="J11"/>
@@ -2888,21 +2910,21 @@
       <c r="L11"/>
       <c r="M11"/>
     </row>
-    <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="55">
+    <row r="12" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="42">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="34" t="s">
+      <c r="B12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="21">
         <v>8</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>95</v>
+      <c r="E12" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
@@ -2911,21 +2933,21 @@
       <c r="L12"/>
       <c r="M12"/>
     </row>
-    <row r="13" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="55">
+    <row r="13" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="42">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="52" t="s">
+      <c r="B13" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="52">
+      <c r="D13" s="39">
         <v>10</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>95</v>
+      <c r="E13" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F13"/>
       <c r="G13"/>
@@ -2934,21 +2956,21 @@
       <c r="L13"/>
       <c r="M13"/>
     </row>
-    <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+    <row r="14" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
         <v>3.1</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="40" t="s">
+      <c r="B14" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="40">
+      <c r="D14" s="27">
         <v>20</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>95</v>
+      <c r="E14" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -2957,21 +2979,21 @@
       <c r="L14"/>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+    <row r="15" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
         <v>3.2</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="34" t="s">
+      <c r="B15" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="21">
         <v>8</v>
       </c>
-      <c r="E15" s="14" t="s">
-        <v>95</v>
+      <c r="E15" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
@@ -2980,21 +3002,21 @@
       <c r="L15"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
+    <row r="16" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
         <v>3.3</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="52" t="s">
+      <c r="B16" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="52">
+      <c r="D16" s="39">
         <v>10</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>95</v>
+      <c r="E16" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -3003,21 +3025,21 @@
       <c r="L16"/>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+    <row r="17" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="40" t="s">
+      <c r="B17" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="27">
         <v>20</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>95</v>
+      <c r="E17" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -3026,21 +3048,21 @@
       <c r="L17"/>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
+    <row r="18" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
         <v>4.2</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="21">
         <v>8</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>95</v>
+      <c r="E18" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
@@ -3049,21 +3071,21 @@
       <c r="L18"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+    <row r="19" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
         <v>4.3</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="52" t="s">
+      <c r="B19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="52">
+      <c r="D19" s="39">
         <v>10</v>
       </c>
-      <c r="E19" s="14" t="s">
-        <v>95</v>
+      <c r="E19" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -3072,21 +3094,21 @@
       <c r="L19"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
+    <row r="20" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="29">
         <v>50</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>95</v>
+      <c r="E20" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F20"/>
       <c r="J20"/>
@@ -3094,12 +3116,12 @@
       <c r="L20"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
+    <row r="21" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
         <v>6</v>
       </c>
-      <c r="B21" s="61" t="s">
-        <v>119</v>
+      <c r="B21" s="47" t="s">
+        <v>114</v>
       </c>
       <c r="F21"/>
       <c r="J21"/>
@@ -3107,21 +3129,21 @@
       <c r="L21"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
+    <row r="22" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
         <v>6.1</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22" s="34" t="s">
+      <c r="B22" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="34">
+      <c r="D22" s="21">
         <v>6</v>
       </c>
-      <c r="E22" s="14" t="s">
-        <v>95</v>
+      <c r="E22" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F22"/>
       <c r="J22"/>
@@ -3129,21 +3151,21 @@
       <c r="L22"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
+    <row r="23" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
         <v>6.2</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C23" s="40" t="s">
+      <c r="B23" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="27">
         <v>3</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>95</v>
+      <c r="E23" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F23"/>
       <c r="J23"/>
@@ -3152,54 +3174,54 @@
       <c r="M23"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
+      <c r="A24" s="13">
         <v>6.3</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C24" s="34" t="s">
+      <c r="B24" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="34">
+      <c r="D24" s="21">
         <v>4</v>
       </c>
-      <c r="E24" s="14" t="s">
-        <v>95</v>
+      <c r="E24" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
+      <c r="A25" s="13">
         <v>6.4</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="40">
+      <c r="D25" s="27">
         <v>15</v>
       </c>
-      <c r="E25" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
+      <c r="E25" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
         <v>6.5</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="52">
+      <c r="D26" s="39">
         <v>20</v>
       </c>
-      <c r="E26" s="14" t="s">
-        <v>95</v>
+      <c r="E26" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F26"/>
       <c r="J26"/>
@@ -3207,12 +3229,12 @@
       <c r="L26"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
+    <row r="27" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
         <v>7</v>
       </c>
-      <c r="B27" s="61" t="s">
-        <v>117</v>
+      <c r="B27" s="47" t="s">
+        <v>112</v>
       </c>
       <c r="F27"/>
       <c r="J27"/>
@@ -3220,21 +3242,21 @@
       <c r="L27"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
+    <row r="28" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
         <v>7.1</v>
       </c>
-      <c r="B28" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C28" s="34" t="s">
+      <c r="B28" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28" s="21">
         <v>6</v>
       </c>
-      <c r="E28" s="14" t="s">
-        <v>95</v>
+      <c r="E28" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F28"/>
       <c r="J28"/>
@@ -3243,79 +3265,79 @@
       <c r="M28"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
+      <c r="A29" s="13">
         <v>7.2</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="40" t="s">
+      <c r="B29" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="40">
+      <c r="D29" s="27">
         <v>3</v>
       </c>
-      <c r="E29" s="14" t="s">
-        <v>95</v>
+      <c r="E29" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
+      <c r="A30" s="13">
         <v>7.3</v>
       </c>
-      <c r="B30" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C30" s="34" t="s">
+      <c r="B30" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="34">
+      <c r="D30" s="21">
         <v>4</v>
       </c>
-      <c r="E30" s="14" t="s">
-        <v>95</v>
+      <c r="E30" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
+      <c r="A31" s="13">
         <v>7.4</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="40">
+      <c r="D31" s="27">
         <v>15</v>
       </c>
-      <c r="E31" s="14" t="s">
-        <v>95</v>
+      <c r="E31" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="14">
+      <c r="A32" s="13">
         <v>7.5</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="52">
+      <c r="D32" s="39">
         <v>20</v>
       </c>
-      <c r="E32" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
+      <c r="E32" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
         <v>8</v>
       </c>
-      <c r="B33" s="61" t="s">
-        <v>122</v>
+      <c r="B33" s="47" t="s">
+        <v>117</v>
       </c>
       <c r="F33"/>
       <c r="J33"/>
@@ -3323,21 +3345,21 @@
       <c r="L33"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
+    <row r="34" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
         <v>8.1</v>
       </c>
-      <c r="B34" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C34" s="34" t="s">
+      <c r="B34" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="34">
+      <c r="D34" s="21">
         <v>6</v>
       </c>
-      <c r="E34" s="14" t="s">
-        <v>95</v>
+      <c r="E34" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F34"/>
       <c r="J34"/>
@@ -3345,21 +3367,21 @@
       <c r="L34"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
+    <row r="35" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B35" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" s="40" t="s">
+      <c r="B35" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="40">
+      <c r="D35" s="27">
         <v>3</v>
       </c>
-      <c r="E35" s="14" t="s">
-        <v>95</v>
+      <c r="E35" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F35"/>
       <c r="J35"/>
@@ -3367,21 +3389,21 @@
       <c r="L35"/>
       <c r="M35"/>
     </row>
-    <row r="36" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
+    <row r="36" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B36" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36" s="34" t="s">
+      <c r="B36" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="34">
+      <c r="D36" s="21">
         <v>4</v>
       </c>
-      <c r="E36" s="14" t="s">
-        <v>95</v>
+      <c r="E36" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F36"/>
       <c r="J36"/>
@@ -3389,21 +3411,21 @@
       <c r="L36"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14">
+    <row r="37" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
         <v>8.4</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="40" t="s">
+      <c r="C37" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="40">
+      <c r="D37" s="27">
         <v>15</v>
       </c>
-      <c r="E37" s="14" t="s">
-        <v>95</v>
+      <c r="E37" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F37"/>
       <c r="J37"/>
@@ -3411,21 +3433,21 @@
       <c r="L37"/>
       <c r="M37"/>
     </row>
-    <row r="38" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14">
+    <row r="38" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13">
         <v>8.5</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="52" t="s">
+      <c r="C38" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="52">
+      <c r="D38" s="39">
         <v>20</v>
       </c>
-      <c r="E38" s="14" t="s">
-        <v>95</v>
+      <c r="E38" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="F38"/>
       <c r="J38"/>
@@ -3434,254 +3456,254 @@
       <c r="M38"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="14">
+      <c r="A39" s="13">
         <v>10</v>
       </c>
-      <c r="B39" s="61" t="s">
+      <c r="B39" s="47" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
+      <c r="A40" s="13">
         <v>10.1</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="C40" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="45">
+      <c r="D40" s="32">
         <v>10</v>
       </c>
-      <c r="E40" s="14" t="s">
-        <v>95</v>
+      <c r="E40" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="14">
+      <c r="A41" s="13">
         <v>10.199999999999999</v>
       </c>
-      <c r="B41" s="56" t="s">
-        <v>123</v>
-      </c>
-      <c r="C41" s="45" t="s">
+      <c r="B41" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="45">
+      <c r="D41" s="32">
         <v>20</v>
       </c>
-      <c r="E41" s="14" t="s">
-        <v>95</v>
+      <c r="E41" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="14">
+      <c r="A42" s="13">
         <v>10.3</v>
       </c>
-      <c r="B42" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="C42" s="45" t="s">
+      <c r="B42" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="45">
+      <c r="D42" s="32">
         <v>5</v>
       </c>
-      <c r="E42" s="14" t="s">
-        <v>95</v>
+      <c r="E42" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="14">
+      <c r="A43" s="13">
         <v>10.4</v>
       </c>
-      <c r="B43" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C43" s="45" t="s">
+      <c r="B43" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="45">
+      <c r="D43" s="32">
         <v>5</v>
       </c>
-      <c r="E43" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="G43" s="14">
+      <c r="E43" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="G43" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="14">
+      <c r="A44" s="13">
         <v>10.5</v>
       </c>
-      <c r="B44" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44" s="45" t="s">
+      <c r="B44" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="45">
+      <c r="D44" s="32">
         <v>20</v>
       </c>
-      <c r="E44" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G44" s="14">
+      <c r="E44" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G44" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="14">
+      <c r="A45" s="13">
         <v>10.7</v>
       </c>
-      <c r="B45" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="C45" s="45" t="s">
+      <c r="B45" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="45">
+      <c r="D45" s="32">
         <v>5</v>
       </c>
-      <c r="E45" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="G45" s="14">
+      <c r="E45" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G45" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="14">
+      <c r="A46" s="13">
         <v>10.4</v>
       </c>
-      <c r="B46" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="C46" s="45" t="s">
+      <c r="B46" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="45">
+      <c r="D46" s="32">
         <v>5</v>
       </c>
-      <c r="E46" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G46" s="14">
+      <c r="E46" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G46" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="C47" s="45" t="s">
+      <c r="B47" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="45">
+      <c r="D47" s="32">
         <v>30</v>
       </c>
-      <c r="E47" s="14" t="s">
-        <v>95</v>
+      <c r="E47" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="45" t="s">
+      <c r="B48" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="45">
+      <c r="D48" s="32">
         <v>5</v>
       </c>
-      <c r="F48" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="G48" s="14">
+      <c r="F48" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G48" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="49" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
-        <v>154</v>
-      </c>
-      <c r="G49" s="14">
+        <v>145</v>
+      </c>
+      <c r="G49" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="50" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
-        <v>155</v>
-      </c>
-      <c r="G50" s="14">
+        <v>146</v>
+      </c>
+      <c r="G50" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="51" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
-        <v>156</v>
-      </c>
-      <c r="G51" s="14">
+        <v>147</v>
+      </c>
+      <c r="G51" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F80"/>
       <c r="J80"/>
       <c r="K80"/>
       <c r="L80"/>
       <c r="M80"/>
     </row>
-    <row r="81" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F81"/>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81"/>
       <c r="M81"/>
     </row>
-    <row r="82" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F82"/>
       <c r="J82"/>
       <c r="K82"/>
       <c r="L82"/>
       <c r="M82"/>
     </row>
-    <row r="83" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F83"/>
       <c r="J83"/>
       <c r="K83"/>
       <c r="L83"/>
       <c r="M83"/>
     </row>
-    <row r="84" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F84"/>
       <c r="J84"/>
       <c r="K84"/>
       <c r="L84"/>
       <c r="M84"/>
     </row>
-    <row r="85" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F85"/>
       <c r="J85"/>
       <c r="K85"/>
       <c r="L85"/>
       <c r="M85"/>
     </row>
-    <row r="86" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F86"/>
       <c r="G86"/>
       <c r="H86"/>
@@ -3690,14 +3712,14 @@
       <c r="L86"/>
       <c r="M86"/>
     </row>
-    <row r="87" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F87"/>
       <c r="J87"/>
       <c r="K87"/>
       <c r="L87"/>
       <c r="M87"/>
     </row>
-    <row r="88" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F88"/>
       <c r="G88"/>
       <c r="H88"/>
@@ -3706,7 +3728,7 @@
       <c r="L88"/>
       <c r="M88"/>
     </row>
-    <row r="89" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F89"/>
       <c r="G89"/>
       <c r="H89"/>
@@ -3715,7 +3737,7 @@
       <c r="L89"/>
       <c r="M89"/>
     </row>
-    <row r="90" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F90"/>
       <c r="G90"/>
       <c r="H90"/>
@@ -3724,7 +3746,7 @@
       <c r="L90"/>
       <c r="M90"/>
     </row>
-    <row r="91" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F91"/>
       <c r="G91"/>
       <c r="H91"/>
@@ -3733,7 +3755,7 @@
       <c r="L91"/>
       <c r="M91"/>
     </row>
-    <row r="92" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F92"/>
       <c r="G92"/>
       <c r="H92"/>
@@ -3742,7 +3764,7 @@
       <c r="L92"/>
       <c r="M92"/>
     </row>
-    <row r="93" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F93"/>
       <c r="G93"/>
       <c r="H93"/>
@@ -3751,7 +3773,7 @@
       <c r="L93"/>
       <c r="M93"/>
     </row>
-    <row r="94" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F94"/>
       <c r="G94"/>
       <c r="H94"/>
@@ -3760,7 +3782,7 @@
       <c r="L94"/>
       <c r="M94"/>
     </row>
-    <row r="95" spans="6:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F95"/>
       <c r="G95"/>
       <c r="H95"/>

</xml_diff>

<commit_message>
add commas to wk1
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767F577A-CE00-4AFE-AE9E-D18E6AD547ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BF277C-427F-48C3-91AF-79BD4D6300AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="2085" windowWidth="21600" windowHeight="11505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32055" yWindow="1605" windowWidth="24585" windowHeight="11505" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -675,11 +675,6 @@
     <t>Spring Break</t>
   </si>
   <si>
-    <t>Class logistics
-Data preparation review
-Linear Regression</t>
-  </si>
-  <si>
     <t>Stratified models, purpose and limitations. 
 What does it mean for a variable to be a moderator? 
 Interpreting Interactions</t>
@@ -703,6 +698,9 @@
   <si>
     <t>[Syllabus](https://norcalbiostat.github.io/MATH456/syllabus_456_S23.html)  
 [Welcome Slides](notes/cn00-welcome.html)</t>
+  </si>
+  <si>
+    <t>Class logistics , Data preparation &amp; Linear Regression reviews</t>
   </si>
 </sst>
 </file>
@@ -1711,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C3:C5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1756,7 +1754,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E2" s="44" t="s">
         <v>168</v>
@@ -2083,9 +2081,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,13 +2136,13 @@
         <v>43122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>56</v>
@@ -2171,7 +2169,7 @@
         <v>138</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>143</v>
@@ -2180,7 +2178,7 @@
         <v>160</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>173</v>
@@ -2201,7 +2199,7 @@
         <v>140</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>161</v>

</xml_diff>

<commit_message>
add something to todays schedule
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55349E75-92AB-4A5D-9F69-AEC354F56967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC0DFAF-EA0F-4CAB-B867-96E869615E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40965" yWindow="960" windowWidth="21150" windowHeight="15375" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -565,11 +565,6 @@
 Download hw1 assignment template file, knit &amp; review what is being asked of you</t>
   </si>
   <si>
-    <t xml:space="preserve">Jump start - write down everything you know about LinReg. 
-Compare to a neighbor. Share with class. 
-Recap on the purpose of linear regression models, assumptions, interpretation of predictors. </t>
-  </si>
-  <si>
     <t>LJ</t>
   </si>
   <si>
@@ -629,10 +624,6 @@
     <t>Wald test
 Multicollinearity
 Variable Selection</t>
-  </si>
-  <si>
-    <t>Choosing between competing models. 
-Wrap up/ Review</t>
   </si>
   <si>
     <t xml:space="preserve">Group Quiz on Model Building
@@ -701,6 +692,15 @@
   <si>
     <t>Group Quiz on class logistics
 Create a [Data preparation reference flowchart](https://norcalbiostat.github.io/MATH456/hw/data_preparation_flowchart.html)</t>
+  </si>
+  <si>
+    <t>Choosing between competing models. 
+Recap: Write down everything you know about LinReg (LJ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump start - write down everything you know about LinReg. (LJ)
+Work as a class to organize these notes in [this google doc](https://docs.google.com/document/d/1l4HDH0VufxOcUe0JhW4CJhhMd6C7TAavt6P1dy_c-oA) 
+Recap on the purpose of linear regression models, assumptions, interpretation of predictors. </t>
   </si>
 </sst>
 </file>
@@ -1754,10 +1754,10 @@
         <v>24</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F2" s="45" t="s">
         <v>114</v>
@@ -1984,7 +1984,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D17" s="64"/>
       <c r="E17" s="65"/>
@@ -2000,7 +2000,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D18" s="64"/>
       <c r="E18" s="65"/>
@@ -2083,7 +2083,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2128,7 +2128,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="40">
         <v>1</v>
       </c>
@@ -2136,22 +2136,22 @@
         <v>43122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>53</v>
@@ -2169,19 +2169,19 @@
         <v>138</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>142</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>58</v>
@@ -2199,19 +2199,19 @@
         <v>140</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>139</v>
       </c>
       <c r="H4" s="66" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -2229,10 +2229,10 @@
         <v>85</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>86</v>
@@ -2259,7 +2259,7 @@
         <v>72</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>70</v>
@@ -2268,7 +2268,7 @@
         <v>69</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -2287,7 +2287,7 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G7" s="33" t="s">
         <v>34</v>
@@ -2311,7 +2311,7 @@
         <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>68</v>
@@ -2327,7 +2327,7 @@
         <v>43171</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
@@ -2418,7 +2418,7 @@
         <v>43199</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2435,7 +2435,7 @@
         <v>43206</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2451,7 +2451,7 @@
         <v>43213</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2467,7 +2467,7 @@
         <v>43220</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2571,7 +2571,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
@@ -2597,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>11</v>
@@ -2631,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>11</v>
@@ -2665,7 +2665,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>11</v>
@@ -2699,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>11</v>
@@ -2782,7 +2782,7 @@
     </row>
     <row r="9" spans="1:13" s="13" customFormat="1" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B9" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -2802,7 +2802,7 @@
     </row>
     <row r="11" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
@@ -2858,7 +2858,7 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
@@ -2880,7 +2880,7 @@
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="17" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>7</v>
@@ -2909,7 +2909,7 @@
     </row>
     <row r="18" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>11</v>
@@ -2949,7 +2949,7 @@
     </row>
     <row r="20" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C20" s="29" t="s">
         <v>12</v>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="21" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C21" s="29" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
add idx and qft insructions
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC0DFAF-EA0F-4CAB-B867-96E869615E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCC93E2-A267-4707-9443-B841F0C92E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -507,9 +507,6 @@
 ASCN Ch 1</t>
   </si>
   <si>
-    <t>ASCN Ch 8</t>
-  </si>
-  <si>
     <t>Review of Linear Regression</t>
   </si>
   <si>
@@ -561,10 +558,6 @@
     <t>Review Week</t>
   </si>
   <si>
-    <t>Read ASCN Ch 8  
-Download hw1 assignment template file, knit &amp; review what is being asked of you</t>
-  </si>
-  <si>
     <t>LJ</t>
   </si>
   <si>
@@ -608,11 +601,6 @@
   </si>
   <si>
     <t>will contain these items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Peer Review
-QFT: Model Building &amp; Variable Selection
-What does it mean for a variable to be a confounder? </t>
   </si>
   <si>
     <t>PMA6 CH9, ASCN 10</t>
@@ -662,11 +650,6 @@
     <t>Spring Break</t>
   </si>
   <si>
-    <t>Stratified models, purpose and limitations. 
-What does it mean for a variable to be a moderator? 
-Interpreting Interactions</t>
-  </si>
-  <si>
     <t>Perform various variable selection techniques
 Identify pros and cons for each method</t>
   </si>
@@ -701,6 +684,22 @@
     <t xml:space="preserve">Jump start - write down everything you know about LinReg. (LJ)
 Work as a class to organize these notes in [this google doc](https://docs.google.com/document/d/1l4HDH0VufxOcUe0JhW4CJhhMd6C7TAavt6P1dy_c-oA) 
 Recap on the purpose of linear regression models, assumptions, interpretation of predictors. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Peer Review
+QFT: Model Building &amp; Variable Selection
+What does it mean for a variable to be a confounder or moderator? </t>
+  </si>
+  <si>
+    <t>Stratified models, purpose and limitations. 
+Interpreting Interactions</t>
+  </si>
+  <si>
+    <t>Read ASCN Ch 9.6, Ch 8  
+Download hw1 assignment template file, knit &amp; review what is being asked of you</t>
+  </si>
+  <si>
+    <t>ASCN Ch 8, Ch 9.6</t>
   </si>
 </sst>
 </file>
@@ -1709,8 +1708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1754,10 +1753,10 @@
         <v>24</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F2" s="45" t="s">
         <v>114</v>
@@ -1779,10 +1778,10 @@
         <v>1.3</v>
       </c>
       <c r="C4" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="D4" s="46" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1793,10 +1792,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>125</v>
+        <v>180</v>
       </c>
       <c r="E5" s="44"/>
       <c r="F5" s="45" t="s">
@@ -1808,10 +1807,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D6" s="56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E6" s="44"/>
       <c r="F6" s="15" t="s">
@@ -1829,7 +1828,7 @@
         <v>117</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E7" s="44"/>
     </row>
@@ -1841,7 +1840,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F8" s="15"/>
     </row>
@@ -1856,11 +1855,11 @@
         <v>122</v>
       </c>
       <c r="D9" s="56" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1894,7 +1893,7 @@
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1955,7 +1954,7 @@
         <v>93</v>
       </c>
       <c r="F15" s="57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1984,7 +1983,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D17" s="64"/>
       <c r="E17" s="65"/>
@@ -2000,7 +1999,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D18" s="64"/>
       <c r="E18" s="65"/>
@@ -2045,7 +2044,7 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D21" s="58"/>
       <c r="F21" s="65"/>
@@ -2081,9 +2080,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2136,22 +2135,22 @@
         <v>43122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>53</v>
@@ -2166,22 +2165,22 @@
         <v>43129</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>58</v>
@@ -2196,22 +2195,22 @@
         <v>43136</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H4" s="66" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -2229,10 +2228,10 @@
         <v>85</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>86</v>
@@ -2259,7 +2258,7 @@
         <v>72</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>70</v>
@@ -2268,7 +2267,7 @@
         <v>69</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -2287,7 +2286,7 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="33" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G7" s="33" t="s">
         <v>34</v>
@@ -2311,7 +2310,7 @@
         <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>68</v>
@@ -2327,7 +2326,7 @@
         <v>43171</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
@@ -2418,7 +2417,7 @@
         <v>43199</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2435,7 +2434,7 @@
         <v>43206</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2451,7 +2450,7 @@
         <v>43213</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2467,7 +2466,7 @@
         <v>43220</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2484,7 +2483,7 @@
         <v>43227</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2571,7 +2570,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
@@ -2597,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>11</v>
@@ -2631,7 +2630,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>11</v>
@@ -2665,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>11</v>
@@ -2699,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>11</v>
@@ -2782,7 +2781,7 @@
     </row>
     <row r="9" spans="1:13" s="13" customFormat="1" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B9" s="42" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
@@ -2791,7 +2790,7 @@
     </row>
     <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -2802,7 +2801,7 @@
     </row>
     <row r="11" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
@@ -2858,7 +2857,7 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
@@ -2880,7 +2879,7 @@
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -2889,7 +2888,7 @@
     </row>
     <row r="17" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>7</v>
@@ -2909,7 +2908,7 @@
     </row>
     <row r="18" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>11</v>
@@ -2949,7 +2948,7 @@
     </row>
     <row r="20" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C20" s="29" t="s">
         <v>12</v>
@@ -2966,7 +2965,7 @@
     </row>
     <row r="21" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C21" s="29" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
fix LJ check in dates
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCC93E2-A267-4707-9443-B841F0C92E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950854EA-EB4A-47C0-A637-7BFC833111F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="181">
   <si>
     <t>Finals Week</t>
   </si>
@@ -1709,20 +1709,20 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.8984375" style="52"/>
+    <col min="1" max="2" width="8.875" style="52"/>
     <col min="3" max="3" width="40" style="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" style="52" customWidth="1"/>
-    <col min="5" max="5" width="44.69921875" style="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.75" style="55" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55" style="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.8984375" style="54"/>
+    <col min="7" max="16384" width="8.875" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="52" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="52" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
         <v>22</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A2" s="53">
         <v>1.1000000000000001</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="53">
         <v>1.2</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="53">
         <v>1.3</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="53">
         <v>2.1</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="53">
         <v>2.2000000000000002</v>
       </c>
@@ -1813,11 +1813,9 @@
         <v>132</v>
       </c>
       <c r="E6" s="44"/>
-      <c r="F6" s="15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>3.1</v>
       </c>
@@ -1831,8 +1829,11 @@
         <v>129</v>
       </c>
       <c r="E7" s="44"/>
-    </row>
-    <row r="8" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="F7" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="53">
         <v>3.2</v>
       </c>
@@ -1844,7 +1845,7 @@
       </c>
       <c r="F8" s="15"/>
     </row>
-    <row r="9" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="53">
         <v>4.0999999999999996</v>
       </c>
@@ -1862,7 +1863,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="53">
         <v>5.0999999999999996</v>
       </c>
@@ -1876,9 +1877,11 @@
         <v>87</v>
       </c>
       <c r="E10" s="19"/>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="F10" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="53">
         <v>6.1</v>
       </c>
@@ -1896,7 +1899,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53">
         <v>7</v>
       </c>
@@ -1911,7 +1914,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="53">
         <v>8</v>
       </c>
@@ -1925,7 +1928,7 @@
       <c r="E13" s="63"/>
       <c r="F13" s="61"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="53">
         <v>9.1</v>
       </c>
@@ -1940,7 +1943,7 @@
       </c>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="53">
         <v>10.1</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="53">
         <v>11.1</v>
       </c>
@@ -1975,7 +1978,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="53">
         <v>12.1</v>
       </c>
@@ -1991,7 +1994,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="53">
         <v>13.1</v>
       </c>
@@ -2007,7 +2010,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="53">
         <v>14.1</v>
       </c>
@@ -2021,7 +2024,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="53">
         <v>15.1</v>
       </c>
@@ -2036,7 +2039,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="53">
         <v>16.100000000000001</v>
       </c>
@@ -2049,7 +2052,7 @@
       <c r="D21" s="58"/>
       <c r="F21" s="65"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="53">
         <v>18.100000000000001</v>
       </c>
@@ -2064,7 +2067,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E26" s="65"/>
     </row>
   </sheetData>
@@ -2085,20 +2088,20 @@
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.09765625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.8984375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.875" style="6" customWidth="1"/>
     <col min="4" max="4" width="36.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="45.8984375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="34.59765625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="45.875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="34.625" style="7" customWidth="1"/>
     <col min="7" max="8" width="38" style="7" customWidth="1"/>
-    <col min="9" max="9" width="35.8984375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="14.8984375" style="6"/>
+    <col min="9" max="9" width="35.875" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="14.875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="40">
         <v>1</v>
       </c>
@@ -2156,7 +2159,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -2186,7 +2189,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -2213,7 +2216,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -2243,7 +2246,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -2270,7 +2273,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -2298,7 +2301,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -2319,7 +2322,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="10">
         <f t="shared" si="0"/>
@@ -2347,7 +2350,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -2370,7 +2373,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -2389,7 +2392,7 @@
       <c r="G11" s="33"/>
       <c r="H11" s="33"/>
     </row>
-    <row r="12" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -2408,7 +2411,7 @@
       <c r="G12" s="33"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -2425,7 +2428,7 @@
       <c r="G13" s="33"/>
       <c r="H13" s="33"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -2441,7 +2444,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -2457,7 +2460,7 @@
       <c r="F15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -2474,7 +2477,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -2491,7 +2494,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>0</v>
       </c>
@@ -2508,10 +2511,10 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G21" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="33"/>
@@ -2520,7 +2523,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -2542,21 +2545,21 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" style="13"/>
+    <col min="1" max="1" width="8.875" style="13"/>
     <col min="2" max="2" width="35" style="13" customWidth="1"/>
-    <col min="3" max="3" width="11.09765625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="6.3984375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="6.375" style="13" customWidth="1"/>
     <col min="5" max="5" width="6" style="13" customWidth="1"/>
-    <col min="6" max="6" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="13" customWidth="1"/>
-    <col min="8" max="8" width="8.8984375" style="13"/>
-    <col min="9" max="9" width="4.59765625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="13"/>
+    <col min="9" max="9" width="4.625" style="13" customWidth="1"/>
+    <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>20</v>
       </c>
@@ -2591,7 +2594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>0</v>
       </c>
@@ -2625,7 +2628,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>0</v>
       </c>
@@ -2659,7 +2662,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>0</v>
       </c>
@@ -2693,7 +2696,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>0</v>
       </c>
@@ -2727,7 +2730,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>0.1</v>
       </c>
@@ -2746,7 +2749,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.2</v>
       </c>
@@ -2764,7 +2767,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.3</v>
       </c>
@@ -2779,7 +2782,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:13" s="13" customFormat="1" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" s="13" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" s="42" t="s">
         <v>146</v>
       </c>
@@ -2788,7 +2791,7 @@
       <c r="L9"/>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="42" t="s">
         <v>149</v>
       </c>
@@ -2799,7 +2802,7 @@
       <c r="L10"/>
       <c r="M10"/>
     </row>
-    <row r="11" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="42" t="s">
         <v>150</v>
       </c>
@@ -2810,7 +2813,7 @@
       <c r="L11"/>
       <c r="M11"/>
     </row>
-    <row r="12" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="42" t="s">
         <v>97</v>
       </c>
@@ -2821,7 +2824,7 @@
       <c r="L12"/>
       <c r="M12"/>
     </row>
-    <row r="13" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="42" t="s">
         <v>99</v>
       </c>
@@ -2831,7 +2834,7 @@
       <c r="L13"/>
       <c r="M13"/>
     </row>
-    <row r="14" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="42" t="s">
         <v>118</v>
       </c>
@@ -2842,7 +2845,7 @@
       <c r="L14"/>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
         <v>96</v>
       </c>
@@ -2864,7 +2867,7 @@
       <c r="L15"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
         <v>98</v>
       </c>
@@ -2886,7 +2889,7 @@
       <c r="L16"/>
       <c r="M16"/>
     </row>
-    <row r="17" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
         <v>148</v>
       </c>
@@ -2906,7 +2909,7 @@
       <c r="L17"/>
       <c r="M17"/>
     </row>
-    <row r="18" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
         <v>147</v>
       </c>
@@ -2926,7 +2929,7 @@
       <c r="L18"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>19</v>
       </c>
@@ -2946,7 +2949,7 @@
       <c r="L19"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>152</v>
       </c>
@@ -2963,7 +2966,7 @@
       <c r="L20"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
         <v>153</v>
       </c>
@@ -2979,56 +2982,56 @@
       <c r="L21"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F22"/>
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
     </row>
-    <row r="50" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F50"/>
       <c r="J50"/>
       <c r="K50"/>
       <c r="L50"/>
       <c r="M50"/>
     </row>
-    <row r="51" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F51"/>
       <c r="J51"/>
       <c r="K51"/>
       <c r="L51"/>
       <c r="M51"/>
     </row>
-    <row r="52" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F52"/>
       <c r="J52"/>
       <c r="K52"/>
       <c r="L52"/>
       <c r="M52"/>
     </row>
-    <row r="53" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F53"/>
       <c r="J53"/>
       <c r="K53"/>
       <c r="L53"/>
       <c r="M53"/>
     </row>
-    <row r="54" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F54"/>
       <c r="J54"/>
       <c r="K54"/>
       <c r="L54"/>
       <c r="M54"/>
     </row>
-    <row r="55" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F55"/>
       <c r="J55"/>
       <c r="K55"/>
       <c r="L55"/>
       <c r="M55"/>
     </row>
-    <row r="56" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F56"/>
       <c r="G56"/>
       <c r="H56"/>
@@ -3037,14 +3040,14 @@
       <c r="L56"/>
       <c r="M56"/>
     </row>
-    <row r="57" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F57"/>
       <c r="J57"/>
       <c r="K57"/>
       <c r="L57"/>
       <c r="M57"/>
     </row>
-    <row r="58" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F58"/>
       <c r="G58"/>
       <c r="H58"/>
@@ -3053,7 +3056,7 @@
       <c r="L58"/>
       <c r="M58"/>
     </row>
-    <row r="59" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F59"/>
       <c r="G59"/>
       <c r="H59"/>
@@ -3062,7 +3065,7 @@
       <c r="L59"/>
       <c r="M59"/>
     </row>
-    <row r="60" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F60"/>
       <c r="G60"/>
       <c r="H60"/>
@@ -3071,7 +3074,7 @@
       <c r="L60"/>
       <c r="M60"/>
     </row>
-    <row r="61" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F61"/>
       <c r="G61"/>
       <c r="H61"/>
@@ -3080,7 +3083,7 @@
       <c r="L61"/>
       <c r="M61"/>
     </row>
-    <row r="62" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F62"/>
       <c r="G62"/>
       <c r="H62"/>
@@ -3089,7 +3092,7 @@
       <c r="L62"/>
       <c r="M62"/>
     </row>
-    <row r="63" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F63"/>
       <c r="G63"/>
       <c r="H63"/>
@@ -3098,7 +3101,7 @@
       <c r="L63"/>
       <c r="M63"/>
     </row>
-    <row r="64" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F64"/>
       <c r="G64"/>
       <c r="H64"/>
@@ -3107,7 +3110,7 @@
       <c r="L64"/>
       <c r="M64"/>
     </row>
-    <row r="65" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F65"/>
       <c r="G65"/>
       <c r="H65"/>
@@ -3134,21 +3137,21 @@
       <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.09765625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.8984375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.875" style="6" customWidth="1"/>
     <col min="4" max="4" width="36.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="38.3984375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="34.59765625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="38.375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="34.625" style="7" customWidth="1"/>
     <col min="7" max="8" width="38" style="7" customWidth="1"/>
-    <col min="9" max="9" width="35.8984375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="24.59765625" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="14.8984375" style="6"/>
+    <col min="9" max="9" width="35.875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="24.625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="14.875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -3180,7 +3183,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="41">
         <v>1</v>
       </c>
@@ -3210,7 +3213,7 @@
       </c>
       <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="41">
         <v>2</v>
       </c>
@@ -3241,7 +3244,7 @@
       </c>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="41">
         <v>3</v>
       </c>
@@ -3268,7 +3271,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="41">
         <v>4</v>
       </c>
@@ -3298,7 +3301,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="106.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="41">
         <v>5</v>
       </c>
@@ -3325,7 +3328,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="40">
         <v>6</v>
       </c>
@@ -3356,7 +3359,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
         <v>7</v>
       </c>
@@ -3381,7 +3384,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -3402,7 +3405,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="10">
         <f t="shared" si="0"/>
@@ -3427,7 +3430,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -3448,7 +3451,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -3475,7 +3478,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -3502,7 +3505,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="66" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -3524,7 +3527,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -3539,7 +3542,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -3561,7 +3564,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -3576,7 +3579,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>0</v>
       </c>
@@ -3591,10 +3594,10 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G21" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="33"/>
@@ -3603,7 +3606,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>

</xml_diff>

<commit_message>
update schedule and add links to hw01
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D48A108-7BB9-4553-A3D8-B8A253595FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84BDB9A-CF64-498D-A54D-A038B84DCAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="182">
   <si>
     <t>Finals Week</t>
   </si>
@@ -473,12 +473,6 @@
 LJ Check in</t>
   </si>
   <si>
-    <t>[[HW 00: Getting Started]](hw/hw00-getting-started.html)</t>
-  </si>
-  <si>
-    <t>[[HW 01: Statistical Modeling]](hw/hw01-model-building.html)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Midterm </t>
   </si>
   <si>
@@ -623,9 +617,6 @@
 </t>
   </si>
   <si>
-    <t>[[Quiz 00]](https://forms.gle/mizdZk4qw8QC5NXT8)</t>
-  </si>
-  <si>
     <t>Correlated Outcomes</t>
   </si>
   <si>
@@ -698,6 +689,18 @@
   <si>
     <t>Multicollinearity
 Variable Selection</t>
+  </si>
+  <si>
+    <t>[Quiz 01](https://forms.gle/97UtRU9bnxswoKzWA)</t>
+  </si>
+  <si>
+    <t>[Quiz 00](https://forms.gle/mizdZk4qw8QC5NXT8)</t>
+  </si>
+  <si>
+    <t>[HW 00: Getting Started](hw/hw00-getting-started.html)</t>
+  </si>
+  <si>
+    <t>[HW 01: Statistical Modeling](hw/hw01-model-building.html)</t>
   </si>
 </sst>
 </file>
@@ -1706,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1751,13 +1754,13 @@
         <v>24</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -1768,7 +1771,7 @@
         <v>48</v>
       </c>
       <c r="D3" s="46" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1776,10 +1779,10 @@
         <v>1.3</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1790,14 +1793,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D5" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="E5" s="44"/>
       <c r="F5" s="45" t="s">
-        <v>115</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1805,10 +1810,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C6" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="56" t="s">
         <v>130</v>
-      </c>
-      <c r="D6" s="56" t="s">
-        <v>132</v>
       </c>
       <c r="E6" s="44"/>
       <c r="F6" s="15"/>
@@ -1821,14 +1826,14 @@
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E7" s="44"/>
       <c r="F7" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -1839,7 +1844,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F8" s="15"/>
     </row>
@@ -1851,14 +1856,14 @@
         <v>4</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D9" s="56" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="57" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1876,7 +1881,7 @@
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.25">
@@ -1894,7 +1899,7 @@
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="57" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1905,7 +1910,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="57" t="s">
@@ -1955,7 +1960,7 @@
         <v>93</v>
       </c>
       <c r="F15" s="57" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1973,7 +1978,7 @@
       </c>
       <c r="E16" s="65"/>
       <c r="F16" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1984,12 +1989,12 @@
         <v>11</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D17" s="64"/>
       <c r="E17" s="65"/>
       <c r="F17" s="57" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2000,12 +2005,12 @@
         <v>12</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D18" s="64"/>
       <c r="E18" s="65"/>
       <c r="F18" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2016,10 +2021,10 @@
         <v>13</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F19" s="65" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2030,11 +2035,11 @@
         <v>14</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D20" s="58"/>
       <c r="F20" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2045,7 +2050,7 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D21" s="58"/>
       <c r="F21" s="65"/>
@@ -2058,11 +2063,11 @@
         <v>90</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E22" s="52"/>
       <c r="F22" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2081,7 +2086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
@@ -2136,22 +2141,22 @@
         <v>43122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>53</v>
@@ -2166,22 +2171,22 @@
         <v>43129</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>58</v>
@@ -2196,22 +2201,22 @@
         <v>43136</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G4" s="67" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I4" s="7"/>
     </row>
@@ -2224,16 +2229,16 @@
         <v>43143</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D5" s="35" t="s">
         <v>85</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>86</v>
@@ -2260,7 +2265,7 @@
         <v>72</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>70</v>
@@ -2269,7 +2274,7 @@
         <v>69</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -2288,7 +2293,7 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="33" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G7" s="33" t="s">
         <v>34</v>
@@ -2312,7 +2317,7 @@
         <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>68</v>
@@ -2328,7 +2333,7 @@
         <v>43171</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
@@ -2419,7 +2424,7 @@
         <v>43199</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2436,7 +2441,7 @@
         <v>43206</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2452,7 +2457,7 @@
         <v>43213</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2468,7 +2473,7 @@
         <v>43220</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2485,7 +2490,7 @@
         <v>43227</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2572,7 +2577,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
@@ -2598,7 +2603,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>11</v>
@@ -2632,7 +2637,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>11</v>
@@ -2666,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>11</v>
@@ -2700,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>11</v>
@@ -2783,7 +2788,7 @@
     </row>
     <row r="9" spans="1:13" s="13" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
@@ -2792,7 +2797,7 @@
     </row>
     <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="42" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -2803,7 +2808,7 @@
     </row>
     <row r="11" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="42" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
@@ -2835,7 +2840,7 @@
     </row>
     <row r="14" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="42" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -2859,7 +2864,7 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
@@ -2881,7 +2886,7 @@
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -2890,7 +2895,7 @@
     </row>
     <row r="17" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>7</v>
@@ -2910,7 +2915,7 @@
     </row>
     <row r="18" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>11</v>
@@ -2950,7 +2955,7 @@
     </row>
     <row r="20" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C20" s="29" t="s">
         <v>12</v>
@@ -2967,7 +2972,7 @@
     </row>
     <row r="21" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C21" s="29" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
update midterm week schedule
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBCCC4F-BFD7-45C0-92F9-C5ECE818C916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED56F762-659A-45BE-B3A4-9015EC09A4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="188">
   <si>
     <t>Finals Week</t>
   </si>
@@ -608,12 +608,6 @@
     <t>Wrap up / reivew</t>
   </si>
   <si>
-    <t xml:space="preserve">Group quiz on Logistic Regression &amp; Classification  
-QFT on Missing Data  
-Effects of non-response
-</t>
-  </si>
-  <si>
     <t>Correlated Outcomes</t>
   </si>
   <si>
@@ -622,9 +616,6 @@
   <si>
     <t>Read ASSN Ch 12  
 Install packages: caret, ROCR</t>
-  </si>
-  <si>
-    <t>Open work day</t>
   </si>
   <si>
     <t>No Class</t>
@@ -707,6 +698,32 @@
   </si>
   <si>
     <t>[Quiz 02](https://forms.gle/fm2XE19fZixwSGnZ9)</t>
+  </si>
+  <si>
+    <t>Explain the effects of missing data. 
+List and define the different missing data mechanisms. 
+Explain the typical methods of handling missing data and the problems with each.
+Explain the mathematical model behind two imputation methods</t>
+  </si>
+  <si>
+    <t>Group quiz on Logistic Regression &amp; Classification  
+QFT on Missing Data  
+Effects of non-response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple imputation is the gold standard of how to analyze data with missing values.
+We'll explore how this algorithm works with some sample data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open work day. Get caught up with late or resubmitted homework. </t>
+  </si>
+  <si>
+    <t>Midterm  (MLR, Variable Selection, LogReg, Classification &amp; Prediction)</t>
+  </si>
+  <si>
+    <t>Review all prior materials. Homework, quizzes, discussion boards, QFT.  
+Draft a 1 page set of notes for each of the 4 topics covered so far. 
+Write 1 serious exam question (don't cheese this)</t>
   </si>
 </sst>
 </file>
@@ -1715,7 +1732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1760,13 +1777,13 @@
         <v>24</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -1802,13 +1819,13 @@
         <v>129</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1838,7 +1855,7 @@
         <v>127</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>121</v>
@@ -1871,7 +1888,7 @@
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="45" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2094,9 +2111,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,22 +2166,22 @@
         <v>43122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>53</v>
@@ -2182,19 +2199,19 @@
         <v>134</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>58</v>
@@ -2212,16 +2229,16 @@
         <v>136</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>153</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G4" s="67" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>135</v>
@@ -2273,7 +2290,7 @@
         <v>72</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>70</v>
@@ -2285,7 +2302,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -2297,23 +2314,23 @@
         <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>65</v>
+        <v>182</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="33" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="G7" s="33" t="s">
         <v>34</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>64</v>
+        <v>184</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -2324,14 +2341,17 @@
       <c r="C8" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>21</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2341,7 +2361,7 @@
         <v>43171</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
@@ -2432,7 +2452,7 @@
         <v>43199</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2449,7 +2469,7 @@
         <v>43206</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2465,7 +2485,7 @@
         <v>43213</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2481,7 +2501,7 @@
         <v>43220</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2799,7 +2819,7 @@
         <v>0.4</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
rebuild schedule to add MI demo page
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED56F762-659A-45BE-B3A4-9015EC09A4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B630B5C-8C82-4833-99DC-17EA97A69D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="188">
   <si>
     <t>Finals Week</t>
   </si>
@@ -715,15 +715,15 @@
 We'll explore how this algorithm works with some sample data. </t>
   </si>
   <si>
-    <t xml:space="preserve">Open work day. Get caught up with late or resubmitted homework. </t>
-  </si>
-  <si>
     <t>Midterm  (MLR, Variable Selection, LogReg, Classification &amp; Prediction)</t>
   </si>
   <si>
     <t>Review all prior materials. Homework, quizzes, discussion boards, QFT.  
 Draft a 1 page set of notes for each of the 4 topics covered so far. 
 Write 1 serious exam question (don't cheese this)</t>
+  </si>
+  <si>
+    <t>[Multiple Imputation Demo](notes/MI_demo.html)</t>
   </si>
 </sst>
 </file>
@@ -1732,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1937,6 +1937,9 @@
       <c r="C12" s="54" t="s">
         <v>114</v>
       </c>
+      <c r="D12" s="52" t="s">
+        <v>187</v>
+      </c>
       <c r="E12" s="19"/>
       <c r="F12" s="57" t="s">
         <v>113</v>
@@ -2111,9 +2114,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,16 +2345,16 @@
         <v>21</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add hw03 to use mi demo as part 1
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B630B5C-8C82-4833-99DC-17EA97A69D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F9CB0A-D97B-4D4A-89E2-117D30E9E2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,9 +534,6 @@
     <t>HW04</t>
   </si>
   <si>
-    <t>HW 03</t>
-  </si>
-  <si>
     <t>Stratification, Moderation &amp; Interaction Terms</t>
   </si>
   <si>
@@ -724,6 +721,9 @@
   </si>
   <si>
     <t>[Multiple Imputation Demo](notes/MI_demo.html)</t>
+  </si>
+  <si>
+    <t>[HW 03: Missing Data](hw/hw03-missing-data.html)</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1126,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1308,6 +1308,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -1777,13 +1783,13 @@
         <v>24</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E2" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="45" t="s">
         <v>176</v>
-      </c>
-      <c r="F2" s="45" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -1819,13 +1825,13 @@
         <v>129</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1855,7 +1861,7 @@
         <v>127</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>121</v>
@@ -1888,7 +1894,7 @@
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1923,8 +1929,8 @@
         <v>92</v>
       </c>
       <c r="E11" s="19"/>
-      <c r="F11" s="57" t="s">
-        <v>133</v>
+      <c r="F11" s="68" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1937,8 +1943,8 @@
       <c r="C12" s="54" t="s">
         <v>114</v>
       </c>
-      <c r="D12" s="52" t="s">
-        <v>187</v>
+      <c r="D12" s="69" t="s">
+        <v>186</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="57" t="s">
@@ -2017,7 +2023,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D17" s="64"/>
       <c r="E17" s="65"/>
@@ -2033,7 +2039,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D18" s="64"/>
       <c r="E18" s="65"/>
@@ -2169,22 +2175,22 @@
         <v>43122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>53</v>
@@ -2199,22 +2205,22 @@
         <v>43129</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="H3" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>58</v>
@@ -2229,22 +2235,22 @@
         <v>43136</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G4" s="67" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I4" s="7"/>
     </row>
@@ -2263,10 +2269,10 @@
         <v>85</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>86</v>
@@ -2293,7 +2299,7 @@
         <v>72</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>70</v>
@@ -2302,7 +2308,7 @@
         <v>69</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -2317,17 +2323,17 @@
         <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G7" s="33" t="s">
         <v>34</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>61</v>
@@ -2345,16 +2351,16 @@
         <v>21</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2364,7 +2370,7 @@
         <v>43171</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
@@ -2455,7 +2461,7 @@
         <v>43199</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2472,7 +2478,7 @@
         <v>43206</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2488,7 +2494,7 @@
         <v>43213</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2504,7 +2510,7 @@
         <v>43220</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2521,7 +2527,7 @@
         <v>43227</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2608,7 +2614,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
@@ -2634,7 +2640,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>11</v>
@@ -2668,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>11</v>
@@ -2702,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>11</v>
@@ -2736,7 +2742,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>11</v>
@@ -2822,7 +2828,7 @@
         <v>0.4</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>7</v>
@@ -2837,7 +2843,7 @@
     </row>
     <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -2848,7 +2854,7 @@
     </row>
     <row r="11" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
@@ -2859,7 +2865,7 @@
     </row>
     <row r="12" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
@@ -2897,7 +2903,7 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
@@ -2919,7 +2925,7 @@
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -2948,7 +2954,7 @@
     </row>
     <row r="18" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>7</v>
@@ -2968,7 +2974,7 @@
     </row>
     <row r="19" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>11</v>
@@ -3006,7 +3012,7 @@
     </row>
     <row r="21" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" s="29" t="s">
         <v>12</v>
@@ -3022,7 +3028,7 @@
     </row>
     <row r="22" spans="2:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C22" s="29" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
finish wk 9 and 10 schedule and PCA hw
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894D4B61-8067-47E2-AC1A-38EF5D85A451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5067E5-3602-4A76-ABCF-F74CE706ACD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31545" yWindow="840" windowWidth="21600" windowHeight="13245" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32985" yWindow="2415" windowWidth="21600" windowHeight="13245" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="206">
   <si>
     <t>Finals Week</t>
   </si>
@@ -750,6 +750,42 @@
   </si>
   <si>
     <t>[HW04: Dimension Reduction](hw/hw04-dimension-reduction.html)</t>
+  </si>
+  <si>
+    <t>Create a latent factor model, visualize and interpret results. 
+Use latent factors as a predictor in another model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how PCA can be used as a dimension reduction technique
+Explain the difference between multivariate and multivariable
+Conduct a PCA using both the correlation and covariance matrix
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use visualization techniques to identify the number of PC's to retain
+Explain the difference between PCA and FA
+Create a latent factor model, visualize and interpret results. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizing and interpreting PC's </t>
+  </si>
+  <si>
+    <t>Introduction to Factor Analysis</t>
+  </si>
+  <si>
+    <t>Read ASCN 15.1-15.3, and PMA6 15.1-15.4</t>
+  </si>
+  <si>
+    <t>Read ASCM 15.4-end, PMA6 15.5-end</t>
+  </si>
+  <si>
+    <t>Factor extraction &amp; scores</t>
+  </si>
+  <si>
+    <t>Factor rotation</t>
+  </si>
+  <si>
+    <t>Quiz. Open work day</t>
   </si>
 </sst>
 </file>
@@ -1764,7 +1800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2153,9 +2189,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,7 +2487,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -2463,7 +2499,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>197</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>190</v>
@@ -2490,14 +2526,22 @@
         <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -2508,11 +2552,21 @@
       <c r="C13" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
+      <c r="D13" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="H13" s="33" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="9">

</xml_diff>

<commit_message>
add quiz 5 and another lj entry
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5067E5-3602-4A76-ABCF-F74CE706ACD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81D7D6F-6A12-4747-A9AB-52B6E861762F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32985" yWindow="2415" windowWidth="21600" windowHeight="13245" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="207">
   <si>
     <t>Finals Week</t>
   </si>
@@ -786,6 +786,9 @@
   </si>
   <si>
     <t>Quiz. Open work day</t>
+  </si>
+  <si>
+    <t>[Quiz 05](https://forms.gle/eHcpdtMPkRe3VXqA6)</t>
   </si>
 </sst>
 </file>
@@ -1800,8 +1803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D35601F-CA8F-4470-84B2-2D8121AF57BF}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2062,6 +2065,9 @@
       <c r="D15" s="64" t="s">
         <v>91</v>
       </c>
+      <c r="E15" s="44" t="s">
+        <v>206</v>
+      </c>
       <c r="F15" s="68" t="s">
         <v>195</v>
       </c>
@@ -2079,7 +2085,7 @@
       <c r="D16" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="65"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="15" t="s">
         <v>118</v>
       </c>
@@ -2095,7 +2101,7 @@
         <v>193</v>
       </c>
       <c r="D17" s="64"/>
-      <c r="E17" s="65"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="57" t="s">
         <v>115</v>
       </c>
@@ -2189,9 +2195,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add marginal effects notes
</commit_message>
<xml_diff>
--- a/schedule_456.xlsx
+++ b/schedule_456.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH456\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26AD270-2F82-40BA-BB0C-7DD92130D3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB293105-938A-49E6-B3ED-0D85E8B515C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="213">
   <si>
     <t>Finals Week</t>
   </si>
@@ -805,6 +805,9 @@
   </si>
   <si>
     <t>HW 06</t>
+  </si>
+  <si>
+    <t>[Marginal Effects](https://norcalbiostat.github.io/MATH456/notes/arginal_effects.html)</t>
   </si>
 </sst>
 </file>
@@ -2164,7 +2167,9 @@
       <c r="C20" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="D20" s="58"/>
+      <c r="D20" s="69" t="s">
+        <v>212</v>
+      </c>
       <c r="F20" s="15"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>